<commit_message>
Property pages working 10-03-2025 added Church added total offerings, lettings and frontsheet all working
</commit_message>
<xml_diff>
--- a/data/Church-receipts-and-payments-2025.xlsx
+++ b/data/Church-receipts-and-payments-2025.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1020" yWindow="1530" windowWidth="23775" windowHeight="13920" tabRatio="776" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-28920" yWindow="-840" windowWidth="29040" windowHeight="15720" tabRatio="776" firstSheet="0" activeTab="5" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="P1 Front page" sheetId="1" state="visible" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="1">'P2 R &amp; P page'!$C$2:$N$41</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'P3 Summ of Orgs'!$C$2:$U$49</definedName>
   </definedNames>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
@@ -806,7 +806,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="326">
+  <cellXfs count="328">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -1330,12 +1330,87 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="46" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="39" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="37" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -1357,85 +1432,38 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0" hidden="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection locked="0" hidden="0"/>
-    </xf>
     <xf numFmtId="167" fontId="22" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="37" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="39" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="45" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
       <protection locked="0" hidden="0"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="43" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -1449,37 +1477,30 @@
     <xf numFmtId="164" fontId="16" fillId="0" borderId="44" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="42" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="16" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="45" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0" hidden="0"/>
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="43" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -1502,32 +1523,17 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="43" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="167" fontId="22" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -2390,164 +2396,164 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
   <cols>
-    <col width="1" customWidth="1" style="248" min="1" max="1"/>
-    <col width="0.42578125" customWidth="1" style="248" min="2" max="2"/>
-    <col width="3.140625" customWidth="1" style="248" min="3" max="3"/>
-    <col width="3.42578125" customWidth="1" style="248" min="4" max="6"/>
-    <col width="30.140625" customWidth="1" style="248" min="7" max="7"/>
-    <col width="0.42578125" customWidth="1" style="248" min="8" max="8"/>
-    <col width="11.42578125" customWidth="1" style="248" min="9" max="9"/>
-    <col width="20" customWidth="1" style="248" min="10" max="10"/>
-    <col width="8.42578125" customWidth="1" style="248" min="11" max="11"/>
-    <col width="11.140625" customWidth="1" style="248" min="12" max="12"/>
-    <col width="2.42578125" customWidth="1" style="248" min="13" max="13"/>
-    <col width="0.85546875" customWidth="1" style="248" min="14" max="14"/>
+    <col width="1" customWidth="1" style="264" min="1" max="1"/>
+    <col width="0.42578125" customWidth="1" style="264" min="2" max="2"/>
+    <col width="3.140625" customWidth="1" style="264" min="3" max="3"/>
+    <col width="3.42578125" customWidth="1" style="264" min="4" max="6"/>
+    <col width="30.140625" customWidth="1" style="264" min="7" max="7"/>
+    <col width="0.42578125" customWidth="1" style="264" min="8" max="8"/>
+    <col width="11.42578125" customWidth="1" style="264" min="9" max="9"/>
+    <col width="20" customWidth="1" style="264" min="10" max="10"/>
+    <col width="8.42578125" customWidth="1" style="264" min="11" max="11"/>
+    <col width="11.140625" customWidth="1" style="264" min="12" max="12"/>
+    <col width="2.42578125" customWidth="1" style="264" min="13" max="13"/>
+    <col width="0.85546875" customWidth="1" style="264" min="14" max="14"/>
   </cols>
   <sheetData>
-    <row r="1" ht="6" customHeight="1" s="248">
-      <c r="B1" s="264" t="n"/>
-      <c r="C1" s="264" t="n"/>
-      <c r="D1" s="264" t="n"/>
-      <c r="E1" s="264" t="n"/>
-      <c r="F1" s="264" t="n"/>
-      <c r="G1" s="264" t="n"/>
-      <c r="H1" s="264" t="n"/>
-      <c r="I1" s="264" t="n"/>
-      <c r="J1" s="264" t="n"/>
-      <c r="K1" s="264" t="n"/>
-      <c r="L1" s="264" t="n"/>
-    </row>
-    <row r="2" ht="15.75" customHeight="1" s="248">
+    <row r="1" ht="6" customHeight="1" s="264">
+      <c r="B1" s="248" t="n"/>
+      <c r="C1" s="248" t="n"/>
+      <c r="D1" s="248" t="n"/>
+      <c r="E1" s="248" t="n"/>
+      <c r="F1" s="248" t="n"/>
+      <c r="G1" s="248" t="n"/>
+      <c r="H1" s="248" t="n"/>
+      <c r="I1" s="248" t="n"/>
+      <c r="J1" s="248" t="n"/>
+      <c r="K1" s="248" t="n"/>
+      <c r="L1" s="248" t="n"/>
+    </row>
+    <row r="2" ht="15.75" customHeight="1" s="264">
       <c r="A2" s="9" t="n"/>
-      <c r="B2" s="247" t="inlineStr">
+      <c r="B2" s="271" t="inlineStr">
         <is>
           <t>CHURCH</t>
         </is>
       </c>
       <c r="N2" s="29" t="n"/>
     </row>
-    <row r="3" ht="15.75" customHeight="1" s="248">
+    <row r="3" ht="15.75" customHeight="1" s="264">
       <c r="A3" s="9" t="n"/>
-      <c r="B3" s="247" t="inlineStr">
+      <c r="B3" s="271" t="inlineStr">
         <is>
           <t xml:space="preserve">        RECEIPTS AND PAYMENTS</t>
         </is>
       </c>
     </row>
-    <row r="4" ht="15.75" customHeight="1" s="248">
+    <row r="4" ht="15.75" customHeight="1" s="264">
       <c r="A4" s="9" t="n"/>
-      <c r="B4" s="247" t="inlineStr">
+      <c r="B4" s="271" t="inlineStr">
         <is>
           <t>ACCOUNTS</t>
         </is>
       </c>
     </row>
-    <row r="5" ht="6.75" customHeight="1" s="248">
+    <row r="5" ht="6.75" customHeight="1" s="264">
       <c r="A5" s="9" t="n"/>
-      <c r="B5" s="264" t="n"/>
-      <c r="C5" s="264" t="n"/>
-      <c r="D5" s="264" t="n"/>
-      <c r="E5" s="264" t="n"/>
-      <c r="F5" s="264" t="n"/>
-      <c r="G5" s="264" t="n"/>
-      <c r="H5" s="264" t="n"/>
-      <c r="I5" s="264" t="n"/>
-      <c r="J5" s="264" t="n"/>
-      <c r="K5" s="264" t="n"/>
-      <c r="L5" s="264" t="n"/>
-    </row>
-    <row r="6" ht="18.75" customHeight="1" s="248">
+      <c r="B5" s="248" t="n"/>
+      <c r="C5" s="248" t="n"/>
+      <c r="D5" s="248" t="n"/>
+      <c r="E5" s="248" t="n"/>
+      <c r="F5" s="248" t="n"/>
+      <c r="G5" s="248" t="n"/>
+      <c r="H5" s="248" t="n"/>
+      <c r="I5" s="248" t="n"/>
+      <c r="J5" s="248" t="n"/>
+      <c r="K5" s="248" t="n"/>
+      <c r="L5" s="248" t="n"/>
+    </row>
+    <row r="6" ht="18.75" customHeight="1" s="264">
       <c r="A6" s="9" t="n"/>
-      <c r="B6" s="250" t="inlineStr">
+      <c r="B6" s="272" t="inlineStr">
         <is>
           <t>THE METHODIST CHURCH</t>
         </is>
       </c>
     </row>
-    <row r="7" ht="9.75" customHeight="1" s="248">
+    <row r="7" ht="9.75" customHeight="1" s="264">
       <c r="A7" s="9" t="n"/>
-      <c r="B7" s="264" t="n"/>
-      <c r="C7" s="264" t="n"/>
-      <c r="D7" s="264" t="n"/>
-      <c r="E7" s="264" t="n"/>
-      <c r="F7" s="264" t="n"/>
-      <c r="G7" s="264" t="n"/>
-      <c r="H7" s="264" t="n"/>
-      <c r="I7" s="264" t="n"/>
-      <c r="J7" s="264" t="n"/>
-      <c r="K7" s="264" t="n"/>
-      <c r="L7" s="264" t="n"/>
-    </row>
-    <row r="8" ht="22.7" customFormat="1" customHeight="1" s="251">
+      <c r="B7" s="248" t="n"/>
+      <c r="C7" s="248" t="n"/>
+      <c r="D7" s="248" t="n"/>
+      <c r="E7" s="248" t="n"/>
+      <c r="F7" s="248" t="n"/>
+      <c r="G7" s="248" t="n"/>
+      <c r="H7" s="248" t="n"/>
+      <c r="I7" s="248" t="n"/>
+      <c r="J7" s="248" t="n"/>
+      <c r="K7" s="248" t="n"/>
+      <c r="L7" s="248" t="n"/>
+    </row>
+    <row r="8" ht="22.7" customFormat="1" customHeight="1" s="273">
       <c r="A8" s="23" t="n"/>
-      <c r="B8" s="250" t="inlineStr">
+      <c r="B8" s="272" t="inlineStr">
         <is>
           <t xml:space="preserve">STANDARD FORM OF ACCOUNTS </t>
         </is>
       </c>
     </row>
-    <row r="9" ht="7.5" customFormat="1" customHeight="1" s="251">
+    <row r="9" ht="7.5" customFormat="1" customHeight="1" s="273">
       <c r="A9" s="23" t="n"/>
-      <c r="B9" s="252" t="n"/>
-    </row>
-    <row r="10" ht="5.25" customHeight="1" s="248">
+      <c r="B9" s="274" t="n"/>
+    </row>
+    <row r="10" ht="5.25" customHeight="1" s="264">
       <c r="A10" s="9" t="n"/>
-      <c r="B10" s="264" t="n"/>
-      <c r="C10" s="264" t="n"/>
-      <c r="D10" s="264" t="n"/>
-      <c r="E10" s="264" t="n"/>
-      <c r="F10" s="264" t="n"/>
-      <c r="G10" s="264" t="n"/>
-      <c r="H10" s="264" t="n"/>
-      <c r="I10" s="264" t="n"/>
-      <c r="J10" s="264" t="n"/>
-      <c r="K10" s="264" t="n"/>
-      <c r="L10" s="264" t="n"/>
-    </row>
-    <row r="11" ht="30.2" customHeight="1" s="248">
+      <c r="B10" s="248" t="n"/>
+      <c r="C10" s="248" t="n"/>
+      <c r="D10" s="248" t="n"/>
+      <c r="E10" s="248" t="n"/>
+      <c r="F10" s="248" t="n"/>
+      <c r="G10" s="248" t="n"/>
+      <c r="H10" s="248" t="n"/>
+      <c r="I10" s="248" t="n"/>
+      <c r="J10" s="248" t="n"/>
+      <c r="K10" s="248" t="n"/>
+      <c r="L10" s="248" t="n"/>
+    </row>
+    <row r="11" ht="30.2" customHeight="1" s="264">
       <c r="A11" s="9" t="n"/>
       <c r="B11" s="35" t="n"/>
-      <c r="C11" s="253">
+      <c r="C11" s="275">
         <f>('Data from streamlit'!C2)</f>
         <v/>
       </c>
-      <c r="D11" s="254" t="n"/>
-      <c r="E11" s="254" t="n"/>
-      <c r="F11" s="254" t="n"/>
-      <c r="G11" s="254" t="n"/>
-      <c r="H11" s="254" t="n"/>
-      <c r="I11" s="254" t="n"/>
-      <c r="J11" s="254" t="n"/>
-      <c r="K11" s="254" t="n"/>
+      <c r="D11" s="276" t="n"/>
+      <c r="E11" s="276" t="n"/>
+      <c r="F11" s="276" t="n"/>
+      <c r="G11" s="276" t="n"/>
+      <c r="H11" s="276" t="n"/>
+      <c r="I11" s="276" t="n"/>
+      <c r="J11" s="276" t="n"/>
+      <c r="K11" s="276" t="n"/>
       <c r="L11" s="245" t="inlineStr">
         <is>
           <t>Church</t>
         </is>
       </c>
     </row>
-    <row r="12" ht="8.449999999999999" customHeight="1" s="248">
+    <row r="12" ht="8.449999999999999" customHeight="1" s="264">
       <c r="A12" s="9" t="n"/>
-      <c r="B12" s="264" t="n"/>
-      <c r="C12" s="264" t="n"/>
-      <c r="D12" s="264" t="n"/>
-      <c r="E12" s="264" t="n"/>
-      <c r="F12" s="264" t="n"/>
-      <c r="G12" s="264" t="n"/>
-      <c r="H12" s="264" t="n"/>
-      <c r="I12" s="264" t="n"/>
-      <c r="J12" s="264" t="n"/>
-      <c r="K12" s="264" t="n"/>
-      <c r="L12" s="264" t="n"/>
-    </row>
-    <row r="13" ht="20.25" customHeight="1" s="248">
+      <c r="B12" s="248" t="n"/>
+      <c r="C12" s="248" t="n"/>
+      <c r="D12" s="248" t="n"/>
+      <c r="E12" s="248" t="n"/>
+      <c r="F12" s="248" t="n"/>
+      <c r="G12" s="248" t="n"/>
+      <c r="H12" s="248" t="n"/>
+      <c r="I12" s="248" t="n"/>
+      <c r="J12" s="248" t="n"/>
+      <c r="K12" s="248" t="n"/>
+      <c r="L12" s="248" t="n"/>
+    </row>
+    <row r="13" ht="20.25" customHeight="1" s="264">
       <c r="A13" s="9" t="n"/>
-      <c r="B13" s="255" t="inlineStr">
+      <c r="B13" s="277" t="inlineStr">
         <is>
           <t xml:space="preserve">        FOR THE YEAR ENDED      </t>
         </is>
       </c>
     </row>
-    <row r="14" ht="8.449999999999999" customHeight="1" s="248">
+    <row r="14" ht="8.449999999999999" customHeight="1" s="264">
       <c r="A14" s="9" t="n"/>
       <c r="B14" s="36" t="n"/>
       <c r="C14" s="36" t="n"/>
@@ -2561,37 +2567,37 @@
       <c r="K14" s="36" t="n"/>
       <c r="L14" s="36" t="n"/>
     </row>
-    <row r="15" ht="20.25" customHeight="1" s="248">
+    <row r="15" ht="20.25" customHeight="1" s="264">
       <c r="A15" s="9" t="n"/>
-      <c r="B15" s="317" t="n">
+      <c r="B15" s="319" t="n">
         <v>45535</v>
       </c>
     </row>
-    <row r="16" ht="3.2" customHeight="1" s="248">
+    <row r="16" ht="3.2" customHeight="1" s="264">
       <c r="A16" s="9" t="n"/>
-      <c r="B16" s="264" t="n"/>
-      <c r="C16" s="264" t="n"/>
-      <c r="D16" s="264" t="n"/>
-      <c r="E16" s="264" t="n"/>
-      <c r="F16" s="264" t="n"/>
-      <c r="G16" s="264" t="n"/>
-      <c r="H16" s="264" t="n"/>
-      <c r="I16" s="264" t="n"/>
-      <c r="J16" s="264" t="n"/>
-      <c r="K16" s="264" t="n"/>
-      <c r="L16" s="264" t="n"/>
-    </row>
-    <row r="17" ht="30.2" customHeight="1" s="248">
+      <c r="B16" s="248" t="n"/>
+      <c r="C16" s="248" t="n"/>
+      <c r="D16" s="248" t="n"/>
+      <c r="E16" s="248" t="n"/>
+      <c r="F16" s="248" t="n"/>
+      <c r="G16" s="248" t="n"/>
+      <c r="H16" s="248" t="n"/>
+      <c r="I16" s="248" t="n"/>
+      <c r="J16" s="248" t="n"/>
+      <c r="K16" s="248" t="n"/>
+      <c r="L16" s="248" t="n"/>
+    </row>
+    <row r="17" ht="30.2" customHeight="1" s="264">
       <c r="A17" s="9" t="n"/>
-      <c r="B17" s="264" t="n"/>
-      <c r="C17" s="253">
+      <c r="B17" s="248" t="n"/>
+      <c r="C17" s="275">
         <f>('Data from streamlit'!C3)</f>
         <v/>
       </c>
-      <c r="D17" s="254" t="n"/>
-      <c r="E17" s="254" t="n"/>
-      <c r="F17" s="254" t="n"/>
-      <c r="G17" s="254" t="n"/>
+      <c r="D17" s="276" t="n"/>
+      <c r="E17" s="276" t="n"/>
+      <c r="F17" s="276" t="n"/>
+      <c r="G17" s="276" t="n"/>
       <c r="H17" s="243" t="n"/>
       <c r="I17" s="244" t="inlineStr">
         <is>
@@ -2603,208 +2609,208 @@
           <t>Circuit no.</t>
         </is>
       </c>
-      <c r="K17" s="256" t="inlineStr">
+      <c r="K17" s="278" t="inlineStr">
         <is>
           <t xml:space="preserve"> 29/31</t>
         </is>
       </c>
-      <c r="L17" s="257" t="n"/>
-    </row>
-    <row r="18" ht="6.75" customHeight="1" s="248">
+      <c r="L17" s="262" t="n"/>
+    </row>
+    <row r="18" ht="6.75" customHeight="1" s="264">
       <c r="A18" s="9" t="n"/>
-      <c r="B18" s="264" t="n"/>
-      <c r="C18" s="264" t="n"/>
-      <c r="D18" s="264" t="n"/>
-      <c r="E18" s="264" t="n"/>
-      <c r="F18" s="264" t="n"/>
-      <c r="G18" s="264" t="n"/>
-      <c r="H18" s="264" t="n"/>
+      <c r="B18" s="248" t="n"/>
+      <c r="C18" s="248" t="n"/>
+      <c r="D18" s="248" t="n"/>
+      <c r="E18" s="248" t="n"/>
+      <c r="F18" s="248" t="n"/>
+      <c r="G18" s="248" t="n"/>
+      <c r="H18" s="248" t="n"/>
       <c r="I18" s="175" t="n"/>
-      <c r="J18" s="264" t="n"/>
-      <c r="K18" s="264" t="n"/>
-      <c r="L18" s="264" t="n"/>
-    </row>
-    <row r="19" ht="26.45" customHeight="1" s="248">
+      <c r="J18" s="248" t="n"/>
+      <c r="K18" s="248" t="n"/>
+      <c r="L18" s="248" t="n"/>
+    </row>
+    <row r="19" ht="26.45" customHeight="1" s="264">
       <c r="A19" s="9" t="n"/>
-      <c r="B19" s="264" t="n"/>
-      <c r="C19" s="259" t="inlineStr">
+      <c r="B19" s="248" t="n"/>
+      <c r="C19" s="280" t="inlineStr">
         <is>
           <t>Registered Charity - Charity Registration number</t>
         </is>
       </c>
-      <c r="J19" s="264" t="n"/>
+      <c r="J19" s="248" t="n"/>
       <c r="K19" s="261" t="n"/>
-      <c r="L19" s="257" t="n"/>
-    </row>
-    <row r="20" ht="7.5" customHeight="1" s="248">
+      <c r="L19" s="262" t="n"/>
+    </row>
+    <row r="20" ht="7.5" customHeight="1" s="264">
       <c r="A20" s="9" t="n"/>
-      <c r="B20" s="264" t="n"/>
-      <c r="C20" s="249" t="n"/>
-      <c r="K20" s="264" t="n"/>
-      <c r="L20" s="264" t="n"/>
+      <c r="B20" s="248" t="n"/>
+      <c r="C20" s="259" t="n"/>
+      <c r="K20" s="248" t="n"/>
+      <c r="L20" s="248" t="n"/>
     </row>
     <row r="21" ht="30.75" customFormat="1" customHeight="1" s="260">
       <c r="A21" s="24" t="n"/>
-      <c r="B21" s="249" t="n"/>
-      <c r="C21" s="249" t="inlineStr">
+      <c r="B21" s="259" t="n"/>
+      <c r="C21" s="259" t="inlineStr">
         <is>
           <t>If not a registered charity His Majesty's Revenue and Customs Gift Aid number</t>
         </is>
       </c>
       <c r="J21" s="213" t="n"/>
-      <c r="K21" s="262" t="n"/>
-      <c r="L21" s="257" t="n"/>
-    </row>
-    <row r="22" ht="72.75" customHeight="1" s="248">
+      <c r="K21" s="263" t="n"/>
+      <c r="L21" s="262" t="n"/>
+    </row>
+    <row r="22" ht="72.75" customHeight="1" s="264">
       <c r="A22" s="9" t="n"/>
-      <c r="B22" s="264" t="n"/>
-      <c r="C22" s="249" t="inlineStr">
+      <c r="B22" s="248" t="n"/>
+      <c r="C22" s="259" t="inlineStr">
         <is>
           <t>(The HMRC number is equivalent to a registered charity number in terms of evidence of charitable status and may be used to give to donors or grant funders wishing to see evidence of the organisation's charitable status.  Methodist charities in England and Wales that are not registered charities are excepted from registration under Statutory Instrument  2014  No.242)</t>
         </is>
       </c>
     </row>
-    <row r="23" ht="14.25" customFormat="1" customHeight="1" s="264">
+    <row r="23" ht="14.25" customFormat="1" customHeight="1" s="248">
       <c r="A23" s="212" t="n"/>
-      <c r="B23" s="263" t="inlineStr">
+      <c r="B23" s="247" t="inlineStr">
         <is>
           <t>Minister:</t>
         </is>
       </c>
     </row>
-    <row r="24" ht="30.2" customFormat="1" customHeight="1" s="264">
+    <row r="24" ht="30.2" customFormat="1" customHeight="1" s="248">
       <c r="A24" s="212" t="n"/>
-      <c r="C24" s="274">
+      <c r="C24" s="269">
         <f>('Data from streamlit'!C8)</f>
         <v/>
       </c>
-      <c r="D24" s="275" t="n"/>
-      <c r="E24" s="275" t="n"/>
-      <c r="F24" s="275" t="n"/>
-      <c r="G24" s="275" t="n"/>
-      <c r="H24" s="275" t="n"/>
-      <c r="I24" s="275" t="n"/>
-      <c r="J24" s="275" t="n"/>
-      <c r="K24" s="275" t="n"/>
-      <c r="L24" s="257" t="n"/>
-    </row>
-    <row r="25" ht="23.25" customFormat="1" customHeight="1" s="264">
+      <c r="D24" s="270" t="n"/>
+      <c r="E24" s="270" t="n"/>
+      <c r="F24" s="270" t="n"/>
+      <c r="G24" s="270" t="n"/>
+      <c r="H24" s="270" t="n"/>
+      <c r="I24" s="270" t="n"/>
+      <c r="J24" s="270" t="n"/>
+      <c r="K24" s="270" t="n"/>
+      <c r="L24" s="262" t="n"/>
+    </row>
+    <row r="25" ht="23.25" customFormat="1" customHeight="1" s="248">
       <c r="A25" s="212" t="n"/>
-      <c r="B25" s="263" t="inlineStr">
+      <c r="B25" s="247" t="inlineStr">
         <is>
           <t>Church Stewards:</t>
         </is>
       </c>
     </row>
-    <row r="26" ht="30.2" customFormat="1" customHeight="1" s="264">
+    <row r="26" ht="30.2" customFormat="1" customHeight="1" s="248">
       <c r="A26" s="212" t="n"/>
-      <c r="C26" s="279">
+      <c r="C26" s="252">
         <f>('Data from streamlit'!C9)</f>
         <v/>
       </c>
-      <c r="D26" s="277" t="n"/>
-      <c r="E26" s="277" t="n"/>
-      <c r="F26" s="277" t="n"/>
-      <c r="G26" s="277" t="n"/>
-      <c r="H26" s="277" t="n"/>
-      <c r="I26" s="276">
+      <c r="D26" s="250" t="n"/>
+      <c r="E26" s="250" t="n"/>
+      <c r="F26" s="250" t="n"/>
+      <c r="G26" s="250" t="n"/>
+      <c r="H26" s="250" t="n"/>
+      <c r="I26" s="249">
         <f>('Data from streamlit'!C10)</f>
         <v/>
       </c>
-      <c r="J26" s="277" t="n"/>
-      <c r="K26" s="277" t="n"/>
-      <c r="L26" s="278" t="n"/>
-    </row>
-    <row r="27" ht="30.2" customFormat="1" customHeight="1" s="264">
+      <c r="J26" s="250" t="n"/>
+      <c r="K26" s="250" t="n"/>
+      <c r="L26" s="251" t="n"/>
+    </row>
+    <row r="27" ht="30.2" customFormat="1" customHeight="1" s="248">
       <c r="A27" s="212" t="n"/>
-      <c r="C27" s="269">
+      <c r="C27" s="258">
         <f>('Data from streamlit'!C11)</f>
         <v/>
       </c>
-      <c r="D27" s="266" t="n"/>
-      <c r="E27" s="266" t="n"/>
-      <c r="F27" s="266" t="n"/>
-      <c r="G27" s="266" t="n"/>
-      <c r="H27" s="266" t="n"/>
-      <c r="I27" s="280">
+      <c r="D27" s="254" t="n"/>
+      <c r="E27" s="254" t="n"/>
+      <c r="F27" s="254" t="n"/>
+      <c r="G27" s="254" t="n"/>
+      <c r="H27" s="254" t="n"/>
+      <c r="I27" s="255">
         <f>('Data from streamlit'!C12)</f>
         <v/>
       </c>
-      <c r="J27" s="266" t="n"/>
-      <c r="K27" s="266" t="n"/>
-      <c r="L27" s="267" t="n"/>
-    </row>
-    <row r="28" ht="30.2" customFormat="1" customHeight="1" s="264">
+      <c r="J27" s="254" t="n"/>
+      <c r="K27" s="254" t="n"/>
+      <c r="L27" s="256" t="n"/>
+    </row>
+    <row r="28" ht="30.2" customFormat="1" customHeight="1" s="248">
       <c r="A28" s="212" t="n"/>
       <c r="B28" s="34" t="n"/>
-      <c r="C28" s="268" t="n"/>
-      <c r="D28" s="266" t="n"/>
-      <c r="E28" s="266" t="n"/>
-      <c r="F28" s="266" t="n"/>
-      <c r="G28" s="266" t="n"/>
-      <c r="H28" s="266" t="n"/>
-      <c r="I28" s="265" t="n"/>
-      <c r="J28" s="266" t="n"/>
-      <c r="K28" s="266" t="n"/>
-      <c r="L28" s="267" t="n"/>
-    </row>
-    <row r="29" ht="30.2" customFormat="1" customHeight="1" s="264">
+      <c r="C28" s="253" t="n"/>
+      <c r="D28" s="254" t="n"/>
+      <c r="E28" s="254" t="n"/>
+      <c r="F28" s="254" t="n"/>
+      <c r="G28" s="254" t="n"/>
+      <c r="H28" s="254" t="n"/>
+      <c r="I28" s="257" t="n"/>
+      <c r="J28" s="254" t="n"/>
+      <c r="K28" s="254" t="n"/>
+      <c r="L28" s="256" t="n"/>
+    </row>
+    <row r="29" ht="30.2" customFormat="1" customHeight="1" s="248">
       <c r="A29" s="212" t="n"/>
       <c r="B29" s="34" t="n"/>
-      <c r="C29" s="268" t="n"/>
-      <c r="D29" s="266" t="n"/>
-      <c r="E29" s="266" t="n"/>
-      <c r="F29" s="266" t="n"/>
-      <c r="G29" s="266" t="n"/>
-      <c r="H29" s="266" t="n"/>
-      <c r="I29" s="265" t="n"/>
-      <c r="J29" s="266" t="n"/>
-      <c r="K29" s="266" t="n"/>
-      <c r="L29" s="267" t="n"/>
-    </row>
-    <row r="30" ht="30.2" customFormat="1" customHeight="1" s="264">
+      <c r="C29" s="253" t="n"/>
+      <c r="D29" s="254" t="n"/>
+      <c r="E29" s="254" t="n"/>
+      <c r="F29" s="254" t="n"/>
+      <c r="G29" s="254" t="n"/>
+      <c r="H29" s="254" t="n"/>
+      <c r="I29" s="257" t="n"/>
+      <c r="J29" s="254" t="n"/>
+      <c r="K29" s="254" t="n"/>
+      <c r="L29" s="256" t="n"/>
+    </row>
+    <row r="30" ht="30.2" customFormat="1" customHeight="1" s="248">
       <c r="A30" s="212" t="n"/>
       <c r="B30" s="34" t="n"/>
-      <c r="C30" s="268" t="n"/>
-      <c r="D30" s="266" t="n"/>
-      <c r="E30" s="266" t="n"/>
-      <c r="F30" s="266" t="n"/>
-      <c r="G30" s="266" t="n"/>
-      <c r="H30" s="266" t="n"/>
-      <c r="I30" s="265" t="n"/>
-      <c r="J30" s="266" t="n"/>
-      <c r="K30" s="266" t="n"/>
-      <c r="L30" s="267" t="n"/>
-    </row>
-    <row r="31" ht="30.2" customFormat="1" customHeight="1" s="264">
+      <c r="C30" s="253" t="n"/>
+      <c r="D30" s="254" t="n"/>
+      <c r="E30" s="254" t="n"/>
+      <c r="F30" s="254" t="n"/>
+      <c r="G30" s="254" t="n"/>
+      <c r="H30" s="254" t="n"/>
+      <c r="I30" s="257" t="n"/>
+      <c r="J30" s="254" t="n"/>
+      <c r="K30" s="254" t="n"/>
+      <c r="L30" s="256" t="n"/>
+    </row>
+    <row r="31" ht="30.2" customFormat="1" customHeight="1" s="248">
       <c r="A31" s="212" t="n"/>
       <c r="B31" s="34" t="n"/>
-      <c r="C31" s="268" t="n"/>
-      <c r="D31" s="266" t="n"/>
-      <c r="E31" s="266" t="n"/>
-      <c r="F31" s="266" t="n"/>
-      <c r="G31" s="266" t="n"/>
-      <c r="H31" s="266" t="n"/>
-      <c r="I31" s="265" t="n"/>
-      <c r="J31" s="266" t="n"/>
-      <c r="K31" s="266" t="n"/>
-      <c r="L31" s="267" t="n"/>
-    </row>
-    <row r="32" ht="30.2" customFormat="1" customHeight="1" s="264">
+      <c r="C31" s="253" t="n"/>
+      <c r="D31" s="254" t="n"/>
+      <c r="E31" s="254" t="n"/>
+      <c r="F31" s="254" t="n"/>
+      <c r="G31" s="254" t="n"/>
+      <c r="H31" s="254" t="n"/>
+      <c r="I31" s="257" t="n"/>
+      <c r="J31" s="254" t="n"/>
+      <c r="K31" s="254" t="n"/>
+      <c r="L31" s="256" t="n"/>
+    </row>
+    <row r="32" ht="30.2" customFormat="1" customHeight="1" s="248">
       <c r="A32" s="212" t="n"/>
       <c r="B32" s="34" t="n"/>
-      <c r="C32" s="273" t="n"/>
-      <c r="D32" s="271" t="n"/>
-      <c r="E32" s="271" t="n"/>
-      <c r="F32" s="271" t="n"/>
-      <c r="G32" s="271" t="n"/>
-      <c r="H32" s="271" t="n"/>
-      <c r="I32" s="270" t="n"/>
-      <c r="J32" s="271" t="n"/>
-      <c r="K32" s="271" t="n"/>
-      <c r="L32" s="272" t="n"/>
-    </row>
-    <row r="33" ht="9" customFormat="1" customHeight="1" s="264">
+      <c r="C32" s="268" t="n"/>
+      <c r="D32" s="266" t="n"/>
+      <c r="E32" s="266" t="n"/>
+      <c r="F32" s="266" t="n"/>
+      <c r="G32" s="266" t="n"/>
+      <c r="H32" s="266" t="n"/>
+      <c r="I32" s="265" t="n"/>
+      <c r="J32" s="266" t="n"/>
+      <c r="K32" s="266" t="n"/>
+      <c r="L32" s="267" t="n"/>
+    </row>
+    <row r="33" ht="9" customFormat="1" customHeight="1" s="248">
       <c r="A33" s="212" t="n"/>
       <c r="B33" s="34" t="n"/>
       <c r="C33" s="34" t="n"/>
@@ -2818,7 +2824,7 @@
       <c r="K33" s="34" t="n"/>
       <c r="L33" s="34" t="n"/>
     </row>
-    <row r="34" hidden="1" ht="3.75" customFormat="1" customHeight="1" s="264">
+    <row r="34" hidden="1" ht="3.75" customFormat="1" customHeight="1" s="248">
       <c r="A34" s="212" t="n"/>
       <c r="B34" s="34" t="n"/>
       <c r="C34" s="34" t="n"/>
@@ -2832,46 +2838,51 @@
       <c r="K34" s="34" t="n"/>
       <c r="L34" s="34" t="n"/>
     </row>
-    <row r="35" ht="14.25" customFormat="1" customHeight="1" s="264">
+    <row r="35" ht="14.25" customFormat="1" customHeight="1" s="248">
       <c r="A35" s="212" t="n"/>
-      <c r="B35" s="263" t="inlineStr">
+      <c r="B35" s="247" t="inlineStr">
         <is>
           <t>Treasurer:</t>
         </is>
       </c>
     </row>
-    <row r="36" ht="30.2" customFormat="1" customHeight="1" s="264">
+    <row r="36" ht="30.2" customFormat="1" customHeight="1" s="248">
       <c r="A36" s="212" t="n"/>
       <c r="B36" s="34" t="n"/>
-      <c r="C36" s="269">
+      <c r="C36" s="258">
         <f>('Data from streamlit'!C13)</f>
         <v/>
       </c>
-      <c r="D36" s="266" t="n"/>
-      <c r="E36" s="266" t="n"/>
-      <c r="F36" s="266" t="n"/>
-      <c r="G36" s="266" t="n"/>
-      <c r="H36" s="266" t="n"/>
-      <c r="I36" s="266" t="n"/>
-      <c r="J36" s="266" t="n"/>
-      <c r="K36" s="266" t="n"/>
-      <c r="L36" s="266" t="n"/>
-    </row>
-    <row r="37" ht="6" customHeight="1" s="248">
+      <c r="D36" s="254" t="n"/>
+      <c r="E36" s="254" t="n"/>
+      <c r="F36" s="254" t="n"/>
+      <c r="G36" s="254" t="n"/>
+      <c r="H36" s="254" t="n"/>
+      <c r="I36" s="254" t="n"/>
+      <c r="J36" s="254" t="n"/>
+      <c r="K36" s="254" t="n"/>
+      <c r="L36" s="254" t="n"/>
+    </row>
+    <row r="37" ht="6" customHeight="1" s="264">
       <c r="A37" s="9" t="n"/>
     </row>
-    <row r="38" ht="6" customHeight="1" s="248"/>
+    <row r="38" ht="6" customHeight="1" s="264"/>
     <row r="40"/>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="B25:L25"/>
-    <mergeCell ref="B23:L23"/>
-    <mergeCell ref="I26:L26"/>
-    <mergeCell ref="C26:H26"/>
-    <mergeCell ref="C28:H28"/>
-    <mergeCell ref="I27:L27"/>
-    <mergeCell ref="I28:L28"/>
-    <mergeCell ref="C27:H27"/>
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="C20:J20"/>
+    <mergeCell ref="B3:L3"/>
+    <mergeCell ref="B4:L4"/>
+    <mergeCell ref="B6:L6"/>
+    <mergeCell ref="B8:L8"/>
+    <mergeCell ref="B9:L9"/>
+    <mergeCell ref="C11:K11"/>
+    <mergeCell ref="B13:L13"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="B15:L15"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C19:I19"/>
     <mergeCell ref="C21:I21"/>
     <mergeCell ref="K19:L19"/>
     <mergeCell ref="K21:L21"/>
@@ -2888,19 +2899,14 @@
     <mergeCell ref="I29:L29"/>
     <mergeCell ref="C22:L22"/>
     <mergeCell ref="C24:L24"/>
-    <mergeCell ref="B2:L2"/>
-    <mergeCell ref="C20:J20"/>
-    <mergeCell ref="B3:L3"/>
-    <mergeCell ref="B4:L4"/>
-    <mergeCell ref="B6:L6"/>
-    <mergeCell ref="B8:L8"/>
-    <mergeCell ref="B9:L9"/>
-    <mergeCell ref="C11:K11"/>
-    <mergeCell ref="B13:L13"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="B15:L15"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C19:I19"/>
+    <mergeCell ref="B25:L25"/>
+    <mergeCell ref="B23:L23"/>
+    <mergeCell ref="I26:L26"/>
+    <mergeCell ref="C26:H26"/>
+    <mergeCell ref="C28:H28"/>
+    <mergeCell ref="I27:L27"/>
+    <mergeCell ref="I28:L28"/>
+    <mergeCell ref="C27:H27"/>
   </mergeCells>
   <pageMargins left="0.3937007874015748" right="0.2362204724409449" top="0.3937007874015748" bottom="0.3937007874015748" header="0.2362204724409449" footer="0.1574803149606299"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -2924,7 +2930,7 @@
   </sheetPr>
   <dimension ref="B1:R42"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showZeros="0" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
@@ -2933,30 +2939,30 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
   <cols>
-    <col width="1.42578125" customWidth="1" style="296" min="1" max="1"/>
-    <col width="0.5703125" customWidth="1" style="296" min="2" max="2"/>
-    <col width="3" bestFit="1" customWidth="1" style="296" min="3" max="3"/>
-    <col width="28.140625" customWidth="1" style="296" min="4" max="4"/>
-    <col width="6" customWidth="1" style="296" min="5" max="5"/>
-    <col width="14" customWidth="1" style="296" min="6" max="6"/>
-    <col width="11.42578125" customWidth="1" style="296" min="7" max="7"/>
-    <col width="10" customWidth="1" style="296" min="8" max="8"/>
-    <col width="0.85546875" customWidth="1" style="296" min="9" max="9"/>
-    <col width="10" customWidth="1" style="296" min="10" max="10"/>
-    <col width="4.85546875" bestFit="1" customWidth="1" style="296" min="11" max="11"/>
-    <col width="0.85546875" customWidth="1" style="296" min="12" max="12"/>
-    <col width="10" customWidth="1" style="296" min="13" max="13"/>
-    <col width="5.42578125" customWidth="1" style="296" min="14" max="14"/>
-    <col width="1" customWidth="1" style="296" min="15" max="15"/>
-    <col width="0.5703125" customWidth="1" style="296" min="16" max="16"/>
-    <col width="10" customWidth="1" style="296" min="17" max="17"/>
-    <col width="6.42578125" customWidth="1" style="296" min="18" max="18"/>
-    <col width="17.5703125" customWidth="1" style="296" min="19" max="19"/>
-    <col width="9.140625" customWidth="1" style="296" min="20" max="28"/>
-    <col width="9.140625" customWidth="1" style="296" min="29" max="16384"/>
+    <col width="1.42578125" customWidth="1" style="289" min="1" max="1"/>
+    <col width="0.5703125" customWidth="1" style="289" min="2" max="2"/>
+    <col width="3" bestFit="1" customWidth="1" style="289" min="3" max="3"/>
+    <col width="28.140625" customWidth="1" style="289" min="4" max="4"/>
+    <col width="6" customWidth="1" style="289" min="5" max="5"/>
+    <col width="14" customWidth="1" style="289" min="6" max="6"/>
+    <col width="11.42578125" customWidth="1" style="289" min="7" max="7"/>
+    <col width="10" customWidth="1" style="289" min="8" max="8"/>
+    <col width="0.85546875" customWidth="1" style="289" min="9" max="9"/>
+    <col width="10" customWidth="1" style="289" min="10" max="10"/>
+    <col width="4.85546875" bestFit="1" customWidth="1" style="289" min="11" max="11"/>
+    <col width="0.85546875" customWidth="1" style="289" min="12" max="12"/>
+    <col width="10" customWidth="1" style="289" min="13" max="13"/>
+    <col width="5.42578125" customWidth="1" style="289" min="14" max="14"/>
+    <col width="1" customWidth="1" style="289" min="15" max="15"/>
+    <col width="0.5703125" customWidth="1" style="289" min="16" max="16"/>
+    <col width="10" customWidth="1" style="289" min="17" max="17"/>
+    <col width="6.42578125" customWidth="1" style="289" min="18" max="18"/>
+    <col width="17.5703125" customWidth="1" style="289" min="19" max="19"/>
+    <col width="9.140625" customWidth="1" style="289" min="20" max="29"/>
+    <col width="9.140625" customWidth="1" style="289" min="30" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" ht="7.5" customHeight="1" s="248">
+    <row r="1" ht="7.5" customHeight="1" s="264">
       <c r="B1" s="8" t="n"/>
       <c r="C1" s="37" t="n"/>
       <c r="D1" s="37" t="n"/>
@@ -2973,27 +2979,27 @@
       <c r="O1" s="8" t="n"/>
       <c r="P1" s="8" t="n"/>
     </row>
-    <row r="2" ht="37.5" customHeight="1" s="248">
+    <row r="2" ht="37.5" customHeight="1" s="264">
       <c r="B2" s="8" t="n"/>
-      <c r="C2" s="295" t="inlineStr">
+      <c r="C2" s="288" t="inlineStr">
         <is>
           <t>ACCOUNTS FOR THE YEAR ENDED 31 AUGUST 2024</t>
         </is>
       </c>
-      <c r="H2" s="299">
+      <c r="H2" s="292">
         <f>'P1 Front page'!$C$11</f>
         <v/>
       </c>
-      <c r="I2" s="254" t="n"/>
-      <c r="J2" s="254" t="n"/>
-      <c r="K2" s="254" t="n"/>
-      <c r="L2" s="254" t="n"/>
-      <c r="M2" s="289" t="inlineStr">
+      <c r="I2" s="276" t="n"/>
+      <c r="J2" s="276" t="n"/>
+      <c r="K2" s="276" t="n"/>
+      <c r="L2" s="276" t="n"/>
+      <c r="M2" s="281" t="inlineStr">
         <is>
           <t>Church</t>
         </is>
       </c>
-      <c r="N2" s="286" t="n"/>
+      <c r="N2" s="282" t="n"/>
       <c r="O2" s="19" t="n"/>
       <c r="P2" s="8" t="n"/>
       <c r="Q2" s="11" t="inlineStr">
@@ -3002,31 +3008,31 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="7.5" customFormat="1" customHeight="1" s="298">
+    <row r="3" ht="7.5" customFormat="1" customHeight="1" s="291">
       <c r="B3" s="131" t="n"/>
       <c r="C3" s="132" t="n"/>
       <c r="D3" s="132" t="n"/>
       <c r="E3" s="132" t="n"/>
       <c r="F3" s="132" t="n"/>
-      <c r="G3" s="297" t="inlineStr">
+      <c r="G3" s="290" t="inlineStr">
         <is>
           <t>Unrestricted Funds</t>
         </is>
       </c>
-      <c r="H3" s="297" t="inlineStr">
+      <c r="H3" s="290" t="inlineStr">
         <is>
           <t>Restricted Funds</t>
         </is>
       </c>
       <c r="I3" s="176" t="n"/>
-      <c r="J3" s="297" t="inlineStr">
+      <c r="J3" s="290" t="inlineStr">
         <is>
           <t>Totals this year</t>
         </is>
       </c>
-      <c r="K3" s="297" t="n"/>
-      <c r="L3" s="297" t="n"/>
-      <c r="M3" s="297" t="inlineStr">
+      <c r="K3" s="290" t="n"/>
+      <c r="L3" s="290" t="n"/>
+      <c r="M3" s="290" t="inlineStr">
         <is>
           <t>Totals last year</t>
         </is>
@@ -3035,7 +3041,7 @@
       <c r="O3" s="4" t="n"/>
       <c r="P3" s="131" t="n"/>
     </row>
-    <row r="4" ht="23.25" customFormat="1" customHeight="1" s="298">
+    <row r="4" ht="23.25" customFormat="1" customHeight="1" s="291">
       <c r="B4" s="131" t="n"/>
       <c r="C4" s="132" t="n"/>
       <c r="D4" s="136" t="inlineStr">
@@ -3046,13 +3052,13 @@
       <c r="E4" s="132" t="n"/>
       <c r="F4" s="132" t="n"/>
       <c r="I4" s="176" t="n"/>
-      <c r="K4" s="297" t="n"/>
-      <c r="L4" s="297" t="n"/>
+      <c r="K4" s="290" t="n"/>
+      <c r="L4" s="290" t="n"/>
       <c r="N4" s="39" t="n"/>
       <c r="O4" s="4" t="n"/>
       <c r="P4" s="131" t="n"/>
     </row>
-    <row r="5" ht="23.25" customFormat="1" customHeight="1" s="298">
+    <row r="5" ht="23.25" customFormat="1" customHeight="1" s="291">
       <c r="B5" s="131" t="n"/>
       <c r="C5" s="40" t="n"/>
       <c r="D5" s="137" t="n"/>
@@ -3085,7 +3091,7 @@
       <c r="O5" s="4" t="n"/>
       <c r="P5" s="131" t="n"/>
     </row>
-    <row r="6" ht="18.75" customHeight="1" s="248">
+    <row r="6" ht="18.75" customHeight="1" s="264">
       <c r="B6" s="8" t="n"/>
       <c r="C6" s="40" t="inlineStr">
         <is>
@@ -3114,7 +3120,7 @@
       <c r="O6" s="14" t="n"/>
       <c r="P6" s="8" t="n"/>
     </row>
-    <row r="7" ht="18.75" customHeight="1" s="248">
+    <row r="7" ht="18.75" customHeight="1" s="264">
       <c r="B7" s="8" t="n"/>
       <c r="C7" s="40" t="inlineStr">
         <is>
@@ -3140,7 +3146,7 @@
       <c r="N7" s="38" t="n"/>
       <c r="P7" s="8" t="n"/>
     </row>
-    <row r="8" ht="27" customHeight="1" s="248">
+    <row r="8" ht="27" customHeight="1" s="264">
       <c r="B8" s="8" t="n"/>
       <c r="C8" s="40" t="inlineStr">
         <is>
@@ -3167,7 +3173,7 @@
       <c r="N8" s="38" t="n"/>
       <c r="P8" s="8" t="n"/>
     </row>
-    <row r="9" ht="18" customHeight="1" s="248">
+    <row r="9" ht="18" customHeight="1" s="264">
       <c r="B9" s="8" t="n"/>
       <c r="C9" s="40" t="inlineStr">
         <is>
@@ -3194,7 +3200,7 @@
       <c r="N9" s="38" t="n"/>
       <c r="P9" s="8" t="n"/>
     </row>
-    <row r="10" ht="18.75" customHeight="1" s="248" thickBot="1">
+    <row r="10" ht="18.75" customHeight="1" s="264" thickBot="1">
       <c r="B10" s="8" t="n"/>
       <c r="C10" s="40" t="inlineStr">
         <is>
@@ -3221,7 +3227,7 @@
       <c r="N10" s="38" t="n"/>
       <c r="P10" s="8" t="n"/>
     </row>
-    <row r="11" ht="17.45" customHeight="1" s="248" thickBot="1">
+    <row r="11" ht="17.45" customHeight="1" s="264" thickBot="1">
       <c r="B11" s="8" t="n"/>
       <c r="C11" s="40" t="inlineStr">
         <is>
@@ -3262,7 +3268,7 @@
       <c r="O11" s="6" t="n"/>
       <c r="P11" s="8" t="n"/>
     </row>
-    <row r="12" ht="8.449999999999999" customHeight="1" s="248">
+    <row r="12" ht="8.449999999999999" customHeight="1" s="264">
       <c r="B12" s="8" t="n"/>
       <c r="C12" s="38" t="n"/>
       <c r="D12" s="38" t="n"/>
@@ -3278,7 +3284,7 @@
       <c r="N12" s="38" t="n"/>
       <c r="P12" s="8" t="n"/>
     </row>
-    <row r="13" ht="18.75" customHeight="1" s="248">
+    <row r="13" ht="18.75" customHeight="1" s="264">
       <c r="B13" s="8" t="n"/>
       <c r="C13" s="38" t="n"/>
       <c r="D13" s="136" t="inlineStr">
@@ -3298,7 +3304,7 @@
       <c r="N13" s="38" t="n"/>
       <c r="P13" s="8" t="n"/>
     </row>
-    <row r="14" ht="18.75" customHeight="1" s="248">
+    <row r="14" ht="18.75" customHeight="1" s="264">
       <c r="B14" s="8" t="n"/>
       <c r="C14" s="40" t="inlineStr">
         <is>
@@ -3322,7 +3328,7 @@
       <c r="N14" s="38" t="n"/>
       <c r="P14" s="8" t="n"/>
     </row>
-    <row r="15" ht="18" customHeight="1" s="248">
+    <row r="15" ht="18" customHeight="1" s="264">
       <c r="B15" s="8" t="n"/>
       <c r="C15" s="40" t="inlineStr">
         <is>
@@ -3349,7 +3355,7 @@
       <c r="N15" s="38" t="n"/>
       <c r="P15" s="8" t="n"/>
     </row>
-    <row r="16" ht="18.75" customHeight="1" s="248">
+    <row r="16" ht="18.75" customHeight="1" s="264">
       <c r="B16" s="8" t="n"/>
       <c r="C16" s="40" t="inlineStr">
         <is>
@@ -3376,7 +3382,7 @@
       <c r="N16" s="38" t="n"/>
       <c r="P16" s="8" t="n"/>
     </row>
-    <row r="17" ht="18.75" customHeight="1" s="248">
+    <row r="17" ht="18.75" customHeight="1" s="264">
       <c r="B17" s="8" t="n"/>
       <c r="C17" s="40" t="inlineStr">
         <is>
@@ -3403,7 +3409,7 @@
       <c r="N17" s="38" t="n"/>
       <c r="P17" s="8" t="n"/>
     </row>
-    <row r="18" ht="26.45" customHeight="1" s="248">
+    <row r="18" ht="26.45" customHeight="1" s="264">
       <c r="B18" s="8" t="n"/>
       <c r="C18" s="40" t="inlineStr">
         <is>
@@ -3430,15 +3436,15 @@
       <c r="N18" s="38" t="n"/>
       <c r="P18" s="8" t="n"/>
     </row>
-    <row r="19" ht="18.75" customHeight="1" s="248">
+    <row r="19" ht="18.75" customHeight="1" s="264">
       <c r="B19" s="8" t="n"/>
       <c r="C19" s="40" t="inlineStr">
         <is>
           <t>b6</t>
         </is>
       </c>
-      <c r="D19" s="300" t="n"/>
-      <c r="E19" s="257" t="n"/>
+      <c r="D19" s="293" t="n"/>
+      <c r="E19" s="262" t="n"/>
       <c r="F19" s="43" t="n"/>
       <c r="G19" s="142" t="n"/>
       <c r="H19" s="142" t="n"/>
@@ -3453,7 +3459,7 @@
       <c r="N19" s="38" t="n"/>
       <c r="P19" s="8" t="n"/>
     </row>
-    <row r="20" ht="18.75" customHeight="1" s="248" thickBot="1">
+    <row r="20" ht="18.75" customHeight="1" s="264" thickBot="1">
       <c r="B20" s="8" t="n"/>
       <c r="C20" s="40" t="inlineStr">
         <is>
@@ -3480,7 +3486,7 @@
       <c r="N20" s="38" t="n"/>
       <c r="P20" s="8" t="n"/>
     </row>
-    <row r="21" ht="18" customHeight="1" s="248" thickBot="1">
+    <row r="21" ht="18" customHeight="1" s="264" thickBot="1">
       <c r="B21" s="8" t="n"/>
       <c r="C21" s="40" t="inlineStr">
         <is>
@@ -3521,7 +3527,7 @@
       <c r="O21" s="7" t="n"/>
       <c r="P21" s="8" t="n"/>
     </row>
-    <row r="22" ht="8.449999999999999" customHeight="1" s="248">
+    <row r="22" ht="8.449999999999999" customHeight="1" s="264">
       <c r="B22" s="8" t="n"/>
       <c r="C22" s="38" t="n"/>
       <c r="D22" s="156" t="n"/>
@@ -3538,7 +3544,7 @@
       <c r="O22" s="7" t="n"/>
       <c r="P22" s="8" t="n"/>
     </row>
-    <row r="23" ht="18.75" customHeight="1" s="248">
+    <row r="23" ht="18.75" customHeight="1" s="264">
       <c r="B23" s="8" t="n"/>
       <c r="C23" s="38" t="n"/>
       <c r="D23" s="136" t="inlineStr">
@@ -3558,7 +3564,7 @@
       <c r="N23" s="38" t="n"/>
       <c r="P23" s="8" t="n"/>
     </row>
-    <row r="24" ht="25.5" customHeight="1" s="248">
+    <row r="24" ht="25.5" customHeight="1" s="264">
       <c r="B24" s="8" t="n"/>
       <c r="C24" s="40" t="inlineStr">
         <is>
@@ -3599,7 +3605,7 @@
       <c r="P24" s="8" t="n"/>
       <c r="Q24" s="17" t="n"/>
     </row>
-    <row r="25" ht="7.5" customHeight="1" s="248">
+    <row r="25" ht="7.5" customHeight="1" s="264">
       <c r="B25" s="8" t="n"/>
       <c r="C25" s="38" t="n"/>
       <c r="D25" s="42" t="n"/>
@@ -3616,7 +3622,7 @@
       <c r="P25" s="8" t="n"/>
       <c r="Q25" s="17" t="n"/>
     </row>
-    <row r="26" ht="33.75" customHeight="1" s="248">
+    <row r="26" ht="33.75" customHeight="1" s="264">
       <c r="B26" s="8" t="n"/>
       <c r="C26" s="40" t="inlineStr">
         <is>
@@ -3656,7 +3662,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" ht="7.5" customHeight="1" s="248">
+    <row r="27" ht="7.5" customHeight="1" s="264">
       <c r="B27" s="8" t="n"/>
       <c r="C27" s="38" t="n"/>
       <c r="D27" s="42" t="n"/>
@@ -3672,19 +3678,19 @@
       <c r="N27" s="38" t="n"/>
       <c r="P27" s="8" t="n"/>
     </row>
-    <row r="28" ht="19.5" customHeight="1" s="248">
+    <row r="28" ht="19.5" customHeight="1" s="264">
       <c r="B28" s="8" t="n"/>
       <c r="C28" s="40" t="inlineStr">
         <is>
           <t>c3</t>
         </is>
       </c>
-      <c r="D28" s="284" t="inlineStr">
+      <c r="D28" s="297" t="inlineStr">
         <is>
           <t xml:space="preserve">Sub total                                                               </t>
         </is>
       </c>
-      <c r="E28" s="254" t="n"/>
+      <c r="E28" s="276" t="n"/>
       <c r="F28" s="157" t="inlineStr">
         <is>
           <t>(c1+c2)</t>
@@ -3712,7 +3718,7 @@
       <c r="N28" s="38" t="n"/>
       <c r="P28" s="8" t="n"/>
     </row>
-    <row r="29" ht="7.5" customHeight="1" s="248">
+    <row r="29" ht="7.5" customHeight="1" s="264">
       <c r="B29" s="8" t="n"/>
       <c r="C29" s="38" t="n"/>
       <c r="D29" s="42" t="n"/>
@@ -3728,7 +3734,7 @@
       <c r="N29" s="38" t="n"/>
       <c r="P29" s="8" t="n"/>
     </row>
-    <row r="30" ht="18" customHeight="1" s="248">
+    <row r="30" ht="18" customHeight="1" s="264">
       <c r="B30" s="8" t="n"/>
       <c r="C30" s="40" t="inlineStr">
         <is>
@@ -3759,7 +3765,7 @@
       <c r="N30" s="38" t="n"/>
       <c r="P30" s="8" t="n"/>
     </row>
-    <row r="31" ht="7.5" customHeight="1" s="248" thickBot="1">
+    <row r="31" ht="7.5" customHeight="1" s="264" thickBot="1">
       <c r="B31" s="8" t="n"/>
       <c r="C31" s="38" t="n"/>
       <c r="D31" s="42" t="n"/>
@@ -3775,7 +3781,7 @@
       <c r="N31" s="38" t="n"/>
       <c r="P31" s="8" t="n"/>
     </row>
-    <row r="32" ht="18" customHeight="1" s="248" thickBot="1">
+    <row r="32" ht="18" customHeight="1" s="264" thickBot="1">
       <c r="B32" s="8" t="n"/>
       <c r="C32" s="40" t="inlineStr">
         <is>
@@ -3833,7 +3839,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" ht="18" customHeight="1" s="248">
+    <row r="33" ht="18" customHeight="1" s="264">
       <c r="B33" s="8" t="n"/>
       <c r="C33" s="38" t="n"/>
       <c r="D33" s="38" t="n"/>
@@ -3849,7 +3855,7 @@
       <c r="N33" s="38" t="n"/>
       <c r="P33" s="8" t="n"/>
     </row>
-    <row r="34" ht="23.25" customHeight="1" s="248" thickBot="1">
+    <row r="34" ht="23.25" customHeight="1" s="264" thickBot="1">
       <c r="B34" s="8" t="n"/>
       <c r="C34" s="38" t="n"/>
       <c r="D34" s="143" t="inlineStr">
@@ -3871,39 +3877,39 @@
     </row>
     <row r="35" ht="37.5" customFormat="1" customHeight="1" s="49">
       <c r="B35" s="53" t="n"/>
-      <c r="C35" s="290" t="inlineStr">
+      <c r="C35" s="283" t="inlineStr">
         <is>
           <t>d</t>
         </is>
       </c>
-      <c r="D35" s="292" t="inlineStr">
+      <c r="D35" s="285" t="inlineStr">
         <is>
           <t xml:space="preserve">FOR INFORMATION ONLY: MONEY RECEIVED AND PASSED ON TO  EXTERNAL ORGANISATIONS                                </t>
         </is>
       </c>
-      <c r="E35" s="293" t="n"/>
-      <c r="F35" s="293" t="n"/>
-      <c r="G35" s="293" t="n"/>
-      <c r="H35" s="293" t="n"/>
-      <c r="I35" s="293" t="n"/>
-      <c r="J35" s="293" t="n"/>
-      <c r="K35" s="293" t="n"/>
-      <c r="L35" s="293" t="n"/>
-      <c r="M35" s="294" t="n"/>
+      <c r="E35" s="286" t="n"/>
+      <c r="F35" s="286" t="n"/>
+      <c r="G35" s="286" t="n"/>
+      <c r="H35" s="286" t="n"/>
+      <c r="I35" s="286" t="n"/>
+      <c r="J35" s="286" t="n"/>
+      <c r="K35" s="286" t="n"/>
+      <c r="L35" s="286" t="n"/>
+      <c r="M35" s="287" t="n"/>
       <c r="P35" s="53" t="n"/>
     </row>
-    <row r="36" ht="13.7" customHeight="1" s="248">
+    <row r="36" ht="13.7" customHeight="1" s="264">
       <c r="B36" s="8" t="n"/>
-      <c r="C36" s="291" t="n"/>
-      <c r="D36" s="287" t="inlineStr">
+      <c r="C36" s="284" t="n"/>
+      <c r="D36" s="299" t="inlineStr">
         <is>
           <t>(these amounts are not to be included in total receipts/payments figures above)</t>
         </is>
       </c>
-      <c r="E36" s="288" t="n"/>
-      <c r="F36" s="288" t="n"/>
-      <c r="G36" s="288" t="n"/>
-      <c r="H36" s="288" t="n"/>
+      <c r="E36" s="300" t="n"/>
+      <c r="F36" s="300" t="n"/>
+      <c r="G36" s="300" t="n"/>
+      <c r="H36" s="300" t="n"/>
       <c r="I36" s="218" t="n"/>
       <c r="J36" s="219" t="inlineStr">
         <is>
@@ -3921,22 +3927,22 @@
       <c r="O36" s="6" t="n"/>
       <c r="P36" s="8" t="n"/>
     </row>
-    <row r="37" ht="31.7" customHeight="1" s="248">
+    <row r="37" ht="31.7" customHeight="1" s="264">
       <c r="B37" s="8" t="n"/>
       <c r="C37" s="50" t="inlineStr">
         <is>
           <t>d1</t>
         </is>
       </c>
-      <c r="D37" s="285" t="inlineStr">
+      <c r="D37" s="298" t="inlineStr">
         <is>
           <t>Balance brought forward from last year</t>
         </is>
       </c>
-      <c r="E37" s="254" t="n"/>
-      <c r="F37" s="254" t="n"/>
-      <c r="G37" s="254" t="n"/>
-      <c r="H37" s="286" t="n"/>
+      <c r="E37" s="276" t="n"/>
+      <c r="F37" s="276" t="n"/>
+      <c r="G37" s="276" t="n"/>
+      <c r="H37" s="282" t="n"/>
       <c r="I37" s="134" t="n"/>
       <c r="J37" s="141">
         <f>+M40</f>
@@ -3949,22 +3955,22 @@
       <c r="O37" s="6" t="n"/>
       <c r="P37" s="8" t="n"/>
     </row>
-    <row r="38" ht="31.7" customHeight="1" s="248">
+    <row r="38" ht="31.7" customHeight="1" s="264">
       <c r="B38" s="8" t="n"/>
       <c r="C38" s="50" t="inlineStr">
         <is>
           <t>d2</t>
         </is>
       </c>
-      <c r="D38" s="285" t="inlineStr">
+      <c r="D38" s="298" t="inlineStr">
         <is>
           <t>Offerings/Gifts - received for external organisations</t>
         </is>
       </c>
-      <c r="E38" s="254" t="n"/>
-      <c r="F38" s="254" t="n"/>
-      <c r="G38" s="254" t="n"/>
-      <c r="H38" s="286" t="n"/>
+      <c r="E38" s="276" t="n"/>
+      <c r="F38" s="276" t="n"/>
+      <c r="G38" s="276" t="n"/>
+      <c r="H38" s="282" t="n"/>
       <c r="I38" s="51" t="n"/>
       <c r="J38" s="141" t="n"/>
       <c r="K38" s="134" t="n"/>
@@ -3973,22 +3979,22 @@
       <c r="N38" s="38" t="n"/>
       <c r="P38" s="8" t="n"/>
     </row>
-    <row r="39" ht="31.7" customHeight="1" s="248" thickBot="1">
+    <row r="39" ht="31.7" customHeight="1" s="264" thickBot="1">
       <c r="B39" s="8" t="n"/>
       <c r="C39" s="50" t="inlineStr">
         <is>
           <t>d3</t>
         </is>
       </c>
-      <c r="D39" s="285" t="inlineStr">
+      <c r="D39" s="298" t="inlineStr">
         <is>
           <t>Offerings/Gifts  - passed to external organisations</t>
         </is>
       </c>
-      <c r="E39" s="254" t="n"/>
-      <c r="F39" s="254" t="n"/>
-      <c r="G39" s="254" t="n"/>
-      <c r="H39" s="286" t="n"/>
+      <c r="E39" s="276" t="n"/>
+      <c r="F39" s="276" t="n"/>
+      <c r="G39" s="276" t="n"/>
+      <c r="H39" s="282" t="n"/>
       <c r="I39" s="51" t="n"/>
       <c r="J39" s="142" t="n"/>
       <c r="K39" s="170" t="n"/>
@@ -3997,22 +4003,22 @@
       <c r="N39" s="38" t="n"/>
       <c r="P39" s="8" t="n"/>
     </row>
-    <row r="40" ht="33.75" customHeight="1" s="248" thickBot="1">
+    <row r="40" ht="33.75" customHeight="1" s="264" thickBot="1">
       <c r="B40" s="8" t="n"/>
       <c r="C40" s="50" t="inlineStr">
         <is>
           <t>d4</t>
         </is>
       </c>
-      <c r="D40" s="281" t="inlineStr">
+      <c r="D40" s="294" t="inlineStr">
         <is>
           <t>BALANCE STILL TO BE PAID                     (d1+d2-d3)</t>
         </is>
       </c>
-      <c r="E40" s="282" t="n"/>
-      <c r="F40" s="282" t="n"/>
-      <c r="G40" s="282" t="n"/>
-      <c r="H40" s="283" t="n"/>
+      <c r="E40" s="295" t="n"/>
+      <c r="F40" s="295" t="n"/>
+      <c r="G40" s="295" t="n"/>
+      <c r="H40" s="296" t="n"/>
       <c r="I40" s="52" t="n"/>
       <c r="J40" s="172">
         <f>SUM(J37+J38-J39)</f>
@@ -4028,11 +4034,11 @@
       <c r="P40" s="8" t="n"/>
       <c r="Q40" s="174" t="n"/>
     </row>
-    <row r="41" ht="6.75" customFormat="1" customHeight="1" s="298">
+    <row r="41" ht="6.75" customFormat="1" customHeight="1" s="291">
       <c r="B41" s="131" t="n"/>
       <c r="P41" s="131" t="n"/>
     </row>
-    <row r="42" ht="2.25" customHeight="1" s="248">
+    <row r="42" ht="2.25" customHeight="1" s="264">
       <c r="B42" s="8" t="n"/>
       <c r="C42" s="8" t="n"/>
       <c r="D42" s="8" t="n"/>
@@ -4049,20 +4055,26 @@
       <c r="O42" s="8" t="n"/>
       <c r="P42" s="8" t="n"/>
     </row>
-    <row r="43" ht="18" customHeight="1" s="248"/>
-    <row r="44" ht="18" customHeight="1" s="248"/>
-    <row r="45" ht="18" customHeight="1" s="248"/>
-    <row r="46" ht="18" customHeight="1" s="248"/>
-    <row r="47" ht="18" customHeight="1" s="248"/>
-    <row r="48" ht="18" customHeight="1" s="248"/>
-    <row r="49" ht="18" customHeight="1" s="248"/>
-    <row r="50" ht="18" customHeight="1" s="248"/>
-    <row r="51" ht="18" customHeight="1" s="248"/>
-    <row r="52" ht="18" customHeight="1" s="248"/>
-    <row r="53" ht="6.75" customHeight="1" s="248"/>
-    <row r="54" ht="6.75" customHeight="1" s="248"/>
+    <row r="43" ht="18" customHeight="1" s="264"/>
+    <row r="44" ht="18" customHeight="1" s="264"/>
+    <row r="45" ht="18" customHeight="1" s="264"/>
+    <row r="46" ht="18" customHeight="1" s="264"/>
+    <row r="47" ht="18" customHeight="1" s="264"/>
+    <row r="48" ht="18" customHeight="1" s="264"/>
+    <row r="49" ht="18" customHeight="1" s="264"/>
+    <row r="50" ht="18" customHeight="1" s="264"/>
+    <row r="51" ht="18" customHeight="1" s="264"/>
+    <row r="52" ht="18" customHeight="1" s="264"/>
+    <row r="53" ht="6.75" customHeight="1" s="264"/>
+    <row r="54" ht="6.75" customHeight="1" s="264"/>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="D40:H40"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D37:H37"/>
+    <mergeCell ref="D38:H38"/>
+    <mergeCell ref="D39:H39"/>
+    <mergeCell ref="D36:H36"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="C35:C36"/>
     <mergeCell ref="D35:M35"/>
@@ -4073,12 +4085,6 @@
     <mergeCell ref="M3:M4"/>
     <mergeCell ref="H2:L2"/>
     <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D40:H40"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D37:H37"/>
-    <mergeCell ref="D38:H38"/>
-    <mergeCell ref="D39:H39"/>
-    <mergeCell ref="D36:H36"/>
   </mergeCells>
   <pageMargins left="0.1574803149606299" right="0.1574803149606299" top="0.2755905511811024" bottom="0.3937007874015748" header="0.1574803149606299" footer="0.2362204724409449"/>
   <pageSetup orientation="portrait" paperSize="9" scale="99"/>
@@ -4107,34 +4113,34 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
   <cols>
-    <col width="1.42578125" customWidth="1" style="248" min="1" max="1"/>
-    <col width="1.140625" customWidth="1" style="248" min="2" max="2"/>
-    <col width="3.42578125" bestFit="1" customWidth="1" style="248" min="3" max="3"/>
-    <col width="25" customWidth="1" style="248" min="4" max="4"/>
-    <col width="1.5703125" customWidth="1" style="248" min="5" max="5"/>
-    <col width="12.85546875" customWidth="1" style="248" min="6" max="6"/>
-    <col width="4" bestFit="1" customWidth="1" style="248" min="7" max="7"/>
-    <col width="0.85546875" customWidth="1" style="248" min="8" max="8"/>
-    <col width="14" customWidth="1" style="248" min="9" max="9"/>
-    <col width="5" customWidth="1" style="248" min="10" max="10"/>
-    <col width="14" customWidth="1" style="248" min="11" max="11"/>
-    <col width="1.42578125" customWidth="1" style="248" min="12" max="12"/>
-    <col width="0.85546875" customWidth="1" style="248" min="13" max="13"/>
-    <col width="15.5703125" customWidth="1" style="248" min="14" max="14"/>
-    <col width="5.5703125" bestFit="1" customWidth="1" style="248" min="15" max="15"/>
-    <col width="0.5703125" customWidth="1" style="248" min="16" max="16"/>
-    <col width="13" customWidth="1" style="248" min="17" max="17"/>
-    <col width="5" bestFit="1" customWidth="1" style="248" min="18" max="18"/>
-    <col width="0.85546875" customWidth="1" style="248" min="19" max="19"/>
-    <col width="15.5703125" customWidth="1" style="248" min="20" max="20"/>
-    <col width="5.85546875" bestFit="1" customWidth="1" style="248" min="21" max="21"/>
-    <col width="1" customWidth="1" style="248" min="22" max="22"/>
-    <col width="9.5703125" customWidth="1" style="248" min="23" max="23"/>
-    <col width="7.85546875" bestFit="1" customWidth="1" style="248" min="25" max="25"/>
-    <col width="2.5703125" customWidth="1" style="248" min="27" max="27"/>
+    <col width="1.42578125" customWidth="1" style="264" min="1" max="1"/>
+    <col width="1.140625" customWidth="1" style="264" min="2" max="2"/>
+    <col width="3.42578125" bestFit="1" customWidth="1" style="264" min="3" max="3"/>
+    <col width="25" customWidth="1" style="264" min="4" max="4"/>
+    <col width="1.5703125" customWidth="1" style="264" min="5" max="5"/>
+    <col width="12.85546875" customWidth="1" style="264" min="6" max="6"/>
+    <col width="4" bestFit="1" customWidth="1" style="264" min="7" max="7"/>
+    <col width="0.85546875" customWidth="1" style="264" min="8" max="8"/>
+    <col width="14" customWidth="1" style="264" min="9" max="9"/>
+    <col width="5" customWidth="1" style="264" min="10" max="10"/>
+    <col width="14" customWidth="1" style="264" min="11" max="11"/>
+    <col width="1.42578125" customWidth="1" style="264" min="12" max="12"/>
+    <col width="0.85546875" customWidth="1" style="264" min="13" max="13"/>
+    <col width="15.5703125" customWidth="1" style="264" min="14" max="14"/>
+    <col width="5.5703125" bestFit="1" customWidth="1" style="264" min="15" max="15"/>
+    <col width="0.5703125" customWidth="1" style="264" min="16" max="16"/>
+    <col width="13" customWidth="1" style="264" min="17" max="17"/>
+    <col width="5" bestFit="1" customWidth="1" style="264" min="18" max="18"/>
+    <col width="0.85546875" customWidth="1" style="264" min="19" max="19"/>
+    <col width="15.5703125" customWidth="1" style="264" min="20" max="20"/>
+    <col width="5.85546875" bestFit="1" customWidth="1" style="264" min="21" max="21"/>
+    <col width="1" customWidth="1" style="264" min="22" max="22"/>
+    <col width="9.5703125" customWidth="1" style="264" min="23" max="23"/>
+    <col width="7.85546875" bestFit="1" customWidth="1" style="264" min="25" max="25"/>
+    <col width="2.5703125" customWidth="1" style="264" min="27" max="27"/>
   </cols>
   <sheetData>
-    <row r="1" ht="8.449999999999999" customHeight="1" s="248">
+    <row r="1" ht="8.449999999999999" customHeight="1" s="264">
       <c r="B1" s="10" t="n"/>
       <c r="C1" s="10" t="n"/>
       <c r="D1" s="53" t="n"/>
@@ -4169,7 +4175,7 @@
       <c r="U1" s="53" t="n"/>
       <c r="V1" s="53" t="n"/>
     </row>
-    <row r="2" ht="27" customHeight="1" s="248">
+    <row r="2" ht="27" customHeight="1" s="264">
       <c r="B2" s="10" t="n"/>
       <c r="C2" s="2" t="n"/>
       <c r="D2" s="49" t="n"/>
@@ -4182,15 +4188,15 @@
       <c r="K2" s="56" t="n"/>
       <c r="L2" s="56" t="n"/>
       <c r="M2" s="56" t="n"/>
-      <c r="N2" s="301">
+      <c r="N2" s="308">
         <f>'P1 Front page'!$C$11</f>
         <v/>
       </c>
-      <c r="O2" s="275" t="n"/>
-      <c r="P2" s="275" t="n"/>
-      <c r="Q2" s="275" t="n"/>
-      <c r="R2" s="275" t="n"/>
-      <c r="S2" s="275" t="n"/>
+      <c r="O2" s="270" t="n"/>
+      <c r="P2" s="270" t="n"/>
+      <c r="Q2" s="270" t="n"/>
+      <c r="R2" s="270" t="n"/>
+      <c r="S2" s="270" t="n"/>
       <c r="T2" s="237" t="inlineStr">
         <is>
           <t>Church</t>
@@ -4204,10 +4210,10 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="25.5" customHeight="1" s="248">
+    <row r="3" ht="25.5" customHeight="1" s="264">
       <c r="B3" s="10" t="n"/>
       <c r="C3" s="2" t="n"/>
-      <c r="D3" s="309" t="inlineStr">
+      <c r="D3" s="305" t="inlineStr">
         <is>
           <t>SUMMARY OF CHURCH ACCOUNTS AND INTERNAL ORGANISATIONS REPORTING TO THE CHURCH COUNCIL</t>
         </is>
@@ -4219,7 +4225,7 @@
       <c r="Y3" s="1" t="n"/>
       <c r="Z3" s="1" t="n"/>
     </row>
-    <row r="4" ht="23.25" customHeight="1" s="248" thickBot="1">
+    <row r="4" ht="23.25" customHeight="1" s="264" thickBot="1">
       <c r="B4" s="10" t="n"/>
       <c r="C4" s="2" t="n"/>
       <c r="D4" s="177" t="inlineStr">
@@ -4250,64 +4256,64 @@
       <c r="U4" s="49" t="n"/>
       <c r="V4" s="53" t="n"/>
     </row>
-    <row r="5" ht="63.75" customHeight="1" s="248">
+    <row r="5" ht="63.75" customHeight="1" s="264">
       <c r="B5" s="10" t="n"/>
       <c r="C5" s="2" t="n"/>
-      <c r="D5" s="303" t="inlineStr">
+      <c r="D5" s="310" t="inlineStr">
         <is>
           <t xml:space="preserve">Summary of the Church accounts for the year ended 31 August 2024 and Internal Organisations reporting to the Church Council/Church Meeting. Note that the funds of an Internal Organisation would normally be Restricted funds unless it could be clearly shown that they could be used for any Methodist purpose.   This section must be completed to arrive at the gross income and expenditure totals of the Church. If gross income exceeds the Accruals threshold, then the Accruals method of accounting AND A DIFFERENT FORM must be used to report the accounts (see Methodist website).  Please refer to the guidance notes regarding transfers between the District and connected  District Organisations. </t>
         </is>
       </c>
-      <c r="E5" s="304" t="n"/>
-      <c r="F5" s="304" t="n"/>
-      <c r="G5" s="304" t="n"/>
-      <c r="H5" s="304" t="n"/>
-      <c r="I5" s="304" t="n"/>
-      <c r="J5" s="304" t="n"/>
-      <c r="K5" s="304" t="n"/>
-      <c r="L5" s="304" t="n"/>
-      <c r="M5" s="304" t="n"/>
-      <c r="N5" s="304" t="n"/>
-      <c r="O5" s="304" t="n"/>
-      <c r="P5" s="304" t="n"/>
-      <c r="Q5" s="304" t="n"/>
-      <c r="R5" s="304" t="n"/>
-      <c r="S5" s="304" t="n"/>
-      <c r="T5" s="305" t="n"/>
+      <c r="E5" s="311" t="n"/>
+      <c r="F5" s="311" t="n"/>
+      <c r="G5" s="311" t="n"/>
+      <c r="H5" s="311" t="n"/>
+      <c r="I5" s="311" t="n"/>
+      <c r="J5" s="311" t="n"/>
+      <c r="K5" s="311" t="n"/>
+      <c r="L5" s="311" t="n"/>
+      <c r="M5" s="311" t="n"/>
+      <c r="N5" s="311" t="n"/>
+      <c r="O5" s="311" t="n"/>
+      <c r="P5" s="311" t="n"/>
+      <c r="Q5" s="311" t="n"/>
+      <c r="R5" s="311" t="n"/>
+      <c r="S5" s="311" t="n"/>
+      <c r="T5" s="312" t="n"/>
       <c r="U5" s="316" t="n"/>
       <c r="V5" s="53" t="n"/>
     </row>
-    <row r="6" ht="3.75" customHeight="1" s="248" thickBot="1">
+    <row r="6" ht="3.75" customHeight="1" s="264" thickBot="1">
       <c r="B6" s="10" t="n"/>
       <c r="C6" s="2" t="n"/>
-      <c r="D6" s="311" t="n"/>
-      <c r="E6" s="282" t="n"/>
-      <c r="F6" s="282" t="n"/>
-      <c r="G6" s="282" t="n"/>
-      <c r="H6" s="282" t="n"/>
-      <c r="I6" s="282" t="n"/>
-      <c r="J6" s="282" t="n"/>
-      <c r="K6" s="282" t="n"/>
-      <c r="L6" s="282" t="n"/>
-      <c r="M6" s="282" t="n"/>
-      <c r="N6" s="282" t="n"/>
-      <c r="O6" s="282" t="n"/>
-      <c r="P6" s="282" t="n"/>
-      <c r="Q6" s="282" t="n"/>
-      <c r="R6" s="282" t="n"/>
-      <c r="S6" s="282" t="n"/>
-      <c r="T6" s="283" t="n"/>
+      <c r="D6" s="306" t="n"/>
+      <c r="E6" s="295" t="n"/>
+      <c r="F6" s="295" t="n"/>
+      <c r="G6" s="295" t="n"/>
+      <c r="H6" s="295" t="n"/>
+      <c r="I6" s="295" t="n"/>
+      <c r="J6" s="295" t="n"/>
+      <c r="K6" s="295" t="n"/>
+      <c r="L6" s="295" t="n"/>
+      <c r="M6" s="295" t="n"/>
+      <c r="N6" s="295" t="n"/>
+      <c r="O6" s="295" t="n"/>
+      <c r="P6" s="295" t="n"/>
+      <c r="Q6" s="295" t="n"/>
+      <c r="R6" s="295" t="n"/>
+      <c r="S6" s="295" t="n"/>
+      <c r="T6" s="296" t="n"/>
       <c r="U6" s="316" t="n"/>
       <c r="V6" s="53" t="n"/>
     </row>
-    <row r="7" ht="6" customHeight="1" s="248">
+    <row r="7" ht="6" customHeight="1" s="264">
       <c r="B7" s="10" t="n"/>
       <c r="C7" s="2" t="n"/>
-      <c r="D7" s="302" t="n"/>
+      <c r="D7" s="309" t="n"/>
       <c r="U7" s="316" t="n"/>
       <c r="V7" s="53" t="n"/>
     </row>
-    <row r="8" ht="35.45" customHeight="1" s="248">
+    <row r="8" ht="35.45" customHeight="1" s="264">
       <c r="B8" s="10" t="n"/>
       <c r="C8" s="2" t="n"/>
       <c r="D8" s="179" t="inlineStr">
@@ -4358,7 +4364,7 @@
       <c r="U8" s="60" t="n"/>
       <c r="V8" s="53" t="n"/>
     </row>
-    <row r="9" ht="24.75" customHeight="1" s="248">
+    <row r="9" ht="24.75" customHeight="1" s="264">
       <c r="B9" s="10" t="n"/>
       <c r="C9" s="16" t="inlineStr">
         <is>
@@ -4391,7 +4397,7 @@
       <c r="U9" s="62" t="n"/>
       <c r="V9" s="53" t="n"/>
     </row>
-    <row r="10" ht="24.75" customHeight="1" s="248">
+    <row r="10" ht="24.75" customHeight="1" s="264">
       <c r="B10" s="10" t="n"/>
       <c r="C10" s="16" t="inlineStr">
         <is>
@@ -4424,7 +4430,7 @@
       <c r="U10" s="62" t="n"/>
       <c r="V10" s="53" t="n"/>
     </row>
-    <row r="11" ht="24.75" customHeight="1" s="248">
+    <row r="11" ht="24.75" customHeight="1" s="264">
       <c r="B11" s="10" t="n"/>
       <c r="C11" s="16" t="inlineStr">
         <is>
@@ -4457,7 +4463,7 @@
       <c r="U11" s="62" t="n"/>
       <c r="V11" s="53" t="n"/>
     </row>
-    <row r="12" ht="24.75" customHeight="1" s="248">
+    <row r="12" ht="24.75" customHeight="1" s="264">
       <c r="B12" s="10" t="n"/>
       <c r="C12" s="16" t="inlineStr">
         <is>
@@ -4490,7 +4496,7 @@
       <c r="U12" s="62" t="n"/>
       <c r="V12" s="53" t="n"/>
     </row>
-    <row r="13" ht="24.75" customHeight="1" s="248">
+    <row r="13" ht="24.75" customHeight="1" s="264">
       <c r="B13" s="10" t="n"/>
       <c r="C13" s="16" t="inlineStr">
         <is>
@@ -4523,7 +4529,7 @@
       <c r="U13" s="62" t="n"/>
       <c r="V13" s="53" t="n"/>
     </row>
-    <row r="14" ht="24.75" customHeight="1" s="248">
+    <row r="14" ht="24.75" customHeight="1" s="264">
       <c r="B14" s="10" t="n"/>
       <c r="C14" s="16" t="inlineStr">
         <is>
@@ -4556,7 +4562,7 @@
       <c r="U14" s="62" t="n"/>
       <c r="V14" s="53" t="n"/>
     </row>
-    <row r="15" ht="24.75" customHeight="1" s="248" thickBot="1">
+    <row r="15" ht="24.75" customHeight="1" s="264" thickBot="1">
       <c r="B15" s="10" t="n"/>
       <c r="C15" s="16" t="inlineStr">
         <is>
@@ -4589,7 +4595,7 @@
       <c r="U15" s="62" t="n"/>
       <c r="V15" s="53" t="n"/>
     </row>
-    <row r="16" ht="25.5" customHeight="1" s="248">
+    <row r="16" ht="25.5" customHeight="1" s="264">
       <c r="B16" s="10" t="n"/>
       <c r="C16" s="16" t="inlineStr">
         <is>
@@ -4655,7 +4661,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" ht="55.5" customHeight="1" s="248" thickBot="1">
+    <row r="17" ht="55.5" customHeight="1" s="264" thickBot="1">
       <c r="B17" s="10" t="n"/>
       <c r="C17" s="16" t="inlineStr">
         <is>
@@ -4730,14 +4736,14 @@
         <v/>
       </c>
     </row>
-    <row r="18" ht="27.75" customHeight="1" s="248" thickBot="1" thickTop="1">
+    <row r="18" ht="27.75" customHeight="1" s="264" thickBot="1" thickTop="1">
       <c r="B18" s="10" t="n"/>
       <c r="C18" s="16" t="inlineStr">
         <is>
           <t>e10</t>
         </is>
       </c>
-      <c r="D18" s="312" t="inlineStr">
+      <c r="D18" s="307" t="inlineStr">
         <is>
           <t>TOTAL CASH FUNDS HELD BY CHURCH</t>
         </is>
@@ -4797,7 +4803,7 @@
       </c>
       <c r="Z18" s="25" t="n"/>
     </row>
-    <row r="19" ht="3.75" customHeight="1" s="248" thickBot="1" thickTop="1">
+    <row r="19" ht="3.75" customHeight="1" s="264" thickBot="1" thickTop="1">
       <c r="B19" s="10" t="n"/>
       <c r="C19" s="2" t="n"/>
       <c r="D19" s="49" t="n"/>
@@ -4820,7 +4826,7 @@
       <c r="U19" s="62" t="n"/>
       <c r="V19" s="53" t="n"/>
     </row>
-    <row r="20" ht="39.2" customHeight="1" s="248" thickBot="1">
+    <row r="20" ht="39.2" customHeight="1" s="264" thickBot="1">
       <c r="B20" s="10" t="n"/>
       <c r="C20" s="2" t="n"/>
       <c r="D20" s="197" t="inlineStr">
@@ -4829,12 +4835,12 @@
         </is>
       </c>
       <c r="E20" s="49" t="n"/>
-      <c r="F20" s="306" t="inlineStr">
+      <c r="F20" s="313" t="inlineStr">
         <is>
           <t>TOTAL RECEIPTS</t>
         </is>
       </c>
-      <c r="G20" s="307" t="n"/>
+      <c r="G20" s="314" t="n"/>
       <c r="H20" s="185" t="n"/>
       <c r="I20" s="211" t="inlineStr">
         <is>
@@ -4848,14 +4854,14 @@
       <c r="N20" s="49" t="n"/>
       <c r="O20" s="62" t="n"/>
       <c r="P20" s="62" t="n"/>
-      <c r="Q20" s="318" t="n"/>
-      <c r="R20" s="318" t="n"/>
-      <c r="S20" s="318" t="n"/>
-      <c r="T20" s="319" t="n"/>
-      <c r="U20" s="318" t="n"/>
-      <c r="V20" s="320" t="n"/>
-    </row>
-    <row r="21" ht="5.25" customHeight="1" s="248">
+      <c r="Q20" s="320" t="n"/>
+      <c r="R20" s="320" t="n"/>
+      <c r="S20" s="320" t="n"/>
+      <c r="T20" s="321" t="n"/>
+      <c r="U20" s="320" t="n"/>
+      <c r="V20" s="322" t="n"/>
+    </row>
+    <row r="21" ht="5.25" customHeight="1" s="264">
       <c r="B21" s="10" t="n"/>
       <c r="C21" s="2" t="n"/>
       <c r="D21" s="49" t="n"/>
@@ -4878,20 +4884,20 @@
       <c r="U21" s="62" t="n"/>
       <c r="V21" s="53" t="n"/>
     </row>
-    <row r="22" ht="3.2" customHeight="1" s="248" thickBot="1">
+    <row r="22" ht="3.2" customHeight="1" s="264" thickBot="1">
       <c r="B22" s="10" t="n"/>
       <c r="C22" s="15" t="n"/>
-      <c r="D22" s="321" t="n"/>
-      <c r="E22" s="321" t="n"/>
-      <c r="F22" s="321" t="n"/>
-      <c r="G22" s="321" t="n"/>
-      <c r="H22" s="321" t="n"/>
-      <c r="I22" s="321" t="n"/>
-      <c r="J22" s="321" t="n"/>
-      <c r="K22" s="321" t="n"/>
-      <c r="L22" s="321" t="n"/>
-      <c r="M22" s="322" t="n"/>
-      <c r="N22" s="322" t="n"/>
+      <c r="D22" s="323" t="n"/>
+      <c r="E22" s="323" t="n"/>
+      <c r="F22" s="323" t="n"/>
+      <c r="G22" s="323" t="n"/>
+      <c r="H22" s="323" t="n"/>
+      <c r="I22" s="323" t="n"/>
+      <c r="J22" s="323" t="n"/>
+      <c r="K22" s="323" t="n"/>
+      <c r="L22" s="323" t="n"/>
+      <c r="M22" s="324" t="n"/>
+      <c r="N22" s="324" t="n"/>
       <c r="O22" s="82" t="n"/>
       <c r="P22" s="82" t="n"/>
       <c r="Q22" s="82" t="n"/>
@@ -4901,20 +4907,20 @@
       <c r="U22" s="82" t="n"/>
       <c r="V22" s="53" t="n"/>
     </row>
-    <row r="23" ht="4.7" customHeight="1" s="248" thickTop="1">
+    <row r="23" ht="4.7" customHeight="1" s="264" thickTop="1">
       <c r="B23" s="10" t="n"/>
       <c r="C23" s="2" t="n"/>
-      <c r="D23" s="323" t="n"/>
-      <c r="E23" s="323" t="n"/>
-      <c r="F23" s="323" t="n"/>
-      <c r="G23" s="323" t="n"/>
-      <c r="H23" s="323" t="n"/>
-      <c r="I23" s="323" t="n"/>
-      <c r="J23" s="323" t="n"/>
-      <c r="K23" s="323" t="n"/>
-      <c r="L23" s="323" t="n"/>
-      <c r="M23" s="324" t="n"/>
-      <c r="N23" s="324" t="n"/>
+      <c r="D23" s="325" t="n"/>
+      <c r="E23" s="325" t="n"/>
+      <c r="F23" s="325" t="n"/>
+      <c r="G23" s="325" t="n"/>
+      <c r="H23" s="325" t="n"/>
+      <c r="I23" s="325" t="n"/>
+      <c r="J23" s="325" t="n"/>
+      <c r="K23" s="325" t="n"/>
+      <c r="L23" s="325" t="n"/>
+      <c r="M23" s="326" t="n"/>
+      <c r="N23" s="326" t="n"/>
       <c r="O23" s="62" t="n"/>
       <c r="P23" s="62" t="n"/>
       <c r="Q23" s="62" t="n"/>
@@ -4924,7 +4930,7 @@
       <c r="U23" s="62" t="n"/>
       <c r="V23" s="53" t="n"/>
     </row>
-    <row r="24" ht="23.25" customHeight="1" s="248" thickBot="1">
+    <row r="24" ht="23.25" customHeight="1" s="264" thickBot="1">
       <c r="B24" s="10" t="n"/>
       <c r="C24" s="2" t="n"/>
       <c r="D24" s="177" t="inlineStr">
@@ -4932,16 +4938,16 @@
           <t>SECTION F</t>
         </is>
       </c>
-      <c r="E24" s="323" t="n"/>
-      <c r="F24" s="323" t="n"/>
-      <c r="G24" s="323" t="n"/>
-      <c r="H24" s="323" t="n"/>
-      <c r="I24" s="323" t="n"/>
-      <c r="J24" s="323" t="n"/>
-      <c r="K24" s="323" t="n"/>
-      <c r="L24" s="323" t="n"/>
-      <c r="M24" s="323" t="n"/>
-      <c r="N24" s="323" t="n"/>
+      <c r="E24" s="325" t="n"/>
+      <c r="F24" s="325" t="n"/>
+      <c r="G24" s="325" t="n"/>
+      <c r="H24" s="325" t="n"/>
+      <c r="I24" s="325" t="n"/>
+      <c r="J24" s="325" t="n"/>
+      <c r="K24" s="325" t="n"/>
+      <c r="L24" s="325" t="n"/>
+      <c r="M24" s="325" t="n"/>
+      <c r="N24" s="325" t="n"/>
       <c r="O24" s="185" t="n"/>
       <c r="P24" s="185" t="n"/>
       <c r="Q24" s="185" t="n"/>
@@ -4951,7 +4957,7 @@
       <c r="U24" s="62" t="n"/>
       <c r="V24" s="53" t="n"/>
     </row>
-    <row r="25" ht="21.2" customHeight="1" s="248">
+    <row r="25" ht="21.2" customHeight="1" s="264">
       <c r="B25" s="10" t="n"/>
       <c r="C25" s="2" t="n"/>
       <c r="D25" s="199" t="inlineStr">
@@ -4978,9 +4984,9 @@
       <c r="U25" s="85" t="n"/>
       <c r="V25" s="53" t="n"/>
     </row>
-    <row r="26" ht="30.75" customHeight="1" s="248">
+    <row r="26" ht="30.75" customHeight="1" s="264">
       <c r="B26" s="10" t="n"/>
-      <c r="C26" s="296" t="n"/>
+      <c r="C26" s="289" t="n"/>
       <c r="D26" s="12" t="inlineStr">
         <is>
           <t>CHURCH - CASH FUNDS HELD at 31 August 2024</t>
@@ -5013,22 +5019,22 @@
       <c r="U26" s="39" t="n"/>
       <c r="V26" s="53" t="n"/>
     </row>
-    <row r="27" ht="24.75" customHeight="1" s="248">
+    <row r="27" ht="24.75" customHeight="1" s="264">
       <c r="B27" s="10" t="n"/>
       <c r="C27" s="5" t="inlineStr">
         <is>
           <t>f1</t>
         </is>
       </c>
-      <c r="D27" s="308" t="inlineStr">
+      <c r="D27" s="302" t="inlineStr">
         <is>
           <t>Cash in hand</t>
         </is>
       </c>
-      <c r="E27" s="254" t="n"/>
-      <c r="F27" s="254" t="n"/>
-      <c r="G27" s="254" t="n"/>
-      <c r="H27" s="286" t="n"/>
+      <c r="E27" s="276" t="n"/>
+      <c r="F27" s="276" t="n"/>
+      <c r="G27" s="276" t="n"/>
+      <c r="H27" s="282" t="n"/>
       <c r="I27" s="87" t="n"/>
       <c r="J27" s="49" t="n"/>
       <c r="K27" s="49" t="n"/>
@@ -5044,22 +5050,22 @@
       <c r="U27" s="93" t="n"/>
       <c r="V27" s="53" t="n"/>
     </row>
-    <row r="28" ht="24.75" customHeight="1" s="248">
+    <row r="28" ht="24.75" customHeight="1" s="264">
       <c r="B28" s="10" t="n"/>
       <c r="C28" s="5" t="inlineStr">
         <is>
           <t>f2</t>
         </is>
       </c>
-      <c r="D28" s="308" t="inlineStr">
+      <c r="D28" s="302" t="inlineStr">
         <is>
           <t>Bank Current Account</t>
         </is>
       </c>
-      <c r="E28" s="254" t="n"/>
-      <c r="F28" s="254" t="n"/>
-      <c r="G28" s="254" t="n"/>
-      <c r="H28" s="286" t="n"/>
+      <c r="E28" s="276" t="n"/>
+      <c r="F28" s="276" t="n"/>
+      <c r="G28" s="276" t="n"/>
+      <c r="H28" s="282" t="n"/>
       <c r="I28" s="93" t="n"/>
       <c r="J28" s="38" t="n"/>
       <c r="K28" s="38" t="n"/>
@@ -5075,22 +5081,22 @@
       <c r="U28" s="93" t="n"/>
       <c r="V28" s="53" t="n"/>
     </row>
-    <row r="29" ht="24.75" customHeight="1" s="248">
+    <row r="29" ht="24.75" customHeight="1" s="264">
       <c r="B29" s="10" t="n"/>
       <c r="C29" s="5" t="inlineStr">
         <is>
           <t>f3</t>
         </is>
       </c>
-      <c r="D29" s="308" t="inlineStr">
+      <c r="D29" s="302" t="inlineStr">
         <is>
           <t>Bank Deposit Account</t>
         </is>
       </c>
-      <c r="E29" s="254" t="n"/>
-      <c r="F29" s="254" t="n"/>
-      <c r="G29" s="254" t="n"/>
-      <c r="H29" s="286" t="n"/>
+      <c r="E29" s="276" t="n"/>
+      <c r="F29" s="276" t="n"/>
+      <c r="G29" s="276" t="n"/>
+      <c r="H29" s="282" t="n"/>
       <c r="I29" s="93" t="n"/>
       <c r="J29" s="38" t="n"/>
       <c r="K29" s="38" t="n"/>
@@ -5106,22 +5112,22 @@
       <c r="U29" s="93" t="n"/>
       <c r="V29" s="53" t="n"/>
     </row>
-    <row r="30" ht="24.75" customHeight="1" s="248">
+    <row r="30" ht="24.75" customHeight="1" s="264">
       <c r="B30" s="10" t="n"/>
       <c r="C30" s="5" t="inlineStr">
         <is>
           <t>f4</t>
         </is>
       </c>
-      <c r="D30" s="308" t="inlineStr">
+      <c r="D30" s="302" t="inlineStr">
         <is>
           <t>Central Finance Board</t>
         </is>
       </c>
-      <c r="E30" s="254" t="n"/>
-      <c r="F30" s="254" t="n"/>
-      <c r="G30" s="254" t="n"/>
-      <c r="H30" s="286" t="n"/>
+      <c r="E30" s="276" t="n"/>
+      <c r="F30" s="276" t="n"/>
+      <c r="G30" s="276" t="n"/>
+      <c r="H30" s="282" t="n"/>
       <c r="I30" s="93" t="n"/>
       <c r="J30" s="38" t="n"/>
       <c r="K30" s="38" t="n"/>
@@ -5137,22 +5143,22 @@
       <c r="U30" s="93" t="n"/>
       <c r="V30" s="53" t="n"/>
     </row>
-    <row r="31" ht="24.75" customHeight="1" s="248">
+    <row r="31" ht="24.75" customHeight="1" s="264">
       <c r="B31" s="9" t="n"/>
       <c r="C31" s="5" t="inlineStr">
         <is>
           <t>f5</t>
         </is>
       </c>
-      <c r="D31" s="308" t="inlineStr">
+      <c r="D31" s="302" t="inlineStr">
         <is>
           <t>Trustees for Methodist Church Purposes</t>
         </is>
       </c>
-      <c r="E31" s="254" t="n"/>
-      <c r="F31" s="254" t="n"/>
-      <c r="G31" s="254" t="n"/>
-      <c r="H31" s="286" t="n"/>
+      <c r="E31" s="276" t="n"/>
+      <c r="F31" s="276" t="n"/>
+      <c r="G31" s="276" t="n"/>
+      <c r="H31" s="282" t="n"/>
       <c r="I31" s="93" t="n"/>
       <c r="J31" s="38" t="n"/>
       <c r="K31" s="38" t="n"/>
@@ -5168,22 +5174,22 @@
       <c r="U31" s="93" t="n"/>
       <c r="V31" s="53" t="n"/>
     </row>
-    <row r="32" ht="24.75" customHeight="1" s="248" thickBot="1">
+    <row r="32" ht="24.75" customHeight="1" s="264" thickBot="1">
       <c r="B32" s="9" t="n"/>
       <c r="C32" s="5" t="inlineStr">
         <is>
           <t>f6</t>
         </is>
       </c>
-      <c r="D32" s="308" t="inlineStr">
+      <c r="D32" s="302" t="inlineStr">
         <is>
           <t>Other funds</t>
         </is>
       </c>
-      <c r="E32" s="254" t="n"/>
-      <c r="F32" s="254" t="n"/>
-      <c r="G32" s="254" t="n"/>
-      <c r="H32" s="286" t="n"/>
+      <c r="E32" s="276" t="n"/>
+      <c r="F32" s="276" t="n"/>
+      <c r="G32" s="276" t="n"/>
+      <c r="H32" s="282" t="n"/>
       <c r="I32" s="93" t="n"/>
       <c r="J32" s="38" t="n"/>
       <c r="K32" s="38" t="n"/>
@@ -5199,22 +5205,22 @@
       <c r="U32" s="97" t="n"/>
       <c r="V32" s="53" t="n"/>
     </row>
-    <row r="33" ht="30.2" customHeight="1" s="248">
+    <row r="33" ht="30.2" customHeight="1" s="264">
       <c r="B33" s="9" t="n"/>
       <c r="C33" s="5" t="inlineStr">
         <is>
           <t>f7</t>
         </is>
       </c>
-      <c r="D33" s="312" t="inlineStr">
+      <c r="D33" s="307" t="inlineStr">
         <is>
           <t xml:space="preserve">SUB TOTAL - Church accounts </t>
         </is>
       </c>
-      <c r="E33" s="254" t="n"/>
-      <c r="F33" s="254" t="n"/>
-      <c r="G33" s="254" t="n"/>
-      <c r="H33" s="286" t="n"/>
+      <c r="E33" s="276" t="n"/>
+      <c r="F33" s="276" t="n"/>
+      <c r="G33" s="276" t="n"/>
+      <c r="H33" s="282" t="n"/>
       <c r="I33" s="93" t="n"/>
       <c r="J33" s="38" t="n"/>
       <c r="K33" s="38" t="n"/>
@@ -5244,22 +5250,22 @@
       </c>
       <c r="V33" s="53" t="n"/>
     </row>
-    <row r="34" ht="32.25" customHeight="1" s="248" thickBot="1">
+    <row r="34" ht="32.25" customHeight="1" s="264" thickBot="1">
       <c r="B34" s="9" t="n"/>
       <c r="C34" s="5" t="inlineStr">
         <is>
           <t>f8</t>
         </is>
       </c>
-      <c r="D34" s="308" t="inlineStr">
+      <c r="D34" s="302" t="inlineStr">
         <is>
           <t>Total funds held by Internal Organisations (the closing balance total from above) (e12)</t>
         </is>
       </c>
-      <c r="E34" s="254" t="n"/>
-      <c r="F34" s="254" t="n"/>
-      <c r="G34" s="254" t="n"/>
-      <c r="H34" s="286" t="n"/>
+      <c r="E34" s="276" t="n"/>
+      <c r="F34" s="276" t="n"/>
+      <c r="G34" s="276" t="n"/>
+      <c r="H34" s="282" t="n"/>
       <c r="I34" s="93" t="n"/>
       <c r="J34" s="38" t="n"/>
       <c r="K34" s="38" t="n"/>
@@ -5299,22 +5305,22 @@
         </is>
       </c>
     </row>
-    <row r="35" ht="30.2" customHeight="1" s="248" thickBot="1" thickTop="1">
+    <row r="35" ht="30.2" customHeight="1" s="264" thickBot="1" thickTop="1">
       <c r="B35" s="9" t="n"/>
       <c r="C35" s="5" t="inlineStr">
         <is>
           <t>f9</t>
         </is>
       </c>
-      <c r="D35" s="312" t="inlineStr">
+      <c r="D35" s="307" t="inlineStr">
         <is>
           <t>TOTAL CASH FUNDS HELD BY CHURCH</t>
         </is>
       </c>
-      <c r="E35" s="254" t="n"/>
-      <c r="F35" s="254" t="n"/>
-      <c r="G35" s="254" t="n"/>
-      <c r="H35" s="286" t="n"/>
+      <c r="E35" s="276" t="n"/>
+      <c r="F35" s="276" t="n"/>
+      <c r="G35" s="276" t="n"/>
+      <c r="H35" s="282" t="n"/>
       <c r="I35" s="93" t="n"/>
       <c r="J35" s="38" t="n"/>
       <c r="K35" s="38" t="n"/>
@@ -5357,7 +5363,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" ht="9" customHeight="1" s="248" thickBot="1" thickTop="1">
+    <row r="36" ht="9" customHeight="1" s="264" thickBot="1" thickTop="1">
       <c r="B36" s="9" t="n"/>
       <c r="C36" s="27" t="n"/>
       <c r="D36" s="203" t="n"/>
@@ -5380,9 +5386,9 @@
       <c r="U36" s="113" t="n"/>
       <c r="V36" s="53" t="n"/>
     </row>
-    <row r="37" ht="6.75" customHeight="1" s="248" thickTop="1">
+    <row r="37" ht="6.75" customHeight="1" s="264" thickTop="1">
       <c r="B37" s="9" t="n"/>
-      <c r="C37" s="296" t="n"/>
+      <c r="C37" s="289" t="n"/>
       <c r="D37" s="204" t="n"/>
       <c r="E37" s="204" t="n"/>
       <c r="F37" s="204" t="n"/>
@@ -5403,9 +5409,9 @@
       <c r="U37" s="115" t="n"/>
       <c r="V37" s="53" t="n"/>
     </row>
-    <row r="38" ht="23.25" customHeight="1" s="248" thickBot="1">
+    <row r="38" ht="23.25" customHeight="1" s="264" thickBot="1">
       <c r="B38" s="9" t="n"/>
-      <c r="C38" s="296" t="n"/>
+      <c r="C38" s="289" t="n"/>
       <c r="D38" s="177" t="inlineStr">
         <is>
           <t>SECTION G</t>
@@ -5438,9 +5444,9 @@
       <c r="U38" s="115" t="n"/>
       <c r="V38" s="53" t="n"/>
     </row>
-    <row r="39" ht="24" customHeight="1" s="248">
+    <row r="39" ht="24" customHeight="1" s="264">
       <c r="B39" s="9" t="n"/>
-      <c r="C39" s="296" t="n"/>
+      <c r="C39" s="289" t="n"/>
       <c r="D39" s="12" t="inlineStr">
         <is>
           <t>OTHER ASSETS and LIABILITIES</t>
@@ -5473,20 +5479,20 @@
       <c r="U39" s="49" t="n"/>
       <c r="V39" s="53" t="n"/>
     </row>
-    <row r="40" ht="30.2" customHeight="1" s="248">
+    <row r="40" ht="30.2" customHeight="1" s="264">
       <c r="B40" s="9" t="n"/>
       <c r="C40" s="5" t="inlineStr">
         <is>
           <t>g1</t>
         </is>
       </c>
-      <c r="D40" s="314" t="inlineStr">
+      <c r="D40" s="304" t="inlineStr">
         <is>
           <t>Investments (include Endowments)</t>
         </is>
       </c>
-      <c r="E40" s="254" t="n"/>
-      <c r="F40" s="254" t="n"/>
+      <c r="E40" s="276" t="n"/>
+      <c r="F40" s="276" t="n"/>
       <c r="G40" s="235" t="n"/>
       <c r="H40" s="205" t="n"/>
       <c r="I40" s="117" t="n"/>
@@ -5504,20 +5510,20 @@
       <c r="U40" s="121" t="n"/>
       <c r="V40" s="53" t="n"/>
     </row>
-    <row r="41" ht="32.25" customHeight="1" s="248">
+    <row r="41" ht="32.25" customHeight="1" s="264">
       <c r="B41" s="9" t="n"/>
       <c r="C41" s="5" t="inlineStr">
         <is>
           <t>g2</t>
         </is>
       </c>
-      <c r="D41" s="310" t="inlineStr">
+      <c r="D41" s="303" t="inlineStr">
         <is>
           <t>Land &amp; Buildings (see notes re Insurance value)</t>
         </is>
       </c>
-      <c r="E41" s="254" t="n"/>
-      <c r="F41" s="254" t="n"/>
+      <c r="E41" s="276" t="n"/>
+      <c r="F41" s="276" t="n"/>
       <c r="G41" s="234" t="n"/>
       <c r="H41" s="206" t="n"/>
       <c r="I41" s="122" t="n"/>
@@ -5535,14 +5541,14 @@
       <c r="U41" s="126" t="n"/>
       <c r="V41" s="53" t="n"/>
     </row>
-    <row r="42" ht="30.2" customHeight="1" s="248">
+    <row r="42" ht="30.2" customHeight="1" s="264">
       <c r="B42" s="9" t="n"/>
       <c r="C42" s="5" t="inlineStr">
         <is>
           <t>g3</t>
         </is>
       </c>
-      <c r="D42" s="310" t="inlineStr">
+      <c r="D42" s="303" t="inlineStr">
         <is>
           <t>Other Assets</t>
         </is>
@@ -5566,7 +5572,7 @@
       <c r="U42" s="126" t="n"/>
       <c r="V42" s="53" t="n"/>
     </row>
-    <row r="43" ht="30.2" customHeight="1" s="248">
+    <row r="43" ht="30.2" customHeight="1" s="264">
       <c r="A43" s="12" t="n"/>
       <c r="B43" s="13" t="n"/>
       <c r="C43" s="5" t="inlineStr">
@@ -5574,15 +5580,15 @@
           <t>g4</t>
         </is>
       </c>
-      <c r="D43" s="308" t="inlineStr">
+      <c r="D43" s="302" t="inlineStr">
         <is>
           <t>Loan(s) - show amount outstanding at year end</t>
         </is>
       </c>
-      <c r="E43" s="254" t="n"/>
-      <c r="F43" s="254" t="n"/>
-      <c r="G43" s="254" t="n"/>
-      <c r="H43" s="286" t="n"/>
+      <c r="E43" s="276" t="n"/>
+      <c r="F43" s="276" t="n"/>
+      <c r="G43" s="276" t="n"/>
+      <c r="H43" s="282" t="n"/>
       <c r="I43" s="127" t="n"/>
       <c r="J43" s="127" t="n"/>
       <c r="K43" s="127" t="n"/>
@@ -5598,20 +5604,20 @@
       <c r="U43" s="126" t="n"/>
       <c r="V43" s="53" t="n"/>
     </row>
-    <row r="44" ht="30.2" customHeight="1" s="248">
+    <row r="44" ht="30.2" customHeight="1" s="264">
       <c r="B44" s="9" t="n"/>
       <c r="C44" s="5" t="inlineStr">
         <is>
           <t>g5</t>
         </is>
       </c>
-      <c r="D44" s="310" t="inlineStr">
+      <c r="D44" s="303" t="inlineStr">
         <is>
           <t xml:space="preserve">Other  Liabilities                </t>
         </is>
       </c>
-      <c r="E44" s="254" t="n"/>
-      <c r="F44" s="254" t="n"/>
+      <c r="E44" s="276" t="n"/>
+      <c r="F44" s="276" t="n"/>
       <c r="G44" s="234" t="n"/>
       <c r="H44" s="207" t="n"/>
       <c r="I44" s="45" t="n"/>
@@ -5631,7 +5637,7 @@
     </row>
     <row r="45">
       <c r="B45" s="9" t="n"/>
-      <c r="C45" s="296" t="n"/>
+      <c r="C45" s="289" t="n"/>
       <c r="D45" s="38" t="n"/>
       <c r="E45" s="38" t="n"/>
       <c r="F45" s="38" t="n"/>
@@ -5652,7 +5658,7 @@
       <c r="U45" s="38" t="n"/>
       <c r="V45" s="53" t="n"/>
     </row>
-    <row r="46" ht="3.2" customHeight="1" s="248">
+    <row r="46" ht="3.2" customHeight="1" s="264">
       <c r="B46" s="9" t="n"/>
       <c r="D46" s="49" t="n"/>
       <c r="E46" s="49" t="n"/>
@@ -5676,7 +5682,7 @@
     </row>
     <row r="47">
       <c r="B47" s="9" t="n"/>
-      <c r="D47" s="313" t="inlineStr">
+      <c r="D47" s="301" t="inlineStr">
         <is>
           <t>f4 Include only Funds held at the Central Finance Board</t>
         </is>
@@ -5695,7 +5701,7 @@
     </row>
     <row r="48">
       <c r="B48" s="9" t="n"/>
-      <c r="D48" s="313" t="inlineStr">
+      <c r="D48" s="301" t="inlineStr">
         <is>
           <t>f5 Include only Funds held at Trustees for Methodist Church Purposes</t>
         </is>
@@ -5738,7 +5744,7 @@
       <c r="U49" s="49" t="n"/>
       <c r="V49" s="53" t="n"/>
     </row>
-    <row r="50" ht="3.2" customHeight="1" s="248">
+    <row r="50" ht="3.2" customHeight="1" s="264">
       <c r="B50" s="9" t="n"/>
       <c r="C50" s="9" t="n"/>
       <c r="D50" s="9" t="n"/>
@@ -5763,6 +5769,18 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="N2:S2"/>
+    <mergeCell ref="D7:T7"/>
+    <mergeCell ref="D5:T5"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="D27:H27"/>
+    <mergeCell ref="D29:H29"/>
+    <mergeCell ref="D3:T3"/>
+    <mergeCell ref="D41:F41"/>
+    <mergeCell ref="D6:T6"/>
+    <mergeCell ref="D33:H33"/>
+    <mergeCell ref="D35:H35"/>
+    <mergeCell ref="D28:H28"/>
     <mergeCell ref="D48:K48"/>
     <mergeCell ref="D30:H30"/>
     <mergeCell ref="D31:H31"/>
@@ -5772,18 +5790,6 @@
     <mergeCell ref="D47:K47"/>
     <mergeCell ref="D40:F40"/>
     <mergeCell ref="D43:H43"/>
-    <mergeCell ref="D29:H29"/>
-    <mergeCell ref="D3:T3"/>
-    <mergeCell ref="D41:F41"/>
-    <mergeCell ref="D6:T6"/>
-    <mergeCell ref="D33:H33"/>
-    <mergeCell ref="D35:H35"/>
-    <mergeCell ref="D28:H28"/>
-    <mergeCell ref="N2:S2"/>
-    <mergeCell ref="D7:T7"/>
-    <mergeCell ref="D5:T5"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="D27:H27"/>
   </mergeCells>
   <pageMargins left="0.1574803149606299" right="0.1574803149606299" top="0.2755905511811024" bottom="0.3543307086614174" header="0.1574803149606299" footer="0.1574803149606299"/>
   <pageSetup orientation="portrait" paperSize="9" scale="59"/>
@@ -5812,7 +5818,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
   <sheetData>
-    <row r="2" ht="15" customHeight="1" s="248">
+    <row r="2" ht="15" customHeight="1" s="264">
       <c r="A2" s="220" t="inlineStr">
         <is>
           <t>Name of Church ……………………………………………………………  No………..</t>
@@ -5827,89 +5833,89 @@
       <c r="H2" s="12" t="n"/>
       <c r="I2" s="12" t="n"/>
     </row>
-    <row r="3" ht="15" customHeight="1" s="248">
+    <row r="3" ht="15" customHeight="1" s="264">
       <c r="A3" s="220" t="n"/>
     </row>
-    <row r="4" ht="15" customHeight="1" s="248">
+    <row r="4" ht="15" customHeight="1" s="264">
       <c r="A4" s="220" t="n"/>
     </row>
-    <row r="5" ht="26.25" customHeight="1" s="248">
+    <row r="5" ht="26.25" customHeight="1" s="264">
       <c r="C5" s="224" t="inlineStr">
         <is>
           <t>Declarations and Scrutiny</t>
         </is>
       </c>
     </row>
-    <row r="6" ht="26.25" customHeight="1" s="248">
+    <row r="6" ht="26.25" customHeight="1" s="264">
       <c r="A6" s="221" t="n"/>
     </row>
-    <row r="7" ht="15" customHeight="1" s="248">
+    <row r="7" ht="15" customHeight="1" s="264">
       <c r="A7" s="315" t="inlineStr">
         <is>
           <t>I confirm that these Receipt and Payment based accounts for the year to 31 August 2024 have been prepared from the records of the Church and that they include all funds under the control of the Church trustees.</t>
         </is>
       </c>
     </row>
-    <row r="8" ht="15" customHeight="1" s="248"/>
-    <row r="9" ht="15" customHeight="1" s="248"/>
-    <row r="10" ht="15" customHeight="1" s="248">
+    <row r="8" ht="15" customHeight="1" s="264"/>
+    <row r="9" ht="15" customHeight="1" s="264"/>
+    <row r="10" ht="15" customHeight="1" s="264">
       <c r="A10" s="220" t="n"/>
     </row>
-    <row r="11" ht="15" customHeight="1" s="248">
+    <row r="11" ht="15" customHeight="1" s="264">
       <c r="A11" s="220" t="n"/>
     </row>
-    <row r="12" ht="15" customHeight="1" s="248">
+    <row r="12" ht="15" customHeight="1" s="264">
       <c r="A12" s="220" t="inlineStr">
         <is>
           <t>Signature of treasurer ………………………………………………………   Date……………………..</t>
         </is>
       </c>
     </row>
-    <row r="13" ht="15" customHeight="1" s="248">
+    <row r="13" ht="15" customHeight="1" s="264">
       <c r="A13" s="220" t="n"/>
     </row>
-    <row r="14" ht="15" customHeight="1" s="248">
+    <row r="14" ht="15" customHeight="1" s="264">
       <c r="A14" s="220" t="inlineStr">
         <is>
           <t>Name and address of treasurer ………………………………………………………………………….</t>
         </is>
       </c>
     </row>
-    <row r="15" ht="15" customHeight="1" s="248">
+    <row r="15" ht="15" customHeight="1" s="264">
       <c r="A15" s="220" t="n"/>
     </row>
-    <row r="16" ht="15" customHeight="1" s="248">
+    <row r="16" ht="15" customHeight="1" s="264">
       <c r="A16" s="220" t="inlineStr">
         <is>
           <t>………………………………………………………………………………….  Post Code………………</t>
         </is>
       </c>
     </row>
-    <row r="17" ht="15" customHeight="1" s="248">
+    <row r="17" ht="15" customHeight="1" s="264">
       <c r="A17" s="220" t="n"/>
     </row>
-    <row r="18" ht="15" customHeight="1" s="248">
+    <row r="18" ht="15" customHeight="1" s="264">
       <c r="A18" s="220" t="n"/>
     </row>
-    <row r="19" ht="15.75" customHeight="1" s="248">
+    <row r="19" ht="15.75" customHeight="1" s="264">
       <c r="A19" s="222" t="inlineStr">
         <is>
           <t>Presentation to the Church trustees</t>
         </is>
       </c>
     </row>
-    <row r="20" ht="15.75" customHeight="1" s="248">
+    <row r="20" ht="15.75" customHeight="1" s="264">
       <c r="A20" s="222" t="n"/>
     </row>
-    <row r="21" ht="15" customHeight="1" s="248">
+    <row r="21" ht="15" customHeight="1" s="264">
       <c r="A21" s="315" t="inlineStr">
         <is>
           <t>I confirm that the annual report and accounts for the year ended 31 August 2024 were/will be* presented to the meeting of the Church trustees held on ……………..</t>
         </is>
       </c>
     </row>
-    <row r="22" ht="15" customHeight="1" s="248"/>
-    <row r="23" ht="15" customHeight="1" s="248">
+    <row r="22" ht="15" customHeight="1" s="264"/>
+    <row r="23" ht="15" customHeight="1" s="264">
       <c r="A23" s="315" t="n"/>
       <c r="B23" s="315" t="n"/>
       <c r="C23" s="315" t="n"/>
@@ -5922,106 +5928,106 @@
       <c r="J23" s="315" t="n"/>
       <c r="K23" s="315" t="n"/>
     </row>
-    <row r="24" ht="15" customHeight="1" s="248">
+    <row r="24" ht="15" customHeight="1" s="264">
       <c r="A24" s="220" t="n"/>
     </row>
-    <row r="25" ht="15" customHeight="1" s="248">
+    <row r="25" ht="15" customHeight="1" s="264">
       <c r="A25" s="220" t="inlineStr">
         <is>
           <t>Signature of the Chair of the meeting  ……………………………………………………………………</t>
         </is>
       </c>
     </row>
-    <row r="26" ht="15" customHeight="1" s="248">
+    <row r="26" ht="15" customHeight="1" s="264">
       <c r="A26" s="220" t="n"/>
     </row>
-    <row r="27" ht="15" customHeight="1" s="248">
+    <row r="27" ht="15" customHeight="1" s="264">
       <c r="A27" s="220" t="inlineStr">
         <is>
           <t>Name of the Chair of the meeting  …………………………………………… Date ……………………</t>
         </is>
       </c>
     </row>
-    <row r="28" ht="15" customHeight="1" s="248">
+    <row r="28" ht="15" customHeight="1" s="264">
       <c r="A28" s="220" t="n"/>
     </row>
-    <row r="29" ht="15" customHeight="1" s="248">
+    <row r="29" ht="15" customHeight="1" s="264">
       <c r="A29" s="220" t="n"/>
     </row>
-    <row r="30" ht="15" customHeight="1" s="248">
+    <row r="30" ht="15" customHeight="1" s="264">
       <c r="A30" s="220" t="n"/>
     </row>
-    <row r="31" ht="15" customHeight="1" s="248">
+    <row r="31" ht="15" customHeight="1" s="264">
       <c r="A31" s="220" t="n"/>
     </row>
-    <row r="32" ht="15" customHeight="1" s="248">
+    <row r="32" ht="15" customHeight="1" s="264">
       <c r="A32" s="220" t="n"/>
     </row>
-    <row r="33" ht="18" customHeight="1" s="248">
+    <row r="33" ht="18" customHeight="1" s="264">
       <c r="C33" s="225" t="inlineStr">
         <is>
           <t xml:space="preserve">Independent Examiner’s Report to the Trustees of the </t>
         </is>
       </c>
     </row>
-    <row r="34" ht="18" customHeight="1" s="248">
+    <row r="34" ht="18" customHeight="1" s="264">
       <c r="A34" s="223" t="n"/>
     </row>
-    <row r="35" ht="18" customHeight="1" s="248">
+    <row r="35" ht="18" customHeight="1" s="264">
       <c r="D35" s="225" t="inlineStr">
         <is>
           <t>……………………..……………………..Church</t>
         </is>
       </c>
     </row>
-    <row r="36" ht="18" customHeight="1" s="248">
+    <row r="36" ht="18" customHeight="1" s="264">
       <c r="A36" s="223" t="n"/>
     </row>
-    <row r="37" ht="15.75" customHeight="1" s="248">
+    <row r="37" ht="15.75" customHeight="1" s="264">
       <c r="E37" s="226" t="inlineStr">
         <is>
           <t>Charity Number …………..</t>
         </is>
       </c>
     </row>
-    <row r="38" ht="15.75" customHeight="1" s="248">
+    <row r="38" ht="15.75" customHeight="1" s="264">
       <c r="A38" s="222" t="n"/>
     </row>
-    <row r="39" ht="15.75" customHeight="1" s="248">
+    <row r="39" ht="15.75" customHeight="1" s="264">
       <c r="A39" s="222" t="n"/>
     </row>
-    <row r="40" ht="15.75" customHeight="1" s="248">
+    <row r="40" ht="15.75" customHeight="1" s="264">
       <c r="A40" s="222" t="inlineStr">
         <is>
           <t>Responsibilities and basis of report</t>
         </is>
       </c>
     </row>
-    <row r="41" ht="15.75" customHeight="1" s="248">
+    <row r="41" ht="15.75" customHeight="1" s="264">
       <c r="A41" s="222" t="n"/>
     </row>
-    <row r="42" ht="15" customHeight="1" s="248">
+    <row r="42" ht="15" customHeight="1" s="264">
       <c r="A42" s="315" t="inlineStr">
         <is>
           <t xml:space="preserve">I report to the trustees on my examination of the accounts of the …………………………………. Church for the year ended 31 August 2024 set out on pages … to ….  As the Church’s trustees, you are responsible for the preparation of the accounts in accordance with the requirements of the Charities Act 2011 (‘the Act’). </t>
         </is>
       </c>
     </row>
-    <row r="43" ht="15" customHeight="1" s="248"/>
-    <row r="44" ht="15" customHeight="1" s="248"/>
-    <row r="45" ht="15" customHeight="1" s="248"/>
-    <row r="46" ht="15" customHeight="1" s="248"/>
-    <row r="47" ht="12.75" customHeight="1" s="248">
+    <row r="43" ht="15" customHeight="1" s="264"/>
+    <row r="44" ht="15" customHeight="1" s="264"/>
+    <row r="45" ht="15" customHeight="1" s="264"/>
+    <row r="46" ht="15" customHeight="1" s="264"/>
+    <row r="47" ht="12.75" customHeight="1" s="264">
       <c r="A47" s="316" t="inlineStr">
         <is>
           <t>I report in respect of my examination of the Church’s accounts carried out under section 145 of the Act and, in carrying out my examination, I have followed all the applicable Directions given by the Charity Commission under section 145(5)(b) of the Act.</t>
         </is>
       </c>
     </row>
-    <row r="48" ht="15" customHeight="1" s="248"/>
-    <row r="49" ht="15" customHeight="1" s="248"/>
+    <row r="48" ht="15" customHeight="1" s="264"/>
+    <row r="49" ht="15" customHeight="1" s="264"/>
     <row r="50"/>
-    <row r="53" ht="15" customHeight="1" s="248">
+    <row r="53" ht="15" customHeight="1" s="264">
       <c r="A53" s="220" t="inlineStr">
         <is>
           <t>* delete or circle as appropriate</t>
@@ -6062,185 +6068,185 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
   <cols>
-    <col width="9.140625" customWidth="1" style="248" min="8" max="9"/>
-    <col width="15" customWidth="1" style="248" min="10" max="10"/>
+    <col width="9.140625" customWidth="1" style="264" min="8" max="9"/>
+    <col width="15" customWidth="1" style="264" min="10" max="10"/>
   </cols>
   <sheetData>
-    <row r="2" ht="15" customHeight="1" s="248">
+    <row r="2" ht="15" customHeight="1" s="264">
       <c r="A2" s="220" t="inlineStr">
         <is>
           <t>Name of Church …………………………………………………………………………  No ………….</t>
         </is>
       </c>
     </row>
-    <row r="3" ht="15" customHeight="1" s="248">
+    <row r="3" ht="15" customHeight="1" s="264">
       <c r="A3" s="220" t="n"/>
     </row>
-    <row r="4" ht="15" customHeight="1" s="248">
+    <row r="4" ht="15" customHeight="1" s="264">
       <c r="A4" s="220" t="n"/>
     </row>
-    <row r="5" ht="15.75" customHeight="1" s="248">
+    <row r="5" ht="15.75" customHeight="1" s="264">
       <c r="A5" s="222" t="inlineStr">
         <is>
           <t>Independent Examiner’s Statement</t>
         </is>
       </c>
     </row>
-    <row r="6" ht="15.75" customHeight="1" s="248">
+    <row r="6" ht="15.75" customHeight="1" s="264">
       <c r="A6" s="222" t="n"/>
     </row>
-    <row r="7" ht="15" customHeight="1" s="248">
+    <row r="7" ht="15" customHeight="1" s="264">
       <c r="A7" s="315" t="inlineStr">
         <is>
           <t>I have completed my examination.  I confirm that no material matters have come to my attention in connection with the examination (other than that disclosed below*) which give me cause to believe that in, any material respect:</t>
         </is>
       </c>
     </row>
-    <row r="8" ht="15" customHeight="1" s="248"/>
-    <row r="9" ht="15" customHeight="1" s="248"/>
-    <row r="10" ht="15" customHeight="1" s="248"/>
-    <row r="11" ht="15" customHeight="1" s="248">
+    <row r="8" ht="15" customHeight="1" s="264"/>
+    <row r="9" ht="15" customHeight="1" s="264"/>
+    <row r="10" ht="15" customHeight="1" s="264"/>
+    <row r="11" ht="15" customHeight="1" s="264">
       <c r="A11" s="220" t="n"/>
     </row>
-    <row r="12" ht="15.75" customHeight="1" s="248">
+    <row r="12" ht="15.75" customHeight="1" s="264">
       <c r="A12" s="227" t="inlineStr">
         <is>
           <t xml:space="preserve">·         the accounting records were not kept in accordance with section 130 of the Act; or </t>
         </is>
       </c>
     </row>
-    <row r="13" ht="15.75" customHeight="1" s="248">
+    <row r="13" ht="15.75" customHeight="1" s="264">
       <c r="A13" s="227" t="inlineStr">
         <is>
           <t>·         the accounts do not accord with the accounting records.</t>
         </is>
       </c>
     </row>
-    <row r="14" ht="15" customHeight="1" s="248">
+    <row r="14" ht="15" customHeight="1" s="264">
       <c r="A14" s="220" t="n"/>
     </row>
-    <row r="15" ht="15" customHeight="1" s="248">
+    <row r="15" ht="15" customHeight="1" s="264">
       <c r="A15" s="220" t="n"/>
     </row>
-    <row r="16" ht="15" customHeight="1" s="248">
+    <row r="16" ht="15" customHeight="1" s="264">
       <c r="A16" s="316" t="inlineStr">
         <is>
           <t>I have no concerns and have come across no other matters in connection with the examination to which attention should be drawn in this report in order to enable a proper understanding of the accounts to be reached.</t>
         </is>
       </c>
     </row>
-    <row r="17" ht="15" customHeight="1" s="248"/>
-    <row r="18" ht="15" customHeight="1" s="248"/>
-    <row r="19" ht="15" customHeight="1" s="248">
+    <row r="17" ht="15" customHeight="1" s="264"/>
+    <row r="18" ht="15" customHeight="1" s="264"/>
+    <row r="19" ht="15" customHeight="1" s="264">
       <c r="A19" s="220" t="n"/>
     </row>
-    <row r="20" ht="15" customHeight="1" s="248">
+    <row r="20" ht="15" customHeight="1" s="264">
       <c r="A20" s="315" t="inlineStr">
         <is>
           <t>I have/have not* obtained independent verification of all investments with the Trustees for Methodist Church Purposes or held in other trusts, bank balances and funds at the Central Finance Board of the Methodist Church which are individually in excess of £10,000 (ten thousand pounds) at the balance sheet date.</t>
         </is>
       </c>
     </row>
-    <row r="21" ht="15" customHeight="1" s="248"/>
-    <row r="22" ht="15" customHeight="1" s="248"/>
-    <row r="23" ht="15" customHeight="1" s="248"/>
-    <row r="24" ht="15" customHeight="1" s="248"/>
-    <row r="25" ht="15" customHeight="1" s="248">
+    <row r="21" ht="15" customHeight="1" s="264"/>
+    <row r="22" ht="15" customHeight="1" s="264"/>
+    <row r="23" ht="15" customHeight="1" s="264"/>
+    <row r="24" ht="15" customHeight="1" s="264"/>
+    <row r="25" ht="15" customHeight="1" s="264">
       <c r="A25" s="220" t="n"/>
     </row>
-    <row r="26" ht="15" customHeight="1" s="248">
+    <row r="26" ht="15" customHeight="1" s="264">
       <c r="A26" s="220" t="n"/>
     </row>
-    <row r="27" ht="15" customHeight="1" s="248">
+    <row r="27" ht="15" customHeight="1" s="264">
       <c r="A27" s="220" t="inlineStr">
         <is>
           <t>Signature of independent examiner   ………………………………………………………………….</t>
         </is>
       </c>
     </row>
-    <row r="28" ht="15" customHeight="1" s="248">
+    <row r="28" ht="15" customHeight="1" s="264">
       <c r="A28" s="220" t="n"/>
     </row>
-    <row r="29" ht="15" customHeight="1" s="248">
+    <row r="29" ht="15" customHeight="1" s="264">
       <c r="A29" s="220" t="inlineStr">
         <is>
           <t>Name of independent examiner  ……………………………………………………………………….</t>
         </is>
       </c>
     </row>
-    <row r="30" ht="15" customHeight="1" s="248">
+    <row r="30" ht="15" customHeight="1" s="264">
       <c r="A30" s="220" t="n"/>
     </row>
-    <row r="31" ht="15" customHeight="1" s="248">
+    <row r="31" ht="15" customHeight="1" s="264">
       <c r="A31" s="220" t="inlineStr">
         <is>
           <t>Relevant professional qualification of independent examiner  ………………………………………</t>
         </is>
       </c>
     </row>
-    <row r="32" ht="15" customHeight="1" s="248">
+    <row r="32" ht="15" customHeight="1" s="264">
       <c r="A32" s="220" t="n"/>
     </row>
-    <row r="33" ht="15" customHeight="1" s="248">
+    <row r="33" ht="15" customHeight="1" s="264">
       <c r="A33" s="220" t="n"/>
     </row>
-    <row r="34" ht="15" customHeight="1" s="248">
+    <row r="34" ht="15" customHeight="1" s="264">
       <c r="A34" s="220" t="inlineStr">
         <is>
           <t>Name of firm (where appropriate)  ………………………………………………………………………</t>
         </is>
       </c>
     </row>
-    <row r="35" ht="15" customHeight="1" s="248">
+    <row r="35" ht="15" customHeight="1" s="264">
       <c r="A35" s="220" t="n"/>
     </row>
-    <row r="36" ht="15" customHeight="1" s="248">
+    <row r="36" ht="15" customHeight="1" s="264">
       <c r="A36" s="220" t="inlineStr">
         <is>
           <t>Address  ……………………………………………………………………………………………………</t>
         </is>
       </c>
     </row>
-    <row r="37" ht="15" customHeight="1" s="248">
+    <row r="37" ht="15" customHeight="1" s="264">
       <c r="A37" s="220" t="n"/>
     </row>
-    <row r="38" ht="15" customHeight="1" s="248">
+    <row r="38" ht="15" customHeight="1" s="264">
       <c r="A38" s="220" t="inlineStr">
         <is>
           <t>………………………………………………………………………………..  Post Code  ………………</t>
         </is>
       </c>
     </row>
-    <row r="39" ht="15" customHeight="1" s="248">
+    <row r="39" ht="15" customHeight="1" s="264">
       <c r="A39" s="220" t="n"/>
     </row>
-    <row r="40" ht="15" customHeight="1" s="248">
+    <row r="40" ht="15" customHeight="1" s="264">
       <c r="A40" s="220" t="inlineStr">
         <is>
           <t>Date  …………………………………………</t>
         </is>
       </c>
     </row>
-    <row r="41" ht="15" customHeight="1" s="248">
+    <row r="41" ht="15" customHeight="1" s="264">
       <c r="A41" s="220" t="n"/>
     </row>
-    <row r="42" ht="15" customHeight="1" s="248">
+    <row r="42" ht="15" customHeight="1" s="264">
       <c r="A42" s="220" t="n"/>
     </row>
-    <row r="43" ht="15" customHeight="1" s="248">
+    <row r="43" ht="15" customHeight="1" s="264">
       <c r="A43" s="220" t="n"/>
     </row>
-    <row r="44" ht="15" customHeight="1" s="248">
+    <row r="44" ht="15" customHeight="1" s="264">
       <c r="A44" s="220" t="n"/>
     </row>
-    <row r="45" ht="15" customHeight="1" s="248">
+    <row r="45" ht="15" customHeight="1" s="264">
       <c r="A45" s="220" t="inlineStr">
         <is>
           <t>*  delete or circle as appropriate</t>
         </is>
       </c>
     </row>
-    <row r="46" ht="15" customHeight="1" s="248">
+    <row r="46" ht="15" customHeight="1" s="264">
       <c r="A46" s="220" t="n"/>
     </row>
     <row r="47">
@@ -6278,7 +6284,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6287,22 +6293,22 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="325" t="inlineStr">
+      <c r="A1" s="327" t="inlineStr">
         <is>
           <t>Unnamed: 0</t>
         </is>
       </c>
-      <c r="B1" s="325" t="inlineStr">
+      <c r="B1" s="327" t="inlineStr">
         <is>
           <t>Unnamed: 1</t>
         </is>
       </c>
-      <c r="C1" s="325" t="inlineStr">
+      <c r="C1" s="327" t="inlineStr">
         <is>
           <t>Unnamed: 2</t>
         </is>
       </c>
-      <c r="D1" s="325" t="inlineStr">
+      <c r="D1" s="327" t="inlineStr">
         <is>
           <t>Unnamed: 3</t>
         </is>
@@ -6486,7 +6492,7 @@
         <v>2025</v>
       </c>
       <c r="C16" t="n">
-        <v>51.5</v>
+        <v>3553.8</v>
       </c>
       <c r="D16" t="inlineStr"/>
     </row>
@@ -6559,24 +6565,48 @@
     <row r="22">
       <c r="A22" t="inlineStr"/>
       <c r="B22" t="inlineStr"/>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>amount</t>
-        </is>
-      </c>
-      <c r="D22" t="n">
-        <v>561.9</v>
-      </c>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr"/>
-      <c r="B23" t="inlineStr"/>
-      <c r="C23" t="inlineStr">
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>LETTINGS</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr"/>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Church Lets</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>amount</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>561.9</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr"/>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Cottage Rents</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
         <is>
           <t>recieved rent</t>
         </is>
       </c>
-      <c r="D23" t="n">
+      <c r="D25" t="n">
         <v>985.6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
improved the church page to add a miscelleneous expenditure and send to a csv file.
</commit_message>
<xml_diff>
--- a/data/Church-receipts-and-payments-2025.xlsx
+++ b/data/Church-receipts-and-payments-2025.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1110" yWindow="660" windowWidth="23775" windowHeight="13920" tabRatio="776" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-26745" yWindow="255" windowWidth="23775" windowHeight="13920" tabRatio="776" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="P1 Front page" sheetId="1" state="visible" r:id="rId1"/>
@@ -797,7 +797,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="326">
+  <cellXfs count="352">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -1081,9 +1081,6 @@
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="29" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="30" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1112,9 +1109,6 @@
     <xf numFmtId="164" fontId="9" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="31" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="16" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="32" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -1321,10 +1315,92 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="46" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="22" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="37" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="16" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0" hidden="0"/>
@@ -1339,96 +1415,33 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0" hidden="0"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection locked="0" hidden="0"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0" hidden="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="14" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0" hidden="0"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="37" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="22" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="43" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="44" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="42" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="16" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
@@ -1453,42 +1466,6 @@
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0" hidden="0"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="43" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="44" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="42" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="43" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
       <protection locked="0" hidden="0"/>
@@ -1510,20 +1487,90 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="43" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="2" fontId="17" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="11" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="28" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="28" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="29" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="31" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="33" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="28" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <protection locked="0" hidden="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="167" fontId="22" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
@@ -2376,171 +2423,171 @@
   </sheetPr>
   <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView topLeftCell="A11" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
   <cols>
-    <col width="1" customWidth="1" style="263" min="1" max="1"/>
-    <col width="0.42578125" customWidth="1" style="263" min="2" max="2"/>
-    <col width="3.140625" customWidth="1" style="263" min="3" max="3"/>
-    <col width="3.42578125" customWidth="1" style="263" min="4" max="6"/>
-    <col width="30.140625" customWidth="1" style="263" min="7" max="7"/>
-    <col width="0.42578125" customWidth="1" style="263" min="8" max="8"/>
-    <col width="11.42578125" customWidth="1" style="263" min="9" max="9"/>
-    <col width="20" customWidth="1" style="263" min="10" max="10"/>
-    <col width="8.42578125" customWidth="1" style="263" min="11" max="11"/>
-    <col width="11.140625" customWidth="1" style="263" min="12" max="12"/>
-    <col width="2.42578125" customWidth="1" style="263" min="13" max="13"/>
-    <col width="0.85546875" customWidth="1" style="263" min="14" max="14"/>
+    <col width="1" customWidth="1" style="244" min="1" max="1"/>
+    <col width="0.42578125" customWidth="1" style="244" min="2" max="2"/>
+    <col width="3.140625" customWidth="1" style="244" min="3" max="3"/>
+    <col width="3.42578125" customWidth="1" style="244" min="4" max="6"/>
+    <col width="30.140625" customWidth="1" style="244" min="7" max="7"/>
+    <col width="0.42578125" customWidth="1" style="244" min="8" max="8"/>
+    <col width="11.42578125" customWidth="1" style="244" min="9" max="9"/>
+    <col width="20" customWidth="1" style="244" min="10" max="10"/>
+    <col width="8.42578125" customWidth="1" style="244" min="11" max="11"/>
+    <col width="11.140625" customWidth="1" style="244" min="12" max="12"/>
+    <col width="2.42578125" customWidth="1" style="244" min="13" max="13"/>
+    <col width="0.85546875" customWidth="1" style="244" min="14" max="14"/>
   </cols>
   <sheetData>
-    <row r="1" ht="6" customHeight="1" s="263">
-      <c r="B1" s="248" t="n"/>
-      <c r="C1" s="248" t="n"/>
-      <c r="D1" s="248" t="n"/>
-      <c r="E1" s="248" t="n"/>
-      <c r="F1" s="248" t="n"/>
-      <c r="G1" s="248" t="n"/>
-      <c r="H1" s="248" t="n"/>
-      <c r="I1" s="248" t="n"/>
-      <c r="J1" s="248" t="n"/>
-      <c r="K1" s="248" t="n"/>
-      <c r="L1" s="248" t="n"/>
-    </row>
-    <row r="2" ht="15.75" customHeight="1" s="263">
+    <row r="1" ht="6" customHeight="1" s="244">
+      <c r="B1" s="260" t="n"/>
+      <c r="C1" s="260" t="n"/>
+      <c r="D1" s="260" t="n"/>
+      <c r="E1" s="260" t="n"/>
+      <c r="F1" s="260" t="n"/>
+      <c r="G1" s="260" t="n"/>
+      <c r="H1" s="260" t="n"/>
+      <c r="I1" s="260" t="n"/>
+      <c r="J1" s="260" t="n"/>
+      <c r="K1" s="260" t="n"/>
+      <c r="L1" s="260" t="n"/>
+    </row>
+    <row r="2" ht="15.75" customHeight="1" s="244">
       <c r="A2" s="9" t="n"/>
-      <c r="B2" s="270" t="inlineStr">
+      <c r="B2" s="243" t="inlineStr">
         <is>
           <t>CHURCH</t>
         </is>
       </c>
       <c r="N2" s="29" t="n"/>
     </row>
-    <row r="3" ht="15.75" customHeight="1" s="263">
+    <row r="3" ht="15.75" customHeight="1" s="244">
       <c r="A3" s="9" t="n"/>
-      <c r="B3" s="270" t="inlineStr">
+      <c r="B3" s="243" t="inlineStr">
         <is>
           <t xml:space="preserve">        RECEIPTS AND PAYMENTS</t>
         </is>
       </c>
     </row>
-    <row r="4" ht="15.75" customHeight="1" s="263">
+    <row r="4" ht="15.75" customHeight="1" s="244">
       <c r="A4" s="9" t="n"/>
-      <c r="B4" s="270" t="inlineStr">
+      <c r="B4" s="243" t="inlineStr">
         <is>
           <t>ACCOUNTS</t>
         </is>
       </c>
     </row>
-    <row r="5" ht="6.75" customHeight="1" s="263">
+    <row r="5" ht="6.75" customHeight="1" s="244">
       <c r="A5" s="9" t="n"/>
-      <c r="B5" s="248" t="n"/>
-      <c r="C5" s="248" t="n"/>
-      <c r="D5" s="248" t="n"/>
-      <c r="E5" s="248" t="n"/>
-      <c r="F5" s="248" t="n"/>
-      <c r="G5" s="248" t="n"/>
-      <c r="H5" s="248" t="n"/>
-      <c r="I5" s="248" t="n"/>
-      <c r="J5" s="248" t="n"/>
-      <c r="K5" s="248" t="n"/>
-      <c r="L5" s="248" t="n"/>
-    </row>
-    <row r="6" ht="18.75" customHeight="1" s="263">
+      <c r="B5" s="260" t="n"/>
+      <c r="C5" s="260" t="n"/>
+      <c r="D5" s="260" t="n"/>
+      <c r="E5" s="260" t="n"/>
+      <c r="F5" s="260" t="n"/>
+      <c r="G5" s="260" t="n"/>
+      <c r="H5" s="260" t="n"/>
+      <c r="I5" s="260" t="n"/>
+      <c r="J5" s="260" t="n"/>
+      <c r="K5" s="260" t="n"/>
+      <c r="L5" s="260" t="n"/>
+    </row>
+    <row r="6" ht="18.75" customHeight="1" s="244">
       <c r="A6" s="9" t="n"/>
-      <c r="B6" s="271" t="inlineStr">
+      <c r="B6" s="246" t="inlineStr">
         <is>
           <t>THE METHODIST CHURCH</t>
         </is>
       </c>
     </row>
-    <row r="7" ht="9.75" customHeight="1" s="263">
+    <row r="7" ht="9.75" customHeight="1" s="244">
       <c r="A7" s="9" t="n"/>
-      <c r="B7" s="248" t="n"/>
-      <c r="C7" s="248" t="n"/>
-      <c r="D7" s="248" t="n"/>
-      <c r="E7" s="248" t="n"/>
-      <c r="F7" s="248" t="n"/>
-      <c r="G7" s="248" t="n"/>
-      <c r="H7" s="248" t="n"/>
-      <c r="I7" s="248" t="n"/>
-      <c r="J7" s="248" t="n"/>
-      <c r="K7" s="248" t="n"/>
-      <c r="L7" s="248" t="n"/>
-    </row>
-    <row r="8" ht="22.7" customFormat="1" customHeight="1" s="272">
+      <c r="B7" s="260" t="n"/>
+      <c r="C7" s="260" t="n"/>
+      <c r="D7" s="260" t="n"/>
+      <c r="E7" s="260" t="n"/>
+      <c r="F7" s="260" t="n"/>
+      <c r="G7" s="260" t="n"/>
+      <c r="H7" s="260" t="n"/>
+      <c r="I7" s="260" t="n"/>
+      <c r="J7" s="260" t="n"/>
+      <c r="K7" s="260" t="n"/>
+      <c r="L7" s="260" t="n"/>
+    </row>
+    <row r="8" ht="22.7" customFormat="1" customHeight="1" s="247">
       <c r="A8" s="23" t="n"/>
-      <c r="B8" s="271" t="inlineStr">
+      <c r="B8" s="246" t="inlineStr">
         <is>
           <t xml:space="preserve">STANDARD FORM OF ACCOUNTS </t>
         </is>
       </c>
     </row>
-    <row r="9" ht="7.5" customFormat="1" customHeight="1" s="272">
+    <row r="9" ht="7.5" customFormat="1" customHeight="1" s="247">
       <c r="A9" s="23" t="n"/>
-      <c r="B9" s="273" t="n"/>
-    </row>
-    <row r="10" ht="5.25" customHeight="1" s="263">
+      <c r="B9" s="248" t="n"/>
+    </row>
+    <row r="10" ht="5.25" customHeight="1" s="244">
       <c r="A10" s="9" t="n"/>
-      <c r="B10" s="248" t="n"/>
-      <c r="C10" s="248" t="n"/>
-      <c r="D10" s="248" t="n"/>
-      <c r="E10" s="248" t="n"/>
-      <c r="F10" s="248" t="n"/>
-      <c r="G10" s="248" t="n"/>
-      <c r="H10" s="248" t="n"/>
-      <c r="I10" s="248" t="n"/>
-      <c r="J10" s="248" t="n"/>
-      <c r="K10" s="248" t="n"/>
-      <c r="L10" s="248" t="n"/>
-    </row>
-    <row r="11" ht="30.2" customHeight="1" s="263">
+      <c r="B10" s="260" t="n"/>
+      <c r="C10" s="260" t="n"/>
+      <c r="D10" s="260" t="n"/>
+      <c r="E10" s="260" t="n"/>
+      <c r="F10" s="260" t="n"/>
+      <c r="G10" s="260" t="n"/>
+      <c r="H10" s="260" t="n"/>
+      <c r="I10" s="260" t="n"/>
+      <c r="J10" s="260" t="n"/>
+      <c r="K10" s="260" t="n"/>
+      <c r="L10" s="260" t="n"/>
+    </row>
+    <row r="11" ht="30.2" customHeight="1" s="244">
       <c r="A11" s="9" t="n"/>
       <c r="B11" s="35" t="n"/>
-      <c r="C11" s="274" t="inlineStr">
+      <c r="C11" s="249" t="inlineStr">
         <is>
           <t>Briggswath and Sleights Methodist</t>
         </is>
       </c>
-      <c r="D11" s="275" t="n"/>
-      <c r="E11" s="275" t="n"/>
-      <c r="F11" s="275" t="n"/>
-      <c r="G11" s="275" t="n"/>
-      <c r="H11" s="275" t="n"/>
-      <c r="I11" s="275" t="n"/>
-      <c r="J11" s="275" t="n"/>
-      <c r="K11" s="275" t="n"/>
-      <c r="L11" s="245" t="inlineStr">
+      <c r="D11" s="250" t="n"/>
+      <c r="E11" s="250" t="n"/>
+      <c r="F11" s="250" t="n"/>
+      <c r="G11" s="250" t="n"/>
+      <c r="H11" s="250" t="n"/>
+      <c r="I11" s="250" t="n"/>
+      <c r="J11" s="250" t="n"/>
+      <c r="K11" s="250" t="n"/>
+      <c r="L11" s="241" t="inlineStr">
         <is>
           <t>Church</t>
         </is>
       </c>
     </row>
-    <row r="12" ht="8.449999999999999" customHeight="1" s="263">
+    <row r="12" ht="8.449999999999999" customHeight="1" s="244">
       <c r="A12" s="9" t="n"/>
-      <c r="B12" s="248" t="n"/>
-      <c r="C12" s="248" t="n"/>
-      <c r="D12" s="248" t="n"/>
-      <c r="E12" s="248" t="n"/>
-      <c r="F12" s="248" t="n"/>
-      <c r="G12" s="248" t="n"/>
-      <c r="H12" s="248" t="n"/>
-      <c r="I12" s="248" t="n"/>
-      <c r="J12" s="248" t="n"/>
-      <c r="K12" s="248" t="n"/>
-      <c r="L12" s="248" t="n"/>
-    </row>
-    <row r="13" ht="20.25" customHeight="1" s="263">
+      <c r="B12" s="260" t="n"/>
+      <c r="C12" s="260" t="n"/>
+      <c r="D12" s="260" t="n"/>
+      <c r="E12" s="260" t="n"/>
+      <c r="F12" s="260" t="n"/>
+      <c r="G12" s="260" t="n"/>
+      <c r="H12" s="260" t="n"/>
+      <c r="I12" s="260" t="n"/>
+      <c r="J12" s="260" t="n"/>
+      <c r="K12" s="260" t="n"/>
+      <c r="L12" s="260" t="n"/>
+    </row>
+    <row r="13" ht="20.25" customHeight="1" s="244">
       <c r="A13" s="9" t="n"/>
-      <c r="B13" s="276" t="inlineStr">
+      <c r="B13" s="251" t="inlineStr">
         <is>
           <t xml:space="preserve">        FOR THE YEAR ENDED      </t>
         </is>
       </c>
     </row>
-    <row r="14" ht="8.449999999999999" customHeight="1" s="263">
+    <row r="14" ht="8.449999999999999" customHeight="1" s="244">
       <c r="A14" s="9" t="n"/>
       <c r="B14" s="36" t="n"/>
       <c r="C14" s="36" t="n"/>
@@ -2554,261 +2601,261 @@
       <c r="K14" s="36" t="n"/>
       <c r="L14" s="36" t="n"/>
     </row>
-    <row r="15" ht="20.25" customHeight="1" s="263">
+    <row r="15" ht="20.25" customHeight="1" s="244">
       <c r="A15" s="9" t="n"/>
-      <c r="B15" s="318" t="n">
+      <c r="B15" s="344" t="n">
         <v>45535</v>
       </c>
     </row>
-    <row r="16" ht="3.2" customHeight="1" s="263">
+    <row r="16" ht="3.2" customHeight="1" s="244">
       <c r="A16" s="9" t="n"/>
-      <c r="B16" s="248" t="n"/>
-      <c r="C16" s="248" t="n"/>
-      <c r="D16" s="248" t="n"/>
-      <c r="E16" s="248" t="n"/>
-      <c r="F16" s="248" t="n"/>
-      <c r="G16" s="248" t="n"/>
-      <c r="H16" s="248" t="n"/>
-      <c r="I16" s="248" t="n"/>
-      <c r="J16" s="248" t="n"/>
-      <c r="K16" s="248" t="n"/>
-      <c r="L16" s="248" t="n"/>
-    </row>
-    <row r="17" ht="30.2" customHeight="1" s="263">
+      <c r="B16" s="260" t="n"/>
+      <c r="C16" s="260" t="n"/>
+      <c r="D16" s="260" t="n"/>
+      <c r="E16" s="260" t="n"/>
+      <c r="F16" s="260" t="n"/>
+      <c r="G16" s="260" t="n"/>
+      <c r="H16" s="260" t="n"/>
+      <c r="I16" s="260" t="n"/>
+      <c r="J16" s="260" t="n"/>
+      <c r="K16" s="260" t="n"/>
+      <c r="L16" s="260" t="n"/>
+    </row>
+    <row r="17" ht="30.2" customHeight="1" s="244">
       <c r="A17" s="9" t="n"/>
-      <c r="B17" s="248" t="n"/>
-      <c r="C17" s="274" t="inlineStr">
+      <c r="B17" s="260" t="n"/>
+      <c r="C17" s="249" t="inlineStr">
         <is>
           <t>North Yorkshire Coast</t>
         </is>
       </c>
-      <c r="D17" s="275" t="n"/>
-      <c r="E17" s="275" t="n"/>
-      <c r="F17" s="275" t="n"/>
-      <c r="G17" s="275" t="n"/>
-      <c r="H17" s="243" t="n"/>
-      <c r="I17" s="244" t="inlineStr">
+      <c r="D17" s="250" t="n"/>
+      <c r="E17" s="250" t="n"/>
+      <c r="F17" s="250" t="n"/>
+      <c r="G17" s="250" t="n"/>
+      <c r="H17" s="239" t="n"/>
+      <c r="I17" s="240" t="inlineStr">
         <is>
           <t>Circuit</t>
         </is>
       </c>
-      <c r="J17" s="243" t="inlineStr">
+      <c r="J17" s="239" t="inlineStr">
         <is>
           <t>Circuit no.</t>
         </is>
       </c>
-      <c r="K17" s="277" t="inlineStr">
+      <c r="K17" s="252" t="inlineStr">
         <is>
           <t>29/31</t>
         </is>
       </c>
-      <c r="L17" s="262" t="n"/>
-    </row>
-    <row r="18" ht="6.75" customHeight="1" s="263">
+      <c r="L17" s="253" t="n"/>
+    </row>
+    <row r="18" ht="6.75" customHeight="1" s="244">
       <c r="A18" s="9" t="n"/>
-      <c r="B18" s="248" t="n"/>
-      <c r="C18" s="248" t="n"/>
-      <c r="D18" s="248" t="n"/>
-      <c r="E18" s="248" t="n"/>
-      <c r="F18" s="248" t="n"/>
-      <c r="G18" s="248" t="n"/>
-      <c r="H18" s="248" t="n"/>
-      <c r="I18" s="175" t="n"/>
-      <c r="J18" s="248" t="n"/>
-      <c r="K18" s="248" t="n"/>
-      <c r="L18" s="248" t="n"/>
-    </row>
-    <row r="19" ht="26.45" customHeight="1" s="263">
+      <c r="B18" s="260" t="n"/>
+      <c r="C18" s="260" t="n"/>
+      <c r="D18" s="260" t="n"/>
+      <c r="E18" s="260" t="n"/>
+      <c r="F18" s="260" t="n"/>
+      <c r="G18" s="260" t="n"/>
+      <c r="H18" s="260" t="n"/>
+      <c r="I18" s="171" t="n"/>
+      <c r="J18" s="260" t="n"/>
+      <c r="K18" s="260" t="n"/>
+      <c r="L18" s="260" t="n"/>
+    </row>
+    <row r="19" ht="26.45" customHeight="1" s="244">
       <c r="A19" s="9" t="n"/>
-      <c r="B19" s="248" t="n"/>
-      <c r="C19" s="279" t="inlineStr">
+      <c r="B19" s="260" t="n"/>
+      <c r="C19" s="255" t="inlineStr">
         <is>
           <t>Registered Charity - Charity Registration number</t>
         </is>
       </c>
-      <c r="J19" s="248" t="n"/>
-      <c r="K19" s="261" t="n"/>
-      <c r="L19" s="262" t="n"/>
-    </row>
-    <row r="20" ht="7.5" customHeight="1" s="263">
+      <c r="J19" s="260" t="n"/>
+      <c r="K19" s="257" t="n"/>
+      <c r="L19" s="253" t="n"/>
+    </row>
+    <row r="20" ht="7.5" customHeight="1" s="244">
       <c r="A20" s="9" t="n"/>
-      <c r="B20" s="248" t="n"/>
-      <c r="C20" s="259" t="n"/>
-      <c r="K20" s="248" t="n"/>
-      <c r="L20" s="248" t="n"/>
-    </row>
-    <row r="21" ht="30.75" customFormat="1" customHeight="1" s="260">
+      <c r="B20" s="260" t="n"/>
+      <c r="C20" s="245" t="n"/>
+      <c r="K20" s="260" t="n"/>
+      <c r="L20" s="260" t="n"/>
+    </row>
+    <row r="21" ht="30.75" customFormat="1" customHeight="1" s="256">
       <c r="A21" s="24" t="n"/>
-      <c r="B21" s="259" t="n"/>
-      <c r="C21" s="259" t="inlineStr">
+      <c r="B21" s="245" t="n"/>
+      <c r="C21" s="245" t="inlineStr">
         <is>
           <t>If not a registered charity His Majesty's Revenue and Customs Gift Aid number</t>
         </is>
       </c>
-      <c r="J21" s="213" t="n"/>
-      <c r="K21" s="316" t="inlineStr">
+      <c r="J21" s="209" t="n"/>
+      <c r="K21" s="258" t="inlineStr">
         <is>
           <t>X65308</t>
         </is>
       </c>
-      <c r="L21" s="262" t="n"/>
-    </row>
-    <row r="22" ht="72.75" customHeight="1" s="263">
+      <c r="L21" s="253" t="n"/>
+    </row>
+    <row r="22" ht="72.75" customHeight="1" s="244">
       <c r="A22" s="9" t="n"/>
-      <c r="B22" s="248" t="n"/>
-      <c r="C22" s="259" t="inlineStr">
+      <c r="B22" s="260" t="n"/>
+      <c r="C22" s="245" t="inlineStr">
         <is>
           <t>(The HMRC number is equivalent to a registered charity number in terms of evidence of charitable status and may be used to give to donors or grant funders wishing to see evidence of the organisation's charitable status.  Methodist charities in England and Wales that are not registered charities are excepted from registration under Statutory Instrument  2014  No.242)</t>
         </is>
       </c>
     </row>
-    <row r="23" ht="14.25" customFormat="1" customHeight="1" s="248">
-      <c r="A23" s="212" t="n"/>
-      <c r="B23" s="247" t="inlineStr">
+    <row r="23" ht="14.25" customFormat="1" customHeight="1" s="260">
+      <c r="A23" s="208" t="n"/>
+      <c r="B23" s="259" t="inlineStr">
         <is>
           <t>Minister:</t>
         </is>
       </c>
     </row>
-    <row r="24" ht="30.2" customFormat="1" customHeight="1" s="248">
-      <c r="A24" s="212" t="n"/>
-      <c r="C24" s="264" t="inlineStr">
+    <row r="24" ht="30.2" customFormat="1" customHeight="1" s="260">
+      <c r="A24" s="208" t="n"/>
+      <c r="C24" s="265" t="inlineStr">
         <is>
           <t>Gareth Phillips</t>
         </is>
       </c>
-      <c r="D24" s="265" t="n"/>
-      <c r="E24" s="265" t="n"/>
-      <c r="F24" s="265" t="n"/>
-      <c r="G24" s="265" t="n"/>
-      <c r="H24" s="265" t="n"/>
-      <c r="I24" s="265" t="n"/>
-      <c r="J24" s="265" t="n"/>
-      <c r="K24" s="265" t="n"/>
-      <c r="L24" s="262" t="n"/>
-    </row>
-    <row r="25" ht="23.25" customFormat="1" customHeight="1" s="248">
-      <c r="A25" s="212" t="n"/>
-      <c r="B25" s="247" t="inlineStr">
+      <c r="D24" s="266" t="n"/>
+      <c r="E24" s="266" t="n"/>
+      <c r="F24" s="266" t="n"/>
+      <c r="G24" s="266" t="n"/>
+      <c r="H24" s="266" t="n"/>
+      <c r="I24" s="266" t="n"/>
+      <c r="J24" s="266" t="n"/>
+      <c r="K24" s="266" t="n"/>
+      <c r="L24" s="253" t="n"/>
+    </row>
+    <row r="25" ht="23.25" customFormat="1" customHeight="1" s="260">
+      <c r="A25" s="208" t="n"/>
+      <c r="B25" s="259" t="inlineStr">
         <is>
           <t>Church Stewards:</t>
         </is>
       </c>
     </row>
-    <row r="26" ht="30.2" customFormat="1" customHeight="1" s="248">
-      <c r="A26" s="212" t="n"/>
-      <c r="C26" s="252" t="inlineStr">
+    <row r="26" ht="30.2" customFormat="1" customHeight="1" s="260">
+      <c r="A26" s="208" t="n"/>
+      <c r="C26" s="274" t="inlineStr">
         <is>
           <t>Ann North</t>
         </is>
       </c>
-      <c r="D26" s="250" t="n"/>
-      <c r="E26" s="250" t="n"/>
-      <c r="F26" s="250" t="n"/>
-      <c r="G26" s="250" t="n"/>
-      <c r="H26" s="250" t="n"/>
-      <c r="I26" s="249" t="inlineStr">
+      <c r="D26" s="272" t="n"/>
+      <c r="E26" s="272" t="n"/>
+      <c r="F26" s="272" t="n"/>
+      <c r="G26" s="272" t="n"/>
+      <c r="H26" s="272" t="n"/>
+      <c r="I26" s="271" t="inlineStr">
         <is>
           <t>Dennis Buck</t>
         </is>
       </c>
-      <c r="J26" s="250" t="n"/>
-      <c r="K26" s="250" t="n"/>
-      <c r="L26" s="251" t="n"/>
-    </row>
-    <row r="27" ht="30.2" customFormat="1" customHeight="1" s="248">
-      <c r="A27" s="212" t="n"/>
-      <c r="C27" s="258" t="inlineStr">
+      <c r="J26" s="272" t="n"/>
+      <c r="K26" s="272" t="n"/>
+      <c r="L26" s="273" t="n"/>
+    </row>
+    <row r="27" ht="30.2" customFormat="1" customHeight="1" s="260">
+      <c r="A27" s="208" t="n"/>
+      <c r="C27" s="276" t="inlineStr">
         <is>
           <t>Peter Brown</t>
         </is>
       </c>
-      <c r="D27" s="254" t="n"/>
-      <c r="E27" s="254" t="n"/>
-      <c r="F27" s="254" t="n"/>
-      <c r="G27" s="254" t="n"/>
-      <c r="H27" s="254" t="n"/>
-      <c r="I27" s="255" t="inlineStr">
+      <c r="D27" s="262" t="n"/>
+      <c r="E27" s="262" t="n"/>
+      <c r="F27" s="262" t="n"/>
+      <c r="G27" s="262" t="n"/>
+      <c r="H27" s="262" t="n"/>
+      <c r="I27" s="275" t="inlineStr">
         <is>
           <t>Sally Wardell</t>
         </is>
       </c>
-      <c r="J27" s="254" t="n"/>
-      <c r="K27" s="254" t="n"/>
-      <c r="L27" s="256" t="n"/>
-    </row>
-    <row r="28" ht="30.2" customFormat="1" customHeight="1" s="248">
-      <c r="A28" s="212" t="n"/>
+      <c r="J27" s="262" t="n"/>
+      <c r="K27" s="262" t="n"/>
+      <c r="L27" s="263" t="n"/>
+    </row>
+    <row r="28" ht="30.2" customFormat="1" customHeight="1" s="260">
+      <c r="A28" s="208" t="n"/>
       <c r="B28" s="34" t="n"/>
-      <c r="C28" s="253" t="n"/>
-      <c r="D28" s="254" t="n"/>
-      <c r="E28" s="254" t="n"/>
-      <c r="F28" s="254" t="n"/>
-      <c r="G28" s="254" t="n"/>
-      <c r="H28" s="254" t="n"/>
-      <c r="I28" s="257" t="n"/>
-      <c r="J28" s="254" t="n"/>
-      <c r="K28" s="254" t="n"/>
-      <c r="L28" s="256" t="n"/>
-    </row>
-    <row r="29" ht="30.2" customFormat="1" customHeight="1" s="248">
-      <c r="A29" s="212" t="n"/>
+      <c r="C28" s="264" t="n"/>
+      <c r="D28" s="262" t="n"/>
+      <c r="E28" s="262" t="n"/>
+      <c r="F28" s="262" t="n"/>
+      <c r="G28" s="262" t="n"/>
+      <c r="H28" s="262" t="n"/>
+      <c r="I28" s="261" t="n"/>
+      <c r="J28" s="262" t="n"/>
+      <c r="K28" s="262" t="n"/>
+      <c r="L28" s="263" t="n"/>
+    </row>
+    <row r="29" ht="30.2" customFormat="1" customHeight="1" s="260">
+      <c r="A29" s="208" t="n"/>
       <c r="B29" s="34" t="n"/>
-      <c r="C29" s="253" t="n"/>
-      <c r="D29" s="254" t="n"/>
-      <c r="E29" s="254" t="n"/>
-      <c r="F29" s="254" t="n"/>
-      <c r="G29" s="254" t="n"/>
-      <c r="H29" s="254" t="n"/>
-      <c r="I29" s="257" t="n"/>
-      <c r="J29" s="254" t="n"/>
-      <c r="K29" s="254" t="n"/>
-      <c r="L29" s="256" t="n"/>
-    </row>
-    <row r="30" ht="30.2" customFormat="1" customHeight="1" s="248">
-      <c r="A30" s="212" t="n"/>
+      <c r="C29" s="264" t="n"/>
+      <c r="D29" s="262" t="n"/>
+      <c r="E29" s="262" t="n"/>
+      <c r="F29" s="262" t="n"/>
+      <c r="G29" s="262" t="n"/>
+      <c r="H29" s="262" t="n"/>
+      <c r="I29" s="261" t="n"/>
+      <c r="J29" s="262" t="n"/>
+      <c r="K29" s="262" t="n"/>
+      <c r="L29" s="263" t="n"/>
+    </row>
+    <row r="30" ht="30.2" customFormat="1" customHeight="1" s="260">
+      <c r="A30" s="208" t="n"/>
       <c r="B30" s="34" t="n"/>
-      <c r="C30" s="253" t="n"/>
-      <c r="D30" s="254" t="n"/>
-      <c r="E30" s="254" t="n"/>
-      <c r="F30" s="254" t="n"/>
-      <c r="G30" s="254" t="n"/>
-      <c r="H30" s="254" t="n"/>
-      <c r="I30" s="257" t="n"/>
-      <c r="J30" s="254" t="n"/>
-      <c r="K30" s="254" t="n"/>
-      <c r="L30" s="256" t="n"/>
-    </row>
-    <row r="31" ht="30.2" customFormat="1" customHeight="1" s="248">
-      <c r="A31" s="212" t="n"/>
+      <c r="C30" s="264" t="n"/>
+      <c r="D30" s="262" t="n"/>
+      <c r="E30" s="262" t="n"/>
+      <c r="F30" s="262" t="n"/>
+      <c r="G30" s="262" t="n"/>
+      <c r="H30" s="262" t="n"/>
+      <c r="I30" s="261" t="n"/>
+      <c r="J30" s="262" t="n"/>
+      <c r="K30" s="262" t="n"/>
+      <c r="L30" s="263" t="n"/>
+    </row>
+    <row r="31" ht="30.2" customFormat="1" customHeight="1" s="260">
+      <c r="A31" s="208" t="n"/>
       <c r="B31" s="34" t="n"/>
-      <c r="C31" s="253" t="n"/>
-      <c r="D31" s="254" t="n"/>
-      <c r="E31" s="254" t="n"/>
-      <c r="F31" s="254" t="n"/>
-      <c r="G31" s="254" t="n"/>
-      <c r="H31" s="254" t="n"/>
-      <c r="I31" s="257" t="n"/>
-      <c r="J31" s="254" t="n"/>
-      <c r="K31" s="254" t="n"/>
-      <c r="L31" s="256" t="n"/>
-    </row>
-    <row r="32" ht="30.2" customFormat="1" customHeight="1" s="248">
-      <c r="A32" s="212" t="n"/>
+      <c r="C31" s="264" t="n"/>
+      <c r="D31" s="262" t="n"/>
+      <c r="E31" s="262" t="n"/>
+      <c r="F31" s="262" t="n"/>
+      <c r="G31" s="262" t="n"/>
+      <c r="H31" s="262" t="n"/>
+      <c r="I31" s="261" t="n"/>
+      <c r="J31" s="262" t="n"/>
+      <c r="K31" s="262" t="n"/>
+      <c r="L31" s="263" t="n"/>
+    </row>
+    <row r="32" ht="30.2" customFormat="1" customHeight="1" s="260">
+      <c r="A32" s="208" t="n"/>
       <c r="B32" s="34" t="n"/>
-      <c r="C32" s="269" t="n"/>
-      <c r="D32" s="267" t="n"/>
-      <c r="E32" s="267" t="n"/>
-      <c r="F32" s="267" t="n"/>
-      <c r="G32" s="267" t="n"/>
-      <c r="H32" s="267" t="n"/>
-      <c r="I32" s="266" t="n"/>
-      <c r="J32" s="267" t="n"/>
-      <c r="K32" s="267" t="n"/>
-      <c r="L32" s="268" t="n"/>
-    </row>
-    <row r="33" ht="9" customFormat="1" customHeight="1" s="248">
-      <c r="A33" s="212" t="n"/>
+      <c r="C32" s="270" t="n"/>
+      <c r="D32" s="268" t="n"/>
+      <c r="E32" s="268" t="n"/>
+      <c r="F32" s="268" t="n"/>
+      <c r="G32" s="268" t="n"/>
+      <c r="H32" s="268" t="n"/>
+      <c r="I32" s="267" t="n"/>
+      <c r="J32" s="268" t="n"/>
+      <c r="K32" s="268" t="n"/>
+      <c r="L32" s="269" t="n"/>
+    </row>
+    <row r="33" ht="9" customFormat="1" customHeight="1" s="260">
+      <c r="A33" s="208" t="n"/>
       <c r="B33" s="34" t="n"/>
       <c r="C33" s="34" t="n"/>
       <c r="D33" s="34" t="n"/>
@@ -2821,8 +2868,8 @@
       <c r="K33" s="34" t="n"/>
       <c r="L33" s="34" t="n"/>
     </row>
-    <row r="34" hidden="1" ht="3.75" customFormat="1" customHeight="1" s="248">
-      <c r="A34" s="212" t="n"/>
+    <row r="34" hidden="1" ht="3.75" customFormat="1" customHeight="1" s="260">
+      <c r="A34" s="208" t="n"/>
       <c r="B34" s="34" t="n"/>
       <c r="C34" s="34" t="n"/>
       <c r="D34" s="34" t="n"/>
@@ -2835,52 +2882,47 @@
       <c r="K34" s="34" t="n"/>
       <c r="L34" s="34" t="n"/>
     </row>
-    <row r="35" ht="14.25" customFormat="1" customHeight="1" s="248">
-      <c r="A35" s="212" t="n"/>
-      <c r="B35" s="247" t="inlineStr">
+    <row r="35" ht="14.25" customFormat="1" customHeight="1" s="260">
+      <c r="A35" s="208" t="n"/>
+      <c r="B35" s="259" t="inlineStr">
         <is>
           <t>Treasurer:</t>
         </is>
       </c>
     </row>
-    <row r="36" ht="30.2" customFormat="1" customHeight="1" s="248">
-      <c r="A36" s="212" t="n"/>
+    <row r="36" ht="30.2" customFormat="1" customHeight="1" s="260">
+      <c r="A36" s="208" t="n"/>
       <c r="B36" s="34" t="n"/>
-      <c r="C36" s="264" t="inlineStr">
+      <c r="C36" s="265" t="inlineStr">
         <is>
           <t>Ann Brown</t>
         </is>
       </c>
-      <c r="D36" s="265" t="n"/>
-      <c r="E36" s="265" t="n"/>
-      <c r="F36" s="265" t="n"/>
-      <c r="G36" s="265" t="n"/>
-      <c r="H36" s="265" t="n"/>
-      <c r="I36" s="265" t="n"/>
-      <c r="J36" s="265" t="n"/>
-      <c r="K36" s="265" t="n"/>
-      <c r="L36" s="262" t="n"/>
-    </row>
-    <row r="37" ht="6" customHeight="1" s="263">
+      <c r="D36" s="266" t="n"/>
+      <c r="E36" s="266" t="n"/>
+      <c r="F36" s="266" t="n"/>
+      <c r="G36" s="266" t="n"/>
+      <c r="H36" s="266" t="n"/>
+      <c r="I36" s="266" t="n"/>
+      <c r="J36" s="266" t="n"/>
+      <c r="K36" s="266" t="n"/>
+      <c r="L36" s="253" t="n"/>
+    </row>
+    <row r="37" ht="6" customHeight="1" s="244">
       <c r="A37" s="9" t="n"/>
     </row>
-    <row r="38" ht="6" customHeight="1" s="263"/>
+    <row r="38" ht="6" customHeight="1" s="244"/>
     <row r="40"/>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="B2:L2"/>
-    <mergeCell ref="C20:J20"/>
-    <mergeCell ref="B3:L3"/>
-    <mergeCell ref="B4:L4"/>
-    <mergeCell ref="B6:L6"/>
-    <mergeCell ref="B8:L8"/>
-    <mergeCell ref="B9:L9"/>
-    <mergeCell ref="C11:K11"/>
-    <mergeCell ref="B13:L13"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="B15:L15"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C19:I19"/>
+    <mergeCell ref="B25:L25"/>
+    <mergeCell ref="B23:L23"/>
+    <mergeCell ref="I26:L26"/>
+    <mergeCell ref="C26:H26"/>
+    <mergeCell ref="C28:H28"/>
+    <mergeCell ref="I27:L27"/>
+    <mergeCell ref="I28:L28"/>
+    <mergeCell ref="C27:H27"/>
     <mergeCell ref="C21:I21"/>
     <mergeCell ref="K19:L19"/>
     <mergeCell ref="K21:L21"/>
@@ -2897,14 +2939,19 @@
     <mergeCell ref="I29:L29"/>
     <mergeCell ref="C22:L22"/>
     <mergeCell ref="C24:L24"/>
-    <mergeCell ref="B25:L25"/>
-    <mergeCell ref="B23:L23"/>
-    <mergeCell ref="I26:L26"/>
-    <mergeCell ref="C26:H26"/>
-    <mergeCell ref="C28:H28"/>
-    <mergeCell ref="I27:L27"/>
-    <mergeCell ref="I28:L28"/>
-    <mergeCell ref="C27:H27"/>
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="C20:J20"/>
+    <mergeCell ref="B3:L3"/>
+    <mergeCell ref="B4:L4"/>
+    <mergeCell ref="B6:L6"/>
+    <mergeCell ref="B8:L8"/>
+    <mergeCell ref="B9:L9"/>
+    <mergeCell ref="C11:K11"/>
+    <mergeCell ref="B13:L13"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="B15:L15"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C19:I19"/>
   </mergeCells>
   <pageMargins left="0.3937007874015748" right="0.2362204724409449" top="0.3937007874015748" bottom="0.3937007874015748" header="0.2362204724409449" footer="0.1574803149606299"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -2928,48 +2975,48 @@
   </sheetPr>
   <dimension ref="B1:R42"/>
   <sheetViews>
-    <sheetView showZeros="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showZeros="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="J10" sqref="J10"/>
+      <selection pane="bottomRight" activeCell="J7" sqref="J7:J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
   <cols>
-    <col width="1.42578125" customWidth="1" style="288" min="1" max="1"/>
-    <col width="0.5703125" customWidth="1" style="288" min="2" max="2"/>
-    <col width="3" bestFit="1" customWidth="1" style="288" min="3" max="3"/>
-    <col width="28.140625" customWidth="1" style="288" min="4" max="4"/>
-    <col width="6" customWidth="1" style="288" min="5" max="5"/>
-    <col width="14" customWidth="1" style="288" min="6" max="6"/>
-    <col width="11.42578125" customWidth="1" style="288" min="7" max="7"/>
-    <col width="10" customWidth="1" style="288" min="8" max="8"/>
-    <col width="0.85546875" customWidth="1" style="288" min="9" max="9"/>
-    <col width="10" customWidth="1" style="288" min="10" max="10"/>
-    <col width="4.85546875" bestFit="1" customWidth="1" style="288" min="11" max="11"/>
-    <col width="0.85546875" customWidth="1" style="288" min="12" max="12"/>
-    <col width="10" customWidth="1" style="288" min="13" max="13"/>
-    <col width="5.42578125" customWidth="1" style="288" min="14" max="14"/>
-    <col width="1" customWidth="1" style="288" min="15" max="15"/>
-    <col width="0.5703125" customWidth="1" style="288" min="16" max="16"/>
-    <col width="10" customWidth="1" style="288" min="17" max="17"/>
-    <col width="6.42578125" customWidth="1" style="288" min="18" max="18"/>
-    <col width="17.5703125" customWidth="1" style="288" min="19" max="19"/>
-    <col width="9.140625" customWidth="1" style="288" min="20" max="32"/>
-    <col width="9.140625" customWidth="1" style="288" min="33" max="16384"/>
+    <col width="1.42578125" customWidth="1" style="292" min="1" max="1"/>
+    <col width="0.5703125" customWidth="1" style="292" min="2" max="2"/>
+    <col width="3" bestFit="1" customWidth="1" style="292" min="3" max="3"/>
+    <col width="28.140625" customWidth="1" style="292" min="4" max="4"/>
+    <col width="6" customWidth="1" style="292" min="5" max="5"/>
+    <col width="14" customWidth="1" style="292" min="6" max="6"/>
+    <col width="11.42578125" customWidth="1" style="330" min="7" max="7"/>
+    <col width="10" customWidth="1" style="292" min="8" max="8"/>
+    <col width="0.85546875" customWidth="1" style="292" min="9" max="9"/>
+    <col width="10" customWidth="1" style="330" min="10" max="10"/>
+    <col width="4.85546875" bestFit="1" customWidth="1" style="292" min="11" max="11"/>
+    <col width="0.85546875" customWidth="1" style="292" min="12" max="12"/>
+    <col width="10" customWidth="1" style="292" min="13" max="13"/>
+    <col width="5.42578125" customWidth="1" style="292" min="14" max="14"/>
+    <col width="1" customWidth="1" style="292" min="15" max="15"/>
+    <col width="0.5703125" customWidth="1" style="292" min="16" max="16"/>
+    <col width="10" customWidth="1" style="292" min="17" max="17"/>
+    <col width="6.42578125" customWidth="1" style="292" min="18" max="18"/>
+    <col width="17.5703125" customWidth="1" style="292" min="19" max="19"/>
+    <col width="9.140625" customWidth="1" style="292" min="20" max="33"/>
+    <col width="9.140625" customWidth="1" style="292" min="34" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" ht="7.5" customHeight="1" s="263">
+    <row r="1" ht="7.5" customHeight="1" s="244">
       <c r="B1" s="8" t="n"/>
       <c r="C1" s="37" t="n"/>
       <c r="D1" s="37" t="n"/>
       <c r="E1" s="37" t="n"/>
       <c r="F1" s="37" t="n"/>
-      <c r="G1" s="37" t="n"/>
+      <c r="G1" s="315" t="n"/>
       <c r="H1" s="37" t="n"/>
       <c r="I1" s="37" t="n"/>
-      <c r="J1" s="37" t="n"/>
+      <c r="J1" s="315" t="n"/>
       <c r="K1" s="37" t="n"/>
       <c r="L1" s="37" t="n"/>
       <c r="M1" s="37" t="n"/>
@@ -2977,27 +3024,27 @@
       <c r="O1" s="8" t="n"/>
       <c r="P1" s="8" t="n"/>
     </row>
-    <row r="2" ht="37.5" customHeight="1" s="263">
+    <row r="2" ht="37.5" customHeight="1" s="244">
       <c r="B2" s="8" t="n"/>
-      <c r="C2" s="287" t="inlineStr">
+      <c r="C2" s="291" t="inlineStr">
         <is>
           <t>ACCOUNTS FOR THE YEAR ENDED 31 AUGUST 2024</t>
         </is>
       </c>
-      <c r="H2" s="291">
+      <c r="H2" s="295">
         <f>'P1 Front page'!$C$11</f>
         <v/>
       </c>
-      <c r="I2" s="275" t="n"/>
-      <c r="J2" s="275" t="n"/>
-      <c r="K2" s="275" t="n"/>
-      <c r="L2" s="275" t="n"/>
-      <c r="M2" s="280" t="inlineStr">
+      <c r="I2" s="250" t="n"/>
+      <c r="J2" s="250" t="n"/>
+      <c r="K2" s="250" t="n"/>
+      <c r="L2" s="250" t="n"/>
+      <c r="M2" s="285" t="inlineStr">
         <is>
           <t>Church</t>
         </is>
       </c>
-      <c r="N2" s="281" t="n"/>
+      <c r="N2" s="282" t="n"/>
       <c r="O2" s="19" t="n"/>
       <c r="P2" s="8" t="n"/>
       <c r="Q2" s="11" t="inlineStr">
@@ -3006,31 +3053,31 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="7.5" customFormat="1" customHeight="1" s="290">
+    <row r="3" ht="7.5" customFormat="1" customHeight="1" s="294">
       <c r="B3" s="131" t="n"/>
       <c r="C3" s="132" t="n"/>
       <c r="D3" s="132" t="n"/>
       <c r="E3" s="132" t="n"/>
       <c r="F3" s="132" t="n"/>
-      <c r="G3" s="289" t="inlineStr">
+      <c r="G3" s="316" t="inlineStr">
         <is>
           <t>Unrestricted Funds</t>
         </is>
       </c>
-      <c r="H3" s="289" t="inlineStr">
+      <c r="H3" s="293" t="inlineStr">
         <is>
           <t>Restricted Funds</t>
         </is>
       </c>
-      <c r="I3" s="176" t="n"/>
-      <c r="J3" s="289" t="inlineStr">
+      <c r="I3" s="172" t="n"/>
+      <c r="J3" s="316" t="inlineStr">
         <is>
           <t>Totals this year</t>
         </is>
       </c>
-      <c r="K3" s="289" t="n"/>
-      <c r="L3" s="289" t="n"/>
-      <c r="M3" s="289" t="inlineStr">
+      <c r="K3" s="293" t="n"/>
+      <c r="L3" s="293" t="n"/>
+      <c r="M3" s="293" t="inlineStr">
         <is>
           <t>Totals last year</t>
         </is>
@@ -3039,7 +3086,7 @@
       <c r="O3" s="4" t="n"/>
       <c r="P3" s="131" t="n"/>
     </row>
-    <row r="4" ht="23.25" customFormat="1" customHeight="1" s="290">
+    <row r="4" ht="23.25" customFormat="1" customHeight="1" s="294">
       <c r="B4" s="131" t="n"/>
       <c r="C4" s="132" t="n"/>
       <c r="D4" s="136" t="inlineStr">
@@ -3049,20 +3096,20 @@
       </c>
       <c r="E4" s="132" t="n"/>
       <c r="F4" s="132" t="n"/>
-      <c r="I4" s="176" t="n"/>
-      <c r="K4" s="289" t="n"/>
-      <c r="L4" s="289" t="n"/>
+      <c r="I4" s="172" t="n"/>
+      <c r="K4" s="293" t="n"/>
+      <c r="L4" s="293" t="n"/>
       <c r="N4" s="39" t="n"/>
       <c r="O4" s="4" t="n"/>
       <c r="P4" s="131" t="n"/>
     </row>
-    <row r="5" ht="23.25" customFormat="1" customHeight="1" s="290">
+    <row r="5" ht="23.25" customFormat="1" customHeight="1" s="294">
       <c r="B5" s="131" t="n"/>
       <c r="C5" s="40" t="n"/>
       <c r="D5" s="137" t="n"/>
       <c r="E5" s="138" t="n"/>
       <c r="F5" s="139" t="n"/>
-      <c r="G5" s="139" t="inlineStr">
+      <c r="G5" s="318" t="inlineStr">
         <is>
           <t>£</t>
         </is>
@@ -3073,7 +3120,7 @@
         </is>
       </c>
       <c r="I5" s="41" t="n"/>
-      <c r="J5" s="139" t="inlineStr">
+      <c r="J5" s="318" t="inlineStr">
         <is>
           <t>£</t>
         </is>
@@ -3089,7 +3136,7 @@
       <c r="O5" s="4" t="n"/>
       <c r="P5" s="131" t="n"/>
     </row>
-    <row r="6" ht="18.75" customHeight="1" s="263">
+    <row r="6" ht="18.75" customHeight="1" s="244">
       <c r="B6" s="8" t="n"/>
       <c r="C6" s="40" t="inlineStr">
         <is>
@@ -3107,10 +3154,10 @@
           <t>Note</t>
         </is>
       </c>
-      <c r="G6" s="139" t="n"/>
+      <c r="G6" s="318" t="n"/>
       <c r="H6" s="139" t="n"/>
       <c r="I6" s="41" t="n"/>
-      <c r="J6" s="139" t="n"/>
+      <c r="J6" s="318" t="n"/>
       <c r="K6" s="140" t="n"/>
       <c r="L6" s="140" t="n"/>
       <c r="M6" s="139" t="n"/>
@@ -3118,7 +3165,7 @@
       <c r="O6" s="14" t="n"/>
       <c r="P6" s="8" t="n"/>
     </row>
-    <row r="7" ht="18.75" customHeight="1" s="263">
+    <row r="7" ht="18.75" customHeight="1" s="244">
       <c r="B7" s="8" t="n"/>
       <c r="C7" s="40" t="inlineStr">
         <is>
@@ -3132,10 +3179,12 @@
       </c>
       <c r="E7" s="42" t="n"/>
       <c r="F7" s="43" t="n"/>
-      <c r="G7" s="141" t="n"/>
+      <c r="G7" s="342" t="n">
+        <v>3553.8</v>
+      </c>
       <c r="H7" s="141" t="n"/>
       <c r="I7" s="38" t="n"/>
-      <c r="J7" s="136" t="n">
+      <c r="J7" s="343" t="n">
         <v>3553.8</v>
       </c>
       <c r="K7" s="134" t="n"/>
@@ -3144,26 +3193,27 @@
       <c r="N7" s="38" t="n"/>
       <c r="P7" s="8" t="n"/>
     </row>
-    <row r="8" ht="27" customHeight="1" s="263">
+    <row r="8" ht="27" customHeight="1" s="244">
       <c r="B8" s="8" t="n"/>
       <c r="C8" s="40" t="inlineStr">
         <is>
           <t>a3</t>
         </is>
       </c>
-      <c r="D8" s="151" t="inlineStr">
+      <c r="D8" s="150" t="inlineStr">
         <is>
           <t>Bank and CFB interest and Investment income</t>
         </is>
       </c>
       <c r="E8" s="42" t="n"/>
       <c r="F8" s="43" t="n"/>
-      <c r="G8" s="141" t="n"/>
+      <c r="G8" s="342" t="n">
+        <v>4480</v>
+      </c>
       <c r="H8" s="141" t="n"/>
       <c r="I8" s="38" t="n"/>
-      <c r="J8" s="136">
-        <f>SUM('Data from streamlit'!D19:D21)</f>
-        <v/>
+      <c r="J8" s="343" t="n">
+        <v>4480</v>
       </c>
       <c r="K8" s="134" t="n"/>
       <c r="L8" s="134" t="n"/>
@@ -3171,7 +3221,7 @@
       <c r="N8" s="38" t="n"/>
       <c r="P8" s="8" t="n"/>
     </row>
-    <row r="9" ht="18" customHeight="1" s="263">
+    <row r="9" ht="18" customHeight="1" s="244">
       <c r="B9" s="8" t="n"/>
       <c r="C9" s="40" t="inlineStr">
         <is>
@@ -3185,12 +3235,13 @@
       </c>
       <c r="E9" s="42" t="n"/>
       <c r="F9" s="43" t="n"/>
-      <c r="G9" s="141" t="n"/>
+      <c r="G9" s="342" t="n">
+        <v>8401.9</v>
+      </c>
       <c r="H9" s="141" t="n"/>
       <c r="I9" s="38" t="n"/>
-      <c r="J9" s="136">
-        <f>SUM('Data from streamlit'!D24:D25)</f>
-        <v/>
+      <c r="J9" s="343" t="n">
+        <v>8401.9</v>
       </c>
       <c r="K9" s="134" t="n"/>
       <c r="L9" s="134" t="n"/>
@@ -3198,7 +3249,7 @@
       <c r="N9" s="38" t="n"/>
       <c r="P9" s="8" t="n"/>
     </row>
-    <row r="10" ht="18.75" customHeight="1" s="263" thickBot="1">
+    <row r="10" ht="18.75" customHeight="1" s="244" thickBot="1">
       <c r="B10" s="8" t="n"/>
       <c r="C10" s="40" t="inlineStr">
         <is>
@@ -3212,12 +3263,13 @@
       </c>
       <c r="E10" s="42" t="n"/>
       <c r="F10" s="43" t="n"/>
-      <c r="G10" s="142" t="n"/>
+      <c r="G10" s="314" t="n">
+        <v>450</v>
+      </c>
       <c r="H10" s="142" t="n"/>
       <c r="I10" s="38" t="n"/>
-      <c r="J10" s="143">
-        <f>SUM(G10:H10)</f>
-        <v/>
+      <c r="J10" s="313" t="n">
+        <v>450</v>
       </c>
       <c r="K10" s="134" t="n"/>
       <c r="L10" s="134" t="n"/>
@@ -3225,7 +3277,7 @@
       <c r="N10" s="38" t="n"/>
       <c r="P10" s="8" t="n"/>
     </row>
-    <row r="11" ht="17.45" customHeight="1" s="263" thickBot="1">
+    <row r="11" ht="17.45" customHeight="1" s="244" thickBot="1">
       <c r="B11" s="8" t="n"/>
       <c r="C11" s="40" t="inlineStr">
         <is>
@@ -3239,7 +3291,7 @@
       </c>
       <c r="E11" s="145" t="n"/>
       <c r="F11" s="146" t="n"/>
-      <c r="G11" s="147">
+      <c r="G11" s="321">
         <f>SUM(G7:G10)</f>
         <v/>
       </c>
@@ -3248,11 +3300,11 @@
         <v/>
       </c>
       <c r="I11" s="148" t="n"/>
-      <c r="J11" s="149">
+      <c r="J11" s="333">
         <f>SUM(J7:J10)</f>
         <v/>
       </c>
-      <c r="K11" s="150" t="inlineStr">
+      <c r="K11" s="149" t="inlineStr">
         <is>
           <t>(a7)</t>
         </is>
@@ -3266,23 +3318,23 @@
       <c r="O11" s="6" t="n"/>
       <c r="P11" s="8" t="n"/>
     </row>
-    <row r="12" ht="8.449999999999999" customHeight="1" s="263">
+    <row r="12" ht="8.449999999999999" customHeight="1" s="244">
       <c r="B12" s="8" t="n"/>
       <c r="C12" s="38" t="n"/>
       <c r="D12" s="38" t="n"/>
       <c r="E12" s="38" t="n"/>
       <c r="F12" s="41" t="n"/>
-      <c r="G12" s="38" t="n"/>
+      <c r="G12" s="322" t="n"/>
       <c r="H12" s="38" t="n"/>
       <c r="I12" s="38" t="n"/>
-      <c r="J12" s="46" t="n"/>
+      <c r="J12" s="334" t="n"/>
       <c r="K12" s="46" t="n"/>
       <c r="L12" s="46" t="n"/>
       <c r="M12" s="38" t="n"/>
       <c r="N12" s="38" t="n"/>
       <c r="P12" s="8" t="n"/>
     </row>
-    <row r="13" ht="18.75" customHeight="1" s="263">
+    <row r="13" ht="18.75" customHeight="1" s="244">
       <c r="B13" s="8" t="n"/>
       <c r="C13" s="38" t="n"/>
       <c r="D13" s="136" t="inlineStr">
@@ -3292,17 +3344,17 @@
       </c>
       <c r="E13" s="38" t="n"/>
       <c r="F13" s="41" t="n"/>
-      <c r="G13" s="38" t="n"/>
+      <c r="G13" s="322" t="n"/>
       <c r="H13" s="38" t="n"/>
       <c r="I13" s="38" t="n"/>
-      <c r="J13" s="46" t="n"/>
+      <c r="J13" s="334" t="n"/>
       <c r="K13" s="46" t="n"/>
       <c r="L13" s="46" t="n"/>
       <c r="M13" s="38" t="n"/>
       <c r="N13" s="38" t="n"/>
       <c r="P13" s="8" t="n"/>
     </row>
-    <row r="14" ht="18.75" customHeight="1" s="263">
+    <row r="14" ht="18.75" customHeight="1" s="244">
       <c r="B14" s="8" t="n"/>
       <c r="C14" s="40" t="inlineStr">
         <is>
@@ -3316,17 +3368,17 @@
       </c>
       <c r="E14" s="138" t="n"/>
       <c r="F14" s="41" t="n"/>
-      <c r="G14" s="38" t="n"/>
+      <c r="G14" s="322" t="n"/>
       <c r="H14" s="38" t="n"/>
       <c r="I14" s="38" t="n"/>
-      <c r="J14" s="38" t="n"/>
+      <c r="J14" s="322" t="n"/>
       <c r="K14" s="38" t="n"/>
       <c r="L14" s="38" t="n"/>
       <c r="M14" s="38" t="n"/>
       <c r="N14" s="38" t="n"/>
       <c r="P14" s="8" t="n"/>
     </row>
-    <row r="15" ht="18" customHeight="1" s="263">
+    <row r="15" ht="18" customHeight="1" s="244">
       <c r="B15" s="8" t="n"/>
       <c r="C15" s="40" t="inlineStr">
         <is>
@@ -3340,10 +3392,10 @@
       </c>
       <c r="E15" s="42" t="n"/>
       <c r="F15" s="43" t="n"/>
-      <c r="G15" s="141" t="n"/>
+      <c r="G15" s="319" t="n"/>
       <c r="H15" s="141" t="n"/>
       <c r="I15" s="38" t="n"/>
-      <c r="J15" s="136">
+      <c r="J15" s="331">
         <f>+G15+H15</f>
         <v/>
       </c>
@@ -3353,7 +3405,7 @@
       <c r="N15" s="38" t="n"/>
       <c r="P15" s="8" t="n"/>
     </row>
-    <row r="16" ht="18.75" customHeight="1" s="263">
+    <row r="16" ht="18.75" customHeight="1" s="244">
       <c r="B16" s="8" t="n"/>
       <c r="C16" s="40" t="inlineStr">
         <is>
@@ -3367,10 +3419,10 @@
       </c>
       <c r="E16" s="42" t="n"/>
       <c r="F16" s="43" t="n"/>
-      <c r="G16" s="141" t="n"/>
+      <c r="G16" s="319" t="n"/>
       <c r="H16" s="141" t="n"/>
       <c r="I16" s="38" t="n"/>
-      <c r="J16" s="136">
+      <c r="J16" s="331">
         <f>+G16+H16</f>
         <v/>
       </c>
@@ -3380,7 +3432,7 @@
       <c r="N16" s="38" t="n"/>
       <c r="P16" s="8" t="n"/>
     </row>
-    <row r="17" ht="18.75" customHeight="1" s="263">
+    <row r="17" ht="18.75" customHeight="1" s="244">
       <c r="B17" s="8" t="n"/>
       <c r="C17" s="40" t="inlineStr">
         <is>
@@ -3394,10 +3446,10 @@
       </c>
       <c r="E17" s="42" t="n"/>
       <c r="F17" s="43" t="n"/>
-      <c r="G17" s="141" t="n"/>
+      <c r="G17" s="319" t="n"/>
       <c r="H17" s="141" t="n"/>
       <c r="I17" s="38" t="n"/>
-      <c r="J17" s="136">
+      <c r="J17" s="331">
         <f>+G17+H17</f>
         <v/>
       </c>
@@ -3407,24 +3459,24 @@
       <c r="N17" s="38" t="n"/>
       <c r="P17" s="8" t="n"/>
     </row>
-    <row r="18" ht="26.45" customHeight="1" s="263">
+    <row r="18" ht="26.45" customHeight="1" s="244">
       <c r="B18" s="8" t="n"/>
       <c r="C18" s="40" t="inlineStr">
         <is>
           <t>b5</t>
         </is>
       </c>
-      <c r="D18" s="151" t="inlineStr">
+      <c r="D18" s="150" t="inlineStr">
         <is>
           <t>Utilities (Insurances, water charges, heating &amp; lighting)</t>
         </is>
       </c>
       <c r="E18" s="42" t="n"/>
       <c r="F18" s="43" t="n"/>
-      <c r="G18" s="141" t="n"/>
+      <c r="G18" s="319" t="n"/>
       <c r="H18" s="141" t="n"/>
       <c r="I18" s="38" t="n"/>
-      <c r="J18" s="136">
+      <c r="J18" s="331">
         <f>+G18+H18</f>
         <v/>
       </c>
@@ -3434,20 +3486,20 @@
       <c r="N18" s="38" t="n"/>
       <c r="P18" s="8" t="n"/>
     </row>
-    <row r="19" ht="18.75" customHeight="1" s="263">
+    <row r="19" ht="18.75" customHeight="1" s="244">
       <c r="B19" s="8" t="n"/>
       <c r="C19" s="40" t="inlineStr">
         <is>
           <t>b6</t>
         </is>
       </c>
-      <c r="D19" s="292" t="n"/>
-      <c r="E19" s="262" t="n"/>
+      <c r="D19" s="296" t="n"/>
+      <c r="E19" s="253" t="n"/>
       <c r="F19" s="43" t="n"/>
-      <c r="G19" s="142" t="n"/>
+      <c r="G19" s="320" t="n"/>
       <c r="H19" s="142" t="n"/>
       <c r="I19" s="38" t="n"/>
-      <c r="J19" s="143">
+      <c r="J19" s="332">
         <f>+G19+H19</f>
         <v/>
       </c>
@@ -3457,7 +3509,7 @@
       <c r="N19" s="38" t="n"/>
       <c r="P19" s="8" t="n"/>
     </row>
-    <row r="20" ht="18.75" customHeight="1" s="263" thickBot="1">
+    <row r="20" ht="18.75" customHeight="1" s="244" thickBot="1">
       <c r="B20" s="8" t="n"/>
       <c r="C20" s="40" t="inlineStr">
         <is>
@@ -3471,10 +3523,10 @@
       </c>
       <c r="E20" s="42" t="n"/>
       <c r="F20" s="43" t="n"/>
-      <c r="G20" s="142" t="n"/>
+      <c r="G20" s="320" t="n"/>
       <c r="H20" s="142" t="n"/>
       <c r="I20" s="38" t="n"/>
-      <c r="J20" s="143">
+      <c r="J20" s="332">
         <f>+G20+H20</f>
         <v/>
       </c>
@@ -3484,65 +3536,65 @@
       <c r="N20" s="38" t="n"/>
       <c r="P20" s="8" t="n"/>
     </row>
-    <row r="21" ht="18" customHeight="1" s="263" thickBot="1">
+    <row r="21" ht="18" customHeight="1" s="244" thickBot="1">
       <c r="B21" s="8" t="n"/>
       <c r="C21" s="40" t="inlineStr">
         <is>
           <t>b8</t>
         </is>
       </c>
-      <c r="D21" s="152" t="inlineStr">
+      <c r="D21" s="151" t="inlineStr">
         <is>
           <t xml:space="preserve">TOTAL PAYMENTS                        </t>
         </is>
       </c>
-      <c r="E21" s="153" t="n"/>
-      <c r="F21" s="154" t="n"/>
-      <c r="G21" s="155">
+      <c r="E21" s="152" t="n"/>
+      <c r="F21" s="153" t="n"/>
+      <c r="G21" s="323">
         <f>SUM(G15:G20)</f>
         <v/>
       </c>
-      <c r="H21" s="155">
+      <c r="H21" s="154">
         <f>SUM(H15:H20)</f>
         <v/>
       </c>
       <c r="I21" s="47" t="n"/>
-      <c r="J21" s="149">
+      <c r="J21" s="333">
         <f>SUM(G21:H21)</f>
         <v/>
       </c>
-      <c r="K21" s="150" t="inlineStr">
+      <c r="K21" s="149" t="inlineStr">
         <is>
           <t>(b9)</t>
         </is>
       </c>
-      <c r="L21" s="156" t="n"/>
-      <c r="M21" s="155">
+      <c r="L21" s="155" t="n"/>
+      <c r="M21" s="154">
         <f>SUM(M15:M20)</f>
         <v/>
       </c>
-      <c r="N21" s="156" t="n"/>
+      <c r="N21" s="155" t="n"/>
       <c r="O21" s="7" t="n"/>
       <c r="P21" s="8" t="n"/>
     </row>
-    <row r="22" ht="8.449999999999999" customHeight="1" s="263">
+    <row r="22" ht="8.449999999999999" customHeight="1" s="244">
       <c r="B22" s="8" t="n"/>
       <c r="C22" s="38" t="n"/>
-      <c r="D22" s="156" t="n"/>
-      <c r="E22" s="156" t="n"/>
+      <c r="D22" s="155" t="n"/>
+      <c r="E22" s="155" t="n"/>
       <c r="F22" s="48" t="n"/>
-      <c r="G22" s="156" t="n"/>
-      <c r="H22" s="156" t="n"/>
+      <c r="G22" s="324" t="n"/>
+      <c r="H22" s="155" t="n"/>
       <c r="I22" s="47" t="n"/>
-      <c r="J22" s="46" t="n"/>
+      <c r="J22" s="334" t="n"/>
       <c r="K22" s="46" t="n"/>
       <c r="L22" s="46" t="n"/>
-      <c r="M22" s="156" t="n"/>
-      <c r="N22" s="156" t="n"/>
+      <c r="M22" s="155" t="n"/>
+      <c r="N22" s="155" t="n"/>
       <c r="O22" s="7" t="n"/>
       <c r="P22" s="8" t="n"/>
     </row>
-    <row r="23" ht="18.75" customHeight="1" s="263">
+    <row r="23" ht="18.75" customHeight="1" s="244">
       <c r="B23" s="8" t="n"/>
       <c r="C23" s="38" t="n"/>
       <c r="D23" s="136" t="inlineStr">
@@ -3552,35 +3604,35 @@
       </c>
       <c r="E23" s="38" t="n"/>
       <c r="F23" s="41" t="n"/>
-      <c r="G23" s="38" t="n"/>
+      <c r="G23" s="322" t="n"/>
       <c r="H23" s="38" t="n"/>
       <c r="I23" s="38" t="n"/>
-      <c r="J23" s="134" t="n"/>
+      <c r="J23" s="335" t="n"/>
       <c r="K23" s="134" t="n"/>
       <c r="L23" s="134" t="n"/>
       <c r="M23" s="38" t="n"/>
       <c r="N23" s="38" t="n"/>
       <c r="P23" s="8" t="n"/>
     </row>
-    <row r="24" ht="25.5" customHeight="1" s="263">
+    <row r="24" ht="25.5" customHeight="1" s="244">
       <c r="B24" s="8" t="n"/>
       <c r="C24" s="40" t="inlineStr">
         <is>
           <t>c1</t>
         </is>
       </c>
-      <c r="D24" s="208" t="inlineStr">
+      <c r="D24" s="204" t="inlineStr">
         <is>
           <t xml:space="preserve">NET RECEIPTS/PAYMENTS FOR THE YEAR            </t>
         </is>
       </c>
       <c r="E24" s="42" t="n"/>
-      <c r="F24" s="157" t="inlineStr">
+      <c r="F24" s="156" t="inlineStr">
         <is>
           <t>(a6-b8)</t>
         </is>
       </c>
-      <c r="G24" s="40">
+      <c r="G24" s="325">
         <f>G11-G21</f>
         <v/>
       </c>
@@ -3589,7 +3641,7 @@
         <v/>
       </c>
       <c r="I24" s="38" t="n"/>
-      <c r="J24" s="136">
+      <c r="J24" s="331">
         <f>SUM(G24:H24)</f>
         <v/>
       </c>
@@ -3603,16 +3655,16 @@
       <c r="P24" s="8" t="n"/>
       <c r="Q24" s="17" t="n"/>
     </row>
-    <row r="25" ht="7.5" customHeight="1" s="263">
+    <row r="25" ht="7.5" customHeight="1" s="244">
       <c r="B25" s="8" t="n"/>
       <c r="C25" s="38" t="n"/>
       <c r="D25" s="42" t="n"/>
       <c r="E25" s="42" t="n"/>
-      <c r="F25" s="158" t="n"/>
-      <c r="G25" s="42" t="n"/>
+      <c r="F25" s="157" t="n"/>
+      <c r="G25" s="326" t="n"/>
       <c r="H25" s="42" t="n"/>
       <c r="I25" s="38" t="n"/>
-      <c r="J25" s="159" t="n"/>
+      <c r="J25" s="336" t="n"/>
       <c r="K25" s="134" t="n"/>
       <c r="L25" s="134" t="n"/>
       <c r="M25" s="42" t="n"/>
@@ -3620,28 +3672,28 @@
       <c r="P25" s="8" t="n"/>
       <c r="Q25" s="17" t="n"/>
     </row>
-    <row r="26" ht="33.75" customHeight="1" s="263">
+    <row r="26" ht="33.75" customHeight="1" s="244">
       <c r="B26" s="8" t="n"/>
       <c r="C26" s="40" t="inlineStr">
         <is>
           <t>c2</t>
         </is>
       </c>
-      <c r="D26" s="151" t="inlineStr">
+      <c r="D26" s="150" t="inlineStr">
         <is>
           <t>Total funds brought forward from last year</t>
         </is>
       </c>
       <c r="E26" s="42" t="n"/>
-      <c r="F26" s="158" t="n"/>
-      <c r="G26" s="141" t="n"/>
+      <c r="F26" s="157" t="n"/>
+      <c r="G26" s="319" t="n"/>
       <c r="H26" s="141" t="n"/>
       <c r="I26" s="38" t="n"/>
-      <c r="J26" s="136">
+      <c r="J26" s="331">
         <f>SUM(G26:H26)</f>
         <v/>
       </c>
-      <c r="K26" s="157" t="inlineStr">
+      <c r="K26" s="156" t="inlineStr">
         <is>
           <t>(c6)</t>
         </is>
@@ -3650,7 +3702,7 @@
       <c r="M26" s="141" t="n"/>
       <c r="N26" s="38" t="n"/>
       <c r="P26" s="8" t="n"/>
-      <c r="Q26" s="214" t="inlineStr">
+      <c r="Q26" s="210" t="inlineStr">
         <is>
           <t>Check Res+Unres total</t>
         </is>
@@ -3660,41 +3712,41 @@
         <v/>
       </c>
     </row>
-    <row r="27" ht="7.5" customHeight="1" s="263">
+    <row r="27" ht="7.5" customHeight="1" s="244">
       <c r="B27" s="8" t="n"/>
       <c r="C27" s="38" t="n"/>
       <c r="D27" s="42" t="n"/>
       <c r="E27" s="42" t="n"/>
-      <c r="F27" s="158" t="n"/>
-      <c r="G27" s="42" t="n"/>
+      <c r="F27" s="157" t="n"/>
+      <c r="G27" s="326" t="n"/>
       <c r="H27" s="42" t="n"/>
       <c r="I27" s="38" t="n"/>
-      <c r="J27" s="160" t="n"/>
+      <c r="J27" s="337" t="n"/>
       <c r="K27" s="140" t="n"/>
       <c r="L27" s="134" t="n"/>
       <c r="M27" s="42" t="n"/>
       <c r="N27" s="38" t="n"/>
       <c r="P27" s="8" t="n"/>
     </row>
-    <row r="28" ht="19.5" customHeight="1" s="263">
+    <row r="28" ht="19.5" customHeight="1" s="244">
       <c r="B28" s="8" t="n"/>
       <c r="C28" s="40" t="inlineStr">
         <is>
           <t>c3</t>
         </is>
       </c>
-      <c r="D28" s="296" t="inlineStr">
+      <c r="D28" s="280" t="inlineStr">
         <is>
           <t xml:space="preserve">Sub total                                                               </t>
         </is>
       </c>
-      <c r="E28" s="275" t="n"/>
-      <c r="F28" s="157" t="inlineStr">
+      <c r="E28" s="250" t="n"/>
+      <c r="F28" s="156" t="inlineStr">
         <is>
           <t>(c1+c2)</t>
         </is>
       </c>
-      <c r="G28" s="40">
+      <c r="G28" s="325">
         <f>G24+G26</f>
         <v/>
       </c>
@@ -3703,7 +3755,7 @@
         <v/>
       </c>
       <c r="I28" s="38" t="n"/>
-      <c r="J28" s="136">
+      <c r="J28" s="331">
         <f>J24+J26</f>
         <v/>
       </c>
@@ -3716,23 +3768,23 @@
       <c r="N28" s="38" t="n"/>
       <c r="P28" s="8" t="n"/>
     </row>
-    <row r="29" ht="7.5" customHeight="1" s="263">
+    <row r="29" ht="7.5" customHeight="1" s="244">
       <c r="B29" s="8" t="n"/>
       <c r="C29" s="38" t="n"/>
       <c r="D29" s="42" t="n"/>
       <c r="E29" s="42" t="n"/>
-      <c r="F29" s="158" t="n"/>
-      <c r="G29" s="42" t="n"/>
+      <c r="F29" s="157" t="n"/>
+      <c r="G29" s="326" t="n"/>
       <c r="H29" s="42" t="n"/>
       <c r="I29" s="38" t="n"/>
-      <c r="J29" s="161" t="n"/>
+      <c r="J29" s="338" t="n"/>
       <c r="K29" s="140" t="n"/>
       <c r="L29" s="134" t="n"/>
       <c r="M29" s="42" t="n"/>
       <c r="N29" s="38" t="n"/>
       <c r="P29" s="8" t="n"/>
     </row>
-    <row r="30" ht="18" customHeight="1" s="263">
+    <row r="30" ht="18" customHeight="1" s="244">
       <c r="B30" s="8" t="n"/>
       <c r="C30" s="40" t="inlineStr">
         <is>
@@ -3745,11 +3797,11 @@
         </is>
       </c>
       <c r="E30" s="42" t="n"/>
-      <c r="F30" s="157" t="n"/>
-      <c r="G30" s="141" t="n"/>
+      <c r="F30" s="156" t="n"/>
+      <c r="G30" s="319" t="n"/>
       <c r="H30" s="141" t="n"/>
       <c r="I30" s="38" t="n"/>
-      <c r="J30" s="136">
+      <c r="J30" s="331">
         <f>SUM(G30:H30)</f>
         <v/>
       </c>
@@ -3763,23 +3815,23 @@
       <c r="N30" s="38" t="n"/>
       <c r="P30" s="8" t="n"/>
     </row>
-    <row r="31" ht="7.5" customHeight="1" s="263" thickBot="1">
+    <row r="31" ht="7.5" customHeight="1" s="244" thickBot="1">
       <c r="B31" s="8" t="n"/>
       <c r="C31" s="38" t="n"/>
       <c r="D31" s="42" t="n"/>
       <c r="E31" s="42" t="n"/>
-      <c r="F31" s="158" t="n"/>
-      <c r="G31" s="162" t="n"/>
-      <c r="H31" s="162" t="n"/>
+      <c r="F31" s="157" t="n"/>
+      <c r="G31" s="327" t="n"/>
+      <c r="H31" s="158" t="n"/>
       <c r="I31" s="38" t="n"/>
-      <c r="J31" s="159" t="n"/>
-      <c r="K31" s="163" t="n"/>
+      <c r="J31" s="336" t="n"/>
+      <c r="K31" s="159" t="n"/>
       <c r="L31" s="134" t="n"/>
-      <c r="M31" s="162" t="n"/>
+      <c r="M31" s="158" t="n"/>
       <c r="N31" s="38" t="n"/>
       <c r="P31" s="8" t="n"/>
     </row>
-    <row r="32" ht="18" customHeight="1" s="263" thickBot="1">
+    <row r="32" ht="18" customHeight="1" s="244" thickBot="1">
       <c r="B32" s="8" t="n"/>
       <c r="C32" s="40" t="inlineStr">
         <is>
@@ -3791,13 +3843,13 @@
           <t xml:space="preserve">TOTAL FUNDS AT END OF YEAR  </t>
         </is>
       </c>
-      <c r="E32" s="164" t="n"/>
-      <c r="F32" s="165" t="inlineStr">
+      <c r="E32" s="160" t="n"/>
+      <c r="F32" s="161" t="inlineStr">
         <is>
           <t>(c3+c4)</t>
         </is>
       </c>
-      <c r="G32" s="147">
+      <c r="G32" s="321">
         <f>G28+G30</f>
         <v/>
       </c>
@@ -3806,11 +3858,11 @@
         <v/>
       </c>
       <c r="I32" s="148" t="n"/>
-      <c r="J32" s="147">
+      <c r="J32" s="321">
         <f>J28+J30</f>
         <v/>
       </c>
-      <c r="K32" s="150" t="inlineStr">
+      <c r="K32" s="149" t="inlineStr">
         <is>
           <t>(c8)</t>
         </is>
@@ -3820,14 +3872,14 @@
         <f>M28+M30</f>
         <v/>
       </c>
-      <c r="N32" s="166" t="inlineStr">
+      <c r="N32" s="162" t="inlineStr">
         <is>
           <t>(c6)</t>
         </is>
       </c>
       <c r="O32" s="20" t="n"/>
       <c r="P32" s="8" t="n"/>
-      <c r="Q32" s="215" t="inlineStr">
+      <c r="Q32" s="211" t="inlineStr">
         <is>
           <t>c6 totals</t>
         </is>
@@ -3837,23 +3889,23 @@
         <v/>
       </c>
     </row>
-    <row r="33" ht="18" customHeight="1" s="263">
+    <row r="33" ht="18" customHeight="1" s="244">
       <c r="B33" s="8" t="n"/>
       <c r="C33" s="38" t="n"/>
       <c r="D33" s="38" t="n"/>
       <c r="E33" s="38" t="n"/>
       <c r="F33" s="41" t="n"/>
-      <c r="G33" s="38" t="n"/>
+      <c r="G33" s="322" t="n"/>
       <c r="H33" s="38" t="n"/>
       <c r="I33" s="38" t="n"/>
-      <c r="J33" s="167" t="n"/>
+      <c r="J33" s="339" t="n"/>
       <c r="K33" s="46" t="n"/>
       <c r="L33" s="46" t="n"/>
-      <c r="M33" s="167" t="n"/>
+      <c r="M33" s="163" t="n"/>
       <c r="N33" s="38" t="n"/>
       <c r="P33" s="8" t="n"/>
     </row>
-    <row r="34" ht="23.25" customHeight="1" s="263" thickBot="1">
+    <row r="34" ht="23.25" customHeight="1" s="244" thickBot="1">
       <c r="B34" s="8" t="n"/>
       <c r="C34" s="38" t="n"/>
       <c r="D34" s="143" t="inlineStr">
@@ -3863,10 +3915,10 @@
       </c>
       <c r="E34" s="38" t="n"/>
       <c r="F34" s="38" t="n"/>
-      <c r="G34" s="38" t="n"/>
+      <c r="G34" s="322" t="n"/>
       <c r="H34" s="38" t="n"/>
       <c r="I34" s="38" t="n"/>
-      <c r="J34" s="134" t="n"/>
+      <c r="J34" s="335" t="n"/>
       <c r="K34" s="134" t="n"/>
       <c r="L34" s="134" t="n"/>
       <c r="M34" s="38" t="n"/>
@@ -3875,48 +3927,48 @@
     </row>
     <row r="35" ht="37.5" customFormat="1" customHeight="1" s="49">
       <c r="B35" s="53" t="n"/>
-      <c r="C35" s="282" t="inlineStr">
+      <c r="C35" s="286" t="inlineStr">
         <is>
           <t>d</t>
         </is>
       </c>
-      <c r="D35" s="284" t="inlineStr">
+      <c r="D35" s="288" t="inlineStr">
         <is>
           <t xml:space="preserve">FOR INFORMATION ONLY: MONEY RECEIVED AND PASSED ON TO  EXTERNAL ORGANISATIONS                                </t>
         </is>
       </c>
-      <c r="E35" s="285" t="n"/>
-      <c r="F35" s="285" t="n"/>
-      <c r="G35" s="285" t="n"/>
-      <c r="H35" s="285" t="n"/>
-      <c r="I35" s="285" t="n"/>
-      <c r="J35" s="285" t="n"/>
-      <c r="K35" s="285" t="n"/>
-      <c r="L35" s="285" t="n"/>
-      <c r="M35" s="286" t="n"/>
+      <c r="E35" s="289" t="n"/>
+      <c r="F35" s="289" t="n"/>
+      <c r="G35" s="289" t="n"/>
+      <c r="H35" s="289" t="n"/>
+      <c r="I35" s="289" t="n"/>
+      <c r="J35" s="289" t="n"/>
+      <c r="K35" s="289" t="n"/>
+      <c r="L35" s="289" t="n"/>
+      <c r="M35" s="290" t="n"/>
       <c r="P35" s="53" t="n"/>
     </row>
-    <row r="36" ht="13.7" customHeight="1" s="263">
+    <row r="36" ht="13.7" customHeight="1" s="244">
       <c r="B36" s="8" t="n"/>
-      <c r="C36" s="283" t="n"/>
-      <c r="D36" s="298" t="inlineStr">
+      <c r="C36" s="287" t="n"/>
+      <c r="D36" s="283" t="inlineStr">
         <is>
           <t>(these amounts are not to be included in total receipts/payments figures above)</t>
         </is>
       </c>
-      <c r="E36" s="299" t="n"/>
-      <c r="F36" s="299" t="n"/>
-      <c r="G36" s="299" t="n"/>
-      <c r="H36" s="299" t="n"/>
-      <c r="I36" s="218" t="n"/>
-      <c r="J36" s="219" t="inlineStr">
+      <c r="E36" s="284" t="n"/>
+      <c r="F36" s="284" t="n"/>
+      <c r="G36" s="284" t="n"/>
+      <c r="H36" s="284" t="n"/>
+      <c r="I36" s="214" t="n"/>
+      <c r="J36" s="340" t="inlineStr">
         <is>
           <t>£</t>
         </is>
       </c>
-      <c r="K36" s="218" t="n"/>
-      <c r="L36" s="168" t="n"/>
-      <c r="M36" s="219" t="inlineStr">
+      <c r="K36" s="214" t="n"/>
+      <c r="L36" s="164" t="n"/>
+      <c r="M36" s="215" t="inlineStr">
         <is>
           <t>£</t>
         </is>
@@ -3925,127 +3977,129 @@
       <c r="O36" s="6" t="n"/>
       <c r="P36" s="8" t="n"/>
     </row>
-    <row r="37" ht="31.7" customHeight="1" s="263">
+    <row r="37" ht="31.7" customHeight="1" s="244">
       <c r="B37" s="8" t="n"/>
       <c r="C37" s="50" t="inlineStr">
         <is>
           <t>d1</t>
         </is>
       </c>
-      <c r="D37" s="297" t="inlineStr">
+      <c r="D37" s="281" t="inlineStr">
         <is>
           <t>Balance brought forward from last year</t>
         </is>
       </c>
-      <c r="E37" s="275" t="n"/>
-      <c r="F37" s="275" t="n"/>
-      <c r="G37" s="275" t="n"/>
-      <c r="H37" s="281" t="n"/>
+      <c r="E37" s="250" t="n"/>
+      <c r="F37" s="250" t="n"/>
+      <c r="G37" s="250" t="n"/>
+      <c r="H37" s="282" t="n"/>
       <c r="I37" s="134" t="n"/>
-      <c r="J37" s="141">
+      <c r="J37" s="319">
         <f>+M40</f>
         <v/>
       </c>
       <c r="K37" s="38" t="n"/>
       <c r="L37" s="38" t="n"/>
-      <c r="M37" s="169" t="n"/>
+      <c r="M37" s="165" t="n"/>
       <c r="N37" s="148" t="n"/>
       <c r="O37" s="6" t="n"/>
       <c r="P37" s="8" t="n"/>
     </row>
-    <row r="38" ht="31.7" customHeight="1" s="263">
+    <row r="38" ht="31.7" customHeight="1" s="244">
       <c r="B38" s="8" t="n"/>
       <c r="C38" s="50" t="inlineStr">
         <is>
           <t>d2</t>
         </is>
       </c>
-      <c r="D38" s="297" t="inlineStr">
+      <c r="D38" s="281" t="inlineStr">
         <is>
           <t>Offerings/Gifts - received for external organisations</t>
         </is>
       </c>
-      <c r="E38" s="275" t="n"/>
-      <c r="F38" s="275" t="n"/>
-      <c r="G38" s="275" t="n"/>
-      <c r="H38" s="281" t="n"/>
+      <c r="E38" s="250" t="n"/>
+      <c r="F38" s="250" t="n"/>
+      <c r="G38" s="250" t="n"/>
+      <c r="H38" s="282" t="n"/>
       <c r="I38" s="51" t="n"/>
-      <c r="J38" s="141" t="n"/>
+      <c r="J38" s="319" t="n"/>
       <c r="K38" s="134" t="n"/>
       <c r="L38" s="134" t="n"/>
-      <c r="M38" s="169" t="n"/>
+      <c r="M38" s="165" t="n"/>
       <c r="N38" s="38" t="n"/>
       <c r="P38" s="8" t="n"/>
     </row>
-    <row r="39" ht="31.7" customHeight="1" s="263" thickBot="1">
+    <row r="39" ht="31.7" customHeight="1" s="244" thickBot="1">
       <c r="B39" s="8" t="n"/>
       <c r="C39" s="50" t="inlineStr">
         <is>
           <t>d3</t>
         </is>
       </c>
-      <c r="D39" s="297" t="inlineStr">
+      <c r="D39" s="281" t="inlineStr">
         <is>
           <t>Offerings/Gifts  - passed to external organisations</t>
         </is>
       </c>
-      <c r="E39" s="275" t="n"/>
-      <c r="F39" s="275" t="n"/>
-      <c r="G39" s="275" t="n"/>
-      <c r="H39" s="281" t="n"/>
+      <c r="E39" s="250" t="n"/>
+      <c r="F39" s="250" t="n"/>
+      <c r="G39" s="250" t="n"/>
+      <c r="H39" s="282" t="n"/>
       <c r="I39" s="51" t="n"/>
-      <c r="J39" s="142" t="n"/>
-      <c r="K39" s="170" t="n"/>
+      <c r="J39" s="320" t="n"/>
+      <c r="K39" s="166" t="n"/>
       <c r="L39" s="134" t="n"/>
-      <c r="M39" s="171" t="n"/>
+      <c r="M39" s="167" t="n"/>
       <c r="N39" s="38" t="n"/>
       <c r="P39" s="8" t="n"/>
     </row>
-    <row r="40" ht="33.75" customHeight="1" s="263" thickBot="1">
+    <row r="40" ht="33.75" customHeight="1" s="244" thickBot="1">
       <c r="B40" s="8" t="n"/>
       <c r="C40" s="50" t="inlineStr">
         <is>
           <t>d4</t>
         </is>
       </c>
-      <c r="D40" s="293" t="inlineStr">
+      <c r="D40" s="277" t="inlineStr">
         <is>
           <t>BALANCE STILL TO BE PAID                     (d1+d2-d3)</t>
         </is>
       </c>
-      <c r="E40" s="294" t="n"/>
-      <c r="F40" s="294" t="n"/>
-      <c r="G40" s="294" t="n"/>
-      <c r="H40" s="295" t="n"/>
+      <c r="E40" s="278" t="n"/>
+      <c r="F40" s="278" t="n"/>
+      <c r="G40" s="278" t="n"/>
+      <c r="H40" s="279" t="n"/>
       <c r="I40" s="52" t="n"/>
-      <c r="J40" s="172">
+      <c r="J40" s="341">
         <f>SUM(J37+J38-J39)</f>
         <v/>
       </c>
-      <c r="K40" s="173" t="n"/>
-      <c r="L40" s="173" t="n"/>
-      <c r="M40" s="172">
+      <c r="K40" s="169" t="n"/>
+      <c r="L40" s="169" t="n"/>
+      <c r="M40" s="168">
         <f>SUM(M37+M38-M39)</f>
         <v/>
       </c>
       <c r="N40" s="38" t="n"/>
       <c r="P40" s="8" t="n"/>
-      <c r="Q40" s="174" t="n"/>
-    </row>
-    <row r="41" ht="6.75" customFormat="1" customHeight="1" s="290">
+      <c r="Q40" s="170" t="n"/>
+    </row>
+    <row r="41" ht="6.75" customFormat="1" customHeight="1" s="294">
       <c r="B41" s="131" t="n"/>
+      <c r="G41" s="328" t="n"/>
+      <c r="J41" s="328" t="n"/>
       <c r="P41" s="131" t="n"/>
     </row>
-    <row r="42" ht="2.25" customHeight="1" s="263">
+    <row r="42" ht="2.25" customHeight="1" s="244">
       <c r="B42" s="8" t="n"/>
       <c r="C42" s="8" t="n"/>
       <c r="D42" s="8" t="n"/>
       <c r="E42" s="8" t="n"/>
       <c r="F42" s="8" t="n"/>
-      <c r="G42" s="8" t="n"/>
+      <c r="G42" s="329" t="n"/>
       <c r="H42" s="8" t="n"/>
       <c r="I42" s="8" t="n"/>
-      <c r="J42" s="8" t="n"/>
+      <c r="J42" s="329" t="n"/>
       <c r="K42" s="8" t="n"/>
       <c r="L42" s="8" t="n"/>
       <c r="M42" s="8" t="n"/>
@@ -4053,26 +4107,20 @@
       <c r="O42" s="8" t="n"/>
       <c r="P42" s="8" t="n"/>
     </row>
-    <row r="43" ht="18" customHeight="1" s="263"/>
-    <row r="44" ht="18" customHeight="1" s="263"/>
-    <row r="45" ht="18" customHeight="1" s="263"/>
-    <row r="46" ht="18" customHeight="1" s="263"/>
-    <row r="47" ht="18" customHeight="1" s="263"/>
-    <row r="48" ht="18" customHeight="1" s="263"/>
-    <row r="49" ht="18" customHeight="1" s="263"/>
-    <row r="50" ht="18" customHeight="1" s="263"/>
-    <row r="51" ht="18" customHeight="1" s="263"/>
-    <row r="52" ht="18" customHeight="1" s="263"/>
-    <row r="53" ht="6.75" customHeight="1" s="263"/>
-    <row r="54" ht="6.75" customHeight="1" s="263"/>
+    <row r="43" ht="18" customHeight="1" s="244"/>
+    <row r="44" ht="18" customHeight="1" s="244"/>
+    <row r="45" ht="18" customHeight="1" s="244"/>
+    <row r="46" ht="18" customHeight="1" s="244"/>
+    <row r="47" ht="18" customHeight="1" s="244"/>
+    <row r="48" ht="18" customHeight="1" s="244"/>
+    <row r="49" ht="18" customHeight="1" s="244"/>
+    <row r="50" ht="18" customHeight="1" s="244"/>
+    <row r="51" ht="18" customHeight="1" s="244"/>
+    <row r="52" ht="18" customHeight="1" s="244"/>
+    <row r="53" ht="6.75" customHeight="1" s="244"/>
+    <row r="54" ht="6.75" customHeight="1" s="244"/>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="D40:H40"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D37:H37"/>
-    <mergeCell ref="D38:H38"/>
-    <mergeCell ref="D39:H39"/>
-    <mergeCell ref="D36:H36"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="C35:C36"/>
     <mergeCell ref="D35:M35"/>
@@ -4083,6 +4131,12 @@
     <mergeCell ref="M3:M4"/>
     <mergeCell ref="H2:L2"/>
     <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D40:H40"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D37:H37"/>
+    <mergeCell ref="D38:H38"/>
+    <mergeCell ref="D39:H39"/>
+    <mergeCell ref="D36:H36"/>
   </mergeCells>
   <pageMargins left="0.1574803149606299" right="0.1574803149606299" top="0.2755905511811024" bottom="0.3937007874015748" header="0.1574803149606299" footer="0.2362204724409449"/>
   <pageSetup orientation="portrait" paperSize="9" scale="99"/>
@@ -4111,34 +4165,34 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
   <cols>
-    <col width="1.42578125" customWidth="1" style="263" min="1" max="1"/>
-    <col width="1.140625" customWidth="1" style="263" min="2" max="2"/>
-    <col width="3.42578125" bestFit="1" customWidth="1" style="263" min="3" max="3"/>
-    <col width="25" customWidth="1" style="263" min="4" max="4"/>
-    <col width="1.5703125" customWidth="1" style="263" min="5" max="5"/>
-    <col width="12.85546875" customWidth="1" style="263" min="6" max="6"/>
-    <col width="4" bestFit="1" customWidth="1" style="263" min="7" max="7"/>
-    <col width="0.85546875" customWidth="1" style="263" min="8" max="8"/>
-    <col width="14" customWidth="1" style="263" min="9" max="9"/>
-    <col width="5" customWidth="1" style="263" min="10" max="10"/>
-    <col width="14" customWidth="1" style="263" min="11" max="11"/>
-    <col width="1.42578125" customWidth="1" style="263" min="12" max="12"/>
-    <col width="0.85546875" customWidth="1" style="263" min="13" max="13"/>
-    <col width="15.5703125" customWidth="1" style="263" min="14" max="14"/>
-    <col width="5.5703125" bestFit="1" customWidth="1" style="263" min="15" max="15"/>
-    <col width="0.5703125" customWidth="1" style="263" min="16" max="16"/>
-    <col width="13" customWidth="1" style="263" min="17" max="17"/>
-    <col width="5" bestFit="1" customWidth="1" style="263" min="18" max="18"/>
-    <col width="0.85546875" customWidth="1" style="263" min="19" max="19"/>
-    <col width="15.5703125" customWidth="1" style="263" min="20" max="20"/>
-    <col width="5.85546875" bestFit="1" customWidth="1" style="263" min="21" max="21"/>
-    <col width="1" customWidth="1" style="263" min="22" max="22"/>
-    <col width="9.5703125" customWidth="1" style="263" min="23" max="23"/>
-    <col width="7.85546875" bestFit="1" customWidth="1" style="263" min="25" max="25"/>
-    <col width="2.5703125" customWidth="1" style="263" min="27" max="27"/>
+    <col width="1.42578125" customWidth="1" style="244" min="1" max="1"/>
+    <col width="1.140625" customWidth="1" style="244" min="2" max="2"/>
+    <col width="3.42578125" bestFit="1" customWidth="1" style="244" min="3" max="3"/>
+    <col width="25" customWidth="1" style="244" min="4" max="4"/>
+    <col width="1.5703125" customWidth="1" style="244" min="5" max="5"/>
+    <col width="12.85546875" customWidth="1" style="244" min="6" max="6"/>
+    <col width="4" bestFit="1" customWidth="1" style="244" min="7" max="7"/>
+    <col width="0.85546875" customWidth="1" style="244" min="8" max="8"/>
+    <col width="14" customWidth="1" style="244" min="9" max="9"/>
+    <col width="5" customWidth="1" style="244" min="10" max="10"/>
+    <col width="14" customWidth="1" style="244" min="11" max="11"/>
+    <col width="1.42578125" customWidth="1" style="244" min="12" max="12"/>
+    <col width="0.85546875" customWidth="1" style="244" min="13" max="13"/>
+    <col width="15.5703125" customWidth="1" style="244" min="14" max="14"/>
+    <col width="5.5703125" bestFit="1" customWidth="1" style="244" min="15" max="15"/>
+    <col width="0.5703125" customWidth="1" style="244" min="16" max="16"/>
+    <col width="13" customWidth="1" style="244" min="17" max="17"/>
+    <col width="5" bestFit="1" customWidth="1" style="244" min="18" max="18"/>
+    <col width="0.85546875" customWidth="1" style="244" min="19" max="19"/>
+    <col width="15.5703125" customWidth="1" style="244" min="20" max="20"/>
+    <col width="5.85546875" bestFit="1" customWidth="1" style="244" min="21" max="21"/>
+    <col width="1" customWidth="1" style="244" min="22" max="22"/>
+    <col width="9.5703125" customWidth="1" style="244" min="23" max="23"/>
+    <col width="7.85546875" bestFit="1" customWidth="1" style="244" min="25" max="25"/>
+    <col width="2.5703125" customWidth="1" style="244" min="27" max="27"/>
   </cols>
   <sheetData>
-    <row r="1" ht="8.449999999999999" customHeight="1" s="263">
+    <row r="1" ht="8.449999999999999" customHeight="1" s="244">
       <c r="B1" s="10" t="n"/>
       <c r="C1" s="10" t="n"/>
       <c r="D1" s="53" t="n"/>
@@ -4173,7 +4227,7 @@
       <c r="U1" s="53" t="n"/>
       <c r="V1" s="53" t="n"/>
     </row>
-    <row r="2" ht="27" customHeight="1" s="263">
+    <row r="2" ht="27" customHeight="1" s="244">
       <c r="B2" s="10" t="n"/>
       <c r="C2" s="2" t="n"/>
       <c r="D2" s="49" t="n"/>
@@ -4186,16 +4240,16 @@
       <c r="K2" s="56" t="n"/>
       <c r="L2" s="56" t="n"/>
       <c r="M2" s="56" t="n"/>
-      <c r="N2" s="307">
+      <c r="N2" s="297">
         <f>'P1 Front page'!$C$11</f>
         <v/>
       </c>
-      <c r="O2" s="265" t="n"/>
-      <c r="P2" s="265" t="n"/>
-      <c r="Q2" s="265" t="n"/>
-      <c r="R2" s="265" t="n"/>
-      <c r="S2" s="265" t="n"/>
-      <c r="T2" s="237" t="inlineStr">
+      <c r="O2" s="266" t="n"/>
+      <c r="P2" s="266" t="n"/>
+      <c r="Q2" s="266" t="n"/>
+      <c r="R2" s="266" t="n"/>
+      <c r="S2" s="266" t="n"/>
+      <c r="T2" s="233" t="inlineStr">
         <is>
           <t>Church</t>
         </is>
@@ -4208,30 +4262,30 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="25.5" customHeight="1" s="263">
+    <row r="3" ht="25.5" customHeight="1" s="244">
       <c r="B3" s="10" t="n"/>
       <c r="C3" s="2" t="n"/>
-      <c r="D3" s="304" t="inlineStr">
+      <c r="D3" s="305" t="inlineStr">
         <is>
           <t>SUMMARY OF CHURCH ACCOUNTS AND INTERNAL ORGANISATIONS REPORTING TO THE CHURCH COUNCIL</t>
         </is>
       </c>
       <c r="U3" s="57" t="n"/>
-      <c r="V3" s="238" t="n"/>
+      <c r="V3" s="234" t="n"/>
       <c r="W3" s="28" t="n"/>
       <c r="X3" s="1" t="n"/>
       <c r="Y3" s="1" t="n"/>
       <c r="Z3" s="1" t="n"/>
     </row>
-    <row r="4" ht="23.25" customHeight="1" s="263" thickBot="1">
+    <row r="4" ht="23.25" customHeight="1" s="244" thickBot="1">
       <c r="B4" s="10" t="n"/>
       <c r="C4" s="2" t="n"/>
-      <c r="D4" s="177" t="inlineStr">
+      <c r="D4" s="173" t="inlineStr">
         <is>
           <t>SECTION E</t>
         </is>
       </c>
-      <c r="E4" s="178" t="inlineStr">
+      <c r="E4" s="174" t="inlineStr">
         <is>
           <t>Please follow the Guidance Notes to complete this page</t>
         </is>
@@ -4254,67 +4308,67 @@
       <c r="U4" s="49" t="n"/>
       <c r="V4" s="53" t="n"/>
     </row>
-    <row r="5" ht="63.75" customHeight="1" s="263">
+    <row r="5" ht="63.75" customHeight="1" s="244">
       <c r="B5" s="10" t="n"/>
       <c r="C5" s="2" t="n"/>
-      <c r="D5" s="309" t="inlineStr">
+      <c r="D5" s="299" t="inlineStr">
         <is>
           <t xml:space="preserve">Summary of the Church accounts for the year ended 31 August 2024 and Internal Organisations reporting to the Church Council/Church Meeting. Note that the funds of an Internal Organisation would normally be Restricted funds unless it could be clearly shown that they could be used for any Methodist purpose.   This section must be completed to arrive at the gross income and expenditure totals of the Church. If gross income exceeds the Accruals threshold, then the Accruals method of accounting AND A DIFFERENT FORM must be used to report the accounts (see Methodist website).  Please refer to the guidance notes regarding transfers between the District and connected  District Organisations. </t>
         </is>
       </c>
-      <c r="E5" s="310" t="n"/>
-      <c r="F5" s="310" t="n"/>
-      <c r="G5" s="310" t="n"/>
-      <c r="H5" s="310" t="n"/>
-      <c r="I5" s="310" t="n"/>
-      <c r="J5" s="310" t="n"/>
-      <c r="K5" s="310" t="n"/>
-      <c r="L5" s="310" t="n"/>
-      <c r="M5" s="310" t="n"/>
-      <c r="N5" s="310" t="n"/>
-      <c r="O5" s="310" t="n"/>
-      <c r="P5" s="310" t="n"/>
-      <c r="Q5" s="310" t="n"/>
-      <c r="R5" s="310" t="n"/>
-      <c r="S5" s="310" t="n"/>
-      <c r="T5" s="311" t="n"/>
-      <c r="U5" s="315" t="n"/>
+      <c r="E5" s="300" t="n"/>
+      <c r="F5" s="300" t="n"/>
+      <c r="G5" s="300" t="n"/>
+      <c r="H5" s="300" t="n"/>
+      <c r="I5" s="300" t="n"/>
+      <c r="J5" s="300" t="n"/>
+      <c r="K5" s="300" t="n"/>
+      <c r="L5" s="300" t="n"/>
+      <c r="M5" s="300" t="n"/>
+      <c r="N5" s="300" t="n"/>
+      <c r="O5" s="300" t="n"/>
+      <c r="P5" s="300" t="n"/>
+      <c r="Q5" s="300" t="n"/>
+      <c r="R5" s="300" t="n"/>
+      <c r="S5" s="300" t="n"/>
+      <c r="T5" s="301" t="n"/>
+      <c r="U5" s="312" t="n"/>
       <c r="V5" s="53" t="n"/>
     </row>
-    <row r="6" ht="3.75" customHeight="1" s="263" thickBot="1">
+    <row r="6" ht="3.75" customHeight="1" s="244" thickBot="1">
       <c r="B6" s="10" t="n"/>
       <c r="C6" s="2" t="n"/>
-      <c r="D6" s="305" t="n"/>
-      <c r="E6" s="294" t="n"/>
-      <c r="F6" s="294" t="n"/>
-      <c r="G6" s="294" t="n"/>
-      <c r="H6" s="294" t="n"/>
-      <c r="I6" s="294" t="n"/>
-      <c r="J6" s="294" t="n"/>
-      <c r="K6" s="294" t="n"/>
-      <c r="L6" s="294" t="n"/>
-      <c r="M6" s="294" t="n"/>
-      <c r="N6" s="294" t="n"/>
-      <c r="O6" s="294" t="n"/>
-      <c r="P6" s="294" t="n"/>
-      <c r="Q6" s="294" t="n"/>
-      <c r="R6" s="294" t="n"/>
-      <c r="S6" s="294" t="n"/>
-      <c r="T6" s="295" t="n"/>
-      <c r="U6" s="315" t="n"/>
+      <c r="D6" s="307" t="n"/>
+      <c r="E6" s="278" t="n"/>
+      <c r="F6" s="278" t="n"/>
+      <c r="G6" s="278" t="n"/>
+      <c r="H6" s="278" t="n"/>
+      <c r="I6" s="278" t="n"/>
+      <c r="J6" s="278" t="n"/>
+      <c r="K6" s="278" t="n"/>
+      <c r="L6" s="278" t="n"/>
+      <c r="M6" s="278" t="n"/>
+      <c r="N6" s="278" t="n"/>
+      <c r="O6" s="278" t="n"/>
+      <c r="P6" s="278" t="n"/>
+      <c r="Q6" s="278" t="n"/>
+      <c r="R6" s="278" t="n"/>
+      <c r="S6" s="278" t="n"/>
+      <c r="T6" s="279" t="n"/>
+      <c r="U6" s="312" t="n"/>
       <c r="V6" s="53" t="n"/>
     </row>
-    <row r="7" ht="6" customHeight="1" s="263">
+    <row r="7" ht="6" customHeight="1" s="244">
       <c r="B7" s="10" t="n"/>
       <c r="C7" s="2" t="n"/>
-      <c r="D7" s="308" t="n"/>
-      <c r="U7" s="315" t="n"/>
+      <c r="D7" s="298" t="n"/>
+      <c r="U7" s="312" t="n"/>
       <c r="V7" s="53" t="n"/>
     </row>
-    <row r="8" ht="35.45" customHeight="1" s="263">
+    <row r="8" ht="35.45" customHeight="1" s="244">
       <c r="B8" s="10" t="n"/>
       <c r="C8" s="2" t="n"/>
-      <c r="D8" s="179" t="inlineStr">
+      <c r="D8" s="175" t="inlineStr">
         <is>
           <t>INTERNAL ORGANISATIONS</t>
         </is>
@@ -4325,35 +4379,35 @@
           <t>Receipts</t>
         </is>
       </c>
-      <c r="G8" s="180" t="n"/>
-      <c r="H8" s="180" t="n"/>
+      <c r="G8" s="176" t="n"/>
+      <c r="H8" s="176" t="n"/>
       <c r="I8" s="59" t="inlineStr">
         <is>
           <t>Payments</t>
         </is>
       </c>
-      <c r="J8" s="180" t="n"/>
+      <c r="J8" s="176" t="n"/>
       <c r="K8" s="59" t="inlineStr">
         <is>
           <t>Net Receipts/ Payments</t>
         </is>
       </c>
-      <c r="L8" s="180" t="n"/>
-      <c r="M8" s="180" t="n"/>
+      <c r="L8" s="176" t="n"/>
+      <c r="M8" s="176" t="n"/>
       <c r="N8" s="59" t="inlineStr">
         <is>
           <t xml:space="preserve"> Adjustments</t>
         </is>
       </c>
-      <c r="O8" s="180" t="n"/>
-      <c r="P8" s="181" t="n"/>
+      <c r="O8" s="176" t="n"/>
+      <c r="P8" s="177" t="n"/>
       <c r="Q8" s="59" t="inlineStr">
         <is>
           <t>Opening balances</t>
         </is>
       </c>
-      <c r="R8" s="182" t="n"/>
-      <c r="S8" s="181" t="n"/>
+      <c r="R8" s="178" t="n"/>
+      <c r="S8" s="177" t="n"/>
       <c r="T8" s="59" t="inlineStr">
         <is>
           <t>Closing balances</t>
@@ -4362,205 +4416,205 @@
       <c r="U8" s="60" t="n"/>
       <c r="V8" s="53" t="n"/>
     </row>
-    <row r="9" ht="24.75" customHeight="1" s="263">
+    <row r="9" ht="24.75" customHeight="1" s="244">
       <c r="B9" s="10" t="n"/>
       <c r="C9" s="16" t="inlineStr">
         <is>
           <t>e1</t>
         </is>
       </c>
-      <c r="D9" s="183" t="n"/>
+      <c r="D9" s="179" t="n"/>
       <c r="E9" s="49" t="n"/>
-      <c r="F9" s="184" t="n"/>
-      <c r="G9" s="185" t="n"/>
+      <c r="F9" s="180" t="n"/>
+      <c r="G9" s="181" t="n"/>
       <c r="H9" s="49" t="n"/>
-      <c r="I9" s="184" t="n"/>
-      <c r="J9" s="185" t="n"/>
-      <c r="K9" s="186">
+      <c r="I9" s="180" t="n"/>
+      <c r="J9" s="181" t="n"/>
+      <c r="K9" s="182">
         <f>+F9-I9</f>
         <v/>
       </c>
-      <c r="L9" s="185" t="n"/>
-      <c r="M9" s="185" t="n"/>
-      <c r="N9" s="184" t="n"/>
-      <c r="O9" s="185" t="n"/>
-      <c r="P9" s="185" t="n"/>
-      <c r="Q9" s="184" t="n"/>
-      <c r="R9" s="185" t="n"/>
-      <c r="S9" s="185" t="n"/>
-      <c r="T9" s="186">
+      <c r="L9" s="181" t="n"/>
+      <c r="M9" s="181" t="n"/>
+      <c r="N9" s="180" t="n"/>
+      <c r="O9" s="181" t="n"/>
+      <c r="P9" s="181" t="n"/>
+      <c r="Q9" s="180" t="n"/>
+      <c r="R9" s="181" t="n"/>
+      <c r="S9" s="181" t="n"/>
+      <c r="T9" s="182">
         <f>+K9+N9+Q9</f>
         <v/>
       </c>
       <c r="U9" s="62" t="n"/>
       <c r="V9" s="53" t="n"/>
     </row>
-    <row r="10" ht="24.75" customHeight="1" s="263">
+    <row r="10" ht="24.75" customHeight="1" s="244">
       <c r="B10" s="10" t="n"/>
       <c r="C10" s="16" t="inlineStr">
         <is>
           <t>e2</t>
         </is>
       </c>
-      <c r="D10" s="183" t="n"/>
+      <c r="D10" s="179" t="n"/>
       <c r="E10" s="49" t="n"/>
-      <c r="F10" s="184" t="n"/>
-      <c r="G10" s="185" t="n"/>
+      <c r="F10" s="180" t="n"/>
+      <c r="G10" s="181" t="n"/>
       <c r="H10" s="49" t="n"/>
-      <c r="I10" s="184" t="n"/>
-      <c r="J10" s="185" t="n"/>
-      <c r="K10" s="186">
+      <c r="I10" s="180" t="n"/>
+      <c r="J10" s="181" t="n"/>
+      <c r="K10" s="182">
         <f>+F10-I10</f>
         <v/>
       </c>
-      <c r="L10" s="185" t="n"/>
-      <c r="M10" s="185" t="n"/>
-      <c r="N10" s="184" t="n"/>
-      <c r="O10" s="185" t="n"/>
-      <c r="P10" s="185" t="n"/>
-      <c r="Q10" s="184" t="n"/>
-      <c r="R10" s="185" t="n"/>
-      <c r="S10" s="185" t="n"/>
-      <c r="T10" s="186">
+      <c r="L10" s="181" t="n"/>
+      <c r="M10" s="181" t="n"/>
+      <c r="N10" s="180" t="n"/>
+      <c r="O10" s="181" t="n"/>
+      <c r="P10" s="181" t="n"/>
+      <c r="Q10" s="180" t="n"/>
+      <c r="R10" s="181" t="n"/>
+      <c r="S10" s="181" t="n"/>
+      <c r="T10" s="182">
         <f>+K10+N10+Q10</f>
         <v/>
       </c>
       <c r="U10" s="62" t="n"/>
       <c r="V10" s="53" t="n"/>
     </row>
-    <row r="11" ht="24.75" customHeight="1" s="263">
+    <row r="11" ht="24.75" customHeight="1" s="244">
       <c r="B11" s="10" t="n"/>
       <c r="C11" s="16" t="inlineStr">
         <is>
           <t>e3</t>
         </is>
       </c>
-      <c r="D11" s="187" t="n"/>
+      <c r="D11" s="183" t="n"/>
       <c r="E11" s="49" t="n"/>
-      <c r="F11" s="184" t="n"/>
-      <c r="G11" s="185" t="n"/>
-      <c r="H11" s="185" t="n"/>
-      <c r="I11" s="184" t="n"/>
-      <c r="J11" s="185" t="n"/>
-      <c r="K11" s="186">
+      <c r="F11" s="180" t="n"/>
+      <c r="G11" s="181" t="n"/>
+      <c r="H11" s="181" t="n"/>
+      <c r="I11" s="180" t="n"/>
+      <c r="J11" s="181" t="n"/>
+      <c r="K11" s="182">
         <f>+F11-I11</f>
         <v/>
       </c>
-      <c r="L11" s="185" t="n"/>
-      <c r="M11" s="185" t="n"/>
-      <c r="N11" s="184" t="n"/>
-      <c r="O11" s="185" t="n"/>
-      <c r="P11" s="185" t="n"/>
-      <c r="Q11" s="184" t="n"/>
-      <c r="R11" s="185" t="n"/>
-      <c r="S11" s="185" t="n"/>
-      <c r="T11" s="186">
+      <c r="L11" s="181" t="n"/>
+      <c r="M11" s="181" t="n"/>
+      <c r="N11" s="180" t="n"/>
+      <c r="O11" s="181" t="n"/>
+      <c r="P11" s="181" t="n"/>
+      <c r="Q11" s="180" t="n"/>
+      <c r="R11" s="181" t="n"/>
+      <c r="S11" s="181" t="n"/>
+      <c r="T11" s="182">
         <f>+K11+N11+Q11</f>
         <v/>
       </c>
       <c r="U11" s="62" t="n"/>
       <c r="V11" s="53" t="n"/>
     </row>
-    <row r="12" ht="24.75" customHeight="1" s="263">
+    <row r="12" ht="24.75" customHeight="1" s="244">
       <c r="B12" s="10" t="n"/>
       <c r="C12" s="16" t="inlineStr">
         <is>
           <t>e4</t>
         </is>
       </c>
-      <c r="D12" s="187" t="n"/>
+      <c r="D12" s="183" t="n"/>
       <c r="E12" s="49" t="n"/>
-      <c r="F12" s="184" t="n"/>
-      <c r="G12" s="185" t="n"/>
-      <c r="H12" s="185" t="n"/>
-      <c r="I12" s="184" t="n"/>
-      <c r="J12" s="185" t="n"/>
-      <c r="K12" s="186">
+      <c r="F12" s="180" t="n"/>
+      <c r="G12" s="181" t="n"/>
+      <c r="H12" s="181" t="n"/>
+      <c r="I12" s="180" t="n"/>
+      <c r="J12" s="181" t="n"/>
+      <c r="K12" s="182">
         <f>+F12-I12</f>
         <v/>
       </c>
-      <c r="L12" s="185" t="n"/>
-      <c r="M12" s="185" t="n"/>
-      <c r="N12" s="184" t="n"/>
-      <c r="O12" s="185" t="n"/>
-      <c r="P12" s="185" t="n"/>
-      <c r="Q12" s="184" t="n"/>
-      <c r="R12" s="185" t="n"/>
-      <c r="S12" s="185" t="n"/>
-      <c r="T12" s="186">
+      <c r="L12" s="181" t="n"/>
+      <c r="M12" s="181" t="n"/>
+      <c r="N12" s="180" t="n"/>
+      <c r="O12" s="181" t="n"/>
+      <c r="P12" s="181" t="n"/>
+      <c r="Q12" s="180" t="n"/>
+      <c r="R12" s="181" t="n"/>
+      <c r="S12" s="181" t="n"/>
+      <c r="T12" s="182">
         <f>+K12+N12+Q12</f>
         <v/>
       </c>
       <c r="U12" s="62" t="n"/>
       <c r="V12" s="53" t="n"/>
     </row>
-    <row r="13" ht="24.75" customHeight="1" s="263">
+    <row r="13" ht="24.75" customHeight="1" s="244">
       <c r="B13" s="10" t="n"/>
       <c r="C13" s="16" t="inlineStr">
         <is>
           <t>e5</t>
         </is>
       </c>
-      <c r="D13" s="187" t="n"/>
+      <c r="D13" s="183" t="n"/>
       <c r="E13" s="49" t="n"/>
-      <c r="F13" s="184" t="n"/>
-      <c r="G13" s="185" t="n"/>
-      <c r="H13" s="185" t="n"/>
-      <c r="I13" s="184" t="n"/>
-      <c r="J13" s="185" t="n"/>
-      <c r="K13" s="186">
+      <c r="F13" s="180" t="n"/>
+      <c r="G13" s="181" t="n"/>
+      <c r="H13" s="181" t="n"/>
+      <c r="I13" s="180" t="n"/>
+      <c r="J13" s="181" t="n"/>
+      <c r="K13" s="182">
         <f>+F13-I13</f>
         <v/>
       </c>
-      <c r="L13" s="185" t="n"/>
-      <c r="M13" s="185" t="n"/>
-      <c r="N13" s="184" t="n"/>
-      <c r="O13" s="185" t="n"/>
-      <c r="P13" s="185" t="n"/>
-      <c r="Q13" s="184" t="n"/>
-      <c r="R13" s="185" t="n"/>
-      <c r="S13" s="185" t="n"/>
-      <c r="T13" s="186">
+      <c r="L13" s="181" t="n"/>
+      <c r="M13" s="181" t="n"/>
+      <c r="N13" s="180" t="n"/>
+      <c r="O13" s="181" t="n"/>
+      <c r="P13" s="181" t="n"/>
+      <c r="Q13" s="180" t="n"/>
+      <c r="R13" s="181" t="n"/>
+      <c r="S13" s="181" t="n"/>
+      <c r="T13" s="182">
         <f>+K13+N13+Q13</f>
         <v/>
       </c>
       <c r="U13" s="62" t="n"/>
       <c r="V13" s="53" t="n"/>
     </row>
-    <row r="14" ht="24.75" customHeight="1" s="263">
+    <row r="14" ht="24.75" customHeight="1" s="244">
       <c r="B14" s="10" t="n"/>
       <c r="C14" s="16" t="inlineStr">
         <is>
           <t>e6</t>
         </is>
       </c>
-      <c r="D14" s="187" t="n"/>
+      <c r="D14" s="183" t="n"/>
       <c r="E14" s="49" t="n"/>
-      <c r="F14" s="184" t="n"/>
-      <c r="G14" s="185" t="n"/>
-      <c r="H14" s="185" t="n"/>
-      <c r="I14" s="184" t="n"/>
-      <c r="J14" s="185" t="n"/>
-      <c r="K14" s="186">
+      <c r="F14" s="180" t="n"/>
+      <c r="G14" s="181" t="n"/>
+      <c r="H14" s="181" t="n"/>
+      <c r="I14" s="180" t="n"/>
+      <c r="J14" s="181" t="n"/>
+      <c r="K14" s="182">
         <f>+F14-I14</f>
         <v/>
       </c>
-      <c r="L14" s="185" t="n"/>
-      <c r="M14" s="185" t="n"/>
-      <c r="N14" s="184" t="n"/>
-      <c r="O14" s="185" t="n"/>
-      <c r="P14" s="185" t="n"/>
-      <c r="Q14" s="184" t="n"/>
-      <c r="R14" s="185" t="n"/>
-      <c r="S14" s="185" t="n"/>
-      <c r="T14" s="186">
+      <c r="L14" s="181" t="n"/>
+      <c r="M14" s="181" t="n"/>
+      <c r="N14" s="180" t="n"/>
+      <c r="O14" s="181" t="n"/>
+      <c r="P14" s="181" t="n"/>
+      <c r="Q14" s="180" t="n"/>
+      <c r="R14" s="181" t="n"/>
+      <c r="S14" s="181" t="n"/>
+      <c r="T14" s="182">
         <f>+K14+N14+Q14</f>
         <v/>
       </c>
       <c r="U14" s="62" t="n"/>
       <c r="V14" s="53" t="n"/>
     </row>
-    <row r="15" ht="24.75" customHeight="1" s="263" thickBot="1">
+    <row r="15" ht="24.75" customHeight="1" s="244" thickBot="1">
       <c r="B15" s="10" t="n"/>
       <c r="C15" s="16" t="inlineStr">
         <is>
@@ -4593,37 +4647,37 @@
       <c r="U15" s="62" t="n"/>
       <c r="V15" s="53" t="n"/>
     </row>
-    <row r="16" ht="25.5" customHeight="1" s="263">
+    <row r="16" ht="25.5" customHeight="1" s="244">
       <c r="B16" s="10" t="n"/>
       <c r="C16" s="16" t="inlineStr">
         <is>
           <t>e8</t>
         </is>
       </c>
-      <c r="D16" s="188" t="inlineStr">
+      <c r="D16" s="184" t="inlineStr">
         <is>
           <t>Sub total of Internal Organisations funds</t>
         </is>
       </c>
       <c r="E16" s="49" t="n"/>
-      <c r="F16" s="189">
+      <c r="F16" s="185">
         <f>SUM(F9:F15)</f>
         <v/>
       </c>
-      <c r="G16" s="190" t="n"/>
-      <c r="H16" s="185" t="n"/>
-      <c r="I16" s="189">
+      <c r="G16" s="186" t="n"/>
+      <c r="H16" s="181" t="n"/>
+      <c r="I16" s="185">
         <f>SUM(I9:I15)</f>
         <v/>
       </c>
-      <c r="J16" s="190" t="n"/>
-      <c r="K16" s="189">
+      <c r="J16" s="186" t="n"/>
+      <c r="K16" s="185">
         <f>SUM(K9:K15)</f>
         <v/>
       </c>
       <c r="L16" s="62" t="n"/>
       <c r="M16" s="62" t="n"/>
-      <c r="N16" s="189">
+      <c r="N16" s="185">
         <f>SUM(N9:N15)</f>
         <v/>
       </c>
@@ -4633,7 +4687,7 @@
         <f>SUM(Q9:Q15)</f>
         <v/>
       </c>
-      <c r="R16" s="239" t="inlineStr">
+      <c r="R16" s="235" t="inlineStr">
         <is>
           <t>(e11)</t>
         </is>
@@ -4643,7 +4697,7 @@
         <f>SUM(T9:T15)</f>
         <v/>
       </c>
-      <c r="U16" s="239" t="inlineStr">
+      <c r="U16" s="235" t="inlineStr">
         <is>
           <t>(e12)</t>
         </is>
@@ -4659,46 +4713,46 @@
         <v/>
       </c>
     </row>
-    <row r="17" ht="55.5" customHeight="1" s="263" thickBot="1">
+    <row r="17" ht="55.5" customHeight="1" s="244" thickBot="1">
       <c r="B17" s="10" t="n"/>
       <c r="C17" s="16" t="inlineStr">
         <is>
           <t>e9</t>
         </is>
       </c>
-      <c r="D17" s="179" t="inlineStr">
+      <c r="D17" s="175" t="inlineStr">
         <is>
           <t>Church accounts (totals brought forward from page 2 - totals column)</t>
         </is>
       </c>
       <c r="E17" s="49" t="n"/>
-      <c r="F17" s="191">
+      <c r="F17" s="187">
         <f>+'P2 R &amp; P page'!J11</f>
         <v/>
       </c>
-      <c r="G17" s="192" t="inlineStr">
+      <c r="G17" s="188" t="inlineStr">
         <is>
           <t>(a7)</t>
         </is>
       </c>
       <c r="H17" s="49" t="n"/>
-      <c r="I17" s="191">
+      <c r="I17" s="187">
         <f>+'P2 R &amp; P page'!J21</f>
         <v/>
       </c>
-      <c r="J17" s="191" t="inlineStr">
+      <c r="J17" s="187" t="inlineStr">
         <is>
           <t>(b9)</t>
         </is>
       </c>
-      <c r="K17" s="191">
+      <c r="K17" s="187">
         <f>+F17-I17</f>
         <v/>
       </c>
-      <c r="L17" s="240" t="n"/>
+      <c r="L17" s="236" t="n"/>
       <c r="M17" s="62" t="n"/>
       <c r="N17" s="68" t="n"/>
-      <c r="O17" s="216" t="inlineStr">
+      <c r="O17" s="343" t="inlineStr">
         <is>
           <t>(c7)</t>
         </is>
@@ -4708,7 +4762,7 @@
         <f>+'P2 R &amp; P page'!J26</f>
         <v/>
       </c>
-      <c r="R17" s="217" t="inlineStr">
+      <c r="R17" s="213" t="inlineStr">
         <is>
           <t>(c6)</t>
         </is>
@@ -4718,7 +4772,7 @@
         <f>+K17+N17+Q17</f>
         <v/>
       </c>
-      <c r="U17" s="217" t="inlineStr">
+      <c r="U17" s="213" t="inlineStr">
         <is>
           <t>(c8)</t>
         </is>
@@ -4734,31 +4788,31 @@
         <v/>
       </c>
     </row>
-    <row r="18" ht="27.75" customHeight="1" s="263" thickBot="1" thickTop="1">
+    <row r="18" ht="27.75" customHeight="1" s="244" thickBot="1" thickTop="1">
       <c r="B18" s="10" t="n"/>
       <c r="C18" s="16" t="inlineStr">
         <is>
           <t>e10</t>
         </is>
       </c>
-      <c r="D18" s="306" t="inlineStr">
+      <c r="D18" s="308" t="inlineStr">
         <is>
           <t>TOTAL CASH FUNDS HELD BY CHURCH</t>
         </is>
       </c>
       <c r="E18" s="49" t="n"/>
-      <c r="F18" s="194">
+      <c r="F18" s="190">
         <f>SUM(F16:F17)</f>
         <v/>
       </c>
       <c r="G18" s="70" t="n"/>
-      <c r="H18" s="185" t="n"/>
-      <c r="I18" s="195">
+      <c r="H18" s="181" t="n"/>
+      <c r="I18" s="191">
         <f>SUM(I16:I17)</f>
         <v/>
       </c>
-      <c r="J18" s="196" t="n"/>
-      <c r="K18" s="195">
+      <c r="J18" s="192" t="n"/>
+      <c r="K18" s="191">
         <f>+F18-I18</f>
         <v/>
       </c>
@@ -4774,7 +4828,7 @@
         <f>SUM(Q16:Q17)</f>
         <v/>
       </c>
-      <c r="R18" s="241" t="inlineStr">
+      <c r="R18" s="237" t="inlineStr">
         <is>
           <t>(x)</t>
         </is>
@@ -4801,17 +4855,17 @@
       </c>
       <c r="Z18" s="25" t="n"/>
     </row>
-    <row r="19" ht="3.75" customHeight="1" s="263" thickBot="1" thickTop="1">
+    <row r="19" ht="3.75" customHeight="1" s="244" thickBot="1" thickTop="1">
       <c r="B19" s="10" t="n"/>
       <c r="C19" s="2" t="n"/>
       <c r="D19" s="49" t="n"/>
       <c r="E19" s="49" t="n"/>
-      <c r="F19" s="185" t="n"/>
-      <c r="G19" s="185" t="n"/>
-      <c r="H19" s="185" t="n"/>
-      <c r="I19" s="185" t="n"/>
-      <c r="J19" s="185" t="n"/>
-      <c r="K19" s="185" t="n"/>
+      <c r="F19" s="181" t="n"/>
+      <c r="G19" s="181" t="n"/>
+      <c r="H19" s="181" t="n"/>
+      <c r="I19" s="181" t="n"/>
+      <c r="J19" s="181" t="n"/>
+      <c r="K19" s="181" t="n"/>
       <c r="L19" s="62" t="n"/>
       <c r="M19" s="62" t="n"/>
       <c r="N19" s="62" t="n"/>
@@ -4824,52 +4878,52 @@
       <c r="U19" s="62" t="n"/>
       <c r="V19" s="53" t="n"/>
     </row>
-    <row r="20" ht="39.2" customHeight="1" s="263" thickBot="1">
+    <row r="20" ht="39.2" customHeight="1" s="244" thickBot="1">
       <c r="B20" s="10" t="n"/>
       <c r="C20" s="2" t="n"/>
-      <c r="D20" s="197" t="inlineStr">
+      <c r="D20" s="193" t="inlineStr">
         <is>
           <t>Continue on a separate sheet if necessary and bring the totals forward</t>
         </is>
       </c>
       <c r="E20" s="49" t="n"/>
-      <c r="F20" s="312" t="inlineStr">
+      <c r="F20" s="302" t="inlineStr">
         <is>
           <t>TOTAL RECEIPTS</t>
         </is>
       </c>
-      <c r="G20" s="313" t="n"/>
-      <c r="H20" s="185" t="n"/>
-      <c r="I20" s="211" t="inlineStr">
+      <c r="G20" s="303" t="n"/>
+      <c r="H20" s="181" t="n"/>
+      <c r="I20" s="207" t="inlineStr">
         <is>
           <t>TOTAL PAYMENTS</t>
         </is>
       </c>
-      <c r="J20" s="209" t="n"/>
-      <c r="K20" s="209" t="n"/>
-      <c r="L20" s="210" t="n"/>
+      <c r="J20" s="205" t="n"/>
+      <c r="K20" s="205" t="n"/>
+      <c r="L20" s="206" t="n"/>
       <c r="M20" s="49" t="n"/>
       <c r="N20" s="49" t="n"/>
       <c r="O20" s="62" t="n"/>
       <c r="P20" s="62" t="n"/>
-      <c r="Q20" s="319" t="n"/>
-      <c r="R20" s="319" t="n"/>
-      <c r="S20" s="319" t="n"/>
-      <c r="T20" s="320" t="n"/>
-      <c r="U20" s="319" t="n"/>
-      <c r="V20" s="321" t="n"/>
-    </row>
-    <row r="21" ht="5.25" customHeight="1" s="263">
+      <c r="Q20" s="345" t="n"/>
+      <c r="R20" s="345" t="n"/>
+      <c r="S20" s="345" t="n"/>
+      <c r="T20" s="346" t="n"/>
+      <c r="U20" s="345" t="n"/>
+      <c r="V20" s="347" t="n"/>
+    </row>
+    <row r="21" ht="5.25" customHeight="1" s="244">
       <c r="B21" s="10" t="n"/>
       <c r="C21" s="2" t="n"/>
       <c r="D21" s="49" t="n"/>
       <c r="E21" s="49" t="n"/>
-      <c r="F21" s="185" t="n"/>
-      <c r="G21" s="185" t="n"/>
-      <c r="H21" s="185" t="n"/>
-      <c r="I21" s="198" t="n"/>
-      <c r="J21" s="198" t="n"/>
-      <c r="K21" s="198" t="n"/>
+      <c r="F21" s="181" t="n"/>
+      <c r="G21" s="181" t="n"/>
+      <c r="H21" s="181" t="n"/>
+      <c r="I21" s="194" t="n"/>
+      <c r="J21" s="194" t="n"/>
+      <c r="K21" s="194" t="n"/>
       <c r="L21" s="79" t="n"/>
       <c r="M21" s="62" t="n"/>
       <c r="N21" s="62" t="n"/>
@@ -4882,20 +4936,20 @@
       <c r="U21" s="62" t="n"/>
       <c r="V21" s="53" t="n"/>
     </row>
-    <row r="22" ht="3.2" customHeight="1" s="263" thickBot="1">
+    <row r="22" ht="3.2" customHeight="1" s="244" thickBot="1">
       <c r="B22" s="10" t="n"/>
       <c r="C22" s="15" t="n"/>
-      <c r="D22" s="322" t="n"/>
-      <c r="E22" s="322" t="n"/>
-      <c r="F22" s="322" t="n"/>
-      <c r="G22" s="322" t="n"/>
-      <c r="H22" s="322" t="n"/>
-      <c r="I22" s="322" t="n"/>
-      <c r="J22" s="322" t="n"/>
-      <c r="K22" s="322" t="n"/>
-      <c r="L22" s="322" t="n"/>
-      <c r="M22" s="323" t="n"/>
-      <c r="N22" s="323" t="n"/>
+      <c r="D22" s="348" t="n"/>
+      <c r="E22" s="348" t="n"/>
+      <c r="F22" s="348" t="n"/>
+      <c r="G22" s="348" t="n"/>
+      <c r="H22" s="348" t="n"/>
+      <c r="I22" s="348" t="n"/>
+      <c r="J22" s="348" t="n"/>
+      <c r="K22" s="348" t="n"/>
+      <c r="L22" s="348" t="n"/>
+      <c r="M22" s="349" t="n"/>
+      <c r="N22" s="349" t="n"/>
       <c r="O22" s="82" t="n"/>
       <c r="P22" s="82" t="n"/>
       <c r="Q22" s="82" t="n"/>
@@ -4905,20 +4959,20 @@
       <c r="U22" s="82" t="n"/>
       <c r="V22" s="53" t="n"/>
     </row>
-    <row r="23" ht="4.7" customHeight="1" s="263" thickTop="1">
+    <row r="23" ht="4.7" customHeight="1" s="244" thickTop="1">
       <c r="B23" s="10" t="n"/>
       <c r="C23" s="2" t="n"/>
-      <c r="D23" s="324" t="n"/>
-      <c r="E23" s="324" t="n"/>
-      <c r="F23" s="324" t="n"/>
-      <c r="G23" s="324" t="n"/>
-      <c r="H23" s="324" t="n"/>
-      <c r="I23" s="324" t="n"/>
-      <c r="J23" s="324" t="n"/>
-      <c r="K23" s="324" t="n"/>
-      <c r="L23" s="324" t="n"/>
-      <c r="M23" s="325" t="n"/>
-      <c r="N23" s="325" t="n"/>
+      <c r="D23" s="350" t="n"/>
+      <c r="E23" s="350" t="n"/>
+      <c r="F23" s="350" t="n"/>
+      <c r="G23" s="350" t="n"/>
+      <c r="H23" s="350" t="n"/>
+      <c r="I23" s="350" t="n"/>
+      <c r="J23" s="350" t="n"/>
+      <c r="K23" s="350" t="n"/>
+      <c r="L23" s="350" t="n"/>
+      <c r="M23" s="351" t="n"/>
+      <c r="N23" s="351" t="n"/>
       <c r="O23" s="62" t="n"/>
       <c r="P23" s="62" t="n"/>
       <c r="Q23" s="62" t="n"/>
@@ -4928,37 +4982,37 @@
       <c r="U23" s="62" t="n"/>
       <c r="V23" s="53" t="n"/>
     </row>
-    <row r="24" ht="23.25" customHeight="1" s="263" thickBot="1">
+    <row r="24" ht="23.25" customHeight="1" s="244" thickBot="1">
       <c r="B24" s="10" t="n"/>
       <c r="C24" s="2" t="n"/>
-      <c r="D24" s="177" t="inlineStr">
+      <c r="D24" s="173" t="inlineStr">
         <is>
           <t>SECTION F</t>
         </is>
       </c>
-      <c r="E24" s="324" t="n"/>
-      <c r="F24" s="324" t="n"/>
-      <c r="G24" s="324" t="n"/>
-      <c r="H24" s="324" t="n"/>
-      <c r="I24" s="324" t="n"/>
-      <c r="J24" s="324" t="n"/>
-      <c r="K24" s="324" t="n"/>
-      <c r="L24" s="324" t="n"/>
-      <c r="M24" s="324" t="n"/>
-      <c r="N24" s="324" t="n"/>
-      <c r="O24" s="185" t="n"/>
-      <c r="P24" s="185" t="n"/>
-      <c r="Q24" s="185" t="n"/>
-      <c r="R24" s="185" t="n"/>
-      <c r="S24" s="185" t="n"/>
-      <c r="T24" s="185" t="n"/>
+      <c r="E24" s="350" t="n"/>
+      <c r="F24" s="350" t="n"/>
+      <c r="G24" s="350" t="n"/>
+      <c r="H24" s="350" t="n"/>
+      <c r="I24" s="350" t="n"/>
+      <c r="J24" s="350" t="n"/>
+      <c r="K24" s="350" t="n"/>
+      <c r="L24" s="350" t="n"/>
+      <c r="M24" s="350" t="n"/>
+      <c r="N24" s="350" t="n"/>
+      <c r="O24" s="181" t="n"/>
+      <c r="P24" s="181" t="n"/>
+      <c r="Q24" s="181" t="n"/>
+      <c r="R24" s="181" t="n"/>
+      <c r="S24" s="181" t="n"/>
+      <c r="T24" s="181" t="n"/>
       <c r="U24" s="62" t="n"/>
       <c r="V24" s="53" t="n"/>
     </row>
-    <row r="25" ht="21.2" customHeight="1" s="263">
+    <row r="25" ht="21.2" customHeight="1" s="244">
       <c r="B25" s="10" t="n"/>
       <c r="C25" s="2" t="n"/>
-      <c r="D25" s="199" t="inlineStr">
+      <c r="D25" s="195" t="inlineStr">
         <is>
           <t>STATEMENT OF ASSETS AND LIABILITIES</t>
         </is>
@@ -4972,19 +5026,19 @@
       <c r="K25" s="49" t="n"/>
       <c r="L25" s="49" t="n"/>
       <c r="M25" s="49" t="n"/>
-      <c r="N25" s="200" t="n"/>
+      <c r="N25" s="196" t="n"/>
       <c r="O25" s="49" t="n"/>
       <c r="P25" s="49" t="n"/>
-      <c r="Q25" s="200" t="n"/>
+      <c r="Q25" s="196" t="n"/>
       <c r="R25" s="49" t="n"/>
       <c r="S25" s="49" t="n"/>
-      <c r="T25" s="200" t="n"/>
+      <c r="T25" s="196" t="n"/>
       <c r="U25" s="85" t="n"/>
       <c r="V25" s="53" t="n"/>
     </row>
-    <row r="26" ht="30.75" customHeight="1" s="263">
+    <row r="26" ht="30.75" customHeight="1" s="244">
       <c r="B26" s="10" t="n"/>
-      <c r="C26" s="288" t="n"/>
+      <c r="C26" s="292" t="n"/>
       <c r="D26" s="12" t="inlineStr">
         <is>
           <t>CHURCH - CASH FUNDS HELD at 31 August 2024</t>
@@ -5017,146 +5071,146 @@
       <c r="U26" s="39" t="n"/>
       <c r="V26" s="53" t="n"/>
     </row>
-    <row r="27" ht="24.75" customHeight="1" s="263">
+    <row r="27" ht="24.75" customHeight="1" s="244">
       <c r="B27" s="10" t="n"/>
       <c r="C27" s="5" t="inlineStr">
         <is>
           <t>f1</t>
         </is>
       </c>
-      <c r="D27" s="301" t="inlineStr">
+      <c r="D27" s="304" t="inlineStr">
         <is>
           <t>Cash in hand</t>
         </is>
       </c>
-      <c r="E27" s="275" t="n"/>
-      <c r="F27" s="275" t="n"/>
-      <c r="G27" s="275" t="n"/>
-      <c r="H27" s="281" t="n"/>
+      <c r="E27" s="250" t="n"/>
+      <c r="F27" s="250" t="n"/>
+      <c r="G27" s="250" t="n"/>
+      <c r="H27" s="282" t="n"/>
       <c r="I27" s="87" t="n"/>
       <c r="J27" s="49" t="n"/>
       <c r="K27" s="49" t="n"/>
       <c r="L27" s="49" t="n"/>
-      <c r="M27" s="201" t="n"/>
+      <c r="M27" s="197" t="n"/>
       <c r="N27" s="141" t="n"/>
-      <c r="O27" s="170" t="n"/>
+      <c r="O27" s="166" t="n"/>
       <c r="P27" s="134" t="n"/>
       <c r="Q27" s="49" t="n"/>
       <c r="R27" s="49" t="n"/>
       <c r="S27" s="91" t="n"/>
-      <c r="T27" s="202" t="n"/>
+      <c r="T27" s="198" t="n"/>
       <c r="U27" s="93" t="n"/>
       <c r="V27" s="53" t="n"/>
     </row>
-    <row r="28" ht="24.75" customHeight="1" s="263">
+    <row r="28" ht="24.75" customHeight="1" s="244">
       <c r="B28" s="10" t="n"/>
       <c r="C28" s="5" t="inlineStr">
         <is>
           <t>f2</t>
         </is>
       </c>
-      <c r="D28" s="301" t="inlineStr">
+      <c r="D28" s="304" t="inlineStr">
         <is>
           <t>Bank Current Account</t>
         </is>
       </c>
-      <c r="E28" s="275" t="n"/>
-      <c r="F28" s="275" t="n"/>
-      <c r="G28" s="275" t="n"/>
-      <c r="H28" s="281" t="n"/>
+      <c r="E28" s="250" t="n"/>
+      <c r="F28" s="250" t="n"/>
+      <c r="G28" s="250" t="n"/>
+      <c r="H28" s="282" t="n"/>
       <c r="I28" s="93" t="n"/>
       <c r="J28" s="38" t="n"/>
       <c r="K28" s="38" t="n"/>
       <c r="L28" s="38" t="n"/>
-      <c r="M28" s="201" t="n"/>
+      <c r="M28" s="197" t="n"/>
       <c r="N28" s="141" t="n"/>
-      <c r="O28" s="170" t="n"/>
+      <c r="O28" s="166" t="n"/>
       <c r="P28" s="134" t="n"/>
       <c r="Q28" s="49" t="n"/>
       <c r="R28" s="49" t="n"/>
       <c r="S28" s="91" t="n"/>
-      <c r="T28" s="202" t="n"/>
+      <c r="T28" s="198" t="n"/>
       <c r="U28" s="93" t="n"/>
       <c r="V28" s="53" t="n"/>
     </row>
-    <row r="29" ht="24.75" customHeight="1" s="263">
+    <row r="29" ht="24.75" customHeight="1" s="244">
       <c r="B29" s="10" t="n"/>
       <c r="C29" s="5" t="inlineStr">
         <is>
           <t>f3</t>
         </is>
       </c>
-      <c r="D29" s="301" t="inlineStr">
+      <c r="D29" s="304" t="inlineStr">
         <is>
           <t>Bank Deposit Account</t>
         </is>
       </c>
-      <c r="E29" s="275" t="n"/>
-      <c r="F29" s="275" t="n"/>
-      <c r="G29" s="275" t="n"/>
-      <c r="H29" s="281" t="n"/>
+      <c r="E29" s="250" t="n"/>
+      <c r="F29" s="250" t="n"/>
+      <c r="G29" s="250" t="n"/>
+      <c r="H29" s="282" t="n"/>
       <c r="I29" s="93" t="n"/>
       <c r="J29" s="38" t="n"/>
       <c r="K29" s="38" t="n"/>
       <c r="L29" s="38" t="n"/>
-      <c r="M29" s="201" t="n"/>
+      <c r="M29" s="197" t="n"/>
       <c r="N29" s="141" t="n"/>
-      <c r="O29" s="170" t="n"/>
+      <c r="O29" s="166" t="n"/>
       <c r="P29" s="134" t="n"/>
       <c r="Q29" s="49" t="n"/>
       <c r="R29" s="49" t="n"/>
       <c r="S29" s="91" t="n"/>
-      <c r="T29" s="202" t="n"/>
+      <c r="T29" s="198" t="n"/>
       <c r="U29" s="93" t="n"/>
       <c r="V29" s="53" t="n"/>
     </row>
-    <row r="30" ht="24.75" customHeight="1" s="263">
+    <row r="30" ht="24.75" customHeight="1" s="244">
       <c r="B30" s="10" t="n"/>
       <c r="C30" s="5" t="inlineStr">
         <is>
           <t>f4</t>
         </is>
       </c>
-      <c r="D30" s="301" t="inlineStr">
+      <c r="D30" s="304" t="inlineStr">
         <is>
           <t>Central Finance Board</t>
         </is>
       </c>
-      <c r="E30" s="275" t="n"/>
-      <c r="F30" s="275" t="n"/>
-      <c r="G30" s="275" t="n"/>
-      <c r="H30" s="281" t="n"/>
+      <c r="E30" s="250" t="n"/>
+      <c r="F30" s="250" t="n"/>
+      <c r="G30" s="250" t="n"/>
+      <c r="H30" s="282" t="n"/>
       <c r="I30" s="93" t="n"/>
       <c r="J30" s="38" t="n"/>
       <c r="K30" s="38" t="n"/>
       <c r="L30" s="38" t="n"/>
-      <c r="M30" s="201" t="n"/>
+      <c r="M30" s="197" t="n"/>
       <c r="N30" s="141" t="n"/>
-      <c r="O30" s="170" t="n"/>
+      <c r="O30" s="166" t="n"/>
       <c r="P30" s="134" t="n"/>
       <c r="Q30" s="49" t="n"/>
       <c r="R30" s="49" t="n"/>
       <c r="S30" s="91" t="n"/>
-      <c r="T30" s="202" t="n"/>
+      <c r="T30" s="198" t="n"/>
       <c r="U30" s="93" t="n"/>
       <c r="V30" s="53" t="n"/>
     </row>
-    <row r="31" ht="24.75" customHeight="1" s="263">
+    <row r="31" ht="24.75" customHeight="1" s="244">
       <c r="B31" s="9" t="n"/>
       <c r="C31" s="5" t="inlineStr">
         <is>
           <t>f5</t>
         </is>
       </c>
-      <c r="D31" s="301" t="inlineStr">
+      <c r="D31" s="304" t="inlineStr">
         <is>
           <t>Trustees for Methodist Church Purposes</t>
         </is>
       </c>
-      <c r="E31" s="275" t="n"/>
-      <c r="F31" s="275" t="n"/>
-      <c r="G31" s="275" t="n"/>
-      <c r="H31" s="281" t="n"/>
+      <c r="E31" s="250" t="n"/>
+      <c r="F31" s="250" t="n"/>
+      <c r="G31" s="250" t="n"/>
+      <c r="H31" s="282" t="n"/>
       <c r="I31" s="93" t="n"/>
       <c r="J31" s="38" t="n"/>
       <c r="K31" s="38" t="n"/>
@@ -5172,22 +5226,22 @@
       <c r="U31" s="93" t="n"/>
       <c r="V31" s="53" t="n"/>
     </row>
-    <row r="32" ht="24.75" customHeight="1" s="263" thickBot="1">
+    <row r="32" ht="24.75" customHeight="1" s="244" thickBot="1">
       <c r="B32" s="9" t="n"/>
       <c r="C32" s="5" t="inlineStr">
         <is>
           <t>f6</t>
         </is>
       </c>
-      <c r="D32" s="301" t="inlineStr">
+      <c r="D32" s="304" t="inlineStr">
         <is>
           <t>Other funds</t>
         </is>
       </c>
-      <c r="E32" s="275" t="n"/>
-      <c r="F32" s="275" t="n"/>
-      <c r="G32" s="275" t="n"/>
-      <c r="H32" s="281" t="n"/>
+      <c r="E32" s="250" t="n"/>
+      <c r="F32" s="250" t="n"/>
+      <c r="G32" s="250" t="n"/>
+      <c r="H32" s="282" t="n"/>
       <c r="I32" s="93" t="n"/>
       <c r="J32" s="38" t="n"/>
       <c r="K32" s="38" t="n"/>
@@ -5203,22 +5257,22 @@
       <c r="U32" s="97" t="n"/>
       <c r="V32" s="53" t="n"/>
     </row>
-    <row r="33" ht="30.2" customHeight="1" s="263">
+    <row r="33" ht="30.2" customHeight="1" s="244">
       <c r="B33" s="9" t="n"/>
       <c r="C33" s="5" t="inlineStr">
         <is>
           <t>f7</t>
         </is>
       </c>
-      <c r="D33" s="306" t="inlineStr">
+      <c r="D33" s="308" t="inlineStr">
         <is>
           <t xml:space="preserve">SUB TOTAL - Church accounts </t>
         </is>
       </c>
-      <c r="E33" s="275" t="n"/>
-      <c r="F33" s="275" t="n"/>
-      <c r="G33" s="275" t="n"/>
-      <c r="H33" s="281" t="n"/>
+      <c r="E33" s="250" t="n"/>
+      <c r="F33" s="250" t="n"/>
+      <c r="G33" s="250" t="n"/>
+      <c r="H33" s="282" t="n"/>
       <c r="I33" s="93" t="n"/>
       <c r="J33" s="38" t="n"/>
       <c r="K33" s="38" t="n"/>
@@ -5248,22 +5302,22 @@
       </c>
       <c r="V33" s="53" t="n"/>
     </row>
-    <row r="34" ht="32.25" customHeight="1" s="263" thickBot="1">
+    <row r="34" ht="32.25" customHeight="1" s="244" thickBot="1">
       <c r="B34" s="9" t="n"/>
       <c r="C34" s="5" t="inlineStr">
         <is>
           <t>f8</t>
         </is>
       </c>
-      <c r="D34" s="301" t="inlineStr">
+      <c r="D34" s="304" t="inlineStr">
         <is>
           <t>Total funds held by Internal Organisations (the closing balance total from above) (e12)</t>
         </is>
       </c>
-      <c r="E34" s="275" t="n"/>
-      <c r="F34" s="275" t="n"/>
-      <c r="G34" s="275" t="n"/>
-      <c r="H34" s="281" t="n"/>
+      <c r="E34" s="250" t="n"/>
+      <c r="F34" s="250" t="n"/>
+      <c r="G34" s="250" t="n"/>
+      <c r="H34" s="282" t="n"/>
       <c r="I34" s="93" t="n"/>
       <c r="J34" s="38" t="n"/>
       <c r="K34" s="38" t="n"/>
@@ -5303,22 +5357,22 @@
         </is>
       </c>
     </row>
-    <row r="35" ht="30.2" customHeight="1" s="263" thickBot="1" thickTop="1">
+    <row r="35" ht="30.2" customHeight="1" s="244" thickBot="1" thickTop="1">
       <c r="B35" s="9" t="n"/>
       <c r="C35" s="5" t="inlineStr">
         <is>
           <t>f9</t>
         </is>
       </c>
-      <c r="D35" s="306" t="inlineStr">
+      <c r="D35" s="308" t="inlineStr">
         <is>
           <t>TOTAL CASH FUNDS HELD BY CHURCH</t>
         </is>
       </c>
-      <c r="E35" s="275" t="n"/>
-      <c r="F35" s="275" t="n"/>
-      <c r="G35" s="275" t="n"/>
-      <c r="H35" s="281" t="n"/>
+      <c r="E35" s="250" t="n"/>
+      <c r="F35" s="250" t="n"/>
+      <c r="G35" s="250" t="n"/>
+      <c r="H35" s="282" t="n"/>
       <c r="I35" s="93" t="n"/>
       <c r="J35" s="38" t="n"/>
       <c r="K35" s="38" t="n"/>
@@ -5333,7 +5387,7 @@
           <t>(x)</t>
         </is>
       </c>
-      <c r="P35" s="242" t="n"/>
+      <c r="P35" s="238" t="n"/>
       <c r="Q35" s="49" t="n"/>
       <c r="R35" s="49" t="n"/>
       <c r="S35" s="38" t="n"/>
@@ -5361,14 +5415,14 @@
         <v/>
       </c>
     </row>
-    <row r="36" ht="9" customHeight="1" s="263" thickBot="1" thickTop="1">
+    <row r="36" ht="9" customHeight="1" s="244" thickBot="1" thickTop="1">
       <c r="B36" s="9" t="n"/>
       <c r="C36" s="27" t="n"/>
-      <c r="D36" s="203" t="n"/>
-      <c r="E36" s="203" t="n"/>
-      <c r="F36" s="203" t="n"/>
-      <c r="G36" s="203" t="n"/>
-      <c r="H36" s="203" t="n"/>
+      <c r="D36" s="199" t="n"/>
+      <c r="E36" s="199" t="n"/>
+      <c r="F36" s="199" t="n"/>
+      <c r="G36" s="199" t="n"/>
+      <c r="H36" s="199" t="n"/>
       <c r="I36" s="110" t="n"/>
       <c r="J36" s="110" t="n"/>
       <c r="K36" s="110" t="n"/>
@@ -5384,14 +5438,14 @@
       <c r="U36" s="113" t="n"/>
       <c r="V36" s="53" t="n"/>
     </row>
-    <row r="37" ht="6.75" customHeight="1" s="263" thickTop="1">
+    <row r="37" ht="6.75" customHeight="1" s="244" thickTop="1">
       <c r="B37" s="9" t="n"/>
-      <c r="C37" s="288" t="n"/>
-      <c r="D37" s="204" t="n"/>
-      <c r="E37" s="204" t="n"/>
-      <c r="F37" s="204" t="n"/>
-      <c r="G37" s="204" t="n"/>
-      <c r="H37" s="204" t="n"/>
+      <c r="C37" s="292" t="n"/>
+      <c r="D37" s="200" t="n"/>
+      <c r="E37" s="200" t="n"/>
+      <c r="F37" s="200" t="n"/>
+      <c r="G37" s="200" t="n"/>
+      <c r="H37" s="200" t="n"/>
       <c r="I37" s="38" t="n"/>
       <c r="J37" s="38" t="n"/>
       <c r="K37" s="38" t="n"/>
@@ -5407,18 +5461,18 @@
       <c r="U37" s="115" t="n"/>
       <c r="V37" s="53" t="n"/>
     </row>
-    <row r="38" ht="23.25" customHeight="1" s="263" thickBot="1">
+    <row r="38" ht="23.25" customHeight="1" s="244" thickBot="1">
       <c r="B38" s="9" t="n"/>
-      <c r="C38" s="288" t="n"/>
-      <c r="D38" s="177" t="inlineStr">
+      <c r="C38" s="292" t="n"/>
+      <c r="D38" s="173" t="inlineStr">
         <is>
           <t>SECTION G</t>
         </is>
       </c>
-      <c r="E38" s="204" t="n"/>
-      <c r="F38" s="204" t="n"/>
-      <c r="G38" s="204" t="n"/>
-      <c r="H38" s="204" t="n"/>
+      <c r="E38" s="200" t="n"/>
+      <c r="F38" s="200" t="n"/>
+      <c r="G38" s="200" t="n"/>
+      <c r="H38" s="200" t="n"/>
       <c r="I38" s="38" t="n"/>
       <c r="J38" s="38" t="n"/>
       <c r="K38" s="38" t="n"/>
@@ -5442,9 +5496,9 @@
       <c r="U38" s="115" t="n"/>
       <c r="V38" s="53" t="n"/>
     </row>
-    <row r="39" ht="24" customHeight="1" s="263">
+    <row r="39" ht="24" customHeight="1" s="244">
       <c r="B39" s="9" t="n"/>
-      <c r="C39" s="288" t="n"/>
+      <c r="C39" s="292" t="n"/>
       <c r="D39" s="12" t="inlineStr">
         <is>
           <t>OTHER ASSETS and LIABILITIES</t>
@@ -5469,7 +5523,7 @@
       <c r="Q39" s="49" t="n"/>
       <c r="R39" s="49" t="n"/>
       <c r="S39" s="49" t="n"/>
-      <c r="T39" s="228" t="inlineStr">
+      <c r="T39" s="224" t="inlineStr">
         <is>
           <t>31 August 2024</t>
         </is>
@@ -5477,22 +5531,22 @@
       <c r="U39" s="49" t="n"/>
       <c r="V39" s="53" t="n"/>
     </row>
-    <row r="40" ht="30.2" customHeight="1" s="263">
+    <row r="40" ht="30.2" customHeight="1" s="244">
       <c r="B40" s="9" t="n"/>
       <c r="C40" s="5" t="inlineStr">
         <is>
           <t>g1</t>
         </is>
       </c>
-      <c r="D40" s="303" t="inlineStr">
+      <c r="D40" s="310" t="inlineStr">
         <is>
           <t>Investments (include Endowments)</t>
         </is>
       </c>
-      <c r="E40" s="275" t="n"/>
-      <c r="F40" s="275" t="n"/>
-      <c r="G40" s="235" t="n"/>
-      <c r="H40" s="205" t="n"/>
+      <c r="E40" s="250" t="n"/>
+      <c r="F40" s="250" t="n"/>
+      <c r="G40" s="231" t="n"/>
+      <c r="H40" s="201" t="n"/>
       <c r="I40" s="117" t="n"/>
       <c r="J40" s="117" t="n"/>
       <c r="K40" s="117" t="n"/>
@@ -5508,22 +5562,22 @@
       <c r="U40" s="121" t="n"/>
       <c r="V40" s="53" t="n"/>
     </row>
-    <row r="41" ht="32.25" customHeight="1" s="263">
+    <row r="41" ht="32.25" customHeight="1" s="244">
       <c r="B41" s="9" t="n"/>
       <c r="C41" s="5" t="inlineStr">
         <is>
           <t>g2</t>
         </is>
       </c>
-      <c r="D41" s="302" t="inlineStr">
+      <c r="D41" s="306" t="inlineStr">
         <is>
           <t>Land &amp; Buildings (see notes re Insurance value)</t>
         </is>
       </c>
-      <c r="E41" s="275" t="n"/>
-      <c r="F41" s="275" t="n"/>
-      <c r="G41" s="234" t="n"/>
-      <c r="H41" s="206" t="n"/>
+      <c r="E41" s="250" t="n"/>
+      <c r="F41" s="250" t="n"/>
+      <c r="G41" s="230" t="n"/>
+      <c r="H41" s="202" t="n"/>
       <c r="I41" s="122" t="n"/>
       <c r="J41" s="122" t="n"/>
       <c r="K41" s="122" t="n"/>
@@ -5539,22 +5593,22 @@
       <c r="U41" s="126" t="n"/>
       <c r="V41" s="53" t="n"/>
     </row>
-    <row r="42" ht="30.2" customHeight="1" s="263">
+    <row r="42" ht="30.2" customHeight="1" s="244">
       <c r="B42" s="9" t="n"/>
       <c r="C42" s="5" t="inlineStr">
         <is>
           <t>g3</t>
         </is>
       </c>
-      <c r="D42" s="302" t="inlineStr">
+      <c r="D42" s="306" t="inlineStr">
         <is>
           <t>Other Assets</t>
         </is>
       </c>
-      <c r="E42" s="234" t="n"/>
-      <c r="F42" s="234" t="n"/>
-      <c r="G42" s="234" t="n"/>
-      <c r="H42" s="206" t="n"/>
+      <c r="E42" s="230" t="n"/>
+      <c r="F42" s="230" t="n"/>
+      <c r="G42" s="230" t="n"/>
+      <c r="H42" s="202" t="n"/>
       <c r="I42" s="122" t="n"/>
       <c r="J42" s="122" t="n"/>
       <c r="K42" s="122" t="n"/>
@@ -5570,7 +5624,7 @@
       <c r="U42" s="126" t="n"/>
       <c r="V42" s="53" t="n"/>
     </row>
-    <row r="43" ht="30.2" customHeight="1" s="263">
+    <row r="43" ht="30.2" customHeight="1" s="244">
       <c r="A43" s="12" t="n"/>
       <c r="B43" s="13" t="n"/>
       <c r="C43" s="5" t="inlineStr">
@@ -5578,15 +5632,15 @@
           <t>g4</t>
         </is>
       </c>
-      <c r="D43" s="301" t="inlineStr">
+      <c r="D43" s="304" t="inlineStr">
         <is>
           <t>Loan(s) - show amount outstanding at year end</t>
         </is>
       </c>
-      <c r="E43" s="275" t="n"/>
-      <c r="F43" s="275" t="n"/>
-      <c r="G43" s="275" t="n"/>
-      <c r="H43" s="281" t="n"/>
+      <c r="E43" s="250" t="n"/>
+      <c r="F43" s="250" t="n"/>
+      <c r="G43" s="250" t="n"/>
+      <c r="H43" s="282" t="n"/>
       <c r="I43" s="127" t="n"/>
       <c r="J43" s="127" t="n"/>
       <c r="K43" s="127" t="n"/>
@@ -5602,22 +5656,22 @@
       <c r="U43" s="126" t="n"/>
       <c r="V43" s="53" t="n"/>
     </row>
-    <row r="44" ht="30.2" customHeight="1" s="263">
+    <row r="44" ht="30.2" customHeight="1" s="244">
       <c r="B44" s="9" t="n"/>
       <c r="C44" s="5" t="inlineStr">
         <is>
           <t>g5</t>
         </is>
       </c>
-      <c r="D44" s="302" t="inlineStr">
+      <c r="D44" s="306" t="inlineStr">
         <is>
           <t xml:space="preserve">Other  Liabilities                </t>
         </is>
       </c>
-      <c r="E44" s="275" t="n"/>
-      <c r="F44" s="275" t="n"/>
-      <c r="G44" s="234" t="n"/>
-      <c r="H44" s="207" t="n"/>
+      <c r="E44" s="250" t="n"/>
+      <c r="F44" s="250" t="n"/>
+      <c r="G44" s="230" t="n"/>
+      <c r="H44" s="203" t="n"/>
       <c r="I44" s="45" t="n"/>
       <c r="J44" s="45" t="n"/>
       <c r="K44" s="45" t="n"/>
@@ -5635,7 +5689,7 @@
     </row>
     <row r="45">
       <c r="B45" s="9" t="n"/>
-      <c r="C45" s="288" t="n"/>
+      <c r="C45" s="292" t="n"/>
       <c r="D45" s="38" t="n"/>
       <c r="E45" s="38" t="n"/>
       <c r="F45" s="38" t="n"/>
@@ -5656,7 +5710,7 @@
       <c r="U45" s="38" t="n"/>
       <c r="V45" s="53" t="n"/>
     </row>
-    <row r="46" ht="3.2" customHeight="1" s="263">
+    <row r="46" ht="3.2" customHeight="1" s="244">
       <c r="B46" s="9" t="n"/>
       <c r="D46" s="49" t="n"/>
       <c r="E46" s="49" t="n"/>
@@ -5680,7 +5734,7 @@
     </row>
     <row r="47">
       <c r="B47" s="9" t="n"/>
-      <c r="D47" s="300" t="inlineStr">
+      <c r="D47" s="309" t="inlineStr">
         <is>
           <t>f4 Include only Funds held at the Central Finance Board</t>
         </is>
@@ -5699,7 +5753,7 @@
     </row>
     <row r="48">
       <c r="B48" s="9" t="n"/>
-      <c r="D48" s="300" t="inlineStr">
+      <c r="D48" s="309" t="inlineStr">
         <is>
           <t>f5 Include only Funds held at Trustees for Methodist Church Purposes</t>
         </is>
@@ -5742,7 +5796,7 @@
       <c r="U49" s="49" t="n"/>
       <c r="V49" s="53" t="n"/>
     </row>
-    <row r="50" ht="3.2" customHeight="1" s="263">
+    <row r="50" ht="3.2" customHeight="1" s="244">
       <c r="B50" s="9" t="n"/>
       <c r="C50" s="9" t="n"/>
       <c r="D50" s="9" t="n"/>
@@ -5767,18 +5821,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="N2:S2"/>
-    <mergeCell ref="D7:T7"/>
-    <mergeCell ref="D5:T5"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="D27:H27"/>
-    <mergeCell ref="D29:H29"/>
-    <mergeCell ref="D3:T3"/>
-    <mergeCell ref="D41:F41"/>
-    <mergeCell ref="D6:T6"/>
-    <mergeCell ref="D33:H33"/>
-    <mergeCell ref="D35:H35"/>
-    <mergeCell ref="D28:H28"/>
     <mergeCell ref="D48:K48"/>
     <mergeCell ref="D30:H30"/>
     <mergeCell ref="D31:H31"/>
@@ -5788,6 +5830,18 @@
     <mergeCell ref="D47:K47"/>
     <mergeCell ref="D40:F40"/>
     <mergeCell ref="D43:H43"/>
+    <mergeCell ref="D29:H29"/>
+    <mergeCell ref="D3:T3"/>
+    <mergeCell ref="D41:F41"/>
+    <mergeCell ref="D6:T6"/>
+    <mergeCell ref="D33:H33"/>
+    <mergeCell ref="D35:H35"/>
+    <mergeCell ref="D28:H28"/>
+    <mergeCell ref="N2:S2"/>
+    <mergeCell ref="D7:T7"/>
+    <mergeCell ref="D5:T5"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="D27:H27"/>
   </mergeCells>
   <pageMargins left="0.1574803149606299" right="0.1574803149606299" top="0.2755905511811024" bottom="0.3543307086614174" header="0.1574803149606299" footer="0.1574803149606299"/>
   <pageSetup orientation="portrait" paperSize="9" scale="59"/>
@@ -5816,8 +5870,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
   <sheetData>
-    <row r="2" ht="15" customHeight="1" s="263">
-      <c r="A2" s="220" t="inlineStr">
+    <row r="2" ht="15" customHeight="1" s="244">
+      <c r="A2" s="216" t="inlineStr">
         <is>
           <t>Name of Church ……………………………………………………………  No………..</t>
         </is>
@@ -5831,202 +5885,202 @@
       <c r="H2" s="12" t="n"/>
       <c r="I2" s="12" t="n"/>
     </row>
-    <row r="3" ht="15" customHeight="1" s="263">
-      <c r="A3" s="220" t="n"/>
-    </row>
-    <row r="4" ht="15" customHeight="1" s="263">
-      <c r="A4" s="220" t="n"/>
-    </row>
-    <row r="5" ht="26.25" customHeight="1" s="263">
-      <c r="C5" s="224" t="inlineStr">
+    <row r="3" ht="15" customHeight="1" s="244">
+      <c r="A3" s="216" t="n"/>
+    </row>
+    <row r="4" ht="15" customHeight="1" s="244">
+      <c r="A4" s="216" t="n"/>
+    </row>
+    <row r="5" ht="26.25" customHeight="1" s="244">
+      <c r="C5" s="220" t="inlineStr">
         <is>
           <t>Declarations and Scrutiny</t>
         </is>
       </c>
     </row>
-    <row r="6" ht="26.25" customHeight="1" s="263">
-      <c r="A6" s="221" t="n"/>
-    </row>
-    <row r="7" ht="15" customHeight="1" s="263">
-      <c r="A7" s="314" t="inlineStr">
+    <row r="6" ht="26.25" customHeight="1" s="244">
+      <c r="A6" s="217" t="n"/>
+    </row>
+    <row r="7" ht="15" customHeight="1" s="244">
+      <c r="A7" s="311" t="inlineStr">
         <is>
           <t>I confirm that these Receipt and Payment based accounts for the year to 31 August 2024 have been prepared from the records of the Church and that they include all funds under the control of the Church trustees.</t>
         </is>
       </c>
     </row>
-    <row r="8" ht="15" customHeight="1" s="263"/>
-    <row r="9" ht="15" customHeight="1" s="263"/>
-    <row r="10" ht="15" customHeight="1" s="263">
-      <c r="A10" s="220" t="n"/>
-    </row>
-    <row r="11" ht="15" customHeight="1" s="263">
-      <c r="A11" s="220" t="n"/>
-    </row>
-    <row r="12" ht="15" customHeight="1" s="263">
-      <c r="A12" s="220" t="inlineStr">
+    <row r="8" ht="15" customHeight="1" s="244"/>
+    <row r="9" ht="15" customHeight="1" s="244"/>
+    <row r="10" ht="15" customHeight="1" s="244">
+      <c r="A10" s="216" t="n"/>
+    </row>
+    <row r="11" ht="15" customHeight="1" s="244">
+      <c r="A11" s="216" t="n"/>
+    </row>
+    <row r="12" ht="15" customHeight="1" s="244">
+      <c r="A12" s="216" t="inlineStr">
         <is>
           <t>Signature of treasurer ………………………………………………………   Date……………………..</t>
         </is>
       </c>
     </row>
-    <row r="13" ht="15" customHeight="1" s="263">
-      <c r="A13" s="220" t="n"/>
-    </row>
-    <row r="14" ht="15" customHeight="1" s="263">
-      <c r="A14" s="220" t="inlineStr">
+    <row r="13" ht="15" customHeight="1" s="244">
+      <c r="A13" s="216" t="n"/>
+    </row>
+    <row r="14" ht="15" customHeight="1" s="244">
+      <c r="A14" s="216" t="inlineStr">
         <is>
           <t>Name and address of treasurer ………………………………………………………………………….</t>
         </is>
       </c>
     </row>
-    <row r="15" ht="15" customHeight="1" s="263">
-      <c r="A15" s="220" t="n"/>
-    </row>
-    <row r="16" ht="15" customHeight="1" s="263">
-      <c r="A16" s="220" t="inlineStr">
+    <row r="15" ht="15" customHeight="1" s="244">
+      <c r="A15" s="216" t="n"/>
+    </row>
+    <row r="16" ht="15" customHeight="1" s="244">
+      <c r="A16" s="216" t="inlineStr">
         <is>
           <t>………………………………………………………………………………….  Post Code………………</t>
         </is>
       </c>
     </row>
-    <row r="17" ht="15" customHeight="1" s="263">
-      <c r="A17" s="220" t="n"/>
-    </row>
-    <row r="18" ht="15" customHeight="1" s="263">
-      <c r="A18" s="220" t="n"/>
-    </row>
-    <row r="19" ht="15.75" customHeight="1" s="263">
-      <c r="A19" s="222" t="inlineStr">
+    <row r="17" ht="15" customHeight="1" s="244">
+      <c r="A17" s="216" t="n"/>
+    </row>
+    <row r="18" ht="15" customHeight="1" s="244">
+      <c r="A18" s="216" t="n"/>
+    </row>
+    <row r="19" ht="15.75" customHeight="1" s="244">
+      <c r="A19" s="218" t="inlineStr">
         <is>
           <t>Presentation to the Church trustees</t>
         </is>
       </c>
     </row>
-    <row r="20" ht="15.75" customHeight="1" s="263">
-      <c r="A20" s="222" t="n"/>
-    </row>
-    <row r="21" ht="15" customHeight="1" s="263">
-      <c r="A21" s="314" t="inlineStr">
+    <row r="20" ht="15.75" customHeight="1" s="244">
+      <c r="A20" s="218" t="n"/>
+    </row>
+    <row r="21" ht="15" customHeight="1" s="244">
+      <c r="A21" s="311" t="inlineStr">
         <is>
           <t>I confirm that the annual report and accounts for the year ended 31 August 2024 were/will be* presented to the meeting of the Church trustees held on ……………..</t>
         </is>
       </c>
     </row>
-    <row r="22" ht="15" customHeight="1" s="263"/>
-    <row r="23" ht="15" customHeight="1" s="263">
-      <c r="A23" s="314" t="n"/>
-      <c r="B23" s="314" t="n"/>
-      <c r="C23" s="314" t="n"/>
-      <c r="D23" s="314" t="n"/>
-      <c r="E23" s="314" t="n"/>
-      <c r="F23" s="314" t="n"/>
-      <c r="G23" s="314" t="n"/>
-      <c r="H23" s="314" t="n"/>
-      <c r="I23" s="314" t="n"/>
-      <c r="J23" s="314" t="n"/>
-      <c r="K23" s="314" t="n"/>
-    </row>
-    <row r="24" ht="15" customHeight="1" s="263">
-      <c r="A24" s="220" t="n"/>
-    </row>
-    <row r="25" ht="15" customHeight="1" s="263">
-      <c r="A25" s="220" t="inlineStr">
+    <row r="22" ht="15" customHeight="1" s="244"/>
+    <row r="23" ht="15" customHeight="1" s="244">
+      <c r="A23" s="311" t="n"/>
+      <c r="B23" s="311" t="n"/>
+      <c r="C23" s="311" t="n"/>
+      <c r="D23" s="311" t="n"/>
+      <c r="E23" s="311" t="n"/>
+      <c r="F23" s="311" t="n"/>
+      <c r="G23" s="311" t="n"/>
+      <c r="H23" s="311" t="n"/>
+      <c r="I23" s="311" t="n"/>
+      <c r="J23" s="311" t="n"/>
+      <c r="K23" s="311" t="n"/>
+    </row>
+    <row r="24" ht="15" customHeight="1" s="244">
+      <c r="A24" s="216" t="n"/>
+    </row>
+    <row r="25" ht="15" customHeight="1" s="244">
+      <c r="A25" s="216" t="inlineStr">
         <is>
           <t>Signature of the Chair of the meeting  ……………………………………………………………………</t>
         </is>
       </c>
     </row>
-    <row r="26" ht="15" customHeight="1" s="263">
-      <c r="A26" s="220" t="n"/>
-    </row>
-    <row r="27" ht="15" customHeight="1" s="263">
-      <c r="A27" s="220" t="inlineStr">
+    <row r="26" ht="15" customHeight="1" s="244">
+      <c r="A26" s="216" t="n"/>
+    </row>
+    <row r="27" ht="15" customHeight="1" s="244">
+      <c r="A27" s="216" t="inlineStr">
         <is>
           <t>Name of the Chair of the meeting  …………………………………………… Date ……………………</t>
         </is>
       </c>
     </row>
-    <row r="28" ht="15" customHeight="1" s="263">
-      <c r="A28" s="220" t="n"/>
-    </row>
-    <row r="29" ht="15" customHeight="1" s="263">
-      <c r="A29" s="220" t="n"/>
-    </row>
-    <row r="30" ht="15" customHeight="1" s="263">
-      <c r="A30" s="220" t="n"/>
-    </row>
-    <row r="31" ht="15" customHeight="1" s="263">
-      <c r="A31" s="220" t="n"/>
-    </row>
-    <row r="32" ht="15" customHeight="1" s="263">
-      <c r="A32" s="220" t="n"/>
-    </row>
-    <row r="33" ht="18" customHeight="1" s="263">
-      <c r="C33" s="225" t="inlineStr">
+    <row r="28" ht="15" customHeight="1" s="244">
+      <c r="A28" s="216" t="n"/>
+    </row>
+    <row r="29" ht="15" customHeight="1" s="244">
+      <c r="A29" s="216" t="n"/>
+    </row>
+    <row r="30" ht="15" customHeight="1" s="244">
+      <c r="A30" s="216" t="n"/>
+    </row>
+    <row r="31" ht="15" customHeight="1" s="244">
+      <c r="A31" s="216" t="n"/>
+    </row>
+    <row r="32" ht="15" customHeight="1" s="244">
+      <c r="A32" s="216" t="n"/>
+    </row>
+    <row r="33" ht="18" customHeight="1" s="244">
+      <c r="C33" s="221" t="inlineStr">
         <is>
           <t xml:space="preserve">Independent Examiner’s Report to the Trustees of the </t>
         </is>
       </c>
     </row>
-    <row r="34" ht="18" customHeight="1" s="263">
-      <c r="A34" s="223" t="n"/>
-    </row>
-    <row r="35" ht="18" customHeight="1" s="263">
-      <c r="D35" s="225" t="inlineStr">
+    <row r="34" ht="18" customHeight="1" s="244">
+      <c r="A34" s="219" t="n"/>
+    </row>
+    <row r="35" ht="18" customHeight="1" s="244">
+      <c r="D35" s="221" t="inlineStr">
         <is>
           <t>……………………..……………………..Church</t>
         </is>
       </c>
     </row>
-    <row r="36" ht="18" customHeight="1" s="263">
-      <c r="A36" s="223" t="n"/>
-    </row>
-    <row r="37" ht="15.75" customHeight="1" s="263">
-      <c r="E37" s="226" t="inlineStr">
+    <row r="36" ht="18" customHeight="1" s="244">
+      <c r="A36" s="219" t="n"/>
+    </row>
+    <row r="37" ht="15.75" customHeight="1" s="244">
+      <c r="E37" s="222" t="inlineStr">
         <is>
           <t>Charity Number …………..</t>
         </is>
       </c>
     </row>
-    <row r="38" ht="15.75" customHeight="1" s="263">
-      <c r="A38" s="222" t="n"/>
-    </row>
-    <row r="39" ht="15.75" customHeight="1" s="263">
-      <c r="A39" s="222" t="n"/>
-    </row>
-    <row r="40" ht="15.75" customHeight="1" s="263">
-      <c r="A40" s="222" t="inlineStr">
+    <row r="38" ht="15.75" customHeight="1" s="244">
+      <c r="A38" s="218" t="n"/>
+    </row>
+    <row r="39" ht="15.75" customHeight="1" s="244">
+      <c r="A39" s="218" t="n"/>
+    </row>
+    <row r="40" ht="15.75" customHeight="1" s="244">
+      <c r="A40" s="218" t="inlineStr">
         <is>
           <t>Responsibilities and basis of report</t>
         </is>
       </c>
     </row>
-    <row r="41" ht="15.75" customHeight="1" s="263">
-      <c r="A41" s="222" t="n"/>
-    </row>
-    <row r="42" ht="15" customHeight="1" s="263">
-      <c r="A42" s="314" t="inlineStr">
+    <row r="41" ht="15.75" customHeight="1" s="244">
+      <c r="A41" s="218" t="n"/>
+    </row>
+    <row r="42" ht="15" customHeight="1" s="244">
+      <c r="A42" s="311" t="inlineStr">
         <is>
           <t xml:space="preserve">I report to the trustees on my examination of the accounts of the …………………………………. Church for the year ended 31 August 2024 set out on pages … to ….  As the Church’s trustees, you are responsible for the preparation of the accounts in accordance with the requirements of the Charities Act 2011 (‘the Act’). </t>
         </is>
       </c>
     </row>
-    <row r="43" ht="15" customHeight="1" s="263"/>
-    <row r="44" ht="15" customHeight="1" s="263"/>
-    <row r="45" ht="15" customHeight="1" s="263"/>
-    <row r="46" ht="15" customHeight="1" s="263"/>
-    <row r="47" ht="12.75" customHeight="1" s="263">
-      <c r="A47" s="315" t="inlineStr">
+    <row r="43" ht="15" customHeight="1" s="244"/>
+    <row r="44" ht="15" customHeight="1" s="244"/>
+    <row r="45" ht="15" customHeight="1" s="244"/>
+    <row r="46" ht="15" customHeight="1" s="244"/>
+    <row r="47" ht="12.75" customHeight="1" s="244">
+      <c r="A47" s="312" t="inlineStr">
         <is>
           <t>I report in respect of my examination of the Church’s accounts carried out under section 145 of the Act and, in carrying out my examination, I have followed all the applicable Directions given by the Charity Commission under section 145(5)(b) of the Act.</t>
         </is>
       </c>
     </row>
-    <row r="48" ht="15" customHeight="1" s="263"/>
-    <row r="49" ht="15" customHeight="1" s="263"/>
+    <row r="48" ht="15" customHeight="1" s="244"/>
+    <row r="49" ht="15" customHeight="1" s="244"/>
     <row r="50"/>
-    <row r="53" ht="15" customHeight="1" s="263">
-      <c r="A53" s="220" t="inlineStr">
+    <row r="53" ht="15" customHeight="1" s="244">
+      <c r="A53" s="216" t="inlineStr">
         <is>
           <t>* delete or circle as appropriate</t>
         </is>
@@ -6066,194 +6120,194 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
   <cols>
-    <col width="9.140625" customWidth="1" style="263" min="8" max="9"/>
-    <col width="15" customWidth="1" style="263" min="10" max="10"/>
+    <col width="9.140625" customWidth="1" style="244" min="8" max="9"/>
+    <col width="15" customWidth="1" style="244" min="10" max="10"/>
   </cols>
   <sheetData>
-    <row r="2" ht="15" customHeight="1" s="263">
-      <c r="A2" s="220" t="inlineStr">
+    <row r="2" ht="15" customHeight="1" s="244">
+      <c r="A2" s="216" t="inlineStr">
         <is>
           <t>Name of Church …………………………………………………………………………  No ………….</t>
         </is>
       </c>
     </row>
-    <row r="3" ht="15" customHeight="1" s="263">
-      <c r="A3" s="220" t="n"/>
-    </row>
-    <row r="4" ht="15" customHeight="1" s="263">
-      <c r="A4" s="220" t="n"/>
-    </row>
-    <row r="5" ht="15.75" customHeight="1" s="263">
-      <c r="A5" s="222" t="inlineStr">
+    <row r="3" ht="15" customHeight="1" s="244">
+      <c r="A3" s="216" t="n"/>
+    </row>
+    <row r="4" ht="15" customHeight="1" s="244">
+      <c r="A4" s="216" t="n"/>
+    </row>
+    <row r="5" ht="15.75" customHeight="1" s="244">
+      <c r="A5" s="218" t="inlineStr">
         <is>
           <t>Independent Examiner’s Statement</t>
         </is>
       </c>
     </row>
-    <row r="6" ht="15.75" customHeight="1" s="263">
-      <c r="A6" s="222" t="n"/>
-    </row>
-    <row r="7" ht="15" customHeight="1" s="263">
-      <c r="A7" s="314" t="inlineStr">
+    <row r="6" ht="15.75" customHeight="1" s="244">
+      <c r="A6" s="218" t="n"/>
+    </row>
+    <row r="7" ht="15" customHeight="1" s="244">
+      <c r="A7" s="311" t="inlineStr">
         <is>
           <t>I have completed my examination.  I confirm that no material matters have come to my attention in connection with the examination (other than that disclosed below*) which give me cause to believe that in, any material respect:</t>
         </is>
       </c>
     </row>
-    <row r="8" ht="15" customHeight="1" s="263"/>
-    <row r="9" ht="15" customHeight="1" s="263"/>
-    <row r="10" ht="15" customHeight="1" s="263"/>
-    <row r="11" ht="15" customHeight="1" s="263">
-      <c r="A11" s="220" t="n"/>
-    </row>
-    <row r="12" ht="15.75" customHeight="1" s="263">
-      <c r="A12" s="227" t="inlineStr">
+    <row r="8" ht="15" customHeight="1" s="244"/>
+    <row r="9" ht="15" customHeight="1" s="244"/>
+    <row r="10" ht="15" customHeight="1" s="244"/>
+    <row r="11" ht="15" customHeight="1" s="244">
+      <c r="A11" s="216" t="n"/>
+    </row>
+    <row r="12" ht="15.75" customHeight="1" s="244">
+      <c r="A12" s="223" t="inlineStr">
         <is>
           <t xml:space="preserve">·         the accounting records were not kept in accordance with section 130 of the Act; or </t>
         </is>
       </c>
     </row>
-    <row r="13" ht="15.75" customHeight="1" s="263">
-      <c r="A13" s="227" t="inlineStr">
+    <row r="13" ht="15.75" customHeight="1" s="244">
+      <c r="A13" s="223" t="inlineStr">
         <is>
           <t>·         the accounts do not accord with the accounting records.</t>
         </is>
       </c>
     </row>
-    <row r="14" ht="15" customHeight="1" s="263">
-      <c r="A14" s="220" t="n"/>
-    </row>
-    <row r="15" ht="15" customHeight="1" s="263">
-      <c r="A15" s="220" t="n"/>
-    </row>
-    <row r="16" ht="15" customHeight="1" s="263">
-      <c r="A16" s="315" t="inlineStr">
+    <row r="14" ht="15" customHeight="1" s="244">
+      <c r="A14" s="216" t="n"/>
+    </row>
+    <row r="15" ht="15" customHeight="1" s="244">
+      <c r="A15" s="216" t="n"/>
+    </row>
+    <row r="16" ht="15" customHeight="1" s="244">
+      <c r="A16" s="312" t="inlineStr">
         <is>
           <t>I have no concerns and have come across no other matters in connection with the examination to which attention should be drawn in this report in order to enable a proper understanding of the accounts to be reached.</t>
         </is>
       </c>
     </row>
-    <row r="17" ht="15" customHeight="1" s="263"/>
-    <row r="18" ht="15" customHeight="1" s="263"/>
-    <row r="19" ht="15" customHeight="1" s="263">
-      <c r="A19" s="220" t="n"/>
-    </row>
-    <row r="20" ht="15" customHeight="1" s="263">
-      <c r="A20" s="314" t="inlineStr">
+    <row r="17" ht="15" customHeight="1" s="244"/>
+    <row r="18" ht="15" customHeight="1" s="244"/>
+    <row r="19" ht="15" customHeight="1" s="244">
+      <c r="A19" s="216" t="n"/>
+    </row>
+    <row r="20" ht="15" customHeight="1" s="244">
+      <c r="A20" s="311" t="inlineStr">
         <is>
           <t>I have/have not* obtained independent verification of all investments with the Trustees for Methodist Church Purposes or held in other trusts, bank balances and funds at the Central Finance Board of the Methodist Church which are individually in excess of £10,000 (ten thousand pounds) at the balance sheet date.</t>
         </is>
       </c>
     </row>
-    <row r="21" ht="15" customHeight="1" s="263"/>
-    <row r="22" ht="15" customHeight="1" s="263"/>
-    <row r="23" ht="15" customHeight="1" s="263"/>
-    <row r="24" ht="15" customHeight="1" s="263"/>
-    <row r="25" ht="15" customHeight="1" s="263">
-      <c r="A25" s="220" t="n"/>
-    </row>
-    <row r="26" ht="15" customHeight="1" s="263">
-      <c r="A26" s="220" t="n"/>
-    </row>
-    <row r="27" ht="15" customHeight="1" s="263">
-      <c r="A27" s="220" t="inlineStr">
+    <row r="21" ht="15" customHeight="1" s="244"/>
+    <row r="22" ht="15" customHeight="1" s="244"/>
+    <row r="23" ht="15" customHeight="1" s="244"/>
+    <row r="24" ht="15" customHeight="1" s="244"/>
+    <row r="25" ht="15" customHeight="1" s="244">
+      <c r="A25" s="216" t="n"/>
+    </row>
+    <row r="26" ht="15" customHeight="1" s="244">
+      <c r="A26" s="216" t="n"/>
+    </row>
+    <row r="27" ht="15" customHeight="1" s="244">
+      <c r="A27" s="216" t="inlineStr">
         <is>
           <t>Signature of independent examiner   ………………………………………………………………….</t>
         </is>
       </c>
     </row>
-    <row r="28" ht="15" customHeight="1" s="263">
-      <c r="A28" s="220" t="n"/>
-    </row>
-    <row r="29" ht="15" customHeight="1" s="263">
-      <c r="A29" s="220" t="inlineStr">
+    <row r="28" ht="15" customHeight="1" s="244">
+      <c r="A28" s="216" t="n"/>
+    </row>
+    <row r="29" ht="15" customHeight="1" s="244">
+      <c r="A29" s="216" t="inlineStr">
         <is>
           <t>Name of independent examiner  ……………………………………………………………………….</t>
         </is>
       </c>
     </row>
-    <row r="30" ht="15" customHeight="1" s="263">
-      <c r="A30" s="220" t="n"/>
-    </row>
-    <row r="31" ht="15" customHeight="1" s="263">
-      <c r="A31" s="220" t="inlineStr">
+    <row r="30" ht="15" customHeight="1" s="244">
+      <c r="A30" s="216" t="n"/>
+    </row>
+    <row r="31" ht="15" customHeight="1" s="244">
+      <c r="A31" s="216" t="inlineStr">
         <is>
           <t>Relevant professional qualification of independent examiner  ………………………………………</t>
         </is>
       </c>
     </row>
-    <row r="32" ht="15" customHeight="1" s="263">
-      <c r="A32" s="220" t="n"/>
-    </row>
-    <row r="33" ht="15" customHeight="1" s="263">
-      <c r="A33" s="220" t="n"/>
-    </row>
-    <row r="34" ht="15" customHeight="1" s="263">
-      <c r="A34" s="220" t="inlineStr">
+    <row r="32" ht="15" customHeight="1" s="244">
+      <c r="A32" s="216" t="n"/>
+    </row>
+    <row r="33" ht="15" customHeight="1" s="244">
+      <c r="A33" s="216" t="n"/>
+    </row>
+    <row r="34" ht="15" customHeight="1" s="244">
+      <c r="A34" s="216" t="inlineStr">
         <is>
           <t>Name of firm (where appropriate)  ………………………………………………………………………</t>
         </is>
       </c>
     </row>
-    <row r="35" ht="15" customHeight="1" s="263">
-      <c r="A35" s="220" t="n"/>
-    </row>
-    <row r="36" ht="15" customHeight="1" s="263">
-      <c r="A36" s="220" t="inlineStr">
+    <row r="35" ht="15" customHeight="1" s="244">
+      <c r="A35" s="216" t="n"/>
+    </row>
+    <row r="36" ht="15" customHeight="1" s="244">
+      <c r="A36" s="216" t="inlineStr">
         <is>
           <t>Address  ……………………………………………………………………………………………………</t>
         </is>
       </c>
     </row>
-    <row r="37" ht="15" customHeight="1" s="263">
-      <c r="A37" s="220" t="n"/>
-    </row>
-    <row r="38" ht="15" customHeight="1" s="263">
-      <c r="A38" s="220" t="inlineStr">
+    <row r="37" ht="15" customHeight="1" s="244">
+      <c r="A37" s="216" t="n"/>
+    </row>
+    <row r="38" ht="15" customHeight="1" s="244">
+      <c r="A38" s="216" t="inlineStr">
         <is>
           <t>………………………………………………………………………………..  Post Code  ………………</t>
         </is>
       </c>
     </row>
-    <row r="39" ht="15" customHeight="1" s="263">
-      <c r="A39" s="220" t="n"/>
-    </row>
-    <row r="40" ht="15" customHeight="1" s="263">
-      <c r="A40" s="220" t="inlineStr">
+    <row r="39" ht="15" customHeight="1" s="244">
+      <c r="A39" s="216" t="n"/>
+    </row>
+    <row r="40" ht="15" customHeight="1" s="244">
+      <c r="A40" s="216" t="inlineStr">
         <is>
           <t>Date  …………………………………………</t>
         </is>
       </c>
     </row>
-    <row r="41" ht="15" customHeight="1" s="263">
-      <c r="A41" s="220" t="n"/>
-    </row>
-    <row r="42" ht="15" customHeight="1" s="263">
-      <c r="A42" s="220" t="n"/>
-    </row>
-    <row r="43" ht="15" customHeight="1" s="263">
-      <c r="A43" s="220" t="n"/>
-    </row>
-    <row r="44" ht="15" customHeight="1" s="263">
-      <c r="A44" s="220" t="n"/>
-    </row>
-    <row r="45" ht="15" customHeight="1" s="263">
-      <c r="A45" s="220" t="inlineStr">
+    <row r="41" ht="15" customHeight="1" s="244">
+      <c r="A41" s="216" t="n"/>
+    </row>
+    <row r="42" ht="15" customHeight="1" s="244">
+      <c r="A42" s="216" t="n"/>
+    </row>
+    <row r="43" ht="15" customHeight="1" s="244">
+      <c r="A43" s="216" t="n"/>
+    </row>
+    <row r="44" ht="15" customHeight="1" s="244">
+      <c r="A44" s="216" t="n"/>
+    </row>
+    <row r="45" ht="15" customHeight="1" s="244">
+      <c r="A45" s="216" t="inlineStr">
         <is>
           <t>*  delete or circle as appropriate</t>
         </is>
       </c>
     </row>
-    <row r="46" ht="15" customHeight="1" s="263">
-      <c r="A46" s="220" t="n"/>
+    <row r="46" ht="15" customHeight="1" s="244">
+      <c r="A46" s="216" t="n"/>
     </row>
     <row r="47">
-      <c r="A47" s="229" t="inlineStr">
+      <c r="A47" s="225" t="inlineStr">
         <is>
           <t>Form Reviewed</t>
         </is>
       </c>
-      <c r="B47" s="230" t="n">
+      <c r="B47" s="226" t="n">
         <v>45505</v>
       </c>
     </row>
@@ -6290,26 +6344,26 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
   <cols>
-    <col width="19.42578125" customWidth="1" style="263" min="2" max="2"/>
+    <col width="19.42578125" customWidth="1" style="244" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="246" t="inlineStr">
+      <c r="A1" s="242" t="inlineStr">
         <is>
           <t>Unnamed: 0</t>
         </is>
       </c>
-      <c r="B1" s="246" t="inlineStr">
+      <c r="B1" s="242" t="inlineStr">
         <is>
           <t>Unnamed: 1</t>
         </is>
       </c>
-      <c r="C1" s="246" t="inlineStr">
+      <c r="C1" s="242" t="inlineStr">
         <is>
           <t>Unnamed: 2</t>
         </is>
       </c>
-      <c r="D1" s="246" t="inlineStr">
+      <c r="D1" s="242" t="inlineStr">
         <is>
           <t>Unnamed: 3</t>
         </is>

</xml_diff>

<commit_message>
New Donations page added and tested, P1 section A and B completed and working for accounting
</commit_message>
<xml_diff>
--- a/data/Church-receipts-and-payments-2025.xlsx
+++ b/data/Church-receipts-and-payments-2025.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-26745" yWindow="255" windowWidth="23775" windowHeight="13920" tabRatio="776" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-26640" yWindow="285" windowWidth="23775" windowHeight="13920" tabRatio="776" firstSheet="0" activeTab="4" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="P1 Front page" sheetId="1" state="visible" r:id="rId1"/>
@@ -11,7 +11,6 @@
     <sheet name="P3 Summ of Orgs" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Declaration and IE" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name=" IE Statement" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Data from streamlit" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_Hlk18748233" localSheetId="4">' IE Statement'!$A$5</definedName>
@@ -32,7 +31,7 @@
     <numFmt numFmtId="166" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="167" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="30">
+  <fonts count="29">
     <font>
       <name val="Arial"/>
       <sz val="10"/>
@@ -184,20 +183,15 @@
       <sz val="20"/>
     </font>
     <font>
-      <name val="Symbol"/>
-      <charset val="2"/>
-      <family val="1"/>
-      <sz val="12"/>
-    </font>
-    <font>
       <name val="Arial"/>
       <family val="2"/>
       <sz val="6"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <b val="1"/>
-      <sz val="10"/>
+      <name val="Wingdings 2"/>
+      <charset val="2"/>
+      <family val="1"/>
+      <sz val="14"/>
     </font>
   </fonts>
   <fills count="3">
@@ -214,7 +208,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="48">
+  <borders count="47">
     <border>
       <left/>
       <right/>
@@ -765,21 +759,6 @@
         <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -797,7 +776,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="352">
+  <cellXfs count="354">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -1259,14 +1238,11 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
     <xf numFmtId="49" fontId="16" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="17" fontId="28" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="17" fontId="27" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -1312,216 +1288,11 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="46" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="22" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="37" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="39" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="43" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="44" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="42" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="45" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="45" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <protection locked="0" hidden="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="43" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="11" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="11" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <protection locked="0" hidden="0"/>
     </xf>
     <xf numFmtId="2" fontId="16" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="2" fontId="17" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="13" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="2" fontId="9" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -1545,7 +1316,6 @@
     <xf numFmtId="2" fontId="16" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="2" fontId="16" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="2" fontId="16" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="2" fontId="4" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="2" fontId="9" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -1570,7 +1340,224 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
       <protection locked="0" hidden="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="39" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="37" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="22" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="45" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="2" fontId="17" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="43" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="44" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="42" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="43" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="45" applyAlignment="1" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" applyProtection="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <protection locked="0" hidden="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="167" fontId="22" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
@@ -2423,171 +2410,171 @@
   </sheetPr>
   <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+    <sheetView topLeftCell="A6" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24:L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
   <cols>
-    <col width="1" customWidth="1" style="244" min="1" max="1"/>
-    <col width="0.42578125" customWidth="1" style="244" min="2" max="2"/>
-    <col width="3.140625" customWidth="1" style="244" min="3" max="3"/>
-    <col width="3.42578125" customWidth="1" style="244" min="4" max="6"/>
-    <col width="30.140625" customWidth="1" style="244" min="7" max="7"/>
-    <col width="0.42578125" customWidth="1" style="244" min="8" max="8"/>
-    <col width="11.42578125" customWidth="1" style="244" min="9" max="9"/>
-    <col width="20" customWidth="1" style="244" min="10" max="10"/>
-    <col width="8.42578125" customWidth="1" style="244" min="11" max="11"/>
-    <col width="11.140625" customWidth="1" style="244" min="12" max="12"/>
-    <col width="2.42578125" customWidth="1" style="244" min="13" max="13"/>
-    <col width="0.85546875" customWidth="1" style="244" min="14" max="14"/>
+    <col width="1" customWidth="1" style="286" min="1" max="1"/>
+    <col width="0.42578125" customWidth="1" style="286" min="2" max="2"/>
+    <col width="3.140625" customWidth="1" style="286" min="3" max="3"/>
+    <col width="3.42578125" customWidth="1" style="286" min="4" max="6"/>
+    <col width="30.140625" customWidth="1" style="286" min="7" max="7"/>
+    <col width="0.42578125" customWidth="1" style="286" min="8" max="8"/>
+    <col width="11.42578125" customWidth="1" style="286" min="9" max="9"/>
+    <col width="20" customWidth="1" style="286" min="10" max="10"/>
+    <col width="8.42578125" customWidth="1" style="286" min="11" max="11"/>
+    <col width="11.140625" customWidth="1" style="286" min="12" max="12"/>
+    <col width="2.42578125" customWidth="1" style="286" min="13" max="13"/>
+    <col width="0.85546875" customWidth="1" style="286" min="14" max="14"/>
   </cols>
   <sheetData>
-    <row r="1" ht="6" customHeight="1" s="244">
-      <c r="B1" s="260" t="n"/>
-      <c r="C1" s="260" t="n"/>
-      <c r="D1" s="260" t="n"/>
-      <c r="E1" s="260" t="n"/>
-      <c r="F1" s="260" t="n"/>
-      <c r="G1" s="260" t="n"/>
-      <c r="H1" s="260" t="n"/>
-      <c r="I1" s="260" t="n"/>
-      <c r="J1" s="260" t="n"/>
-      <c r="K1" s="260" t="n"/>
-      <c r="L1" s="260" t="n"/>
-    </row>
-    <row r="2" ht="15.75" customHeight="1" s="244">
+    <row r="1" ht="6" customHeight="1" s="286">
+      <c r="B1" s="270" t="n"/>
+      <c r="C1" s="270" t="n"/>
+      <c r="D1" s="270" t="n"/>
+      <c r="E1" s="270" t="n"/>
+      <c r="F1" s="270" t="n"/>
+      <c r="G1" s="270" t="n"/>
+      <c r="H1" s="270" t="n"/>
+      <c r="I1" s="270" t="n"/>
+      <c r="J1" s="270" t="n"/>
+      <c r="K1" s="270" t="n"/>
+      <c r="L1" s="270" t="n"/>
+    </row>
+    <row r="2" ht="15.75" customHeight="1" s="286">
       <c r="A2" s="9" t="n"/>
-      <c r="B2" s="243" t="inlineStr">
+      <c r="B2" s="293" t="inlineStr">
         <is>
           <t>CHURCH</t>
         </is>
       </c>
       <c r="N2" s="29" t="n"/>
     </row>
-    <row r="3" ht="15.75" customHeight="1" s="244">
+    <row r="3" ht="15.75" customHeight="1" s="286">
       <c r="A3" s="9" t="n"/>
-      <c r="B3" s="243" t="inlineStr">
+      <c r="B3" s="293" t="inlineStr">
         <is>
           <t xml:space="preserve">        RECEIPTS AND PAYMENTS</t>
         </is>
       </c>
     </row>
-    <row r="4" ht="15.75" customHeight="1" s="244">
+    <row r="4" ht="15.75" customHeight="1" s="286">
       <c r="A4" s="9" t="n"/>
-      <c r="B4" s="243" t="inlineStr">
+      <c r="B4" s="293" t="inlineStr">
         <is>
           <t>ACCOUNTS</t>
         </is>
       </c>
     </row>
-    <row r="5" ht="6.75" customHeight="1" s="244">
+    <row r="5" ht="6.75" customHeight="1" s="286">
       <c r="A5" s="9" t="n"/>
-      <c r="B5" s="260" t="n"/>
-      <c r="C5" s="260" t="n"/>
-      <c r="D5" s="260" t="n"/>
-      <c r="E5" s="260" t="n"/>
-      <c r="F5" s="260" t="n"/>
-      <c r="G5" s="260" t="n"/>
-      <c r="H5" s="260" t="n"/>
-      <c r="I5" s="260" t="n"/>
-      <c r="J5" s="260" t="n"/>
-      <c r="K5" s="260" t="n"/>
-      <c r="L5" s="260" t="n"/>
-    </row>
-    <row r="6" ht="18.75" customHeight="1" s="244">
+      <c r="B5" s="270" t="n"/>
+      <c r="C5" s="270" t="n"/>
+      <c r="D5" s="270" t="n"/>
+      <c r="E5" s="270" t="n"/>
+      <c r="F5" s="270" t="n"/>
+      <c r="G5" s="270" t="n"/>
+      <c r="H5" s="270" t="n"/>
+      <c r="I5" s="270" t="n"/>
+      <c r="J5" s="270" t="n"/>
+      <c r="K5" s="270" t="n"/>
+      <c r="L5" s="270" t="n"/>
+    </row>
+    <row r="6" ht="18.75" customHeight="1" s="286">
       <c r="A6" s="9" t="n"/>
-      <c r="B6" s="246" t="inlineStr">
+      <c r="B6" s="294" t="inlineStr">
         <is>
           <t>THE METHODIST CHURCH</t>
         </is>
       </c>
     </row>
-    <row r="7" ht="9.75" customHeight="1" s="244">
+    <row r="7" ht="9.75" customHeight="1" s="286">
       <c r="A7" s="9" t="n"/>
-      <c r="B7" s="260" t="n"/>
-      <c r="C7" s="260" t="n"/>
-      <c r="D7" s="260" t="n"/>
-      <c r="E7" s="260" t="n"/>
-      <c r="F7" s="260" t="n"/>
-      <c r="G7" s="260" t="n"/>
-      <c r="H7" s="260" t="n"/>
-      <c r="I7" s="260" t="n"/>
-      <c r="J7" s="260" t="n"/>
-      <c r="K7" s="260" t="n"/>
-      <c r="L7" s="260" t="n"/>
-    </row>
-    <row r="8" ht="22.7" customFormat="1" customHeight="1" s="247">
+      <c r="B7" s="270" t="n"/>
+      <c r="C7" s="270" t="n"/>
+      <c r="D7" s="270" t="n"/>
+      <c r="E7" s="270" t="n"/>
+      <c r="F7" s="270" t="n"/>
+      <c r="G7" s="270" t="n"/>
+      <c r="H7" s="270" t="n"/>
+      <c r="I7" s="270" t="n"/>
+      <c r="J7" s="270" t="n"/>
+      <c r="K7" s="270" t="n"/>
+      <c r="L7" s="270" t="n"/>
+    </row>
+    <row r="8" ht="22.7" customFormat="1" customHeight="1" s="295">
       <c r="A8" s="23" t="n"/>
-      <c r="B8" s="246" t="inlineStr">
+      <c r="B8" s="294" t="inlineStr">
         <is>
           <t xml:space="preserve">STANDARD FORM OF ACCOUNTS </t>
         </is>
       </c>
     </row>
-    <row r="9" ht="7.5" customFormat="1" customHeight="1" s="247">
+    <row r="9" ht="7.5" customFormat="1" customHeight="1" s="295">
       <c r="A9" s="23" t="n"/>
-      <c r="B9" s="248" t="n"/>
-    </row>
-    <row r="10" ht="5.25" customHeight="1" s="244">
+      <c r="B9" s="296" t="n"/>
+    </row>
+    <row r="10" ht="5.25" customHeight="1" s="286">
       <c r="A10" s="9" t="n"/>
-      <c r="B10" s="260" t="n"/>
-      <c r="C10" s="260" t="n"/>
-      <c r="D10" s="260" t="n"/>
-      <c r="E10" s="260" t="n"/>
-      <c r="F10" s="260" t="n"/>
-      <c r="G10" s="260" t="n"/>
-      <c r="H10" s="260" t="n"/>
-      <c r="I10" s="260" t="n"/>
-      <c r="J10" s="260" t="n"/>
-      <c r="K10" s="260" t="n"/>
-      <c r="L10" s="260" t="n"/>
-    </row>
-    <row r="11" ht="30.2" customHeight="1" s="244">
+      <c r="B10" s="270" t="n"/>
+      <c r="C10" s="270" t="n"/>
+      <c r="D10" s="270" t="n"/>
+      <c r="E10" s="270" t="n"/>
+      <c r="F10" s="270" t="n"/>
+      <c r="G10" s="270" t="n"/>
+      <c r="H10" s="270" t="n"/>
+      <c r="I10" s="270" t="n"/>
+      <c r="J10" s="270" t="n"/>
+      <c r="K10" s="270" t="n"/>
+      <c r="L10" s="270" t="n"/>
+    </row>
+    <row r="11" ht="30.2" customHeight="1" s="286">
       <c r="A11" s="9" t="n"/>
       <c r="B11" s="35" t="n"/>
-      <c r="C11" s="249" t="inlineStr">
+      <c r="C11" s="297" t="inlineStr">
         <is>
           <t>Briggswath and Sleights Methodist</t>
         </is>
       </c>
-      <c r="D11" s="250" t="n"/>
-      <c r="E11" s="250" t="n"/>
-      <c r="F11" s="250" t="n"/>
-      <c r="G11" s="250" t="n"/>
-      <c r="H11" s="250" t="n"/>
-      <c r="I11" s="250" t="n"/>
-      <c r="J11" s="250" t="n"/>
-      <c r="K11" s="250" t="n"/>
-      <c r="L11" s="241" t="inlineStr">
+      <c r="D11" s="298" t="n"/>
+      <c r="E11" s="298" t="n"/>
+      <c r="F11" s="298" t="n"/>
+      <c r="G11" s="298" t="n"/>
+      <c r="H11" s="298" t="n"/>
+      <c r="I11" s="298" t="n"/>
+      <c r="J11" s="298" t="n"/>
+      <c r="K11" s="298" t="n"/>
+      <c r="L11" s="240" t="inlineStr">
         <is>
           <t>Church</t>
         </is>
       </c>
     </row>
-    <row r="12" ht="8.449999999999999" customHeight="1" s="244">
+    <row r="12" ht="8.449999999999999" customHeight="1" s="286">
       <c r="A12" s="9" t="n"/>
-      <c r="B12" s="260" t="n"/>
-      <c r="C12" s="260" t="n"/>
-      <c r="D12" s="260" t="n"/>
-      <c r="E12" s="260" t="n"/>
-      <c r="F12" s="260" t="n"/>
-      <c r="G12" s="260" t="n"/>
-      <c r="H12" s="260" t="n"/>
-      <c r="I12" s="260" t="n"/>
-      <c r="J12" s="260" t="n"/>
-      <c r="K12" s="260" t="n"/>
-      <c r="L12" s="260" t="n"/>
-    </row>
-    <row r="13" ht="20.25" customHeight="1" s="244">
+      <c r="B12" s="270" t="n"/>
+      <c r="C12" s="270" t="n"/>
+      <c r="D12" s="270" t="n"/>
+      <c r="E12" s="270" t="n"/>
+      <c r="F12" s="270" t="n"/>
+      <c r="G12" s="270" t="n"/>
+      <c r="H12" s="270" t="n"/>
+      <c r="I12" s="270" t="n"/>
+      <c r="J12" s="270" t="n"/>
+      <c r="K12" s="270" t="n"/>
+      <c r="L12" s="270" t="n"/>
+    </row>
+    <row r="13" ht="20.25" customHeight="1" s="286">
       <c r="A13" s="9" t="n"/>
-      <c r="B13" s="251" t="inlineStr">
+      <c r="B13" s="299" t="inlineStr">
         <is>
           <t xml:space="preserve">        FOR THE YEAR ENDED      </t>
         </is>
       </c>
     </row>
-    <row r="14" ht="8.449999999999999" customHeight="1" s="244">
+    <row r="14" ht="8.449999999999999" customHeight="1" s="286">
       <c r="A14" s="9" t="n"/>
       <c r="B14" s="36" t="n"/>
       <c r="C14" s="36" t="n"/>
@@ -2601,148 +2588,148 @@
       <c r="K14" s="36" t="n"/>
       <c r="L14" s="36" t="n"/>
     </row>
-    <row r="15" ht="20.25" customHeight="1" s="244">
+    <row r="15" ht="20.25" customHeight="1" s="286">
       <c r="A15" s="9" t="n"/>
-      <c r="B15" s="344" t="n">
+      <c r="B15" s="346" t="n">
         <v>45535</v>
       </c>
     </row>
-    <row r="16" ht="3.2" customHeight="1" s="244">
+    <row r="16" ht="3.2" customHeight="1" s="286">
       <c r="A16" s="9" t="n"/>
-      <c r="B16" s="260" t="n"/>
-      <c r="C16" s="260" t="n"/>
-      <c r="D16" s="260" t="n"/>
-      <c r="E16" s="260" t="n"/>
-      <c r="F16" s="260" t="n"/>
-      <c r="G16" s="260" t="n"/>
-      <c r="H16" s="260" t="n"/>
-      <c r="I16" s="260" t="n"/>
-      <c r="J16" s="260" t="n"/>
-      <c r="K16" s="260" t="n"/>
-      <c r="L16" s="260" t="n"/>
-    </row>
-    <row r="17" ht="30.2" customHeight="1" s="244">
+      <c r="B16" s="270" t="n"/>
+      <c r="C16" s="270" t="n"/>
+      <c r="D16" s="270" t="n"/>
+      <c r="E16" s="270" t="n"/>
+      <c r="F16" s="270" t="n"/>
+      <c r="G16" s="270" t="n"/>
+      <c r="H16" s="270" t="n"/>
+      <c r="I16" s="270" t="n"/>
+      <c r="J16" s="270" t="n"/>
+      <c r="K16" s="270" t="n"/>
+      <c r="L16" s="270" t="n"/>
+    </row>
+    <row r="17" ht="30.2" customHeight="1" s="286">
       <c r="A17" s="9" t="n"/>
-      <c r="B17" s="260" t="n"/>
-      <c r="C17" s="249" t="inlineStr">
+      <c r="B17" s="270" t="n"/>
+      <c r="C17" s="297" t="inlineStr">
         <is>
           <t>North Yorkshire Coast</t>
         </is>
       </c>
-      <c r="D17" s="250" t="n"/>
-      <c r="E17" s="250" t="n"/>
-      <c r="F17" s="250" t="n"/>
-      <c r="G17" s="250" t="n"/>
-      <c r="H17" s="239" t="n"/>
-      <c r="I17" s="240" t="inlineStr">
+      <c r="D17" s="298" t="n"/>
+      <c r="E17" s="298" t="n"/>
+      <c r="F17" s="298" t="n"/>
+      <c r="G17" s="298" t="n"/>
+      <c r="H17" s="238" t="n"/>
+      <c r="I17" s="239" t="inlineStr">
         <is>
           <t>Circuit</t>
         </is>
       </c>
-      <c r="J17" s="239" t="inlineStr">
+      <c r="J17" s="238" t="inlineStr">
         <is>
           <t>Circuit no.</t>
         </is>
       </c>
-      <c r="K17" s="252" t="inlineStr">
+      <c r="K17" s="300" t="inlineStr">
         <is>
           <t>29/31</t>
         </is>
       </c>
-      <c r="L17" s="253" t="n"/>
-    </row>
-    <row r="18" ht="6.75" customHeight="1" s="244">
+      <c r="L17" s="284" t="n"/>
+    </row>
+    <row r="18" ht="6.75" customHeight="1" s="286">
       <c r="A18" s="9" t="n"/>
-      <c r="B18" s="260" t="n"/>
-      <c r="C18" s="260" t="n"/>
-      <c r="D18" s="260" t="n"/>
-      <c r="E18" s="260" t="n"/>
-      <c r="F18" s="260" t="n"/>
-      <c r="G18" s="260" t="n"/>
-      <c r="H18" s="260" t="n"/>
+      <c r="B18" s="270" t="n"/>
+      <c r="C18" s="270" t="n"/>
+      <c r="D18" s="270" t="n"/>
+      <c r="E18" s="270" t="n"/>
+      <c r="F18" s="270" t="n"/>
+      <c r="G18" s="270" t="n"/>
+      <c r="H18" s="270" t="n"/>
       <c r="I18" s="171" t="n"/>
-      <c r="J18" s="260" t="n"/>
-      <c r="K18" s="260" t="n"/>
-      <c r="L18" s="260" t="n"/>
-    </row>
-    <row r="19" ht="26.45" customHeight="1" s="244">
+      <c r="J18" s="270" t="n"/>
+      <c r="K18" s="270" t="n"/>
+      <c r="L18" s="270" t="n"/>
+    </row>
+    <row r="19" ht="26.45" customHeight="1" s="286">
       <c r="A19" s="9" t="n"/>
-      <c r="B19" s="260" t="n"/>
-      <c r="C19" s="255" t="inlineStr">
+      <c r="B19" s="270" t="n"/>
+      <c r="C19" s="302" t="inlineStr">
         <is>
           <t>Registered Charity - Charity Registration number</t>
         </is>
       </c>
-      <c r="J19" s="260" t="n"/>
-      <c r="K19" s="257" t="n"/>
-      <c r="L19" s="253" t="n"/>
-    </row>
-    <row r="20" ht="7.5" customHeight="1" s="244">
+      <c r="J19" s="270" t="n"/>
+      <c r="K19" s="283" t="n"/>
+      <c r="L19" s="284" t="n"/>
+    </row>
+    <row r="20" ht="7.5" customHeight="1" s="286">
       <c r="A20" s="9" t="n"/>
-      <c r="B20" s="260" t="n"/>
-      <c r="C20" s="245" t="n"/>
-      <c r="K20" s="260" t="n"/>
-      <c r="L20" s="260" t="n"/>
-    </row>
-    <row r="21" ht="30.75" customFormat="1" customHeight="1" s="256">
+      <c r="B20" s="270" t="n"/>
+      <c r="C20" s="281" t="n"/>
+      <c r="K20" s="270" t="n"/>
+      <c r="L20" s="270" t="n"/>
+    </row>
+    <row r="21" ht="30.75" customFormat="1" customHeight="1" s="282">
       <c r="A21" s="24" t="n"/>
-      <c r="B21" s="245" t="n"/>
-      <c r="C21" s="245" t="inlineStr">
+      <c r="B21" s="281" t="n"/>
+      <c r="C21" s="281" t="inlineStr">
         <is>
           <t>If not a registered charity His Majesty's Revenue and Customs Gift Aid number</t>
         </is>
       </c>
       <c r="J21" s="209" t="n"/>
-      <c r="K21" s="258" t="inlineStr">
+      <c r="K21" s="285" t="inlineStr">
         <is>
           <t>X65308</t>
         </is>
       </c>
-      <c r="L21" s="253" t="n"/>
-    </row>
-    <row r="22" ht="72.75" customHeight="1" s="244">
+      <c r="L21" s="284" t="n"/>
+    </row>
+    <row r="22" ht="72.75" customHeight="1" s="286">
       <c r="A22" s="9" t="n"/>
-      <c r="B22" s="260" t="n"/>
-      <c r="C22" s="245" t="inlineStr">
+      <c r="B22" s="270" t="n"/>
+      <c r="C22" s="281" t="inlineStr">
         <is>
           <t>(The HMRC number is equivalent to a registered charity number in terms of evidence of charitable status and may be used to give to donors or grant funders wishing to see evidence of the organisation's charitable status.  Methodist charities in England and Wales that are not registered charities are excepted from registration under Statutory Instrument  2014  No.242)</t>
         </is>
       </c>
     </row>
-    <row r="23" ht="14.25" customFormat="1" customHeight="1" s="260">
+    <row r="23" ht="14.25" customFormat="1" customHeight="1" s="270">
       <c r="A23" s="208" t="n"/>
-      <c r="B23" s="259" t="inlineStr">
+      <c r="B23" s="269" t="inlineStr">
         <is>
           <t>Minister:</t>
         </is>
       </c>
     </row>
-    <row r="24" ht="30.2" customFormat="1" customHeight="1" s="260">
+    <row r="24" ht="30.2" customFormat="1" customHeight="1" s="270">
       <c r="A24" s="208" t="n"/>
-      <c r="C24" s="265" t="inlineStr">
+      <c r="C24" s="287" t="inlineStr">
         <is>
           <t>Gareth Phillips</t>
         </is>
       </c>
-      <c r="D24" s="266" t="n"/>
-      <c r="E24" s="266" t="n"/>
-      <c r="F24" s="266" t="n"/>
-      <c r="G24" s="266" t="n"/>
-      <c r="H24" s="266" t="n"/>
-      <c r="I24" s="266" t="n"/>
-      <c r="J24" s="266" t="n"/>
-      <c r="K24" s="266" t="n"/>
-      <c r="L24" s="253" t="n"/>
-    </row>
-    <row r="25" ht="23.25" customFormat="1" customHeight="1" s="260">
+      <c r="D24" s="288" t="n"/>
+      <c r="E24" s="288" t="n"/>
+      <c r="F24" s="288" t="n"/>
+      <c r="G24" s="288" t="n"/>
+      <c r="H24" s="288" t="n"/>
+      <c r="I24" s="288" t="n"/>
+      <c r="J24" s="288" t="n"/>
+      <c r="K24" s="288" t="n"/>
+      <c r="L24" s="284" t="n"/>
+    </row>
+    <row r="25" ht="23.25" customFormat="1" customHeight="1" s="270">
       <c r="A25" s="208" t="n"/>
-      <c r="B25" s="259" t="inlineStr">
+      <c r="B25" s="269" t="inlineStr">
         <is>
           <t>Church Stewards:</t>
         </is>
       </c>
     </row>
-    <row r="26" ht="30.2" customFormat="1" customHeight="1" s="260">
+    <row r="26" ht="30.2" customFormat="1" customHeight="1" s="270">
       <c r="A26" s="208" t="n"/>
       <c r="C26" s="274" t="inlineStr">
         <is>
@@ -2763,98 +2750,98 @@
       <c r="K26" s="272" t="n"/>
       <c r="L26" s="273" t="n"/>
     </row>
-    <row r="27" ht="30.2" customFormat="1" customHeight="1" s="260">
+    <row r="27" ht="30.2" customFormat="1" customHeight="1" s="270">
       <c r="A27" s="208" t="n"/>
-      <c r="C27" s="276" t="inlineStr">
+      <c r="C27" s="280" t="inlineStr">
         <is>
           <t>Peter Brown</t>
         </is>
       </c>
-      <c r="D27" s="262" t="n"/>
-      <c r="E27" s="262" t="n"/>
-      <c r="F27" s="262" t="n"/>
-      <c r="G27" s="262" t="n"/>
-      <c r="H27" s="262" t="n"/>
-      <c r="I27" s="275" t="inlineStr">
+      <c r="D27" s="276" t="n"/>
+      <c r="E27" s="276" t="n"/>
+      <c r="F27" s="276" t="n"/>
+      <c r="G27" s="276" t="n"/>
+      <c r="H27" s="276" t="n"/>
+      <c r="I27" s="277" t="inlineStr">
         <is>
           <t>Sally Wardell</t>
         </is>
       </c>
-      <c r="J27" s="262" t="n"/>
-      <c r="K27" s="262" t="n"/>
-      <c r="L27" s="263" t="n"/>
-    </row>
-    <row r="28" ht="30.2" customFormat="1" customHeight="1" s="260">
+      <c r="J27" s="276" t="n"/>
+      <c r="K27" s="276" t="n"/>
+      <c r="L27" s="278" t="n"/>
+    </row>
+    <row r="28" ht="30.2" customFormat="1" customHeight="1" s="270">
       <c r="A28" s="208" t="n"/>
       <c r="B28" s="34" t="n"/>
-      <c r="C28" s="264" t="n"/>
-      <c r="D28" s="262" t="n"/>
-      <c r="E28" s="262" t="n"/>
-      <c r="F28" s="262" t="n"/>
-      <c r="G28" s="262" t="n"/>
-      <c r="H28" s="262" t="n"/>
-      <c r="I28" s="261" t="n"/>
-      <c r="J28" s="262" t="n"/>
-      <c r="K28" s="262" t="n"/>
-      <c r="L28" s="263" t="n"/>
-    </row>
-    <row r="29" ht="30.2" customFormat="1" customHeight="1" s="260">
+      <c r="C28" s="275" t="n"/>
+      <c r="D28" s="276" t="n"/>
+      <c r="E28" s="276" t="n"/>
+      <c r="F28" s="276" t="n"/>
+      <c r="G28" s="276" t="n"/>
+      <c r="H28" s="276" t="n"/>
+      <c r="I28" s="279" t="n"/>
+      <c r="J28" s="276" t="n"/>
+      <c r="K28" s="276" t="n"/>
+      <c r="L28" s="278" t="n"/>
+    </row>
+    <row r="29" ht="30.2" customFormat="1" customHeight="1" s="270">
       <c r="A29" s="208" t="n"/>
       <c r="B29" s="34" t="n"/>
-      <c r="C29" s="264" t="n"/>
-      <c r="D29" s="262" t="n"/>
-      <c r="E29" s="262" t="n"/>
-      <c r="F29" s="262" t="n"/>
-      <c r="G29" s="262" t="n"/>
-      <c r="H29" s="262" t="n"/>
-      <c r="I29" s="261" t="n"/>
-      <c r="J29" s="262" t="n"/>
-      <c r="K29" s="262" t="n"/>
-      <c r="L29" s="263" t="n"/>
-    </row>
-    <row r="30" ht="30.2" customFormat="1" customHeight="1" s="260">
+      <c r="C29" s="275" t="n"/>
+      <c r="D29" s="276" t="n"/>
+      <c r="E29" s="276" t="n"/>
+      <c r="F29" s="276" t="n"/>
+      <c r="G29" s="276" t="n"/>
+      <c r="H29" s="276" t="n"/>
+      <c r="I29" s="279" t="n"/>
+      <c r="J29" s="276" t="n"/>
+      <c r="K29" s="276" t="n"/>
+      <c r="L29" s="278" t="n"/>
+    </row>
+    <row r="30" ht="30.2" customFormat="1" customHeight="1" s="270">
       <c r="A30" s="208" t="n"/>
       <c r="B30" s="34" t="n"/>
-      <c r="C30" s="264" t="n"/>
-      <c r="D30" s="262" t="n"/>
-      <c r="E30" s="262" t="n"/>
-      <c r="F30" s="262" t="n"/>
-      <c r="G30" s="262" t="n"/>
-      <c r="H30" s="262" t="n"/>
-      <c r="I30" s="261" t="n"/>
-      <c r="J30" s="262" t="n"/>
-      <c r="K30" s="262" t="n"/>
-      <c r="L30" s="263" t="n"/>
-    </row>
-    <row r="31" ht="30.2" customFormat="1" customHeight="1" s="260">
+      <c r="C30" s="275" t="n"/>
+      <c r="D30" s="276" t="n"/>
+      <c r="E30" s="276" t="n"/>
+      <c r="F30" s="276" t="n"/>
+      <c r="G30" s="276" t="n"/>
+      <c r="H30" s="276" t="n"/>
+      <c r="I30" s="279" t="n"/>
+      <c r="J30" s="276" t="n"/>
+      <c r="K30" s="276" t="n"/>
+      <c r="L30" s="278" t="n"/>
+    </row>
+    <row r="31" ht="30.2" customFormat="1" customHeight="1" s="270">
       <c r="A31" s="208" t="n"/>
       <c r="B31" s="34" t="n"/>
-      <c r="C31" s="264" t="n"/>
-      <c r="D31" s="262" t="n"/>
-      <c r="E31" s="262" t="n"/>
-      <c r="F31" s="262" t="n"/>
-      <c r="G31" s="262" t="n"/>
-      <c r="H31" s="262" t="n"/>
-      <c r="I31" s="261" t="n"/>
-      <c r="J31" s="262" t="n"/>
-      <c r="K31" s="262" t="n"/>
-      <c r="L31" s="263" t="n"/>
-    </row>
-    <row r="32" ht="30.2" customFormat="1" customHeight="1" s="260">
+      <c r="C31" s="275" t="n"/>
+      <c r="D31" s="276" t="n"/>
+      <c r="E31" s="276" t="n"/>
+      <c r="F31" s="276" t="n"/>
+      <c r="G31" s="276" t="n"/>
+      <c r="H31" s="276" t="n"/>
+      <c r="I31" s="279" t="n"/>
+      <c r="J31" s="276" t="n"/>
+      <c r="K31" s="276" t="n"/>
+      <c r="L31" s="278" t="n"/>
+    </row>
+    <row r="32" ht="30.2" customFormat="1" customHeight="1" s="270">
       <c r="A32" s="208" t="n"/>
       <c r="B32" s="34" t="n"/>
-      <c r="C32" s="270" t="n"/>
-      <c r="D32" s="268" t="n"/>
-      <c r="E32" s="268" t="n"/>
-      <c r="F32" s="268" t="n"/>
-      <c r="G32" s="268" t="n"/>
-      <c r="H32" s="268" t="n"/>
-      <c r="I32" s="267" t="n"/>
-      <c r="J32" s="268" t="n"/>
-      <c r="K32" s="268" t="n"/>
-      <c r="L32" s="269" t="n"/>
-    </row>
-    <row r="33" ht="9" customFormat="1" customHeight="1" s="260">
+      <c r="C32" s="292" t="n"/>
+      <c r="D32" s="290" t="n"/>
+      <c r="E32" s="290" t="n"/>
+      <c r="F32" s="290" t="n"/>
+      <c r="G32" s="290" t="n"/>
+      <c r="H32" s="290" t="n"/>
+      <c r="I32" s="289" t="n"/>
+      <c r="J32" s="290" t="n"/>
+      <c r="K32" s="290" t="n"/>
+      <c r="L32" s="291" t="n"/>
+    </row>
+    <row r="33" ht="9" customFormat="1" customHeight="1" s="270">
       <c r="A33" s="208" t="n"/>
       <c r="B33" s="34" t="n"/>
       <c r="C33" s="34" t="n"/>
@@ -2868,7 +2855,7 @@
       <c r="K33" s="34" t="n"/>
       <c r="L33" s="34" t="n"/>
     </row>
-    <row r="34" hidden="1" ht="3.75" customFormat="1" customHeight="1" s="260">
+    <row r="34" hidden="1" ht="3.75" customFormat="1" customHeight="1" s="270">
       <c r="A34" s="208" t="n"/>
       <c r="B34" s="34" t="n"/>
       <c r="C34" s="34" t="n"/>
@@ -2882,47 +2869,52 @@
       <c r="K34" s="34" t="n"/>
       <c r="L34" s="34" t="n"/>
     </row>
-    <row r="35" ht="14.25" customFormat="1" customHeight="1" s="260">
+    <row r="35" ht="14.25" customFormat="1" customHeight="1" s="270">
       <c r="A35" s="208" t="n"/>
-      <c r="B35" s="259" t="inlineStr">
+      <c r="B35" s="269" t="inlineStr">
         <is>
           <t>Treasurer:</t>
         </is>
       </c>
     </row>
-    <row r="36" ht="30.2" customFormat="1" customHeight="1" s="260">
+    <row r="36" ht="30.2" customFormat="1" customHeight="1" s="270">
       <c r="A36" s="208" t="n"/>
       <c r="B36" s="34" t="n"/>
-      <c r="C36" s="265" t="inlineStr">
+      <c r="C36" s="287" t="inlineStr">
         <is>
           <t>Ann Brown</t>
         </is>
       </c>
-      <c r="D36" s="266" t="n"/>
-      <c r="E36" s="266" t="n"/>
-      <c r="F36" s="266" t="n"/>
-      <c r="G36" s="266" t="n"/>
-      <c r="H36" s="266" t="n"/>
-      <c r="I36" s="266" t="n"/>
-      <c r="J36" s="266" t="n"/>
-      <c r="K36" s="266" t="n"/>
-      <c r="L36" s="253" t="n"/>
-    </row>
-    <row r="37" ht="6" customHeight="1" s="244">
+      <c r="D36" s="288" t="n"/>
+      <c r="E36" s="288" t="n"/>
+      <c r="F36" s="288" t="n"/>
+      <c r="G36" s="288" t="n"/>
+      <c r="H36" s="288" t="n"/>
+      <c r="I36" s="288" t="n"/>
+      <c r="J36" s="288" t="n"/>
+      <c r="K36" s="288" t="n"/>
+      <c r="L36" s="284" t="n"/>
+    </row>
+    <row r="37" ht="6" customHeight="1" s="286">
       <c r="A37" s="9" t="n"/>
     </row>
-    <row r="38" ht="6" customHeight="1" s="244"/>
+    <row r="38" ht="6" customHeight="1" s="286"/>
     <row r="40"/>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="B25:L25"/>
-    <mergeCell ref="B23:L23"/>
-    <mergeCell ref="I26:L26"/>
-    <mergeCell ref="C26:H26"/>
-    <mergeCell ref="C28:H28"/>
-    <mergeCell ref="I27:L27"/>
-    <mergeCell ref="I28:L28"/>
-    <mergeCell ref="C27:H27"/>
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="C20:J20"/>
+    <mergeCell ref="B3:L3"/>
+    <mergeCell ref="B4:L4"/>
+    <mergeCell ref="B6:L6"/>
+    <mergeCell ref="B8:L8"/>
+    <mergeCell ref="B9:L9"/>
+    <mergeCell ref="C11:K11"/>
+    <mergeCell ref="B13:L13"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="B15:L15"/>
+    <mergeCell ref="C17:G17"/>
+    <mergeCell ref="C19:I19"/>
     <mergeCell ref="C21:I21"/>
     <mergeCell ref="K19:L19"/>
     <mergeCell ref="K21:L21"/>
@@ -2939,19 +2931,14 @@
     <mergeCell ref="I29:L29"/>
     <mergeCell ref="C22:L22"/>
     <mergeCell ref="C24:L24"/>
-    <mergeCell ref="B2:L2"/>
-    <mergeCell ref="C20:J20"/>
-    <mergeCell ref="B3:L3"/>
-    <mergeCell ref="B4:L4"/>
-    <mergeCell ref="B6:L6"/>
-    <mergeCell ref="B8:L8"/>
-    <mergeCell ref="B9:L9"/>
-    <mergeCell ref="C11:K11"/>
-    <mergeCell ref="B13:L13"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="B15:L15"/>
-    <mergeCell ref="C17:G17"/>
-    <mergeCell ref="C19:I19"/>
+    <mergeCell ref="B25:L25"/>
+    <mergeCell ref="B23:L23"/>
+    <mergeCell ref="I26:L26"/>
+    <mergeCell ref="C26:H26"/>
+    <mergeCell ref="C28:H28"/>
+    <mergeCell ref="I27:L27"/>
+    <mergeCell ref="I28:L28"/>
+    <mergeCell ref="C27:H27"/>
   </mergeCells>
   <pageMargins left="0.3937007874015748" right="0.2362204724409449" top="0.3937007874015748" bottom="0.3937007874015748" header="0.2362204724409449" footer="0.1574803149606299"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -2975,8 +2962,8 @@
   </sheetPr>
   <dimension ref="B1:R42"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
+    <sheetView showZeros="0" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="6" ySplit="5" topLeftCell="G26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
       <selection pane="bottomRight" activeCell="J7" sqref="J7:J10"/>
@@ -2984,39 +2971,39 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
   <cols>
-    <col width="1.42578125" customWidth="1" style="292" min="1" max="1"/>
-    <col width="0.5703125" customWidth="1" style="292" min="2" max="2"/>
-    <col width="3" bestFit="1" customWidth="1" style="292" min="3" max="3"/>
-    <col width="28.140625" customWidth="1" style="292" min="4" max="4"/>
-    <col width="6" customWidth="1" style="292" min="5" max="5"/>
-    <col width="14" customWidth="1" style="292" min="6" max="6"/>
-    <col width="11.42578125" customWidth="1" style="330" min="7" max="7"/>
-    <col width="10" customWidth="1" style="292" min="8" max="8"/>
-    <col width="0.85546875" customWidth="1" style="292" min="9" max="9"/>
-    <col width="10" customWidth="1" style="330" min="10" max="10"/>
-    <col width="4.85546875" bestFit="1" customWidth="1" style="292" min="11" max="11"/>
-    <col width="0.85546875" customWidth="1" style="292" min="12" max="12"/>
-    <col width="10" customWidth="1" style="292" min="13" max="13"/>
-    <col width="5.42578125" customWidth="1" style="292" min="14" max="14"/>
-    <col width="1" customWidth="1" style="292" min="15" max="15"/>
-    <col width="0.5703125" customWidth="1" style="292" min="16" max="16"/>
-    <col width="10" customWidth="1" style="292" min="17" max="17"/>
-    <col width="6.42578125" customWidth="1" style="292" min="18" max="18"/>
-    <col width="17.5703125" customWidth="1" style="292" min="19" max="19"/>
-    <col width="9.140625" customWidth="1" style="292" min="20" max="33"/>
-    <col width="9.140625" customWidth="1" style="292" min="34" max="16384"/>
+    <col width="1.42578125" customWidth="1" style="311" min="1" max="1"/>
+    <col width="0.5703125" customWidth="1" style="311" min="2" max="2"/>
+    <col width="3" bestFit="1" customWidth="1" style="311" min="3" max="3"/>
+    <col width="28.140625" customWidth="1" style="311" min="4" max="4"/>
+    <col width="6" customWidth="1" style="311" min="5" max="5"/>
+    <col width="14" customWidth="1" style="311" min="6" max="6"/>
+    <col width="11.42578125" customWidth="1" style="312" min="7" max="7"/>
+    <col width="10" customWidth="1" style="311" min="8" max="8"/>
+    <col width="0.85546875" customWidth="1" style="311" min="9" max="9"/>
+    <col width="10" customWidth="1" style="312" min="10" max="10"/>
+    <col width="4.85546875" bestFit="1" customWidth="1" style="311" min="11" max="11"/>
+    <col width="0.85546875" customWidth="1" style="311" min="12" max="12"/>
+    <col width="10" customWidth="1" style="311" min="13" max="13"/>
+    <col width="5.42578125" customWidth="1" style="311" min="14" max="14"/>
+    <col width="1" customWidth="1" style="311" min="15" max="15"/>
+    <col width="0.5703125" customWidth="1" style="311" min="16" max="16"/>
+    <col width="10" customWidth="1" style="311" min="17" max="17"/>
+    <col width="6.42578125" customWidth="1" style="311" min="18" max="18"/>
+    <col width="17.5703125" customWidth="1" style="311" min="19" max="19"/>
+    <col width="9.140625" customWidth="1" style="311" min="20" max="34"/>
+    <col width="9.140625" customWidth="1" style="311" min="35" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" ht="7.5" customHeight="1" s="244">
+    <row r="1" ht="7.5" customHeight="1" s="286">
       <c r="B1" s="8" t="n"/>
       <c r="C1" s="37" t="n"/>
       <c r="D1" s="37" t="n"/>
       <c r="E1" s="37" t="n"/>
       <c r="F1" s="37" t="n"/>
-      <c r="G1" s="315" t="n"/>
+      <c r="G1" s="243" t="n"/>
       <c r="H1" s="37" t="n"/>
       <c r="I1" s="37" t="n"/>
-      <c r="J1" s="315" t="n"/>
+      <c r="J1" s="243" t="n"/>
       <c r="K1" s="37" t="n"/>
       <c r="L1" s="37" t="n"/>
       <c r="M1" s="37" t="n"/>
@@ -3024,27 +3011,27 @@
       <c r="O1" s="8" t="n"/>
       <c r="P1" s="8" t="n"/>
     </row>
-    <row r="2" ht="37.5" customHeight="1" s="244">
+    <row r="2" ht="37.5" customHeight="1" s="286">
       <c r="B2" s="8" t="n"/>
-      <c r="C2" s="291" t="inlineStr">
+      <c r="C2" s="310" t="inlineStr">
         <is>
           <t>ACCOUNTS FOR THE YEAR ENDED 31 AUGUST 2024</t>
         </is>
       </c>
-      <c r="H2" s="295">
+      <c r="H2" s="316">
         <f>'P1 Front page'!$C$11</f>
         <v/>
       </c>
-      <c r="I2" s="250" t="n"/>
-      <c r="J2" s="250" t="n"/>
-      <c r="K2" s="250" t="n"/>
-      <c r="L2" s="250" t="n"/>
-      <c r="M2" s="285" t="inlineStr">
+      <c r="I2" s="298" t="n"/>
+      <c r="J2" s="298" t="n"/>
+      <c r="K2" s="298" t="n"/>
+      <c r="L2" s="298" t="n"/>
+      <c r="M2" s="303" t="inlineStr">
         <is>
           <t>Church</t>
         </is>
       </c>
-      <c r="N2" s="282" t="n"/>
+      <c r="N2" s="304" t="n"/>
       <c r="O2" s="19" t="n"/>
       <c r="P2" s="8" t="n"/>
       <c r="Q2" s="11" t="inlineStr">
@@ -3053,31 +3040,31 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="7.5" customFormat="1" customHeight="1" s="294">
+    <row r="3" ht="7.5" customFormat="1" customHeight="1" s="314">
       <c r="B3" s="131" t="n"/>
       <c r="C3" s="132" t="n"/>
       <c r="D3" s="132" t="n"/>
       <c r="E3" s="132" t="n"/>
       <c r="F3" s="132" t="n"/>
-      <c r="G3" s="316" t="inlineStr">
+      <c r="G3" s="313" t="inlineStr">
         <is>
           <t>Unrestricted Funds</t>
         </is>
       </c>
-      <c r="H3" s="293" t="inlineStr">
+      <c r="H3" s="315" t="inlineStr">
         <is>
           <t>Restricted Funds</t>
         </is>
       </c>
       <c r="I3" s="172" t="n"/>
-      <c r="J3" s="316" t="inlineStr">
+      <c r="J3" s="313" t="inlineStr">
         <is>
           <t>Totals this year</t>
         </is>
       </c>
-      <c r="K3" s="293" t="n"/>
-      <c r="L3" s="293" t="n"/>
-      <c r="M3" s="293" t="inlineStr">
+      <c r="K3" s="315" t="n"/>
+      <c r="L3" s="315" t="n"/>
+      <c r="M3" s="315" t="inlineStr">
         <is>
           <t>Totals last year</t>
         </is>
@@ -3086,7 +3073,7 @@
       <c r="O3" s="4" t="n"/>
       <c r="P3" s="131" t="n"/>
     </row>
-    <row r="4" ht="23.25" customFormat="1" customHeight="1" s="294">
+    <row r="4" ht="23.25" customFormat="1" customHeight="1" s="314">
       <c r="B4" s="131" t="n"/>
       <c r="C4" s="132" t="n"/>
       <c r="D4" s="136" t="inlineStr">
@@ -3097,19 +3084,19 @@
       <c r="E4" s="132" t="n"/>
       <c r="F4" s="132" t="n"/>
       <c r="I4" s="172" t="n"/>
-      <c r="K4" s="293" t="n"/>
-      <c r="L4" s="293" t="n"/>
+      <c r="K4" s="315" t="n"/>
+      <c r="L4" s="315" t="n"/>
       <c r="N4" s="39" t="n"/>
       <c r="O4" s="4" t="n"/>
       <c r="P4" s="131" t="n"/>
     </row>
-    <row r="5" ht="23.25" customFormat="1" customHeight="1" s="294">
+    <row r="5" ht="23.25" customFormat="1" customHeight="1" s="314">
       <c r="B5" s="131" t="n"/>
       <c r="C5" s="40" t="n"/>
       <c r="D5" s="137" t="n"/>
       <c r="E5" s="138" t="n"/>
       <c r="F5" s="139" t="n"/>
-      <c r="G5" s="318" t="inlineStr">
+      <c r="G5" s="245" t="inlineStr">
         <is>
           <t>£</t>
         </is>
@@ -3120,7 +3107,7 @@
         </is>
       </c>
       <c r="I5" s="41" t="n"/>
-      <c r="J5" s="318" t="inlineStr">
+      <c r="J5" s="245" t="inlineStr">
         <is>
           <t>£</t>
         </is>
@@ -3136,7 +3123,7 @@
       <c r="O5" s="4" t="n"/>
       <c r="P5" s="131" t="n"/>
     </row>
-    <row r="6" ht="18.75" customHeight="1" s="244">
+    <row r="6" ht="18.75" customHeight="1" s="286">
       <c r="B6" s="8" t="n"/>
       <c r="C6" s="40" t="inlineStr">
         <is>
@@ -3154,10 +3141,10 @@
           <t>Note</t>
         </is>
       </c>
-      <c r="G6" s="318" t="n"/>
+      <c r="G6" s="245" t="n"/>
       <c r="H6" s="139" t="n"/>
       <c r="I6" s="41" t="n"/>
-      <c r="J6" s="318" t="n"/>
+      <c r="J6" s="245" t="n"/>
       <c r="K6" s="140" t="n"/>
       <c r="L6" s="140" t="n"/>
       <c r="M6" s="139" t="n"/>
@@ -3165,7 +3152,7 @@
       <c r="O6" s="14" t="n"/>
       <c r="P6" s="8" t="n"/>
     </row>
-    <row r="7" ht="18.75" customHeight="1" s="244">
+    <row r="7" ht="18.75" customHeight="1" s="286">
       <c r="B7" s="8" t="n"/>
       <c r="C7" s="40" t="inlineStr">
         <is>
@@ -3179,12 +3166,12 @@
       </c>
       <c r="E7" s="42" t="n"/>
       <c r="F7" s="43" t="n"/>
-      <c r="G7" s="342" t="n">
+      <c r="G7" s="268" t="n">
         <v>3553.8</v>
       </c>
       <c r="H7" s="141" t="n"/>
       <c r="I7" s="38" t="n"/>
-      <c r="J7" s="343" t="n">
+      <c r="J7" s="212" t="n">
         <v>3553.8</v>
       </c>
       <c r="K7" s="134" t="n"/>
@@ -3193,7 +3180,7 @@
       <c r="N7" s="38" t="n"/>
       <c r="P7" s="8" t="n"/>
     </row>
-    <row r="8" ht="27" customHeight="1" s="244">
+    <row r="8" ht="27" customHeight="1" s="286">
       <c r="B8" s="8" t="n"/>
       <c r="C8" s="40" t="inlineStr">
         <is>
@@ -3207,12 +3194,12 @@
       </c>
       <c r="E8" s="42" t="n"/>
       <c r="F8" s="43" t="n"/>
-      <c r="G8" s="342" t="n">
+      <c r="G8" s="268" t="n">
         <v>4480</v>
       </c>
       <c r="H8" s="141" t="n"/>
       <c r="I8" s="38" t="n"/>
-      <c r="J8" s="343" t="n">
+      <c r="J8" s="212" t="n">
         <v>4480</v>
       </c>
       <c r="K8" s="134" t="n"/>
@@ -3221,7 +3208,7 @@
       <c r="N8" s="38" t="n"/>
       <c r="P8" s="8" t="n"/>
     </row>
-    <row r="9" ht="18" customHeight="1" s="244">
+    <row r="9" ht="18" customHeight="1" s="286">
       <c r="B9" s="8" t="n"/>
       <c r="C9" s="40" t="inlineStr">
         <is>
@@ -3235,12 +3222,12 @@
       </c>
       <c r="E9" s="42" t="n"/>
       <c r="F9" s="43" t="n"/>
-      <c r="G9" s="342" t="n">
+      <c r="G9" s="268" t="n">
         <v>8401.9</v>
       </c>
       <c r="H9" s="141" t="n"/>
       <c r="I9" s="38" t="n"/>
-      <c r="J9" s="343" t="n">
+      <c r="J9" s="212" t="n">
         <v>8401.9</v>
       </c>
       <c r="K9" s="134" t="n"/>
@@ -3249,7 +3236,7 @@
       <c r="N9" s="38" t="n"/>
       <c r="P9" s="8" t="n"/>
     </row>
-    <row r="10" ht="18.75" customHeight="1" s="244" thickBot="1">
+    <row r="10" ht="18.75" customHeight="1" s="286" thickBot="1">
       <c r="B10" s="8" t="n"/>
       <c r="C10" s="40" t="inlineStr">
         <is>
@@ -3263,12 +3250,12 @@
       </c>
       <c r="E10" s="42" t="n"/>
       <c r="F10" s="43" t="n"/>
-      <c r="G10" s="314" t="n">
+      <c r="G10" s="242" t="n">
         <v>450</v>
       </c>
       <c r="H10" s="142" t="n"/>
       <c r="I10" s="38" t="n"/>
-      <c r="J10" s="313" t="n">
+      <c r="J10" s="241" t="n">
         <v>450</v>
       </c>
       <c r="K10" s="134" t="n"/>
@@ -3277,7 +3264,7 @@
       <c r="N10" s="38" t="n"/>
       <c r="P10" s="8" t="n"/>
     </row>
-    <row r="11" ht="17.45" customHeight="1" s="244" thickBot="1">
+    <row r="11" ht="17.45" customHeight="1" s="286" thickBot="1">
       <c r="B11" s="8" t="n"/>
       <c r="C11" s="40" t="inlineStr">
         <is>
@@ -3291,7 +3278,7 @@
       </c>
       <c r="E11" s="145" t="n"/>
       <c r="F11" s="146" t="n"/>
-      <c r="G11" s="321">
+      <c r="G11" s="248">
         <f>SUM(G7:G10)</f>
         <v/>
       </c>
@@ -3300,7 +3287,7 @@
         <v/>
       </c>
       <c r="I11" s="148" t="n"/>
-      <c r="J11" s="333">
+      <c r="J11" s="259">
         <f>SUM(J7:J10)</f>
         <v/>
       </c>
@@ -3318,23 +3305,23 @@
       <c r="O11" s="6" t="n"/>
       <c r="P11" s="8" t="n"/>
     </row>
-    <row r="12" ht="8.449999999999999" customHeight="1" s="244">
+    <row r="12" ht="8.449999999999999" customHeight="1" s="286">
       <c r="B12" s="8" t="n"/>
       <c r="C12" s="38" t="n"/>
       <c r="D12" s="38" t="n"/>
       <c r="E12" s="38" t="n"/>
       <c r="F12" s="41" t="n"/>
-      <c r="G12" s="322" t="n"/>
+      <c r="G12" s="249" t="n"/>
       <c r="H12" s="38" t="n"/>
       <c r="I12" s="38" t="n"/>
-      <c r="J12" s="334" t="n"/>
+      <c r="J12" s="260" t="n"/>
       <c r="K12" s="46" t="n"/>
       <c r="L12" s="46" t="n"/>
       <c r="M12" s="38" t="n"/>
       <c r="N12" s="38" t="n"/>
       <c r="P12" s="8" t="n"/>
     </row>
-    <row r="13" ht="18.75" customHeight="1" s="244">
+    <row r="13" ht="18.75" customHeight="1" s="286">
       <c r="B13" s="8" t="n"/>
       <c r="C13" s="38" t="n"/>
       <c r="D13" s="136" t="inlineStr">
@@ -3344,17 +3331,17 @@
       </c>
       <c r="E13" s="38" t="n"/>
       <c r="F13" s="41" t="n"/>
-      <c r="G13" s="322" t="n"/>
+      <c r="G13" s="249" t="n"/>
       <c r="H13" s="38" t="n"/>
       <c r="I13" s="38" t="n"/>
-      <c r="J13" s="334" t="n"/>
+      <c r="J13" s="260" t="n"/>
       <c r="K13" s="46" t="n"/>
       <c r="L13" s="46" t="n"/>
       <c r="M13" s="38" t="n"/>
       <c r="N13" s="38" t="n"/>
       <c r="P13" s="8" t="n"/>
     </row>
-    <row r="14" ht="18.75" customHeight="1" s="244">
+    <row r="14" ht="18.75" customHeight="1" s="286">
       <c r="B14" s="8" t="n"/>
       <c r="C14" s="40" t="inlineStr">
         <is>
@@ -3368,17 +3355,17 @@
       </c>
       <c r="E14" s="138" t="n"/>
       <c r="F14" s="41" t="n"/>
-      <c r="G14" s="322" t="n"/>
+      <c r="G14" s="249" t="n"/>
       <c r="H14" s="38" t="n"/>
       <c r="I14" s="38" t="n"/>
-      <c r="J14" s="322" t="n"/>
+      <c r="J14" s="249" t="n"/>
       <c r="K14" s="38" t="n"/>
       <c r="L14" s="38" t="n"/>
       <c r="M14" s="38" t="n"/>
       <c r="N14" s="38" t="n"/>
       <c r="P14" s="8" t="n"/>
     </row>
-    <row r="15" ht="18" customHeight="1" s="244">
+    <row r="15" ht="18" customHeight="1" s="286">
       <c r="B15" s="8" t="n"/>
       <c r="C15" s="40" t="inlineStr">
         <is>
@@ -3392,12 +3379,13 @@
       </c>
       <c r="E15" s="42" t="n"/>
       <c r="F15" s="43" t="n"/>
-      <c r="G15" s="319" t="n"/>
+      <c r="G15" s="246" t="n">
+        <v>3750</v>
+      </c>
       <c r="H15" s="141" t="n"/>
       <c r="I15" s="38" t="n"/>
-      <c r="J15" s="331">
-        <f>+G15+H15</f>
-        <v/>
+      <c r="J15" s="257" t="n">
+        <v>3750</v>
       </c>
       <c r="K15" s="134" t="n"/>
       <c r="L15" s="134" t="n"/>
@@ -3405,7 +3393,7 @@
       <c r="N15" s="38" t="n"/>
       <c r="P15" s="8" t="n"/>
     </row>
-    <row r="16" ht="18.75" customHeight="1" s="244">
+    <row r="16" ht="18.75" customHeight="1" s="286">
       <c r="B16" s="8" t="n"/>
       <c r="C16" s="40" t="inlineStr">
         <is>
@@ -3419,12 +3407,13 @@
       </c>
       <c r="E16" s="42" t="n"/>
       <c r="F16" s="43" t="n"/>
-      <c r="G16" s="319" t="n"/>
+      <c r="G16" s="246" t="n">
+        <v>261.55</v>
+      </c>
       <c r="H16" s="141" t="n"/>
       <c r="I16" s="38" t="n"/>
-      <c r="J16" s="331">
-        <f>+G16+H16</f>
-        <v/>
+      <c r="J16" s="257" t="n">
+        <v>261.55</v>
       </c>
       <c r="K16" s="134" t="n"/>
       <c r="L16" s="134" t="n"/>
@@ -3432,7 +3421,7 @@
       <c r="N16" s="38" t="n"/>
       <c r="P16" s="8" t="n"/>
     </row>
-    <row r="17" ht="18.75" customHeight="1" s="244">
+    <row r="17" ht="18.75" customHeight="1" s="286">
       <c r="B17" s="8" t="n"/>
       <c r="C17" s="40" t="inlineStr">
         <is>
@@ -3446,12 +3435,13 @@
       </c>
       <c r="E17" s="42" t="n"/>
       <c r="F17" s="43" t="n"/>
-      <c r="G17" s="319" t="n"/>
+      <c r="G17" s="246" t="n">
+        <v>600</v>
+      </c>
       <c r="H17" s="141" t="n"/>
       <c r="I17" s="38" t="n"/>
-      <c r="J17" s="331">
-        <f>+G17+H17</f>
-        <v/>
+      <c r="J17" s="257" t="n">
+        <v>600</v>
       </c>
       <c r="K17" s="134" t="n"/>
       <c r="L17" s="134" t="n"/>
@@ -3459,7 +3449,7 @@
       <c r="N17" s="38" t="n"/>
       <c r="P17" s="8" t="n"/>
     </row>
-    <row r="18" ht="26.45" customHeight="1" s="244">
+    <row r="18" ht="26.45" customHeight="1" s="286">
       <c r="B18" s="8" t="n"/>
       <c r="C18" s="40" t="inlineStr">
         <is>
@@ -3473,12 +3463,13 @@
       </c>
       <c r="E18" s="42" t="n"/>
       <c r="F18" s="43" t="n"/>
-      <c r="G18" s="319" t="n"/>
+      <c r="G18" s="246" t="n">
+        <v>832.9</v>
+      </c>
       <c r="H18" s="141" t="n"/>
       <c r="I18" s="38" t="n"/>
-      <c r="J18" s="331">
-        <f>+G18+H18</f>
-        <v/>
+      <c r="J18" s="257" t="n">
+        <v>832.9</v>
       </c>
       <c r="K18" s="134" t="n"/>
       <c r="L18" s="134" t="n"/>
@@ -3486,20 +3477,20 @@
       <c r="N18" s="38" t="n"/>
       <c r="P18" s="8" t="n"/>
     </row>
-    <row r="19" ht="18.75" customHeight="1" s="244">
+    <row r="19" ht="18.75" customHeight="1" s="286">
       <c r="B19" s="8" t="n"/>
       <c r="C19" s="40" t="inlineStr">
         <is>
           <t>b6</t>
         </is>
       </c>
-      <c r="D19" s="296" t="n"/>
-      <c r="E19" s="253" t="n"/>
+      <c r="D19" s="317" t="n"/>
+      <c r="E19" s="284" t="n"/>
       <c r="F19" s="43" t="n"/>
-      <c r="G19" s="320" t="n"/>
+      <c r="G19" s="247" t="n"/>
       <c r="H19" s="142" t="n"/>
       <c r="I19" s="38" t="n"/>
-      <c r="J19" s="332">
+      <c r="J19" s="258">
         <f>+G19+H19</f>
         <v/>
       </c>
@@ -3509,7 +3500,7 @@
       <c r="N19" s="38" t="n"/>
       <c r="P19" s="8" t="n"/>
     </row>
-    <row r="20" ht="18.75" customHeight="1" s="244" thickBot="1">
+    <row r="20" ht="18.75" customHeight="1" s="286" thickBot="1">
       <c r="B20" s="8" t="n"/>
       <c r="C20" s="40" t="inlineStr">
         <is>
@@ -3523,12 +3514,13 @@
       </c>
       <c r="E20" s="42" t="n"/>
       <c r="F20" s="43" t="n"/>
-      <c r="G20" s="320" t="n"/>
+      <c r="G20" s="247" t="n">
+        <v>280.25</v>
+      </c>
       <c r="H20" s="142" t="n"/>
       <c r="I20" s="38" t="n"/>
-      <c r="J20" s="332">
-        <f>+G20+H20</f>
-        <v/>
+      <c r="J20" s="258" t="n">
+        <v>280.25</v>
       </c>
       <c r="K20" s="134" t="n"/>
       <c r="L20" s="134" t="n"/>
@@ -3536,7 +3528,7 @@
       <c r="N20" s="38" t="n"/>
       <c r="P20" s="8" t="n"/>
     </row>
-    <row r="21" ht="18" customHeight="1" s="244" thickBot="1">
+    <row r="21" ht="18" customHeight="1" s="286" thickBot="1">
       <c r="B21" s="8" t="n"/>
       <c r="C21" s="40" t="inlineStr">
         <is>
@@ -3550,7 +3542,7 @@
       </c>
       <c r="E21" s="152" t="n"/>
       <c r="F21" s="153" t="n"/>
-      <c r="G21" s="323">
+      <c r="G21" s="250">
         <f>SUM(G15:G20)</f>
         <v/>
       </c>
@@ -3559,7 +3551,7 @@
         <v/>
       </c>
       <c r="I21" s="47" t="n"/>
-      <c r="J21" s="333">
+      <c r="J21" s="259">
         <f>SUM(G21:H21)</f>
         <v/>
       </c>
@@ -3577,16 +3569,16 @@
       <c r="O21" s="7" t="n"/>
       <c r="P21" s="8" t="n"/>
     </row>
-    <row r="22" ht="8.449999999999999" customHeight="1" s="244">
+    <row r="22" ht="8.449999999999999" customHeight="1" s="286">
       <c r="B22" s="8" t="n"/>
       <c r="C22" s="38" t="n"/>
       <c r="D22" s="155" t="n"/>
       <c r="E22" s="155" t="n"/>
       <c r="F22" s="48" t="n"/>
-      <c r="G22" s="324" t="n"/>
+      <c r="G22" s="251" t="n"/>
       <c r="H22" s="155" t="n"/>
       <c r="I22" s="47" t="n"/>
-      <c r="J22" s="334" t="n"/>
+      <c r="J22" s="260" t="n"/>
       <c r="K22" s="46" t="n"/>
       <c r="L22" s="46" t="n"/>
       <c r="M22" s="155" t="n"/>
@@ -3594,7 +3586,7 @@
       <c r="O22" s="7" t="n"/>
       <c r="P22" s="8" t="n"/>
     </row>
-    <row r="23" ht="18.75" customHeight="1" s="244">
+    <row r="23" ht="18.75" customHeight="1" s="286">
       <c r="B23" s="8" t="n"/>
       <c r="C23" s="38" t="n"/>
       <c r="D23" s="136" t="inlineStr">
@@ -3604,17 +3596,17 @@
       </c>
       <c r="E23" s="38" t="n"/>
       <c r="F23" s="41" t="n"/>
-      <c r="G23" s="322" t="n"/>
+      <c r="G23" s="249" t="n"/>
       <c r="H23" s="38" t="n"/>
       <c r="I23" s="38" t="n"/>
-      <c r="J23" s="335" t="n"/>
+      <c r="J23" s="261" t="n"/>
       <c r="K23" s="134" t="n"/>
       <c r="L23" s="134" t="n"/>
       <c r="M23" s="38" t="n"/>
       <c r="N23" s="38" t="n"/>
       <c r="P23" s="8" t="n"/>
     </row>
-    <row r="24" ht="25.5" customHeight="1" s="244">
+    <row r="24" ht="25.5" customHeight="1" s="286">
       <c r="B24" s="8" t="n"/>
       <c r="C24" s="40" t="inlineStr">
         <is>
@@ -3632,7 +3624,7 @@
           <t>(a6-b8)</t>
         </is>
       </c>
-      <c r="G24" s="325">
+      <c r="G24" s="252">
         <f>G11-G21</f>
         <v/>
       </c>
@@ -3641,7 +3633,7 @@
         <v/>
       </c>
       <c r="I24" s="38" t="n"/>
-      <c r="J24" s="331">
+      <c r="J24" s="257">
         <f>SUM(G24:H24)</f>
         <v/>
       </c>
@@ -3655,16 +3647,16 @@
       <c r="P24" s="8" t="n"/>
       <c r="Q24" s="17" t="n"/>
     </row>
-    <row r="25" ht="7.5" customHeight="1" s="244">
+    <row r="25" ht="7.5" customHeight="1" s="286">
       <c r="B25" s="8" t="n"/>
       <c r="C25" s="38" t="n"/>
       <c r="D25" s="42" t="n"/>
       <c r="E25" s="42" t="n"/>
       <c r="F25" s="157" t="n"/>
-      <c r="G25" s="326" t="n"/>
+      <c r="G25" s="253" t="n"/>
       <c r="H25" s="42" t="n"/>
       <c r="I25" s="38" t="n"/>
-      <c r="J25" s="336" t="n"/>
+      <c r="J25" s="262" t="n"/>
       <c r="K25" s="134" t="n"/>
       <c r="L25" s="134" t="n"/>
       <c r="M25" s="42" t="n"/>
@@ -3672,7 +3664,7 @@
       <c r="P25" s="8" t="n"/>
       <c r="Q25" s="17" t="n"/>
     </row>
-    <row r="26" ht="33.75" customHeight="1" s="244">
+    <row r="26" ht="33.75" customHeight="1" s="286">
       <c r="B26" s="8" t="n"/>
       <c r="C26" s="40" t="inlineStr">
         <is>
@@ -3686,10 +3678,10 @@
       </c>
       <c r="E26" s="42" t="n"/>
       <c r="F26" s="157" t="n"/>
-      <c r="G26" s="319" t="n"/>
+      <c r="G26" s="246" t="n"/>
       <c r="H26" s="141" t="n"/>
       <c r="I26" s="38" t="n"/>
-      <c r="J26" s="331">
+      <c r="J26" s="257">
         <f>SUM(G26:H26)</f>
         <v/>
       </c>
@@ -3712,41 +3704,41 @@
         <v/>
       </c>
     </row>
-    <row r="27" ht="7.5" customHeight="1" s="244">
+    <row r="27" ht="7.5" customHeight="1" s="286">
       <c r="B27" s="8" t="n"/>
       <c r="C27" s="38" t="n"/>
       <c r="D27" s="42" t="n"/>
       <c r="E27" s="42" t="n"/>
       <c r="F27" s="157" t="n"/>
-      <c r="G27" s="326" t="n"/>
+      <c r="G27" s="253" t="n"/>
       <c r="H27" s="42" t="n"/>
       <c r="I27" s="38" t="n"/>
-      <c r="J27" s="337" t="n"/>
+      <c r="J27" s="263" t="n"/>
       <c r="K27" s="140" t="n"/>
       <c r="L27" s="134" t="n"/>
       <c r="M27" s="42" t="n"/>
       <c r="N27" s="38" t="n"/>
       <c r="P27" s="8" t="n"/>
     </row>
-    <row r="28" ht="19.5" customHeight="1" s="244">
+    <row r="28" ht="19.5" customHeight="1" s="286">
       <c r="B28" s="8" t="n"/>
       <c r="C28" s="40" t="inlineStr">
         <is>
           <t>c3</t>
         </is>
       </c>
-      <c r="D28" s="280" t="inlineStr">
+      <c r="D28" s="321" t="inlineStr">
         <is>
           <t xml:space="preserve">Sub total                                                               </t>
         </is>
       </c>
-      <c r="E28" s="250" t="n"/>
+      <c r="E28" s="298" t="n"/>
       <c r="F28" s="156" t="inlineStr">
         <is>
           <t>(c1+c2)</t>
         </is>
       </c>
-      <c r="G28" s="325">
+      <c r="G28" s="252">
         <f>G24+G26</f>
         <v/>
       </c>
@@ -3755,7 +3747,7 @@
         <v/>
       </c>
       <c r="I28" s="38" t="n"/>
-      <c r="J28" s="331">
+      <c r="J28" s="257">
         <f>J24+J26</f>
         <v/>
       </c>
@@ -3768,23 +3760,23 @@
       <c r="N28" s="38" t="n"/>
       <c r="P28" s="8" t="n"/>
     </row>
-    <row r="29" ht="7.5" customHeight="1" s="244">
+    <row r="29" ht="7.5" customHeight="1" s="286">
       <c r="B29" s="8" t="n"/>
       <c r="C29" s="38" t="n"/>
       <c r="D29" s="42" t="n"/>
       <c r="E29" s="42" t="n"/>
       <c r="F29" s="157" t="n"/>
-      <c r="G29" s="326" t="n"/>
+      <c r="G29" s="253" t="n"/>
       <c r="H29" s="42" t="n"/>
       <c r="I29" s="38" t="n"/>
-      <c r="J29" s="338" t="n"/>
+      <c r="J29" s="264" t="n"/>
       <c r="K29" s="140" t="n"/>
       <c r="L29" s="134" t="n"/>
       <c r="M29" s="42" t="n"/>
       <c r="N29" s="38" t="n"/>
       <c r="P29" s="8" t="n"/>
     </row>
-    <row r="30" ht="18" customHeight="1" s="244">
+    <row r="30" ht="18" customHeight="1" s="286">
       <c r="B30" s="8" t="n"/>
       <c r="C30" s="40" t="inlineStr">
         <is>
@@ -3798,10 +3790,10 @@
       </c>
       <c r="E30" s="42" t="n"/>
       <c r="F30" s="156" t="n"/>
-      <c r="G30" s="319" t="n"/>
+      <c r="G30" s="246" t="n"/>
       <c r="H30" s="141" t="n"/>
       <c r="I30" s="38" t="n"/>
-      <c r="J30" s="331">
+      <c r="J30" s="257">
         <f>SUM(G30:H30)</f>
         <v/>
       </c>
@@ -3815,23 +3807,23 @@
       <c r="N30" s="38" t="n"/>
       <c r="P30" s="8" t="n"/>
     </row>
-    <row r="31" ht="7.5" customHeight="1" s="244" thickBot="1">
+    <row r="31" ht="7.5" customHeight="1" s="286" thickBot="1">
       <c r="B31" s="8" t="n"/>
       <c r="C31" s="38" t="n"/>
       <c r="D31" s="42" t="n"/>
       <c r="E31" s="42" t="n"/>
       <c r="F31" s="157" t="n"/>
-      <c r="G31" s="327" t="n"/>
+      <c r="G31" s="254" t="n"/>
       <c r="H31" s="158" t="n"/>
       <c r="I31" s="38" t="n"/>
-      <c r="J31" s="336" t="n"/>
+      <c r="J31" s="262" t="n"/>
       <c r="K31" s="159" t="n"/>
       <c r="L31" s="134" t="n"/>
       <c r="M31" s="158" t="n"/>
       <c r="N31" s="38" t="n"/>
       <c r="P31" s="8" t="n"/>
     </row>
-    <row r="32" ht="18" customHeight="1" s="244" thickBot="1">
+    <row r="32" ht="18" customHeight="1" s="286" thickBot="1">
       <c r="B32" s="8" t="n"/>
       <c r="C32" s="40" t="inlineStr">
         <is>
@@ -3849,7 +3841,7 @@
           <t>(c3+c4)</t>
         </is>
       </c>
-      <c r="G32" s="321">
+      <c r="G32" s="248">
         <f>G28+G30</f>
         <v/>
       </c>
@@ -3858,7 +3850,7 @@
         <v/>
       </c>
       <c r="I32" s="148" t="n"/>
-      <c r="J32" s="321">
+      <c r="J32" s="248">
         <f>J28+J30</f>
         <v/>
       </c>
@@ -3889,23 +3881,23 @@
         <v/>
       </c>
     </row>
-    <row r="33" ht="18" customHeight="1" s="244">
+    <row r="33" ht="18" customHeight="1" s="286">
       <c r="B33" s="8" t="n"/>
       <c r="C33" s="38" t="n"/>
       <c r="D33" s="38" t="n"/>
       <c r="E33" s="38" t="n"/>
       <c r="F33" s="41" t="n"/>
-      <c r="G33" s="322" t="n"/>
+      <c r="G33" s="249" t="n"/>
       <c r="H33" s="38" t="n"/>
       <c r="I33" s="38" t="n"/>
-      <c r="J33" s="339" t="n"/>
+      <c r="J33" s="265" t="n"/>
       <c r="K33" s="46" t="n"/>
       <c r="L33" s="46" t="n"/>
       <c r="M33" s="163" t="n"/>
       <c r="N33" s="38" t="n"/>
       <c r="P33" s="8" t="n"/>
     </row>
-    <row r="34" ht="23.25" customHeight="1" s="244" thickBot="1">
+    <row r="34" ht="23.25" customHeight="1" s="286" thickBot="1">
       <c r="B34" s="8" t="n"/>
       <c r="C34" s="38" t="n"/>
       <c r="D34" s="143" t="inlineStr">
@@ -3915,10 +3907,10 @@
       </c>
       <c r="E34" s="38" t="n"/>
       <c r="F34" s="38" t="n"/>
-      <c r="G34" s="322" t="n"/>
+      <c r="G34" s="249" t="n"/>
       <c r="H34" s="38" t="n"/>
       <c r="I34" s="38" t="n"/>
-      <c r="J34" s="335" t="n"/>
+      <c r="J34" s="261" t="n"/>
       <c r="K34" s="134" t="n"/>
       <c r="L34" s="134" t="n"/>
       <c r="M34" s="38" t="n"/>
@@ -3927,41 +3919,41 @@
     </row>
     <row r="35" ht="37.5" customFormat="1" customHeight="1" s="49">
       <c r="B35" s="53" t="n"/>
-      <c r="C35" s="286" t="inlineStr">
+      <c r="C35" s="305" t="inlineStr">
         <is>
           <t>d</t>
         </is>
       </c>
-      <c r="D35" s="288" t="inlineStr">
+      <c r="D35" s="307" t="inlineStr">
         <is>
           <t xml:space="preserve">FOR INFORMATION ONLY: MONEY RECEIVED AND PASSED ON TO  EXTERNAL ORGANISATIONS                                </t>
         </is>
       </c>
-      <c r="E35" s="289" t="n"/>
-      <c r="F35" s="289" t="n"/>
-      <c r="G35" s="289" t="n"/>
-      <c r="H35" s="289" t="n"/>
-      <c r="I35" s="289" t="n"/>
-      <c r="J35" s="289" t="n"/>
-      <c r="K35" s="289" t="n"/>
-      <c r="L35" s="289" t="n"/>
-      <c r="M35" s="290" t="n"/>
+      <c r="E35" s="308" t="n"/>
+      <c r="F35" s="308" t="n"/>
+      <c r="G35" s="308" t="n"/>
+      <c r="H35" s="308" t="n"/>
+      <c r="I35" s="308" t="n"/>
+      <c r="J35" s="308" t="n"/>
+      <c r="K35" s="308" t="n"/>
+      <c r="L35" s="308" t="n"/>
+      <c r="M35" s="309" t="n"/>
       <c r="P35" s="53" t="n"/>
     </row>
-    <row r="36" ht="13.7" customHeight="1" s="244">
+    <row r="36" ht="13.7" customHeight="1" s="286">
       <c r="B36" s="8" t="n"/>
-      <c r="C36" s="287" t="n"/>
-      <c r="D36" s="283" t="inlineStr">
+      <c r="C36" s="306" t="n"/>
+      <c r="D36" s="323" t="inlineStr">
         <is>
           <t>(these amounts are not to be included in total receipts/payments figures above)</t>
         </is>
       </c>
-      <c r="E36" s="284" t="n"/>
-      <c r="F36" s="284" t="n"/>
-      <c r="G36" s="284" t="n"/>
-      <c r="H36" s="284" t="n"/>
+      <c r="E36" s="324" t="n"/>
+      <c r="F36" s="324" t="n"/>
+      <c r="G36" s="324" t="n"/>
+      <c r="H36" s="324" t="n"/>
       <c r="I36" s="214" t="n"/>
-      <c r="J36" s="340" t="inlineStr">
+      <c r="J36" s="266" t="inlineStr">
         <is>
           <t>£</t>
         </is>
@@ -3977,24 +3969,24 @@
       <c r="O36" s="6" t="n"/>
       <c r="P36" s="8" t="n"/>
     </row>
-    <row r="37" ht="31.7" customHeight="1" s="244">
+    <row r="37" ht="31.7" customHeight="1" s="286">
       <c r="B37" s="8" t="n"/>
       <c r="C37" s="50" t="inlineStr">
         <is>
           <t>d1</t>
         </is>
       </c>
-      <c r="D37" s="281" t="inlineStr">
+      <c r="D37" s="322" t="inlineStr">
         <is>
           <t>Balance brought forward from last year</t>
         </is>
       </c>
-      <c r="E37" s="250" t="n"/>
-      <c r="F37" s="250" t="n"/>
-      <c r="G37" s="250" t="n"/>
-      <c r="H37" s="282" t="n"/>
+      <c r="E37" s="298" t="n"/>
+      <c r="F37" s="298" t="n"/>
+      <c r="G37" s="298" t="n"/>
+      <c r="H37" s="304" t="n"/>
       <c r="I37" s="134" t="n"/>
-      <c r="J37" s="319">
+      <c r="J37" s="246">
         <f>+M40</f>
         <v/>
       </c>
@@ -4005,72 +3997,72 @@
       <c r="O37" s="6" t="n"/>
       <c r="P37" s="8" t="n"/>
     </row>
-    <row r="38" ht="31.7" customHeight="1" s="244">
+    <row r="38" ht="31.7" customHeight="1" s="286">
       <c r="B38" s="8" t="n"/>
       <c r="C38" s="50" t="inlineStr">
         <is>
           <t>d2</t>
         </is>
       </c>
-      <c r="D38" s="281" t="inlineStr">
+      <c r="D38" s="322" t="inlineStr">
         <is>
           <t>Offerings/Gifts - received for external organisations</t>
         </is>
       </c>
-      <c r="E38" s="250" t="n"/>
-      <c r="F38" s="250" t="n"/>
-      <c r="G38" s="250" t="n"/>
-      <c r="H38" s="282" t="n"/>
+      <c r="E38" s="298" t="n"/>
+      <c r="F38" s="298" t="n"/>
+      <c r="G38" s="298" t="n"/>
+      <c r="H38" s="304" t="n"/>
       <c r="I38" s="51" t="n"/>
-      <c r="J38" s="319" t="n"/>
+      <c r="J38" s="246" t="n"/>
       <c r="K38" s="134" t="n"/>
       <c r="L38" s="134" t="n"/>
       <c r="M38" s="165" t="n"/>
       <c r="N38" s="38" t="n"/>
       <c r="P38" s="8" t="n"/>
     </row>
-    <row r="39" ht="31.7" customHeight="1" s="244" thickBot="1">
+    <row r="39" ht="31.7" customHeight="1" s="286" thickBot="1">
       <c r="B39" s="8" t="n"/>
       <c r="C39" s="50" t="inlineStr">
         <is>
           <t>d3</t>
         </is>
       </c>
-      <c r="D39" s="281" t="inlineStr">
+      <c r="D39" s="322" t="inlineStr">
         <is>
           <t>Offerings/Gifts  - passed to external organisations</t>
         </is>
       </c>
-      <c r="E39" s="250" t="n"/>
-      <c r="F39" s="250" t="n"/>
-      <c r="G39" s="250" t="n"/>
-      <c r="H39" s="282" t="n"/>
+      <c r="E39" s="298" t="n"/>
+      <c r="F39" s="298" t="n"/>
+      <c r="G39" s="298" t="n"/>
+      <c r="H39" s="304" t="n"/>
       <c r="I39" s="51" t="n"/>
-      <c r="J39" s="320" t="n"/>
+      <c r="J39" s="247" t="n"/>
       <c r="K39" s="166" t="n"/>
       <c r="L39" s="134" t="n"/>
       <c r="M39" s="167" t="n"/>
       <c r="N39" s="38" t="n"/>
       <c r="P39" s="8" t="n"/>
     </row>
-    <row r="40" ht="33.75" customHeight="1" s="244" thickBot="1">
+    <row r="40" ht="33.75" customHeight="1" s="286" thickBot="1">
       <c r="B40" s="8" t="n"/>
       <c r="C40" s="50" t="inlineStr">
         <is>
           <t>d4</t>
         </is>
       </c>
-      <c r="D40" s="277" t="inlineStr">
+      <c r="D40" s="318" t="inlineStr">
         <is>
           <t>BALANCE STILL TO BE PAID                     (d1+d2-d3)</t>
         </is>
       </c>
-      <c r="E40" s="278" t="n"/>
-      <c r="F40" s="278" t="n"/>
-      <c r="G40" s="278" t="n"/>
-      <c r="H40" s="279" t="n"/>
+      <c r="E40" s="319" t="n"/>
+      <c r="F40" s="319" t="n"/>
+      <c r="G40" s="319" t="n"/>
+      <c r="H40" s="320" t="n"/>
       <c r="I40" s="52" t="n"/>
-      <c r="J40" s="341">
+      <c r="J40" s="267">
         <f>SUM(J37+J38-J39)</f>
         <v/>
       </c>
@@ -4084,22 +4076,22 @@
       <c r="P40" s="8" t="n"/>
       <c r="Q40" s="170" t="n"/>
     </row>
-    <row r="41" ht="6.75" customFormat="1" customHeight="1" s="294">
+    <row r="41" ht="6.75" customFormat="1" customHeight="1" s="314">
       <c r="B41" s="131" t="n"/>
-      <c r="G41" s="328" t="n"/>
-      <c r="J41" s="328" t="n"/>
+      <c r="G41" s="244" t="n"/>
+      <c r="J41" s="244" t="n"/>
       <c r="P41" s="131" t="n"/>
     </row>
-    <row r="42" ht="2.25" customHeight="1" s="244">
+    <row r="42" ht="2.25" customHeight="1" s="286">
       <c r="B42" s="8" t="n"/>
       <c r="C42" s="8" t="n"/>
       <c r="D42" s="8" t="n"/>
       <c r="E42" s="8" t="n"/>
       <c r="F42" s="8" t="n"/>
-      <c r="G42" s="329" t="n"/>
+      <c r="G42" s="255" t="n"/>
       <c r="H42" s="8" t="n"/>
       <c r="I42" s="8" t="n"/>
-      <c r="J42" s="329" t="n"/>
+      <c r="J42" s="255" t="n"/>
       <c r="K42" s="8" t="n"/>
       <c r="L42" s="8" t="n"/>
       <c r="M42" s="8" t="n"/>
@@ -4107,20 +4099,26 @@
       <c r="O42" s="8" t="n"/>
       <c r="P42" s="8" t="n"/>
     </row>
-    <row r="43" ht="18" customHeight="1" s="244"/>
-    <row r="44" ht="18" customHeight="1" s="244"/>
-    <row r="45" ht="18" customHeight="1" s="244"/>
-    <row r="46" ht="18" customHeight="1" s="244"/>
-    <row r="47" ht="18" customHeight="1" s="244"/>
-    <row r="48" ht="18" customHeight="1" s="244"/>
-    <row r="49" ht="18" customHeight="1" s="244"/>
-    <row r="50" ht="18" customHeight="1" s="244"/>
-    <row r="51" ht="18" customHeight="1" s="244"/>
-    <row r="52" ht="18" customHeight="1" s="244"/>
-    <row r="53" ht="6.75" customHeight="1" s="244"/>
-    <row r="54" ht="6.75" customHeight="1" s="244"/>
+    <row r="43" ht="18" customHeight="1" s="286"/>
+    <row r="44" ht="18" customHeight="1" s="286"/>
+    <row r="45" ht="18" customHeight="1" s="286"/>
+    <row r="46" ht="18" customHeight="1" s="286"/>
+    <row r="47" ht="18" customHeight="1" s="286"/>
+    <row r="48" ht="18" customHeight="1" s="286"/>
+    <row r="49" ht="18" customHeight="1" s="286"/>
+    <row r="50" ht="18" customHeight="1" s="286"/>
+    <row r="51" ht="18" customHeight="1" s="286"/>
+    <row r="52" ht="18" customHeight="1" s="286"/>
+    <row r="53" ht="6.75" customHeight="1" s="286"/>
+    <row r="54" ht="6.75" customHeight="1" s="286"/>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="D40:H40"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D37:H37"/>
+    <mergeCell ref="D38:H38"/>
+    <mergeCell ref="D39:H39"/>
+    <mergeCell ref="D36:H36"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="C35:C36"/>
     <mergeCell ref="D35:M35"/>
@@ -4131,12 +4129,6 @@
     <mergeCell ref="M3:M4"/>
     <mergeCell ref="H2:L2"/>
     <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D40:H40"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D37:H37"/>
-    <mergeCell ref="D38:H38"/>
-    <mergeCell ref="D39:H39"/>
-    <mergeCell ref="D36:H36"/>
   </mergeCells>
   <pageMargins left="0.1574803149606299" right="0.1574803149606299" top="0.2755905511811024" bottom="0.3937007874015748" header="0.1574803149606299" footer="0.2362204724409449"/>
   <pageSetup orientation="portrait" paperSize="9" scale="99"/>
@@ -4159,40 +4151,40 @@
   </sheetPr>
   <dimension ref="A1:Z50"/>
   <sheetViews>
-    <sheetView showZeros="0" showWhiteSpace="0" view="pageLayout" topLeftCell="A38" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView showZeros="0" showWhiteSpace="0" view="pageLayout" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
   <cols>
-    <col width="1.42578125" customWidth="1" style="244" min="1" max="1"/>
-    <col width="1.140625" customWidth="1" style="244" min="2" max="2"/>
-    <col width="3.42578125" bestFit="1" customWidth="1" style="244" min="3" max="3"/>
-    <col width="25" customWidth="1" style="244" min="4" max="4"/>
-    <col width="1.5703125" customWidth="1" style="244" min="5" max="5"/>
-    <col width="12.85546875" customWidth="1" style="244" min="6" max="6"/>
-    <col width="4" bestFit="1" customWidth="1" style="244" min="7" max="7"/>
-    <col width="0.85546875" customWidth="1" style="244" min="8" max="8"/>
-    <col width="14" customWidth="1" style="244" min="9" max="9"/>
-    <col width="5" customWidth="1" style="244" min="10" max="10"/>
-    <col width="14" customWidth="1" style="244" min="11" max="11"/>
-    <col width="1.42578125" customWidth="1" style="244" min="12" max="12"/>
-    <col width="0.85546875" customWidth="1" style="244" min="13" max="13"/>
-    <col width="15.5703125" customWidth="1" style="244" min="14" max="14"/>
-    <col width="5.5703125" bestFit="1" customWidth="1" style="244" min="15" max="15"/>
-    <col width="0.5703125" customWidth="1" style="244" min="16" max="16"/>
-    <col width="13" customWidth="1" style="244" min="17" max="17"/>
-    <col width="5" bestFit="1" customWidth="1" style="244" min="18" max="18"/>
-    <col width="0.85546875" customWidth="1" style="244" min="19" max="19"/>
-    <col width="15.5703125" customWidth="1" style="244" min="20" max="20"/>
-    <col width="5.85546875" bestFit="1" customWidth="1" style="244" min="21" max="21"/>
-    <col width="1" customWidth="1" style="244" min="22" max="22"/>
-    <col width="9.5703125" customWidth="1" style="244" min="23" max="23"/>
-    <col width="7.85546875" bestFit="1" customWidth="1" style="244" min="25" max="25"/>
-    <col width="2.5703125" customWidth="1" style="244" min="27" max="27"/>
+    <col width="1.42578125" customWidth="1" style="286" min="1" max="1"/>
+    <col width="1.140625" customWidth="1" style="286" min="2" max="2"/>
+    <col width="3.42578125" bestFit="1" customWidth="1" style="286" min="3" max="3"/>
+    <col width="25" customWidth="1" style="286" min="4" max="4"/>
+    <col width="1.5703125" customWidth="1" style="286" min="5" max="5"/>
+    <col width="12.85546875" customWidth="1" style="286" min="6" max="6"/>
+    <col width="4" bestFit="1" customWidth="1" style="286" min="7" max="7"/>
+    <col width="0.85546875" customWidth="1" style="286" min="8" max="8"/>
+    <col width="14" customWidth="1" style="286" min="9" max="9"/>
+    <col width="5" customWidth="1" style="286" min="10" max="10"/>
+    <col width="14" customWidth="1" style="286" min="11" max="11"/>
+    <col width="1.42578125" customWidth="1" style="286" min="12" max="12"/>
+    <col width="0.85546875" customWidth="1" style="286" min="13" max="13"/>
+    <col width="15.5703125" customWidth="1" style="286" min="14" max="14"/>
+    <col width="5.5703125" bestFit="1" customWidth="1" style="286" min="15" max="15"/>
+    <col width="0.5703125" customWidth="1" style="286" min="16" max="16"/>
+    <col width="13" customWidth="1" style="286" min="17" max="17"/>
+    <col width="5" bestFit="1" customWidth="1" style="286" min="18" max="18"/>
+    <col width="0.85546875" customWidth="1" style="286" min="19" max="19"/>
+    <col width="15.5703125" customWidth="1" style="286" min="20" max="20"/>
+    <col width="5.85546875" bestFit="1" customWidth="1" style="286" min="21" max="21"/>
+    <col width="1" customWidth="1" style="286" min="22" max="22"/>
+    <col width="9.5703125" customWidth="1" style="286" min="23" max="23"/>
+    <col width="7.85546875" bestFit="1" customWidth="1" style="286" min="25" max="25"/>
+    <col width="2.5703125" customWidth="1" style="286" min="27" max="27"/>
   </cols>
   <sheetData>
-    <row r="1" ht="8.449999999999999" customHeight="1" s="244">
+    <row r="1" ht="8.449999999999999" customHeight="1" s="286">
       <c r="B1" s="10" t="n"/>
       <c r="C1" s="10" t="n"/>
       <c r="D1" s="53" t="n"/>
@@ -4227,7 +4219,7 @@
       <c r="U1" s="53" t="n"/>
       <c r="V1" s="53" t="n"/>
     </row>
-    <row r="2" ht="27" customHeight="1" s="244">
+    <row r="2" ht="27" customHeight="1" s="286">
       <c r="B2" s="10" t="n"/>
       <c r="C2" s="2" t="n"/>
       <c r="D2" s="49" t="n"/>
@@ -4240,16 +4232,16 @@
       <c r="K2" s="56" t="n"/>
       <c r="L2" s="56" t="n"/>
       <c r="M2" s="56" t="n"/>
-      <c r="N2" s="297">
+      <c r="N2" s="332">
         <f>'P1 Front page'!$C$11</f>
         <v/>
       </c>
-      <c r="O2" s="266" t="n"/>
-      <c r="P2" s="266" t="n"/>
-      <c r="Q2" s="266" t="n"/>
-      <c r="R2" s="266" t="n"/>
-      <c r="S2" s="266" t="n"/>
-      <c r="T2" s="233" t="inlineStr">
+      <c r="O2" s="288" t="n"/>
+      <c r="P2" s="288" t="n"/>
+      <c r="Q2" s="288" t="n"/>
+      <c r="R2" s="288" t="n"/>
+      <c r="S2" s="288" t="n"/>
+      <c r="T2" s="232" t="inlineStr">
         <is>
           <t>Church</t>
         </is>
@@ -4262,22 +4254,22 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="25.5" customHeight="1" s="244">
+    <row r="3" ht="25.5" customHeight="1" s="286">
       <c r="B3" s="10" t="n"/>
       <c r="C3" s="2" t="n"/>
-      <c r="D3" s="305" t="inlineStr">
+      <c r="D3" s="329" t="inlineStr">
         <is>
           <t>SUMMARY OF CHURCH ACCOUNTS AND INTERNAL ORGANISATIONS REPORTING TO THE CHURCH COUNCIL</t>
         </is>
       </c>
       <c r="U3" s="57" t="n"/>
-      <c r="V3" s="234" t="n"/>
+      <c r="V3" s="233" t="n"/>
       <c r="W3" s="28" t="n"/>
       <c r="X3" s="1" t="n"/>
       <c r="Y3" s="1" t="n"/>
       <c r="Z3" s="1" t="n"/>
     </row>
-    <row r="4" ht="23.25" customHeight="1" s="244" thickBot="1">
+    <row r="4" ht="23.25" customHeight="1" s="286" thickBot="1">
       <c r="B4" s="10" t="n"/>
       <c r="C4" s="2" t="n"/>
       <c r="D4" s="173" t="inlineStr">
@@ -4308,64 +4300,64 @@
       <c r="U4" s="49" t="n"/>
       <c r="V4" s="53" t="n"/>
     </row>
-    <row r="5" ht="63.75" customHeight="1" s="244">
+    <row r="5" ht="63.75" customHeight="1" s="286">
       <c r="B5" s="10" t="n"/>
       <c r="C5" s="2" t="n"/>
-      <c r="D5" s="299" t="inlineStr">
+      <c r="D5" s="334" t="inlineStr">
         <is>
           <t xml:space="preserve">Summary of the Church accounts for the year ended 31 August 2024 and Internal Organisations reporting to the Church Council/Church Meeting. Note that the funds of an Internal Organisation would normally be Restricted funds unless it could be clearly shown that they could be used for any Methodist purpose.   This section must be completed to arrive at the gross income and expenditure totals of the Church. If gross income exceeds the Accruals threshold, then the Accruals method of accounting AND A DIFFERENT FORM must be used to report the accounts (see Methodist website).  Please refer to the guidance notes regarding transfers between the District and connected  District Organisations. </t>
         </is>
       </c>
-      <c r="E5" s="300" t="n"/>
-      <c r="F5" s="300" t="n"/>
-      <c r="G5" s="300" t="n"/>
-      <c r="H5" s="300" t="n"/>
-      <c r="I5" s="300" t="n"/>
-      <c r="J5" s="300" t="n"/>
-      <c r="K5" s="300" t="n"/>
-      <c r="L5" s="300" t="n"/>
-      <c r="M5" s="300" t="n"/>
-      <c r="N5" s="300" t="n"/>
-      <c r="O5" s="300" t="n"/>
-      <c r="P5" s="300" t="n"/>
-      <c r="Q5" s="300" t="n"/>
-      <c r="R5" s="300" t="n"/>
-      <c r="S5" s="300" t="n"/>
-      <c r="T5" s="301" t="n"/>
-      <c r="U5" s="312" t="n"/>
+      <c r="E5" s="335" t="n"/>
+      <c r="F5" s="335" t="n"/>
+      <c r="G5" s="335" t="n"/>
+      <c r="H5" s="335" t="n"/>
+      <c r="I5" s="335" t="n"/>
+      <c r="J5" s="335" t="n"/>
+      <c r="K5" s="335" t="n"/>
+      <c r="L5" s="335" t="n"/>
+      <c r="M5" s="335" t="n"/>
+      <c r="N5" s="335" t="n"/>
+      <c r="O5" s="335" t="n"/>
+      <c r="P5" s="335" t="n"/>
+      <c r="Q5" s="335" t="n"/>
+      <c r="R5" s="335" t="n"/>
+      <c r="S5" s="335" t="n"/>
+      <c r="T5" s="336" t="n"/>
+      <c r="U5" s="340" t="n"/>
       <c r="V5" s="53" t="n"/>
     </row>
-    <row r="6" ht="3.75" customHeight="1" s="244" thickBot="1">
+    <row r="6" ht="3.75" customHeight="1" s="286" thickBot="1">
       <c r="B6" s="10" t="n"/>
       <c r="C6" s="2" t="n"/>
-      <c r="D6" s="307" t="n"/>
-      <c r="E6" s="278" t="n"/>
-      <c r="F6" s="278" t="n"/>
-      <c r="G6" s="278" t="n"/>
-      <c r="H6" s="278" t="n"/>
-      <c r="I6" s="278" t="n"/>
-      <c r="J6" s="278" t="n"/>
-      <c r="K6" s="278" t="n"/>
-      <c r="L6" s="278" t="n"/>
-      <c r="M6" s="278" t="n"/>
-      <c r="N6" s="278" t="n"/>
-      <c r="O6" s="278" t="n"/>
-      <c r="P6" s="278" t="n"/>
-      <c r="Q6" s="278" t="n"/>
-      <c r="R6" s="278" t="n"/>
-      <c r="S6" s="278" t="n"/>
-      <c r="T6" s="279" t="n"/>
-      <c r="U6" s="312" t="n"/>
+      <c r="D6" s="330" t="n"/>
+      <c r="E6" s="319" t="n"/>
+      <c r="F6" s="319" t="n"/>
+      <c r="G6" s="319" t="n"/>
+      <c r="H6" s="319" t="n"/>
+      <c r="I6" s="319" t="n"/>
+      <c r="J6" s="319" t="n"/>
+      <c r="K6" s="319" t="n"/>
+      <c r="L6" s="319" t="n"/>
+      <c r="M6" s="319" t="n"/>
+      <c r="N6" s="319" t="n"/>
+      <c r="O6" s="319" t="n"/>
+      <c r="P6" s="319" t="n"/>
+      <c r="Q6" s="319" t="n"/>
+      <c r="R6" s="319" t="n"/>
+      <c r="S6" s="319" t="n"/>
+      <c r="T6" s="320" t="n"/>
+      <c r="U6" s="340" t="n"/>
       <c r="V6" s="53" t="n"/>
     </row>
-    <row r="7" ht="6" customHeight="1" s="244">
+    <row r="7" ht="6" customHeight="1" s="286">
       <c r="B7" s="10" t="n"/>
       <c r="C7" s="2" t="n"/>
-      <c r="D7" s="298" t="n"/>
-      <c r="U7" s="312" t="n"/>
+      <c r="D7" s="333" t="n"/>
+      <c r="U7" s="340" t="n"/>
       <c r="V7" s="53" t="n"/>
     </row>
-    <row r="8" ht="35.45" customHeight="1" s="244">
+    <row r="8" ht="35.45" customHeight="1" s="286">
       <c r="B8" s="10" t="n"/>
       <c r="C8" s="2" t="n"/>
       <c r="D8" s="175" t="inlineStr">
@@ -4416,7 +4408,7 @@
       <c r="U8" s="60" t="n"/>
       <c r="V8" s="53" t="n"/>
     </row>
-    <row r="9" ht="24.75" customHeight="1" s="244">
+    <row r="9" ht="24.75" customHeight="1" s="286">
       <c r="B9" s="10" t="n"/>
       <c r="C9" s="16" t="inlineStr">
         <is>
@@ -4449,7 +4441,7 @@
       <c r="U9" s="62" t="n"/>
       <c r="V9" s="53" t="n"/>
     </row>
-    <row r="10" ht="24.75" customHeight="1" s="244">
+    <row r="10" ht="24.75" customHeight="1" s="286">
       <c r="B10" s="10" t="n"/>
       <c r="C10" s="16" t="inlineStr">
         <is>
@@ -4482,7 +4474,7 @@
       <c r="U10" s="62" t="n"/>
       <c r="V10" s="53" t="n"/>
     </row>
-    <row r="11" ht="24.75" customHeight="1" s="244">
+    <row r="11" ht="24.75" customHeight="1" s="286">
       <c r="B11" s="10" t="n"/>
       <c r="C11" s="16" t="inlineStr">
         <is>
@@ -4515,7 +4507,7 @@
       <c r="U11" s="62" t="n"/>
       <c r="V11" s="53" t="n"/>
     </row>
-    <row r="12" ht="24.75" customHeight="1" s="244">
+    <row r="12" ht="24.75" customHeight="1" s="286">
       <c r="B12" s="10" t="n"/>
       <c r="C12" s="16" t="inlineStr">
         <is>
@@ -4548,7 +4540,7 @@
       <c r="U12" s="62" t="n"/>
       <c r="V12" s="53" t="n"/>
     </row>
-    <row r="13" ht="24.75" customHeight="1" s="244">
+    <row r="13" ht="24.75" customHeight="1" s="286">
       <c r="B13" s="10" t="n"/>
       <c r="C13" s="16" t="inlineStr">
         <is>
@@ -4581,7 +4573,7 @@
       <c r="U13" s="62" t="n"/>
       <c r="V13" s="53" t="n"/>
     </row>
-    <row r="14" ht="24.75" customHeight="1" s="244">
+    <row r="14" ht="24.75" customHeight="1" s="286">
       <c r="B14" s="10" t="n"/>
       <c r="C14" s="16" t="inlineStr">
         <is>
@@ -4614,7 +4606,7 @@
       <c r="U14" s="62" t="n"/>
       <c r="V14" s="53" t="n"/>
     </row>
-    <row r="15" ht="24.75" customHeight="1" s="244" thickBot="1">
+    <row r="15" ht="24.75" customHeight="1" s="286" thickBot="1">
       <c r="B15" s="10" t="n"/>
       <c r="C15" s="16" t="inlineStr">
         <is>
@@ -4647,7 +4639,7 @@
       <c r="U15" s="62" t="n"/>
       <c r="V15" s="53" t="n"/>
     </row>
-    <row r="16" ht="25.5" customHeight="1" s="244">
+    <row r="16" ht="25.5" customHeight="1" s="286">
       <c r="B16" s="10" t="n"/>
       <c r="C16" s="16" t="inlineStr">
         <is>
@@ -4687,7 +4679,7 @@
         <f>SUM(Q9:Q15)</f>
         <v/>
       </c>
-      <c r="R16" s="235" t="inlineStr">
+      <c r="R16" s="234" t="inlineStr">
         <is>
           <t>(e11)</t>
         </is>
@@ -4697,7 +4689,7 @@
         <f>SUM(T9:T15)</f>
         <v/>
       </c>
-      <c r="U16" s="235" t="inlineStr">
+      <c r="U16" s="234" t="inlineStr">
         <is>
           <t>(e12)</t>
         </is>
@@ -4713,7 +4705,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" ht="55.5" customHeight="1" s="244" thickBot="1">
+    <row r="17" ht="55.5" customHeight="1" s="286" thickBot="1">
       <c r="B17" s="10" t="n"/>
       <c r="C17" s="16" t="inlineStr">
         <is>
@@ -4749,10 +4741,10 @@
         <f>+F17-I17</f>
         <v/>
       </c>
-      <c r="L17" s="236" t="n"/>
+      <c r="L17" s="235" t="n"/>
       <c r="M17" s="62" t="n"/>
       <c r="N17" s="68" t="n"/>
-      <c r="O17" s="343" t="inlineStr">
+      <c r="O17" s="212" t="inlineStr">
         <is>
           <t>(c7)</t>
         </is>
@@ -4788,14 +4780,14 @@
         <v/>
       </c>
     </row>
-    <row r="18" ht="27.75" customHeight="1" s="244" thickBot="1" thickTop="1">
+    <row r="18" ht="27.75" customHeight="1" s="286" thickBot="1" thickTop="1">
       <c r="B18" s="10" t="n"/>
       <c r="C18" s="16" t="inlineStr">
         <is>
           <t>e10</t>
         </is>
       </c>
-      <c r="D18" s="308" t="inlineStr">
+      <c r="D18" s="331" t="inlineStr">
         <is>
           <t>TOTAL CASH FUNDS HELD BY CHURCH</t>
         </is>
@@ -4828,7 +4820,7 @@
         <f>SUM(Q16:Q17)</f>
         <v/>
       </c>
-      <c r="R18" s="237" t="inlineStr">
+      <c r="R18" s="236" t="inlineStr">
         <is>
           <t>(x)</t>
         </is>
@@ -4855,7 +4847,7 @@
       </c>
       <c r="Z18" s="25" t="n"/>
     </row>
-    <row r="19" ht="3.75" customHeight="1" s="244" thickBot="1" thickTop="1">
+    <row r="19" ht="3.75" customHeight="1" s="286" thickBot="1" thickTop="1">
       <c r="B19" s="10" t="n"/>
       <c r="C19" s="2" t="n"/>
       <c r="D19" s="49" t="n"/>
@@ -4878,7 +4870,7 @@
       <c r="U19" s="62" t="n"/>
       <c r="V19" s="53" t="n"/>
     </row>
-    <row r="20" ht="39.2" customHeight="1" s="244" thickBot="1">
+    <row r="20" ht="39.2" customHeight="1" s="286" thickBot="1">
       <c r="B20" s="10" t="n"/>
       <c r="C20" s="2" t="n"/>
       <c r="D20" s="193" t="inlineStr">
@@ -4887,12 +4879,12 @@
         </is>
       </c>
       <c r="E20" s="49" t="n"/>
-      <c r="F20" s="302" t="inlineStr">
+      <c r="F20" s="337" t="inlineStr">
         <is>
           <t>TOTAL RECEIPTS</t>
         </is>
       </c>
-      <c r="G20" s="303" t="n"/>
+      <c r="G20" s="338" t="n"/>
       <c r="H20" s="181" t="n"/>
       <c r="I20" s="207" t="inlineStr">
         <is>
@@ -4906,14 +4898,14 @@
       <c r="N20" s="49" t="n"/>
       <c r="O20" s="62" t="n"/>
       <c r="P20" s="62" t="n"/>
-      <c r="Q20" s="345" t="n"/>
-      <c r="R20" s="345" t="n"/>
-      <c r="S20" s="345" t="n"/>
-      <c r="T20" s="346" t="n"/>
-      <c r="U20" s="345" t="n"/>
-      <c r="V20" s="347" t="n"/>
-    </row>
-    <row r="21" ht="5.25" customHeight="1" s="244">
+      <c r="Q20" s="347" t="n"/>
+      <c r="R20" s="347" t="n"/>
+      <c r="S20" s="347" t="n"/>
+      <c r="T20" s="348" t="n"/>
+      <c r="U20" s="347" t="n"/>
+      <c r="V20" s="349" t="n"/>
+    </row>
+    <row r="21" ht="5.25" customHeight="1" s="286">
       <c r="B21" s="10" t="n"/>
       <c r="C21" s="2" t="n"/>
       <c r="D21" s="49" t="n"/>
@@ -4936,20 +4928,20 @@
       <c r="U21" s="62" t="n"/>
       <c r="V21" s="53" t="n"/>
     </row>
-    <row r="22" ht="3.2" customHeight="1" s="244" thickBot="1">
+    <row r="22" ht="3.2" customHeight="1" s="286" thickBot="1">
       <c r="B22" s="10" t="n"/>
       <c r="C22" s="15" t="n"/>
-      <c r="D22" s="348" t="n"/>
-      <c r="E22" s="348" t="n"/>
-      <c r="F22" s="348" t="n"/>
-      <c r="G22" s="348" t="n"/>
-      <c r="H22" s="348" t="n"/>
-      <c r="I22" s="348" t="n"/>
-      <c r="J22" s="348" t="n"/>
-      <c r="K22" s="348" t="n"/>
-      <c r="L22" s="348" t="n"/>
-      <c r="M22" s="349" t="n"/>
-      <c r="N22" s="349" t="n"/>
+      <c r="D22" s="350" t="n"/>
+      <c r="E22" s="350" t="n"/>
+      <c r="F22" s="350" t="n"/>
+      <c r="G22" s="350" t="n"/>
+      <c r="H22" s="350" t="n"/>
+      <c r="I22" s="350" t="n"/>
+      <c r="J22" s="350" t="n"/>
+      <c r="K22" s="350" t="n"/>
+      <c r="L22" s="350" t="n"/>
+      <c r="M22" s="351" t="n"/>
+      <c r="N22" s="351" t="n"/>
       <c r="O22" s="82" t="n"/>
       <c r="P22" s="82" t="n"/>
       <c r="Q22" s="82" t="n"/>
@@ -4959,20 +4951,20 @@
       <c r="U22" s="82" t="n"/>
       <c r="V22" s="53" t="n"/>
     </row>
-    <row r="23" ht="4.7" customHeight="1" s="244" thickTop="1">
+    <row r="23" ht="4.7" customHeight="1" s="286" thickTop="1">
       <c r="B23" s="10" t="n"/>
       <c r="C23" s="2" t="n"/>
-      <c r="D23" s="350" t="n"/>
-      <c r="E23" s="350" t="n"/>
-      <c r="F23" s="350" t="n"/>
-      <c r="G23" s="350" t="n"/>
-      <c r="H23" s="350" t="n"/>
-      <c r="I23" s="350" t="n"/>
-      <c r="J23" s="350" t="n"/>
-      <c r="K23" s="350" t="n"/>
-      <c r="L23" s="350" t="n"/>
-      <c r="M23" s="351" t="n"/>
-      <c r="N23" s="351" t="n"/>
+      <c r="D23" s="352" t="n"/>
+      <c r="E23" s="352" t="n"/>
+      <c r="F23" s="352" t="n"/>
+      <c r="G23" s="352" t="n"/>
+      <c r="H23" s="352" t="n"/>
+      <c r="I23" s="352" t="n"/>
+      <c r="J23" s="352" t="n"/>
+      <c r="K23" s="352" t="n"/>
+      <c r="L23" s="352" t="n"/>
+      <c r="M23" s="353" t="n"/>
+      <c r="N23" s="353" t="n"/>
       <c r="O23" s="62" t="n"/>
       <c r="P23" s="62" t="n"/>
       <c r="Q23" s="62" t="n"/>
@@ -4982,7 +4974,7 @@
       <c r="U23" s="62" t="n"/>
       <c r="V23" s="53" t="n"/>
     </row>
-    <row r="24" ht="23.25" customHeight="1" s="244" thickBot="1">
+    <row r="24" ht="23.25" customHeight="1" s="286" thickBot="1">
       <c r="B24" s="10" t="n"/>
       <c r="C24" s="2" t="n"/>
       <c r="D24" s="173" t="inlineStr">
@@ -4990,16 +4982,16 @@
           <t>SECTION F</t>
         </is>
       </c>
-      <c r="E24" s="350" t="n"/>
-      <c r="F24" s="350" t="n"/>
-      <c r="G24" s="350" t="n"/>
-      <c r="H24" s="350" t="n"/>
-      <c r="I24" s="350" t="n"/>
-      <c r="J24" s="350" t="n"/>
-      <c r="K24" s="350" t="n"/>
-      <c r="L24" s="350" t="n"/>
-      <c r="M24" s="350" t="n"/>
-      <c r="N24" s="350" t="n"/>
+      <c r="E24" s="352" t="n"/>
+      <c r="F24" s="352" t="n"/>
+      <c r="G24" s="352" t="n"/>
+      <c r="H24" s="352" t="n"/>
+      <c r="I24" s="352" t="n"/>
+      <c r="J24" s="352" t="n"/>
+      <c r="K24" s="352" t="n"/>
+      <c r="L24" s="352" t="n"/>
+      <c r="M24" s="352" t="n"/>
+      <c r="N24" s="352" t="n"/>
       <c r="O24" s="181" t="n"/>
       <c r="P24" s="181" t="n"/>
       <c r="Q24" s="181" t="n"/>
@@ -5009,7 +5001,7 @@
       <c r="U24" s="62" t="n"/>
       <c r="V24" s="53" t="n"/>
     </row>
-    <row r="25" ht="21.2" customHeight="1" s="244">
+    <row r="25" ht="21.2" customHeight="1" s="286">
       <c r="B25" s="10" t="n"/>
       <c r="C25" s="2" t="n"/>
       <c r="D25" s="195" t="inlineStr">
@@ -5036,9 +5028,9 @@
       <c r="U25" s="85" t="n"/>
       <c r="V25" s="53" t="n"/>
     </row>
-    <row r="26" ht="30.75" customHeight="1" s="244">
+    <row r="26" ht="30.75" customHeight="1" s="286">
       <c r="B26" s="10" t="n"/>
-      <c r="C26" s="292" t="n"/>
+      <c r="C26" s="311" t="n"/>
       <c r="D26" s="12" t="inlineStr">
         <is>
           <t>CHURCH - CASH FUNDS HELD at 31 August 2024</t>
@@ -5071,22 +5063,22 @@
       <c r="U26" s="39" t="n"/>
       <c r="V26" s="53" t="n"/>
     </row>
-    <row r="27" ht="24.75" customHeight="1" s="244">
+    <row r="27" ht="24.75" customHeight="1" s="286">
       <c r="B27" s="10" t="n"/>
       <c r="C27" s="5" t="inlineStr">
         <is>
           <t>f1</t>
         </is>
       </c>
-      <c r="D27" s="304" t="inlineStr">
+      <c r="D27" s="326" t="inlineStr">
         <is>
           <t>Cash in hand</t>
         </is>
       </c>
-      <c r="E27" s="250" t="n"/>
-      <c r="F27" s="250" t="n"/>
-      <c r="G27" s="250" t="n"/>
-      <c r="H27" s="282" t="n"/>
+      <c r="E27" s="298" t="n"/>
+      <c r="F27" s="298" t="n"/>
+      <c r="G27" s="298" t="n"/>
+      <c r="H27" s="304" t="n"/>
       <c r="I27" s="87" t="n"/>
       <c r="J27" s="49" t="n"/>
       <c r="K27" s="49" t="n"/>
@@ -5102,22 +5094,22 @@
       <c r="U27" s="93" t="n"/>
       <c r="V27" s="53" t="n"/>
     </row>
-    <row r="28" ht="24.75" customHeight="1" s="244">
+    <row r="28" ht="24.75" customHeight="1" s="286">
       <c r="B28" s="10" t="n"/>
       <c r="C28" s="5" t="inlineStr">
         <is>
           <t>f2</t>
         </is>
       </c>
-      <c r="D28" s="304" t="inlineStr">
+      <c r="D28" s="326" t="inlineStr">
         <is>
           <t>Bank Current Account</t>
         </is>
       </c>
-      <c r="E28" s="250" t="n"/>
-      <c r="F28" s="250" t="n"/>
-      <c r="G28" s="250" t="n"/>
-      <c r="H28" s="282" t="n"/>
+      <c r="E28" s="298" t="n"/>
+      <c r="F28" s="298" t="n"/>
+      <c r="G28" s="298" t="n"/>
+      <c r="H28" s="304" t="n"/>
       <c r="I28" s="93" t="n"/>
       <c r="J28" s="38" t="n"/>
       <c r="K28" s="38" t="n"/>
@@ -5133,22 +5125,22 @@
       <c r="U28" s="93" t="n"/>
       <c r="V28" s="53" t="n"/>
     </row>
-    <row r="29" ht="24.75" customHeight="1" s="244">
+    <row r="29" ht="24.75" customHeight="1" s="286">
       <c r="B29" s="10" t="n"/>
       <c r="C29" s="5" t="inlineStr">
         <is>
           <t>f3</t>
         </is>
       </c>
-      <c r="D29" s="304" t="inlineStr">
+      <c r="D29" s="326" t="inlineStr">
         <is>
           <t>Bank Deposit Account</t>
         </is>
       </c>
-      <c r="E29" s="250" t="n"/>
-      <c r="F29" s="250" t="n"/>
-      <c r="G29" s="250" t="n"/>
-      <c r="H29" s="282" t="n"/>
+      <c r="E29" s="298" t="n"/>
+      <c r="F29" s="298" t="n"/>
+      <c r="G29" s="298" t="n"/>
+      <c r="H29" s="304" t="n"/>
       <c r="I29" s="93" t="n"/>
       <c r="J29" s="38" t="n"/>
       <c r="K29" s="38" t="n"/>
@@ -5164,22 +5156,22 @@
       <c r="U29" s="93" t="n"/>
       <c r="V29" s="53" t="n"/>
     </row>
-    <row r="30" ht="24.75" customHeight="1" s="244">
+    <row r="30" ht="24.75" customHeight="1" s="286">
       <c r="B30" s="10" t="n"/>
       <c r="C30" s="5" t="inlineStr">
         <is>
           <t>f4</t>
         </is>
       </c>
-      <c r="D30" s="304" t="inlineStr">
+      <c r="D30" s="326" t="inlineStr">
         <is>
           <t>Central Finance Board</t>
         </is>
       </c>
-      <c r="E30" s="250" t="n"/>
-      <c r="F30" s="250" t="n"/>
-      <c r="G30" s="250" t="n"/>
-      <c r="H30" s="282" t="n"/>
+      <c r="E30" s="298" t="n"/>
+      <c r="F30" s="298" t="n"/>
+      <c r="G30" s="298" t="n"/>
+      <c r="H30" s="304" t="n"/>
       <c r="I30" s="93" t="n"/>
       <c r="J30" s="38" t="n"/>
       <c r="K30" s="38" t="n"/>
@@ -5195,22 +5187,22 @@
       <c r="U30" s="93" t="n"/>
       <c r="V30" s="53" t="n"/>
     </row>
-    <row r="31" ht="24.75" customHeight="1" s="244">
+    <row r="31" ht="24.75" customHeight="1" s="286">
       <c r="B31" s="9" t="n"/>
       <c r="C31" s="5" t="inlineStr">
         <is>
           <t>f5</t>
         </is>
       </c>
-      <c r="D31" s="304" t="inlineStr">
+      <c r="D31" s="326" t="inlineStr">
         <is>
           <t>Trustees for Methodist Church Purposes</t>
         </is>
       </c>
-      <c r="E31" s="250" t="n"/>
-      <c r="F31" s="250" t="n"/>
-      <c r="G31" s="250" t="n"/>
-      <c r="H31" s="282" t="n"/>
+      <c r="E31" s="298" t="n"/>
+      <c r="F31" s="298" t="n"/>
+      <c r="G31" s="298" t="n"/>
+      <c r="H31" s="304" t="n"/>
       <c r="I31" s="93" t="n"/>
       <c r="J31" s="38" t="n"/>
       <c r="K31" s="38" t="n"/>
@@ -5226,22 +5218,22 @@
       <c r="U31" s="93" t="n"/>
       <c r="V31" s="53" t="n"/>
     </row>
-    <row r="32" ht="24.75" customHeight="1" s="244" thickBot="1">
+    <row r="32" ht="24.75" customHeight="1" s="286" thickBot="1">
       <c r="B32" s="9" t="n"/>
       <c r="C32" s="5" t="inlineStr">
         <is>
           <t>f6</t>
         </is>
       </c>
-      <c r="D32" s="304" t="inlineStr">
+      <c r="D32" s="326" t="inlineStr">
         <is>
           <t>Other funds</t>
         </is>
       </c>
-      <c r="E32" s="250" t="n"/>
-      <c r="F32" s="250" t="n"/>
-      <c r="G32" s="250" t="n"/>
-      <c r="H32" s="282" t="n"/>
+      <c r="E32" s="298" t="n"/>
+      <c r="F32" s="298" t="n"/>
+      <c r="G32" s="298" t="n"/>
+      <c r="H32" s="304" t="n"/>
       <c r="I32" s="93" t="n"/>
       <c r="J32" s="38" t="n"/>
       <c r="K32" s="38" t="n"/>
@@ -5257,22 +5249,22 @@
       <c r="U32" s="97" t="n"/>
       <c r="V32" s="53" t="n"/>
     </row>
-    <row r="33" ht="30.2" customHeight="1" s="244">
+    <row r="33" ht="30.2" customHeight="1" s="286">
       <c r="B33" s="9" t="n"/>
       <c r="C33" s="5" t="inlineStr">
         <is>
           <t>f7</t>
         </is>
       </c>
-      <c r="D33" s="308" t="inlineStr">
+      <c r="D33" s="331" t="inlineStr">
         <is>
           <t xml:space="preserve">SUB TOTAL - Church accounts </t>
         </is>
       </c>
-      <c r="E33" s="250" t="n"/>
-      <c r="F33" s="250" t="n"/>
-      <c r="G33" s="250" t="n"/>
-      <c r="H33" s="282" t="n"/>
+      <c r="E33" s="298" t="n"/>
+      <c r="F33" s="298" t="n"/>
+      <c r="G33" s="298" t="n"/>
+      <c r="H33" s="304" t="n"/>
       <c r="I33" s="93" t="n"/>
       <c r="J33" s="38" t="n"/>
       <c r="K33" s="38" t="n"/>
@@ -5302,22 +5294,22 @@
       </c>
       <c r="V33" s="53" t="n"/>
     </row>
-    <row r="34" ht="32.25" customHeight="1" s="244" thickBot="1">
+    <row r="34" ht="32.25" customHeight="1" s="286" thickBot="1">
       <c r="B34" s="9" t="n"/>
       <c r="C34" s="5" t="inlineStr">
         <is>
           <t>f8</t>
         </is>
       </c>
-      <c r="D34" s="304" t="inlineStr">
+      <c r="D34" s="326" t="inlineStr">
         <is>
           <t>Total funds held by Internal Organisations (the closing balance total from above) (e12)</t>
         </is>
       </c>
-      <c r="E34" s="250" t="n"/>
-      <c r="F34" s="250" t="n"/>
-      <c r="G34" s="250" t="n"/>
-      <c r="H34" s="282" t="n"/>
+      <c r="E34" s="298" t="n"/>
+      <c r="F34" s="298" t="n"/>
+      <c r="G34" s="298" t="n"/>
+      <c r="H34" s="304" t="n"/>
       <c r="I34" s="93" t="n"/>
       <c r="J34" s="38" t="n"/>
       <c r="K34" s="38" t="n"/>
@@ -5357,22 +5349,22 @@
         </is>
       </c>
     </row>
-    <row r="35" ht="30.2" customHeight="1" s="244" thickBot="1" thickTop="1">
+    <row r="35" ht="30.2" customHeight="1" s="286" thickBot="1" thickTop="1">
       <c r="B35" s="9" t="n"/>
       <c r="C35" s="5" t="inlineStr">
         <is>
           <t>f9</t>
         </is>
       </c>
-      <c r="D35" s="308" t="inlineStr">
+      <c r="D35" s="331" t="inlineStr">
         <is>
           <t>TOTAL CASH FUNDS HELD BY CHURCH</t>
         </is>
       </c>
-      <c r="E35" s="250" t="n"/>
-      <c r="F35" s="250" t="n"/>
-      <c r="G35" s="250" t="n"/>
-      <c r="H35" s="282" t="n"/>
+      <c r="E35" s="298" t="n"/>
+      <c r="F35" s="298" t="n"/>
+      <c r="G35" s="298" t="n"/>
+      <c r="H35" s="304" t="n"/>
       <c r="I35" s="93" t="n"/>
       <c r="J35" s="38" t="n"/>
       <c r="K35" s="38" t="n"/>
@@ -5387,7 +5379,7 @@
           <t>(x)</t>
         </is>
       </c>
-      <c r="P35" s="238" t="n"/>
+      <c r="P35" s="237" t="n"/>
       <c r="Q35" s="49" t="n"/>
       <c r="R35" s="49" t="n"/>
       <c r="S35" s="38" t="n"/>
@@ -5415,7 +5407,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" ht="9" customHeight="1" s="244" thickBot="1" thickTop="1">
+    <row r="36" ht="9" customHeight="1" s="286" thickBot="1" thickTop="1">
       <c r="B36" s="9" t="n"/>
       <c r="C36" s="27" t="n"/>
       <c r="D36" s="199" t="n"/>
@@ -5438,9 +5430,9 @@
       <c r="U36" s="113" t="n"/>
       <c r="V36" s="53" t="n"/>
     </row>
-    <row r="37" ht="6.75" customHeight="1" s="244" thickTop="1">
+    <row r="37" ht="6.75" customHeight="1" s="286" thickTop="1">
       <c r="B37" s="9" t="n"/>
-      <c r="C37" s="292" t="n"/>
+      <c r="C37" s="311" t="n"/>
       <c r="D37" s="200" t="n"/>
       <c r="E37" s="200" t="n"/>
       <c r="F37" s="200" t="n"/>
@@ -5461,9 +5453,9 @@
       <c r="U37" s="115" t="n"/>
       <c r="V37" s="53" t="n"/>
     </row>
-    <row r="38" ht="23.25" customHeight="1" s="244" thickBot="1">
+    <row r="38" ht="23.25" customHeight="1" s="286" thickBot="1">
       <c r="B38" s="9" t="n"/>
-      <c r="C38" s="292" t="n"/>
+      <c r="C38" s="311" t="n"/>
       <c r="D38" s="173" t="inlineStr">
         <is>
           <t>SECTION G</t>
@@ -5496,9 +5488,9 @@
       <c r="U38" s="115" t="n"/>
       <c r="V38" s="53" t="n"/>
     </row>
-    <row r="39" ht="24" customHeight="1" s="244">
+    <row r="39" ht="24" customHeight="1" s="286">
       <c r="B39" s="9" t="n"/>
-      <c r="C39" s="292" t="n"/>
+      <c r="C39" s="311" t="n"/>
       <c r="D39" s="12" t="inlineStr">
         <is>
           <t>OTHER ASSETS and LIABILITIES</t>
@@ -5523,7 +5515,7 @@
       <c r="Q39" s="49" t="n"/>
       <c r="R39" s="49" t="n"/>
       <c r="S39" s="49" t="n"/>
-      <c r="T39" s="224" t="inlineStr">
+      <c r="T39" s="223" t="inlineStr">
         <is>
           <t>31 August 2024</t>
         </is>
@@ -5531,21 +5523,21 @@
       <c r="U39" s="49" t="n"/>
       <c r="V39" s="53" t="n"/>
     </row>
-    <row r="40" ht="30.2" customHeight="1" s="244">
+    <row r="40" ht="30.2" customHeight="1" s="286">
       <c r="B40" s="9" t="n"/>
       <c r="C40" s="5" t="inlineStr">
         <is>
           <t>g1</t>
         </is>
       </c>
-      <c r="D40" s="310" t="inlineStr">
+      <c r="D40" s="328" t="inlineStr">
         <is>
           <t>Investments (include Endowments)</t>
         </is>
       </c>
-      <c r="E40" s="250" t="n"/>
-      <c r="F40" s="250" t="n"/>
-      <c r="G40" s="231" t="n"/>
+      <c r="E40" s="298" t="n"/>
+      <c r="F40" s="298" t="n"/>
+      <c r="G40" s="230" t="n"/>
       <c r="H40" s="201" t="n"/>
       <c r="I40" s="117" t="n"/>
       <c r="J40" s="117" t="n"/>
@@ -5562,21 +5554,21 @@
       <c r="U40" s="121" t="n"/>
       <c r="V40" s="53" t="n"/>
     </row>
-    <row r="41" ht="32.25" customHeight="1" s="244">
+    <row r="41" ht="32.25" customHeight="1" s="286">
       <c r="B41" s="9" t="n"/>
       <c r="C41" s="5" t="inlineStr">
         <is>
           <t>g2</t>
         </is>
       </c>
-      <c r="D41" s="306" t="inlineStr">
+      <c r="D41" s="327" t="inlineStr">
         <is>
           <t>Land &amp; Buildings (see notes re Insurance value)</t>
         </is>
       </c>
-      <c r="E41" s="250" t="n"/>
-      <c r="F41" s="250" t="n"/>
-      <c r="G41" s="230" t="n"/>
+      <c r="E41" s="298" t="n"/>
+      <c r="F41" s="298" t="n"/>
+      <c r="G41" s="229" t="n"/>
       <c r="H41" s="202" t="n"/>
       <c r="I41" s="122" t="n"/>
       <c r="J41" s="122" t="n"/>
@@ -5593,21 +5585,21 @@
       <c r="U41" s="126" t="n"/>
       <c r="V41" s="53" t="n"/>
     </row>
-    <row r="42" ht="30.2" customHeight="1" s="244">
+    <row r="42" ht="30.2" customHeight="1" s="286">
       <c r="B42" s="9" t="n"/>
       <c r="C42" s="5" t="inlineStr">
         <is>
           <t>g3</t>
         </is>
       </c>
-      <c r="D42" s="306" t="inlineStr">
+      <c r="D42" s="327" t="inlineStr">
         <is>
           <t>Other Assets</t>
         </is>
       </c>
-      <c r="E42" s="230" t="n"/>
-      <c r="F42" s="230" t="n"/>
-      <c r="G42" s="230" t="n"/>
+      <c r="E42" s="229" t="n"/>
+      <c r="F42" s="229" t="n"/>
+      <c r="G42" s="229" t="n"/>
       <c r="H42" s="202" t="n"/>
       <c r="I42" s="122" t="n"/>
       <c r="J42" s="122" t="n"/>
@@ -5624,7 +5616,7 @@
       <c r="U42" s="126" t="n"/>
       <c r="V42" s="53" t="n"/>
     </row>
-    <row r="43" ht="30.2" customHeight="1" s="244">
+    <row r="43" ht="30.2" customHeight="1" s="286">
       <c r="A43" s="12" t="n"/>
       <c r="B43" s="13" t="n"/>
       <c r="C43" s="5" t="inlineStr">
@@ -5632,15 +5624,15 @@
           <t>g4</t>
         </is>
       </c>
-      <c r="D43" s="304" t="inlineStr">
+      <c r="D43" s="326" t="inlineStr">
         <is>
           <t>Loan(s) - show amount outstanding at year end</t>
         </is>
       </c>
-      <c r="E43" s="250" t="n"/>
-      <c r="F43" s="250" t="n"/>
-      <c r="G43" s="250" t="n"/>
-      <c r="H43" s="282" t="n"/>
+      <c r="E43" s="298" t="n"/>
+      <c r="F43" s="298" t="n"/>
+      <c r="G43" s="298" t="n"/>
+      <c r="H43" s="304" t="n"/>
       <c r="I43" s="127" t="n"/>
       <c r="J43" s="127" t="n"/>
       <c r="K43" s="127" t="n"/>
@@ -5656,21 +5648,21 @@
       <c r="U43" s="126" t="n"/>
       <c r="V43" s="53" t="n"/>
     </row>
-    <row r="44" ht="30.2" customHeight="1" s="244">
+    <row r="44" ht="30.2" customHeight="1" s="286">
       <c r="B44" s="9" t="n"/>
       <c r="C44" s="5" t="inlineStr">
         <is>
           <t>g5</t>
         </is>
       </c>
-      <c r="D44" s="306" t="inlineStr">
+      <c r="D44" s="327" t="inlineStr">
         <is>
           <t xml:space="preserve">Other  Liabilities                </t>
         </is>
       </c>
-      <c r="E44" s="250" t="n"/>
-      <c r="F44" s="250" t="n"/>
-      <c r="G44" s="230" t="n"/>
+      <c r="E44" s="298" t="n"/>
+      <c r="F44" s="298" t="n"/>
+      <c r="G44" s="229" t="n"/>
       <c r="H44" s="203" t="n"/>
       <c r="I44" s="45" t="n"/>
       <c r="J44" s="45" t="n"/>
@@ -5689,7 +5681,7 @@
     </row>
     <row r="45">
       <c r="B45" s="9" t="n"/>
-      <c r="C45" s="292" t="n"/>
+      <c r="C45" s="311" t="n"/>
       <c r="D45" s="38" t="n"/>
       <c r="E45" s="38" t="n"/>
       <c r="F45" s="38" t="n"/>
@@ -5710,7 +5702,7 @@
       <c r="U45" s="38" t="n"/>
       <c r="V45" s="53" t="n"/>
     </row>
-    <row r="46" ht="3.2" customHeight="1" s="244">
+    <row r="46" ht="3.2" customHeight="1" s="286">
       <c r="B46" s="9" t="n"/>
       <c r="D46" s="49" t="n"/>
       <c r="E46" s="49" t="n"/>
@@ -5734,7 +5726,7 @@
     </row>
     <row r="47">
       <c r="B47" s="9" t="n"/>
-      <c r="D47" s="309" t="inlineStr">
+      <c r="D47" s="325" t="inlineStr">
         <is>
           <t>f4 Include only Funds held at the Central Finance Board</t>
         </is>
@@ -5753,7 +5745,7 @@
     </row>
     <row r="48">
       <c r="B48" s="9" t="n"/>
-      <c r="D48" s="309" t="inlineStr">
+      <c r="D48" s="325" t="inlineStr">
         <is>
           <t>f5 Include only Funds held at Trustees for Methodist Church Purposes</t>
         </is>
@@ -5796,7 +5788,7 @@
       <c r="U49" s="49" t="n"/>
       <c r="V49" s="53" t="n"/>
     </row>
-    <row r="50" ht="3.2" customHeight="1" s="244">
+    <row r="50" ht="3.2" customHeight="1" s="286">
       <c r="B50" s="9" t="n"/>
       <c r="C50" s="9" t="n"/>
       <c r="D50" s="9" t="n"/>
@@ -5821,6 +5813,18 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="N2:S2"/>
+    <mergeCell ref="D7:T7"/>
+    <mergeCell ref="D5:T5"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="D27:H27"/>
+    <mergeCell ref="D29:H29"/>
+    <mergeCell ref="D3:T3"/>
+    <mergeCell ref="D41:F41"/>
+    <mergeCell ref="D6:T6"/>
+    <mergeCell ref="D33:H33"/>
+    <mergeCell ref="D35:H35"/>
+    <mergeCell ref="D28:H28"/>
     <mergeCell ref="D48:K48"/>
     <mergeCell ref="D30:H30"/>
     <mergeCell ref="D31:H31"/>
@@ -5830,18 +5834,6 @@
     <mergeCell ref="D47:K47"/>
     <mergeCell ref="D40:F40"/>
     <mergeCell ref="D43:H43"/>
-    <mergeCell ref="D29:H29"/>
-    <mergeCell ref="D3:T3"/>
-    <mergeCell ref="D41:F41"/>
-    <mergeCell ref="D6:T6"/>
-    <mergeCell ref="D33:H33"/>
-    <mergeCell ref="D35:H35"/>
-    <mergeCell ref="D28:H28"/>
-    <mergeCell ref="N2:S2"/>
-    <mergeCell ref="D7:T7"/>
-    <mergeCell ref="D5:T5"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="D27:H27"/>
   </mergeCells>
   <pageMargins left="0.1574803149606299" right="0.1574803149606299" top="0.2755905511811024" bottom="0.3543307086614174" header="0.1574803149606299" footer="0.1574803149606299"/>
   <pageSetup orientation="portrait" paperSize="9" scale="59"/>
@@ -5864,222 +5856,242 @@
   </sheetPr>
   <dimension ref="A2:K53"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I58" sqref="I57:I58"/>
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
   <sheetData>
-    <row r="2" ht="15" customHeight="1" s="244">
+    <row r="2" ht="15" customHeight="1" s="286">
       <c r="A2" s="216" t="inlineStr">
         <is>
           <t>Name of Church ……………………………………………………………  No………..</t>
         </is>
       </c>
       <c r="B2" s="12" t="n"/>
-      <c r="C2" s="12" t="n"/>
-      <c r="D2" s="12" t="n"/>
-      <c r="E2" s="12" t="n"/>
-      <c r="F2" s="12" t="n"/>
-      <c r="G2" s="12" t="n"/>
-      <c r="H2" s="12" t="n"/>
-      <c r="I2" s="12" t="n"/>
-    </row>
-    <row r="3" ht="15" customHeight="1" s="244">
+      <c r="C2" s="344">
+        <f>'P1 Front page'!$C$11</f>
+        <v/>
+      </c>
+      <c r="D2" s="342" t="n"/>
+      <c r="E2" s="342" t="n"/>
+      <c r="F2" s="342" t="n"/>
+      <c r="G2" s="342" t="n"/>
+      <c r="H2" s="342" t="n"/>
+      <c r="I2" s="342" t="n"/>
+      <c r="J2" s="342" t="n"/>
+      <c r="K2" s="342" t="n"/>
+    </row>
+    <row r="3" ht="15" customHeight="1" s="286">
       <c r="A3" s="216" t="n"/>
     </row>
-    <row r="4" ht="15" customHeight="1" s="244">
+    <row r="4" ht="15" customHeight="1" s="286">
       <c r="A4" s="216" t="n"/>
     </row>
-    <row r="5" ht="26.25" customHeight="1" s="244">
+    <row r="5" ht="26.25" customHeight="1" s="286">
       <c r="C5" s="220" t="inlineStr">
         <is>
           <t>Declarations and Scrutiny</t>
         </is>
       </c>
     </row>
-    <row r="6" ht="26.25" customHeight="1" s="244">
+    <row r="6" ht="26.25" customHeight="1" s="286">
       <c r="A6" s="217" t="n"/>
     </row>
-    <row r="7" ht="15" customHeight="1" s="244">
-      <c r="A7" s="311" t="inlineStr">
+    <row r="7" ht="15" customHeight="1" s="286">
+      <c r="A7" s="339" t="inlineStr">
         <is>
           <t>I confirm that these Receipt and Payment based accounts for the year to 31 August 2024 have been prepared from the records of the Church and that they include all funds under the control of the Church trustees.</t>
         </is>
       </c>
     </row>
-    <row r="8" ht="15" customHeight="1" s="244"/>
-    <row r="9" ht="15" customHeight="1" s="244"/>
-    <row r="10" ht="15" customHeight="1" s="244">
+    <row r="8" ht="15" customHeight="1" s="286"/>
+    <row r="9" ht="15" customHeight="1" s="286"/>
+    <row r="10" ht="15" customHeight="1" s="286">
       <c r="A10" s="216" t="n"/>
     </row>
-    <row r="11" ht="15" customHeight="1" s="244">
+    <row r="11" ht="15" customHeight="1" s="286">
       <c r="A11" s="216" t="n"/>
     </row>
-    <row r="12" ht="15" customHeight="1" s="244">
+    <row r="12" ht="15" customHeight="1" s="286">
       <c r="A12" s="216" t="inlineStr">
         <is>
           <t>Signature of treasurer ………………………………………………………   Date……………………..</t>
         </is>
       </c>
     </row>
-    <row r="13" ht="15" customHeight="1" s="244">
+    <row r="13" ht="15" customHeight="1" s="286">
       <c r="A13" s="216" t="n"/>
     </row>
-    <row r="14" ht="15" customHeight="1" s="244">
+    <row r="14" ht="15" customHeight="1" s="286">
       <c r="A14" s="216" t="inlineStr">
         <is>
           <t>Name and address of treasurer ………………………………………………………………………….</t>
         </is>
       </c>
-    </row>
-    <row r="15" ht="15" customHeight="1" s="244">
+      <c r="E14" s="343">
+        <f>'P1 Front page'!$C$36</f>
+        <v/>
+      </c>
+      <c r="F14" s="341" t="n"/>
+      <c r="G14" s="341" t="n"/>
+      <c r="H14" s="341" t="n"/>
+    </row>
+    <row r="15" ht="15" customHeight="1" s="286">
       <c r="A15" s="216" t="n"/>
     </row>
-    <row r="16" ht="15" customHeight="1" s="244">
+    <row r="16" ht="15" customHeight="1" s="286">
       <c r="A16" s="216" t="inlineStr">
         <is>
           <t>………………………………………………………………………………….  Post Code………………</t>
         </is>
       </c>
     </row>
-    <row r="17" ht="15" customHeight="1" s="244">
+    <row r="17" ht="15" customHeight="1" s="286">
       <c r="A17" s="216" t="n"/>
     </row>
-    <row r="18" ht="15" customHeight="1" s="244">
+    <row r="18" ht="15" customHeight="1" s="286">
       <c r="A18" s="216" t="n"/>
     </row>
-    <row r="19" ht="15.75" customHeight="1" s="244">
+    <row r="19" ht="15.75" customHeight="1" s="286">
       <c r="A19" s="218" t="inlineStr">
         <is>
           <t>Presentation to the Church trustees</t>
         </is>
       </c>
     </row>
-    <row r="20" ht="15.75" customHeight="1" s="244">
+    <row r="20" ht="15.75" customHeight="1" s="286">
       <c r="A20" s="218" t="n"/>
     </row>
-    <row r="21" ht="15" customHeight="1" s="244">
-      <c r="A21" s="311" t="inlineStr">
+    <row r="21" ht="15" customHeight="1" s="286">
+      <c r="A21" s="339" t="inlineStr">
         <is>
           <t>I confirm that the annual report and accounts for the year ended 31 August 2024 were/will be* presented to the meeting of the Church trustees held on ……………..</t>
         </is>
       </c>
     </row>
-    <row r="22" ht="15" customHeight="1" s="244"/>
-    <row r="23" ht="15" customHeight="1" s="244">
-      <c r="A23" s="311" t="n"/>
-      <c r="B23" s="311" t="n"/>
-      <c r="C23" s="311" t="n"/>
-      <c r="D23" s="311" t="n"/>
-      <c r="E23" s="311" t="n"/>
-      <c r="F23" s="311" t="n"/>
-      <c r="G23" s="311" t="n"/>
-      <c r="H23" s="311" t="n"/>
-      <c r="I23" s="311" t="n"/>
-      <c r="J23" s="311" t="n"/>
-      <c r="K23" s="311" t="n"/>
-    </row>
-    <row r="24" ht="15" customHeight="1" s="244">
+    <row r="22" ht="15" customHeight="1" s="286"/>
+    <row r="23" ht="15" customHeight="1" s="286">
+      <c r="A23" s="339" t="n"/>
+      <c r="B23" s="339" t="n"/>
+      <c r="C23" s="339" t="n"/>
+      <c r="D23" s="339" t="n"/>
+      <c r="E23" s="339" t="n"/>
+      <c r="F23" s="339" t="n"/>
+      <c r="G23" s="339" t="n"/>
+      <c r="H23" s="339" t="n"/>
+      <c r="I23" s="339" t="n"/>
+      <c r="J23" s="339" t="n"/>
+      <c r="K23" s="339" t="n"/>
+    </row>
+    <row r="24" ht="15" customHeight="1" s="286">
       <c r="A24" s="216" t="n"/>
     </row>
-    <row r="25" ht="15" customHeight="1" s="244">
+    <row r="25" ht="15" customHeight="1" s="286">
       <c r="A25" s="216" t="inlineStr">
         <is>
           <t>Signature of the Chair of the meeting  ……………………………………………………………………</t>
         </is>
       </c>
     </row>
-    <row r="26" ht="15" customHeight="1" s="244">
+    <row r="26" ht="15" customHeight="1" s="286">
       <c r="A26" s="216" t="n"/>
     </row>
-    <row r="27" ht="15" customHeight="1" s="244">
+    <row r="27" ht="15" customHeight="1" s="286">
       <c r="A27" s="216" t="inlineStr">
         <is>
           <t>Name of the Chair of the meeting  …………………………………………… Date ……………………</t>
         </is>
       </c>
-    </row>
-    <row r="28" ht="15" customHeight="1" s="244">
+      <c r="E27" s="343">
+        <f>'P1 Front page'!$C$24</f>
+        <v/>
+      </c>
+      <c r="F27" s="341" t="n"/>
+      <c r="G27" s="341" t="n"/>
+      <c r="H27" s="341" t="n"/>
+      <c r="I27" s="341" t="n"/>
+    </row>
+    <row r="28" ht="15" customHeight="1" s="286">
       <c r="A28" s="216" t="n"/>
     </row>
-    <row r="29" ht="15" customHeight="1" s="244">
+    <row r="29" ht="15" customHeight="1" s="286">
       <c r="A29" s="216" t="n"/>
     </row>
-    <row r="30" ht="15" customHeight="1" s="244">
+    <row r="30" ht="15" customHeight="1" s="286">
       <c r="A30" s="216" t="n"/>
     </row>
-    <row r="31" ht="15" customHeight="1" s="244">
+    <row r="31" ht="15" customHeight="1" s="286">
       <c r="A31" s="216" t="n"/>
     </row>
-    <row r="32" ht="15" customHeight="1" s="244">
+    <row r="32" ht="15" customHeight="1" s="286">
       <c r="A32" s="216" t="n"/>
     </row>
-    <row r="33" ht="18" customHeight="1" s="244">
+    <row r="33" ht="18" customHeight="1" s="286">
       <c r="C33" s="221" t="inlineStr">
         <is>
           <t xml:space="preserve">Independent Examiner’s Report to the Trustees of the </t>
         </is>
       </c>
     </row>
-    <row r="34" ht="18" customHeight="1" s="244">
+    <row r="34" ht="18" customHeight="1" s="286">
       <c r="A34" s="219" t="n"/>
     </row>
-    <row r="35" ht="18" customHeight="1" s="244">
+    <row r="35" ht="18" customHeight="1" s="286">
       <c r="D35" s="221" t="inlineStr">
         <is>
           <t>……………………..……………………..Church</t>
         </is>
       </c>
     </row>
-    <row r="36" ht="18" customHeight="1" s="244">
+    <row r="36" ht="18" customHeight="1" s="286">
       <c r="A36" s="219" t="n"/>
     </row>
-    <row r="37" ht="15.75" customHeight="1" s="244">
+    <row r="37" ht="15.75" customHeight="1" s="286">
       <c r="E37" s="222" t="inlineStr">
         <is>
           <t>Charity Number …………..</t>
         </is>
       </c>
     </row>
-    <row r="38" ht="15.75" customHeight="1" s="244">
+    <row r="38" ht="15.75" customHeight="1" s="286">
       <c r="A38" s="218" t="n"/>
     </row>
-    <row r="39" ht="15.75" customHeight="1" s="244">
+    <row r="39" ht="15.75" customHeight="1" s="286">
       <c r="A39" s="218" t="n"/>
     </row>
-    <row r="40" ht="15.75" customHeight="1" s="244">
+    <row r="40" ht="15.75" customHeight="1" s="286">
       <c r="A40" s="218" t="inlineStr">
         <is>
           <t>Responsibilities and basis of report</t>
         </is>
       </c>
     </row>
-    <row r="41" ht="15.75" customHeight="1" s="244">
+    <row r="41" ht="15.75" customHeight="1" s="286">
       <c r="A41" s="218" t="n"/>
     </row>
-    <row r="42" ht="15" customHeight="1" s="244">
-      <c r="A42" s="311" t="inlineStr">
+    <row r="42" ht="15" customHeight="1" s="286">
+      <c r="A42" s="339" t="inlineStr">
         <is>
           <t xml:space="preserve">I report to the trustees on my examination of the accounts of the …………………………………. Church for the year ended 31 August 2024 set out on pages … to ….  As the Church’s trustees, you are responsible for the preparation of the accounts in accordance with the requirements of the Charities Act 2011 (‘the Act’). </t>
         </is>
       </c>
     </row>
-    <row r="43" ht="15" customHeight="1" s="244"/>
-    <row r="44" ht="15" customHeight="1" s="244"/>
-    <row r="45" ht="15" customHeight="1" s="244"/>
-    <row r="46" ht="15" customHeight="1" s="244"/>
-    <row r="47" ht="12.75" customHeight="1" s="244">
-      <c r="A47" s="312" t="inlineStr">
+    <row r="43" ht="15" customHeight="1" s="286"/>
+    <row r="44" ht="15" customHeight="1" s="286"/>
+    <row r="45" ht="15" customHeight="1" s="286"/>
+    <row r="46" ht="15" customHeight="1" s="286"/>
+    <row r="47" ht="12.75" customHeight="1" s="286">
+      <c r="A47" s="340" t="inlineStr">
         <is>
           <t>I report in respect of my examination of the Church’s accounts carried out under section 145 of the Act and, in carrying out my examination, I have followed all the applicable Directions given by the Charity Commission under section 145(5)(b) of the Act.</t>
         </is>
       </c>
     </row>
-    <row r="48" ht="15" customHeight="1" s="244"/>
-    <row r="49" ht="15" customHeight="1" s="244"/>
+    <row r="48" ht="15" customHeight="1" s="286"/>
+    <row r="49" ht="15" customHeight="1" s="286"/>
     <row r="50"/>
-    <row r="53" ht="15" customHeight="1" s="244">
+    <row r="53" ht="15" customHeight="1" s="286">
       <c r="A53" s="216" t="inlineStr">
         <is>
           <t>* delete or circle as appropriate</t>
@@ -6114,200 +6126,210 @@
   </sheetPr>
   <dimension ref="A2:J47"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
   <cols>
-    <col width="9.140625" customWidth="1" style="244" min="8" max="9"/>
-    <col width="15" customWidth="1" style="244" min="10" max="10"/>
+    <col width="9.140625" customWidth="1" style="286" min="8" max="9"/>
+    <col width="15" customWidth="1" style="286" min="10" max="10"/>
   </cols>
   <sheetData>
-    <row r="2" ht="15" customHeight="1" s="244">
+    <row r="2" ht="15" customHeight="1" s="286">
       <c r="A2" s="216" t="inlineStr">
         <is>
           <t>Name of Church …………………………………………………………………………  No ………….</t>
         </is>
       </c>
     </row>
-    <row r="3" ht="15" customHeight="1" s="244">
+    <row r="3" ht="15" customHeight="1" s="286">
       <c r="A3" s="216" t="n"/>
     </row>
-    <row r="4" ht="15" customHeight="1" s="244">
+    <row r="4" ht="15" customHeight="1" s="286">
       <c r="A4" s="216" t="n"/>
     </row>
-    <row r="5" ht="15.75" customHeight="1" s="244">
+    <row r="5" ht="15.75" customHeight="1" s="286">
       <c r="A5" s="218" t="inlineStr">
         <is>
           <t>Independent Examiner’s Statement</t>
         </is>
       </c>
     </row>
-    <row r="6" ht="15.75" customHeight="1" s="244">
+    <row r="6" ht="15.75" customHeight="1" s="286">
       <c r="A6" s="218" t="n"/>
     </row>
-    <row r="7" ht="15" customHeight="1" s="244">
-      <c r="A7" s="311" t="inlineStr">
+    <row r="7" ht="15" customHeight="1" s="286">
+      <c r="A7" s="339" t="inlineStr">
         <is>
           <t>I have completed my examination.  I confirm that no material matters have come to my attention in connection with the examination (other than that disclosed below*) which give me cause to believe that in, any material respect:</t>
         </is>
       </c>
     </row>
-    <row r="8" ht="15" customHeight="1" s="244"/>
-    <row r="9" ht="15" customHeight="1" s="244"/>
-    <row r="10" ht="15" customHeight="1" s="244"/>
-    <row r="11" ht="15" customHeight="1" s="244">
+    <row r="8" ht="15" customHeight="1" s="286"/>
+    <row r="9" ht="15" customHeight="1" s="286"/>
+    <row r="10" ht="15" customHeight="1" s="286"/>
+    <row r="11" ht="15" customHeight="1" s="286">
       <c r="A11" s="216" t="n"/>
     </row>
-    <row r="12" ht="15.75" customHeight="1" s="244">
-      <c r="A12" s="223" t="inlineStr">
-        <is>
-          <t xml:space="preserve">·         the accounting records were not kept in accordance with section 130 of the Act; or </t>
-        </is>
-      </c>
-    </row>
-    <row r="13" ht="15.75" customHeight="1" s="244">
-      <c r="A13" s="223" t="inlineStr">
-        <is>
-          <t>·         the accounts do not accord with the accounting records.</t>
-        </is>
-      </c>
-    </row>
-    <row r="14" ht="15" customHeight="1" s="244">
+    <row r="12" ht="15.75" customHeight="1" s="286">
+      <c r="A12" s="345" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> £</t>
+        </is>
+      </c>
+      <c r="B12" s="117" t="inlineStr">
+        <is>
+          <t xml:space="preserve">the accounting records were not kept in accordance with section 130 of the Act; or </t>
+        </is>
+      </c>
+    </row>
+    <row r="13" ht="15.75" customHeight="1" s="286">
+      <c r="A13" s="345" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> £</t>
+        </is>
+      </c>
+      <c r="B13" s="117" t="inlineStr">
+        <is>
+          <t>the accounts do not accord with the accounting records.</t>
+        </is>
+      </c>
+    </row>
+    <row r="14" ht="15" customHeight="1" s="286">
       <c r="A14" s="216" t="n"/>
     </row>
-    <row r="15" ht="15" customHeight="1" s="244">
+    <row r="15" ht="15" customHeight="1" s="286">
       <c r="A15" s="216" t="n"/>
     </row>
-    <row r="16" ht="15" customHeight="1" s="244">
-      <c r="A16" s="312" t="inlineStr">
+    <row r="16" ht="15" customHeight="1" s="286">
+      <c r="A16" s="340" t="inlineStr">
         <is>
           <t>I have no concerns and have come across no other matters in connection with the examination to which attention should be drawn in this report in order to enable a proper understanding of the accounts to be reached.</t>
         </is>
       </c>
     </row>
-    <row r="17" ht="15" customHeight="1" s="244"/>
-    <row r="18" ht="15" customHeight="1" s="244"/>
-    <row r="19" ht="15" customHeight="1" s="244">
+    <row r="17" ht="15" customHeight="1" s="286"/>
+    <row r="18" ht="15" customHeight="1" s="286"/>
+    <row r="19" ht="15" customHeight="1" s="286">
       <c r="A19" s="216" t="n"/>
     </row>
-    <row r="20" ht="15" customHeight="1" s="244">
-      <c r="A20" s="311" t="inlineStr">
+    <row r="20" ht="15" customHeight="1" s="286">
+      <c r="A20" s="339" t="inlineStr">
         <is>
           <t>I have/have not* obtained independent verification of all investments with the Trustees for Methodist Church Purposes or held in other trusts, bank balances and funds at the Central Finance Board of the Methodist Church which are individually in excess of £10,000 (ten thousand pounds) at the balance sheet date.</t>
         </is>
       </c>
     </row>
-    <row r="21" ht="15" customHeight="1" s="244"/>
-    <row r="22" ht="15" customHeight="1" s="244"/>
-    <row r="23" ht="15" customHeight="1" s="244"/>
-    <row r="24" ht="15" customHeight="1" s="244"/>
-    <row r="25" ht="15" customHeight="1" s="244">
+    <row r="21" ht="15" customHeight="1" s="286"/>
+    <row r="22" ht="15" customHeight="1" s="286"/>
+    <row r="23" ht="15" customHeight="1" s="286"/>
+    <row r="24" ht="15" customHeight="1" s="286"/>
+    <row r="25" ht="15" customHeight="1" s="286">
       <c r="A25" s="216" t="n"/>
     </row>
-    <row r="26" ht="15" customHeight="1" s="244">
+    <row r="26" ht="15" customHeight="1" s="286">
       <c r="A26" s="216" t="n"/>
     </row>
-    <row r="27" ht="15" customHeight="1" s="244">
+    <row r="27" ht="15" customHeight="1" s="286">
       <c r="A27" s="216" t="inlineStr">
         <is>
           <t>Signature of independent examiner   ………………………………………………………………….</t>
         </is>
       </c>
     </row>
-    <row r="28" ht="15" customHeight="1" s="244">
+    <row r="28" ht="15" customHeight="1" s="286">
       <c r="A28" s="216" t="n"/>
     </row>
-    <row r="29" ht="15" customHeight="1" s="244">
+    <row r="29" ht="15" customHeight="1" s="286">
       <c r="A29" s="216" t="inlineStr">
         <is>
           <t>Name of independent examiner  ……………………………………………………………………….</t>
         </is>
       </c>
     </row>
-    <row r="30" ht="15" customHeight="1" s="244">
+    <row r="30" ht="15" customHeight="1" s="286">
       <c r="A30" s="216" t="n"/>
     </row>
-    <row r="31" ht="15" customHeight="1" s="244">
+    <row r="31" ht="15" customHeight="1" s="286">
       <c r="A31" s="216" t="inlineStr">
         <is>
           <t>Relevant professional qualification of independent examiner  ………………………………………</t>
         </is>
       </c>
     </row>
-    <row r="32" ht="15" customHeight="1" s="244">
+    <row r="32" ht="15" customHeight="1" s="286">
       <c r="A32" s="216" t="n"/>
     </row>
-    <row r="33" ht="15" customHeight="1" s="244">
+    <row r="33" ht="15" customHeight="1" s="286">
       <c r="A33" s="216" t="n"/>
     </row>
-    <row r="34" ht="15" customHeight="1" s="244">
+    <row r="34" ht="15" customHeight="1" s="286">
       <c r="A34" s="216" t="inlineStr">
         <is>
           <t>Name of firm (where appropriate)  ………………………………………………………………………</t>
         </is>
       </c>
     </row>
-    <row r="35" ht="15" customHeight="1" s="244">
+    <row r="35" ht="15" customHeight="1" s="286">
       <c r="A35" s="216" t="n"/>
     </row>
-    <row r="36" ht="15" customHeight="1" s="244">
+    <row r="36" ht="15" customHeight="1" s="286">
       <c r="A36" s="216" t="inlineStr">
         <is>
           <t>Address  ……………………………………………………………………………………………………</t>
         </is>
       </c>
     </row>
-    <row r="37" ht="15" customHeight="1" s="244">
+    <row r="37" ht="15" customHeight="1" s="286">
       <c r="A37" s="216" t="n"/>
     </row>
-    <row r="38" ht="15" customHeight="1" s="244">
+    <row r="38" ht="15" customHeight="1" s="286">
       <c r="A38" s="216" t="inlineStr">
         <is>
           <t>………………………………………………………………………………..  Post Code  ………………</t>
         </is>
       </c>
     </row>
-    <row r="39" ht="15" customHeight="1" s="244">
+    <row r="39" ht="15" customHeight="1" s="286">
       <c r="A39" s="216" t="n"/>
     </row>
-    <row r="40" ht="15" customHeight="1" s="244">
+    <row r="40" ht="15" customHeight="1" s="286">
       <c r="A40" s="216" t="inlineStr">
         <is>
           <t>Date  …………………………………………</t>
         </is>
       </c>
     </row>
-    <row r="41" ht="15" customHeight="1" s="244">
+    <row r="41" ht="15" customHeight="1" s="286">
       <c r="A41" s="216" t="n"/>
     </row>
-    <row r="42" ht="15" customHeight="1" s="244">
+    <row r="42" ht="15" customHeight="1" s="286">
       <c r="A42" s="216" t="n"/>
     </row>
-    <row r="43" ht="15" customHeight="1" s="244">
+    <row r="43" ht="15" customHeight="1" s="286">
       <c r="A43" s="216" t="n"/>
     </row>
-    <row r="44" ht="15" customHeight="1" s="244">
+    <row r="44" ht="15" customHeight="1" s="286">
       <c r="A44" s="216" t="n"/>
     </row>
-    <row r="45" ht="15" customHeight="1" s="244">
+    <row r="45" ht="15" customHeight="1" s="286">
       <c r="A45" s="216" t="inlineStr">
         <is>
           <t>*  delete or circle as appropriate</t>
         </is>
       </c>
     </row>
-    <row r="46" ht="15" customHeight="1" s="244">
+    <row r="46" ht="15" customHeight="1" s="286">
       <c r="A46" s="216" t="n"/>
     </row>
     <row r="47">
-      <c r="A47" s="225" t="inlineStr">
+      <c r="A47" s="224" t="inlineStr">
         <is>
           <t>Form Reviewed</t>
         </is>
       </c>
-      <c r="B47" s="226" t="n">
+      <c r="B47" s="225" t="n">
         <v>45505</v>
       </c>
     </row>
@@ -6328,283 +6350,4 @@
     <firstFooter/>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D25"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
-  <cols>
-    <col width="19.42578125" customWidth="1" style="244" min="2" max="2"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="242" t="inlineStr">
-        <is>
-          <t>Unnamed: 0</t>
-        </is>
-      </c>
-      <c r="B1" s="242" t="inlineStr">
-        <is>
-          <t>Unnamed: 1</t>
-        </is>
-      </c>
-      <c r="C1" s="242" t="inlineStr">
-        <is>
-          <t>Unnamed: 2</t>
-        </is>
-      </c>
-      <c r="D1" s="242" t="inlineStr">
-        <is>
-          <t>Unnamed: 3</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Briggswath &amp; Sleights Methodist Church</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>circuit</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> North Yorkshire Coast Circuit</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>district</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Yorkshire North and East</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>number</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> 29/31</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Role</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>minister</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Gareth Phillips</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>steward1</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Ann North</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>steward2</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Dennis Buck</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>steward3</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Peter Brown</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>steward4</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Sally Wardell</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>treasurer</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Ann Brown</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Total offering (including gift aid)</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="B16" t="n">
-        <v>2025</v>
-      </c>
-      <c r="C16" t="n">
-        <v>3553.8</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Bank</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Balance</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>Interest</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>CFB</t>
-        </is>
-      </c>
-      <c r="C19" t="n">
-        <v>71</v>
-      </c>
-      <c r="D19" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>TMCP</t>
-        </is>
-      </c>
-      <c r="C20" t="n">
-        <v>156291.9</v>
-      </c>
-      <c r="D20" t="n">
-        <v>4480</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>HSBC</t>
-        </is>
-      </c>
-      <c r="C21" t="n">
-        <v>11350</v>
-      </c>
-      <c r="D21" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>LETTINGS</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Church Lets</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>amount</t>
-        </is>
-      </c>
-      <c r="D24" t="n">
-        <v>561.9</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Cottage Rents</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>rent</t>
-        </is>
-      </c>
-      <c r="D25" t="n">
-        <v>7840</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>